<commit_message>
Refine presets categories and remove chance always
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -197,7 +197,7 @@
     <ns0:row r="4">
       <ns0:c r="A4" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>CSM</ns0:t>
+          <ns0:t>Presets</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B4" t="inlineStr" s="2">
@@ -234,7 +234,7 @@
     <ns0:row r="5">
       <ns0:c r="A5" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM</ns0:t>
+          <ns0:t>Presets</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B5" t="inlineStr" s="0">
@@ -271,86 +271,86 @@
     <ns0:row r="6">
       <ns0:c r="A6" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B6" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third Person Distribution</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C6" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D6" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>First Person Only</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E6" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>First Person Only | Mixed (Rare Third Person) | Mixed | Mostly Third Person | Third Person Only</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F6" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CameraDistributionProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G6" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Controls how often third-person killcam appears when Camera Mode is Default.</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="7">
-      <ns0:c r="A7" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B7" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Camera Mode</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C7" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D7" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Default (Preset)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E7" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Default (Preset) | First Person Only | Third Person Only</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F7" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CameraModeProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G7" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Default = Third Person Distribution decides. First Person only disables killcam. Third Person only forces third-person killcam when eligible.</ns0:t>
+      <ns0:c r="A7" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Preset Settings</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B7" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C7" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D7" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E7" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F7" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G7" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="8">
       <ns0:c r="A8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM</ns0:t>
+          <ns0:t>Preset Settings</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Intensity Preset</ns0:t>
+          <ns0:t>Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C8" t="inlineStr" s="0">
@@ -360,34 +360,34 @@
       </ns0:c>
       <ns0:c r="D8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Balanced</ns0:t>
+          <ns0:t>First Person Only</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Subtle | Balanced | Dramatic | Cinematic | Epic</ns0:t>
+          <ns0:t>First Person Only | Mixed (Rare Third Person) | Mixed | Mostly Third Person | Third Person Only</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>PresetProvider</ns0:t>
+          <ns0:t>CameraDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Intensity profile. Subtle = brief, Balanced = default, Dramatic = stronger, Cinematic = dramatic, Epic = extreme</ns0:t>
+          <ns0:t>Controls how often third-person killcam appears when Camera Mode is Default.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="9">
       <ns0:c r="A9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM</ns0:t>
+          <ns0:t>Preset Settings</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance Preset</ns0:t>
+          <ns0:t>Camera Mode</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C9" t="inlineStr" s="0">
@@ -397,34 +397,34 @@
       </ns0:c>
       <ns0:c r="D9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (Cooldown Only)</ns0:t>
+          <ns0:t>Default (Preset)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (Cooldown Only) | Rare | Balanced | Frequent | Always (100%)</ns0:t>
+          <ns0:t>Default (Preset) | First Person Only | Third Person Only</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ChancePresetProvider</ns0:t>
+          <ns0:t>CameraModeProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger chance values. Off means chance is ignored (cooldown only).</ns0:t>
+          <ns0:t>Default = Third Person Distribution decides. First Person only disables killcam. Third Person only forces third-person killcam when eligible.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="10">
       <ns0:c r="A10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM</ns0:t>
+          <ns0:t>Preset Settings</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown Preset</ns0:t>
+          <ns0:t>Intensity Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C10" t="inlineStr" s="0">
@@ -439,29 +439,29 @@
       </ns0:c>
       <ns0:c r="E10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (No Cooldown) | Short | Balanced | Long | Extended</ns0:t>
+          <ns0:t>Subtle | Balanced | Dramatic | Cinematic | Epic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CooldownPresetProvider</ns0:t>
+          <ns0:t>PresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger cooldown values. Off disables cooldown.</ns0:t>
+          <ns0:t>Intensity profile. Subtle = brief, Balanced = default, Dramatic = stronger, Cinematic = dramatic, Epic = extreme</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="11">
       <ns0:c r="A11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM</ns0:t>
+          <ns0:t>Preset Settings</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration Preset</ns0:t>
+          <ns0:t>Chance Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C11" t="inlineStr" s="0">
@@ -471,34 +471,34 @@
       </ns0:c>
       <ns0:c r="D11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Balanced</ns0:t>
+          <ns0:t>Off (Cooldown Only)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Short | Balanced | Long | Extended</ns0:t>
+          <ns0:t>Off (Cooldown Only) | Rare | Balanced | Frequent</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>DurationPresetProvider</ns0:t>
+          <ns0:t>ChancePresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger duration values.</ns0:t>
+          <ns0:t>Sets per-trigger chance values. Off means chance is ignored (cooldown only).</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="12">
       <ns0:c r="A12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM</ns0:t>
+          <ns0:t>Preset Settings</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smoothness Preset</ns0:t>
+          <ns0:t>Cooldown Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C12" t="inlineStr" s="0">
@@ -513,29 +513,29 @@
       </ns0:c>
       <ns0:c r="E12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Very Snappy | Snappy | Balanced | Smooth | Cinematic | Ultra Smooth</ns0:t>
+          <ns0:t>Off (No Cooldown) | Short | Balanced | Long | Extended</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>CooldownPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger transition speed values (lower = smoother).</ns0:t>
+          <ns0:t>Sets per-trigger cooldown values. Off disables cooldown.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="13">
       <ns0:c r="A13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM</ns0:t>
+          <ns0:t>Preset Settings</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger Profile</ns0:t>
+          <ns0:t>Duration Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C13" t="inlineStr" s="0">
@@ -545,34 +545,34 @@
       </ns0:c>
       <ns0:c r="D13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>All Triggers</ns0:t>
+          <ns0:t>Balanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only</ns0:t>
+          <ns0:t>Short | Balanced | Long | Extended</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerProfileProvider</ns0:t>
+          <ns0:t>DurationPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
+          <ns0:t>Sets per-trigger duration values.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="14">
       <ns0:c r="A14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM</ns0:t>
+          <ns0:t>Preset Settings</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Cooldown</ns0:t>
+          <ns0:t>Smoothness Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C14" t="inlineStr" s="0">
@@ -582,34 +582,34 @@
       </ns0:c>
       <ns0:c r="D14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3s</ns0:t>
+          <ns0:t>Balanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
+          <ns0:t>Very Snappy | Snappy | Balanced | Smooth | Cinematic | Ultra Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CooldownProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
+          <ns0:t>Sets per-trigger transition speed values (lower = smoother).</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="15">
       <ns0:c r="A15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM</ns0:t>
+          <ns0:t>Preset Settings</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Smoothing</ns0:t>
+          <ns0:t>Trigger Profile</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C15" t="inlineStr" s="0">
@@ -619,108 +619,108 @@
       </ns0:c>
       <ns0:c r="D15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger</ns0:t>
+          <ns0:t>All Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
+          <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>GlobalSmoothingProvider</ns0:t>
+          <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Override transition speed for all triggers. Per Trigger uses per-trigger smoothing (plus Smoothness Preset).</ns0:t>
+          <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="16">
       <ns0:c r="A16" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B16" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Haptic Feedback</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C16" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D16" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Medium</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E16" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F16" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>HapticIntensityProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G16" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="17">
-      <ns0:c r="A17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Dynamic Intensity</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Scale intensity based on damage dealt</ns0:t>
+      <ns0:c r="A17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Global Overrides</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="18">
       <ns0:c r="A18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM</ns0:t>
+          <ns0:t>Global Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Threshold</ns0:t>
+          <ns0:t>Global Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="0">
@@ -730,34 +730,34 @@
       </ns0:c>
       <ns0:c r="D18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
+          <ns0:t>3s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t>CooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
+          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM</ns0:t>
+          <ns0:t>Global Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Min Group</ns0:t>
+          <ns0:t>Global Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="0">
@@ -767,118 +767,118 @@
       </ns0:c>
       <ns0:c r="D19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 enemies</ns0:t>
+          <ns0:t>Per Trigger</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
+          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>MinEnemyGroupProvider</ns0:t>
+          <ns0:t>GlobalSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Minimum enemies in wave for Last Enemy to trigger</ns0:t>
+          <ns0:t>Override transition speed for all triggers. Per Trigger uses per-trigger smoothing (plus Smoothness Preset).</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Global Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Haptic Feedback</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Medium</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off | Light | Medium | Strong</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>HapticIntensityProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
-      <ns0:c r="A21" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B21" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C21" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D21" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E21" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F21" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G21" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Global Overrides</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Dynamic Intensity</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Scale intensity based on damage dealt</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
       <ns0:c r="A22" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B22" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Kill</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C22" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D22" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E22" t="inlineStr" s="0">
@@ -893,155 +893,155 @@
       </ns0:c>
       <ns0:c r="G22" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="23">
-      <ns0:c r="A23" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B23" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C23" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D23" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E23" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F23" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G23" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+      <ns0:c r="A23" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Trigger Conditions</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B23" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C23" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D23" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E23" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F23" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G23" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="24">
       <ns0:c r="A24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>Trigger Conditions</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismemberment</ns0:t>
+          <ns0:t>Last Stand Threshold</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>15%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B25" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C25" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D25" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E25" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F25" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G25" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="26">
+      <ns0:c r="A26" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B25" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C25" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D25" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E25" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F25" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G25" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="26">
-      <ns0:c r="A26" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B26" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C26" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D26" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E26" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F26" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G26" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+      <ns0:c r="B26" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C26" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D26" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E26" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F26" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G26" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1053,7 +1053,7 @@
       </ns0:c>
       <ns0:c r="B27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand</ns0:t>
+          <ns0:t>Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C27" t="inlineStr" s="0">
@@ -1078,7 +1078,7 @@
       </ns0:c>
       <ns0:c r="G27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1090,7 +1090,7 @@
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry</ns0:t>
+          <ns0:t>Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C28" t="inlineStr" s="0">
@@ -1115,29 +1115,29 @@
       </ns0:c>
       <ns0:c r="G28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on successful weapon deflections</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="29">
       <ns0:c r="A29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E29" t="inlineStr" s="0">
@@ -1152,56 +1152,56 @@
       </ns0:c>
       <ns0:c r="G29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="30">
-      <ns0:c r="A30" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B30" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C30" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D30" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E30" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F30" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G30" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Triggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="31">
       <ns0:c r="A31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Enable Killcam</ns0:t>
+          <ns0:t>Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C31" t="inlineStr" s="0">
@@ -1211,7 +1211,7 @@
       </ns0:c>
       <ns0:c r="D31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E31" t="inlineStr" s="0">
@@ -1226,155 +1226,155 @@
       </ns0:c>
       <ns0:c r="G31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>WARNING: May cause VR motion sickness</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="32">
       <ns0:c r="A32" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B32" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera Distance</ns0:t>
+          <ns0:t>Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C32" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D32" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3m</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E32" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F32" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G32" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="33">
       <ns0:c r="A33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera Height</ns0:t>
+          <ns0:t>Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Trigger on successful weapon deflections</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="34">
       <ns0:c r="A34" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B34" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C34" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D34" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E34" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F34" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G34" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="35">
+      <ns0:c r="A35" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Orbit Speed</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="35">
-      <ns0:c r="A35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>On Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Trigger killcam on decapitation kills</ns0:t>
+      <ns0:c r="B35" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C35" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D35" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E35" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F35" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G35" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1386,7 +1386,7 @@
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On Critical Kill</ns0:t>
+          <ns0:t>Enable Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="0">
@@ -1396,7 +1396,7 @@
       </ns0:c>
       <ns0:c r="D36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E36" t="inlineStr" s="0">
@@ -1411,7 +1411,7 @@
       </ns0:c>
       <ns0:c r="G36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger killcam on critical (head/neck) kills</ns0:t>
+          <ns0:t>WARNING: May cause VR motion sickness</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1423,32 +1423,32 @@
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On Last Enemy</ns0:t>
+          <ns0:t>Camera Distance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>3m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger killcam when killing the last enemy</ns0:t>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1460,289 +1460,291 @@
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Show Player Body</ns0:t>
+          <ns0:t>Camera Height</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>1.5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Show player body during killcam (third-person view)</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="39">
       <ns0:c r="A39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Orbit Speed</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="40">
-      <ns0:c r="A40" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B40" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C40" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D40" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E40" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F40" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G40" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Killcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>On Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Trigger killcam on decapitation kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="41">
       <ns0:c r="A41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Chance</ns0:t>
+          <ns0:t>On Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>25%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Trigger killcam on critical (head/neck) kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="42">
       <ns0:c r="A42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Time Scale</ns0:t>
+          <ns0:t>On Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.35x</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Trigger killcam when killing the last enemy</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="43">
       <ns0:c r="A43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Duration</ns0:t>
+          <ns0:t>Show Player Body</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.0s</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Show player body during killcam (third-person view)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="44">
       <ns0:c r="A44" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B44" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C44" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D44" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E44" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F44" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G44" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="45">
+      <ns0:c r="A45" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B44" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Basic Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C44" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D44" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>5.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E44" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F44" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G44" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="45">
-      <ns0:c r="A45" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B45" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Basic Smoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C45" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D45" s="0">
-        <ns0:v>8</ns0:v>
-      </ns0:c>
-      <ns0:c r="E45" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F45" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G45" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+      <ns0:c r="B45" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C45" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D45" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E45" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F45" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G45" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1754,7 +1756,7 @@
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Third Person Distribution</ns0:t>
+          <ns0:t>Basic Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C46" t="inlineStr" s="0">
@@ -1764,108 +1766,108 @@
       </ns0:c>
       <ns0:c r="D46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>25%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="47">
       <ns0:c r="A47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Basic Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.35x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="48">
-      <ns0:c r="A48" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B48" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C48" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D48" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E48" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F48" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G48" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Basic Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomDurationProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="49">
       <ns0:c r="A49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Chance</ns0:t>
+          <ns0:t>Basic Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C49" t="inlineStr" s="0">
@@ -1875,34 +1877,34 @@
       </ns0:c>
       <ns0:c r="D49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>75%</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="50">
       <ns0:c r="A50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Time Scale</ns0:t>
+          <ns0:t>Basic Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C50" t="inlineStr" s="0">
@@ -1910,36 +1912,34 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.25x</ns0:t>
-        </ns0:is>
+      <ns0:c r="D50" s="0">
+        <ns0:v>8</ns0:v>
       </ns0:c>
       <ns0:c r="E50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="51">
       <ns0:c r="A51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Duration</ns0:t>
+          <ns0:t>Basic Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C51" t="inlineStr" s="0">
@@ -1949,94 +1949,96 @@
       </ns0:c>
       <ns0:c r="D51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="52">
       <ns0:c r="A52" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B52" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C52" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D52" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E52" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F52" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G52" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="53">
+      <ns0:c r="A53" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B52" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Critical Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C52" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D52" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>5.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E52" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F52" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G52" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="53">
-      <ns0:c r="A53" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B53" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Critical Smoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C53" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D53" s="0">
-        <ns0:v>8</ns0:v>
-      </ns0:c>
-      <ns0:c r="E53" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F53" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G53" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+      <ns0:c r="B53" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C53" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D53" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E53" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F53" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G53" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2048,7 +2050,7 @@
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Third Person Distribution</ns0:t>
+          <ns0:t>Critical Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C54" t="inlineStr" s="0">
@@ -2058,108 +2060,108 @@
       </ns0:c>
       <ns0:c r="D54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>75%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="55">
       <ns0:c r="A55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Critical Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="56">
-      <ns0:c r="A56" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B56" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C56" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D56" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E56" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F56" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G56" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Critical Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Critical Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomDurationProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="57">
       <ns0:c r="A57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Chance</ns0:t>
+          <ns0:t>Critical Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C57" t="inlineStr" s="0">
@@ -2169,34 +2171,34 @@
       </ns0:c>
       <ns0:c r="D57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>60%</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="58">
       <ns0:c r="A58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Time Scale</ns0:t>
+          <ns0:t>Critical Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C58" t="inlineStr" s="0">
@@ -2204,36 +2206,34 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D58" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.30x</ns0:t>
-        </ns0:is>
+      <ns0:c r="D58" s="0">
+        <ns0:v>8</ns0:v>
       </ns0:c>
       <ns0:c r="E58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="59">
       <ns0:c r="A59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Duration</ns0:t>
+          <ns0:t>Critical Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C59" t="inlineStr" s="0">
@@ -2243,94 +2243,96 @@
       </ns0:c>
       <ns0:c r="D59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="60">
       <ns0:c r="A60" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="61">
+      <ns0:c r="A61" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B60" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Dismember Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C60" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D60" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>5.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E60" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F60" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G60" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="61">
-      <ns0:c r="A61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Dismember Smoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D61" s="0">
-        <ns0:v>8</ns0:v>
-      </ns0:c>
-      <ns0:c r="E61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+      <ns0:c r="B61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2342,7 +2344,7 @@
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Third Person Distribution</ns0:t>
+          <ns0:t>Dismember Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C62" t="inlineStr" s="0">
@@ -2352,108 +2354,108 @@
       </ns0:c>
       <ns0:c r="D62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>60%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="63">
       <ns0:c r="A63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Dismember Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.30x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="64">
-      <ns0:c r="A64" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B64" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C64" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D64" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E64" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F64" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G64" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Dismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Dismember Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomDurationProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="65">
       <ns0:c r="A65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Chance</ns0:t>
+          <ns0:t>Dismember Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="0">
@@ -2463,34 +2465,34 @@
       </ns0:c>
       <ns0:c r="D65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>90%</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="66">
       <ns0:c r="A66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Time Scale</ns0:t>
+          <ns0:t>Dismember Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="0">
@@ -2498,36 +2500,34 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D66" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.20x</ns0:t>
-        </ns0:is>
+      <ns0:c r="D66" s="0">
+        <ns0:v>8</ns0:v>
       </ns0:c>
       <ns0:c r="E66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="67">
       <ns0:c r="A67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Duration</ns0:t>
+          <ns0:t>Dismember Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C67" t="inlineStr" s="0">
@@ -2537,94 +2537,96 @@
       </ns0:c>
       <ns0:c r="D67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="68">
       <ns0:c r="A68" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B68" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C68" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D68" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E68" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F68" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G68" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="69">
+      <ns0:c r="A69" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B68" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Decapitation Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C68" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D68" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>4.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E68" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F68" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G68" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="69">
-      <ns0:c r="A69" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B69" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Decapitation Smoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C69" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D69" s="0">
-        <ns0:v>6</ns0:v>
-      </ns0:c>
-      <ns0:c r="E69" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F69" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G69" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+      <ns0:c r="B69" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C69" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D69" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E69" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F69" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G69" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2636,7 +2638,7 @@
       </ns0:c>
       <ns0:c r="B70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Third Person Distribution</ns0:t>
+          <ns0:t>Decapitation Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C70" t="inlineStr" s="0">
@@ -2646,108 +2648,108 @@
       </ns0:c>
       <ns0:c r="D70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>90%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="71">
       <ns0:c r="A71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Decapitation Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="72">
-      <ns0:c r="A72" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B72" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C72" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D72" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E72" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F72" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G72" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Decapitation Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomDurationProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="73">
       <ns0:c r="A73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Chance</ns0:t>
+          <ns0:t>Decapitation Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C73" t="inlineStr" s="0">
@@ -2757,34 +2759,34 @@
       </ns0:c>
       <ns0:c r="D73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>100%</ns0:t>
+          <ns0:t>4.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="74">
       <ns0:c r="A74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Time Scale</ns0:t>
+          <ns0:t>Decapitation Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C74" t="inlineStr" s="0">
@@ -2792,36 +2794,34 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D74" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.20x</ns0:t>
-        </ns0:is>
+      <ns0:c r="D74" s="0">
+        <ns0:v>6</ns0:v>
       </ns0:c>
       <ns0:c r="E74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="75">
       <ns0:c r="A75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Duration</ns0:t>
+          <ns0:t>Decapitation Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="0">
@@ -2831,94 +2831,96 @@
       </ns0:c>
       <ns0:c r="D75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="76">
       <ns0:c r="A76" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B76" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C76" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D76" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E76" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F76" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G76" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="77">
+      <ns0:c r="A77" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B76" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Enemy Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C76" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D76" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E76" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F76" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G76" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="77">
-      <ns0:c r="A77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Enemy Smoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D77" s="0">
-        <ns0:v>4</ns0:v>
-      </ns0:c>
-      <ns0:c r="E77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+      <ns0:c r="B77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2930,7 +2932,7 @@
       </ns0:c>
       <ns0:c r="B78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Third Person Distribution</ns0:t>
+          <ns0:t>Last Enemy Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C78" t="inlineStr" s="0">
@@ -2940,108 +2942,108 @@
       </ns0:c>
       <ns0:c r="D78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="79">
       <ns0:c r="A79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Last Enemy Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="80">
-      <ns0:c r="A80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Enemy Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>3.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomDurationProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="81">
       <ns0:c r="A81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Time Scale</ns0:t>
+          <ns0:t>Last Enemy Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="0">
@@ -3051,34 +3053,34 @@
       </ns0:c>
       <ns0:c r="D81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.15x</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="82">
       <ns0:c r="A82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Duration</ns0:t>
+          <ns0:t>Last Enemy Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="0">
@@ -3086,36 +3088,34 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D82" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>5.0s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D82" s="0">
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="E82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="83">
       <ns0:c r="A83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Cooldown</ns0:t>
+          <ns0:t>Last Enemy Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="0">
@@ -3125,143 +3125,145 @@
       </ns0:c>
       <ns0:c r="D83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>45.0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="84">
       <ns0:c r="A84" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="85">
+      <ns0:c r="A85" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Stand Smoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D84" s="0">
-        <ns0:v>4</ns0:v>
-      </ns0:c>
-      <ns0:c r="E84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="85">
-      <ns0:c r="A85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G85" t="inlineStr" s="0">
+      <ns0:c r="B85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G85" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="86">
-      <ns0:c r="A86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Stand Time Scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.15x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="87">
       <ns0:c r="A87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Chance</ns0:t>
+          <ns0:t>Last Stand Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C87" t="inlineStr" s="0">
@@ -3271,34 +3273,34 @@
       </ns0:c>
       <ns0:c r="D87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>50%</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="88">
       <ns0:c r="A88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Time Scale</ns0:t>
+          <ns0:t>Last Stand Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="0">
@@ -3308,34 +3310,34 @@
       </ns0:c>
       <ns0:c r="D88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.30x</ns0:t>
+          <ns0:t>45.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
       <ns0:c r="A89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Duration</ns0:t>
+          <ns0:t>Last Stand Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C89" t="inlineStr" s="0">
@@ -3343,205 +3345,388 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D89" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1.2s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D89" s="0">
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="E89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="90">
       <ns0:c r="A90" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="91">
+      <ns0:c r="A91" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Parry Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>7.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="91">
-      <ns0:c r="A91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Parry Smoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D91" s="0">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+      <ns0:c r="B91" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C91" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D91" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E91" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F91" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G91" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="92">
       <ns0:c r="A92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Parry Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>50%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="93">
-      <ns0:c r="A93" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B93" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C93" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D93" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E93" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F93" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G93" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Parry Time Scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.30x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="94">
       <ns0:c r="A94" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t>Custom: Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B94" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Parry Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C94" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D94" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.2s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E94" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F94" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomDurationProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G94" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="95">
+      <ns0:c r="A95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Parry Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>7.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomCooldownProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="96">
+      <ns0:c r="A96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Parry Smoothing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D96" s="0">
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Transition speed</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="97">
+      <ns0:c r="A97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="98">
+      <ns0:c r="A98" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CSM Advanced</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B94" t="inlineStr" s="0">
+      <ns0:c r="B98" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C98" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D98" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E98" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F98" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G98" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="99">
+      <ns0:c r="A99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B99" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Debug Logging</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C94" t="inlineStr" s="0">
+      <ns0:c r="C99" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D94" t="inlineStr" s="0">
+      <ns0:c r="D99" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E94" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F94" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G94" t="inlineStr" s="0">
+      <ns0:c r="E99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G99" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
@@ -3626,7 +3811,7 @@
       </ns0:c>
       <ns0:c r="B6" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (Cooldown Only) | Rare | Balanced | Frequent | Always (100%)</ns0:t>
+          <ns0:t>Off (Cooldown Only) | Rare | Balanced | Frequent</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Move Last Stand threshold into triggers
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -900,7 +900,7 @@
     <ns0:row r="23">
       <ns0:c r="A23" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>Trigger Conditions</ns0:t>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="2">
@@ -937,59 +937,59 @@
     <ns0:row r="24">
       <ns0:c r="A24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger Conditions</ns0:t>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Threshold</ns0:t>
+          <ns0:t>Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E25" t="inlineStr" s="0">
@@ -1004,44 +1004,44 @@
       </ns0:c>
       <ns0:c r="G25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="26">
-      <ns0:c r="A26" t="inlineStr" s="2">
+      <ns0:c r="A26" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B26" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C26" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D26" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E26" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F26" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G26" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Dismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1053,7 +1053,7 @@
       </ns0:c>
       <ns0:c r="B27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Kill</ns0:t>
+          <ns0:t>Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C27" t="inlineStr" s="0">
@@ -1078,7 +1078,7 @@
       </ns0:c>
       <ns0:c r="G27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1090,7 +1090,7 @@
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Kill</ns0:t>
+          <ns0:t>Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C28" t="inlineStr" s="0">
@@ -1115,7 +1115,7 @@
       </ns0:c>
       <ns0:c r="G28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1127,7 +1127,7 @@
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismemberment</ns0:t>
+          <ns0:t>Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C29" t="inlineStr" s="0">
@@ -1152,7 +1152,7 @@
       </ns0:c>
       <ns0:c r="G29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1164,32 +1164,32 @@
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation</ns0:t>
+          <ns0:t>Last Stand Threshold</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>15%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1201,7 +1201,7 @@
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy</ns0:t>
+          <ns0:t>Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C31" t="inlineStr" s="0">
@@ -1226,29 +1226,29 @@
       </ns0:c>
       <ns0:c r="G31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+          <ns0:t>Trigger on successful weapon deflections</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="32">
       <ns0:c r="A32" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B32" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C32" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D32" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E32" t="inlineStr" s="0">
@@ -1263,66 +1263,66 @@
       </ns0:c>
       <ns0:c r="G32" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="33">
-      <ns0:c r="A33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Trigger on successful weapon deflections</ns0:t>
+      <ns0:c r="A33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CSM Killcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="34">
       <ns0:c r="A34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Enable Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E34" t="inlineStr" s="0">
@@ -1337,44 +1337,44 @@
       </ns0:c>
       <ns0:c r="G34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>WARNING: May cause VR motion sickness</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="35">
-      <ns0:c r="A35" t="inlineStr" s="2">
+      <ns0:c r="A35" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B35" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C35" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D35" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E35" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F35" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G35" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Camera Distance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>3m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1386,32 +1386,32 @@
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Enable Killcam</ns0:t>
+          <ns0:t>Camera Height</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>1.5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>WARNING: May cause VR motion sickness</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1423,7 +1423,7 @@
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera Distance</ns0:t>
+          <ns0:t>Orbit Speed</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C37" t="inlineStr" s="0">
@@ -1433,22 +1433,22 @@
       </ns0:c>
       <ns0:c r="D37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3m</ns0:t>
+          <ns0:t>Slow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
+          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1460,32 +1460,32 @@
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera Height</ns0:t>
+          <ns0:t>On Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Trigger killcam on decapitation kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1497,32 +1497,32 @@
       </ns0:c>
       <ns0:c r="B39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Orbit Speed</ns0:t>
+          <ns0:t>On Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slow</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
+          <ns0:t>Trigger killcam on critical (head/neck) kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1534,7 +1534,7 @@
       </ns0:c>
       <ns0:c r="B40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On Decapitation</ns0:t>
+          <ns0:t>On Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C40" t="inlineStr" s="0">
@@ -1559,7 +1559,7 @@
       </ns0:c>
       <ns0:c r="G40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger killcam on decapitation kills</ns0:t>
+          <ns0:t>Trigger killcam when killing the last enemy</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1571,7 +1571,7 @@
       </ns0:c>
       <ns0:c r="B41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On Critical Kill</ns0:t>
+          <ns0:t>Show Player Body</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C41" t="inlineStr" s="0">
@@ -1596,29 +1596,29 @@
       </ns0:c>
       <ns0:c r="G41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger killcam on critical (head/neck) kills</ns0:t>
+          <ns0:t>Show player body during killcam (third-person view)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="42">
       <ns0:c r="A42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On Last Enemy</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E42" t="inlineStr" s="0">
@@ -1633,118 +1633,118 @@
       </ns0:c>
       <ns0:c r="G42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger killcam when killing the last enemy</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="43">
-      <ns0:c r="A43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Show Player Body</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Show player body during killcam (third-person view)</ns0:t>
+      <ns0:c r="A43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="44">
       <ns0:c r="A44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Basic Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>25%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="45">
-      <ns0:c r="A45" t="inlineStr" s="2">
+      <ns0:c r="A45" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B45" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C45" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D45" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E45" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F45" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G45" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Basic Time Scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.35x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1756,7 +1756,7 @@
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Chance</ns0:t>
+          <ns0:t>Basic Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C46" t="inlineStr" s="0">
@@ -1766,22 +1766,22 @@
       </ns0:c>
       <ns0:c r="D46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>25%</ns0:t>
+          <ns0:t>1.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1793,7 +1793,7 @@
       </ns0:c>
       <ns0:c r="B47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Time Scale</ns0:t>
+          <ns0:t>Basic Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C47" t="inlineStr" s="0">
@@ -1803,22 +1803,22 @@
       </ns0:c>
       <ns0:c r="D47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.35x</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1830,7 +1830,7 @@
       </ns0:c>
       <ns0:c r="B48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Duration</ns0:t>
+          <ns0:t>Basic Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C48" t="inlineStr" s="0">
@@ -1838,24 +1838,22 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D48" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1.0s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D48" s="0">
+        <ns0:v>8</ns0:v>
       </ns0:c>
       <ns0:c r="E48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1867,7 +1865,7 @@
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Cooldown</ns0:t>
+          <ns0:t>Basic Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C49" t="inlineStr" s="0">
@@ -1877,168 +1875,170 @@
       </ns0:c>
       <ns0:c r="D49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="50">
       <ns0:c r="A50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Smoothing</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D50" s="0">
-        <ns0:v>8</ns0:v>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D50" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="51">
-      <ns0:c r="A51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Basic Third Person Distribution</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+      <ns0:c r="A51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Critical Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="52">
       <ns0:c r="A52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Critical Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>75%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="53">
-      <ns0:c r="A53" t="inlineStr" s="2">
+      <ns0:c r="A53" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B53" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C53" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D53" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E53" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F53" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G53" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Critical Time Scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.25x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2050,7 +2050,7 @@
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Chance</ns0:t>
+          <ns0:t>Critical Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C54" t="inlineStr" s="0">
@@ -2060,22 +2060,22 @@
       </ns0:c>
       <ns0:c r="D54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>75%</ns0:t>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2087,7 +2087,7 @@
       </ns0:c>
       <ns0:c r="B55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Time Scale</ns0:t>
+          <ns0:t>Critical Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C55" t="inlineStr" s="0">
@@ -2097,22 +2097,22 @@
       </ns0:c>
       <ns0:c r="D55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.25x</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2124,7 +2124,7 @@
       </ns0:c>
       <ns0:c r="B56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Duration</ns0:t>
+          <ns0:t>Critical Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C56" t="inlineStr" s="0">
@@ -2132,24 +2132,22 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D56" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1.5s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D56" s="0">
+        <ns0:v>8</ns0:v>
       </ns0:c>
       <ns0:c r="E56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2161,7 +2159,7 @@
       </ns0:c>
       <ns0:c r="B57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Cooldown</ns0:t>
+          <ns0:t>Critical Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C57" t="inlineStr" s="0">
@@ -2171,168 +2169,170 @@
       </ns0:c>
       <ns0:c r="D57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="58">
       <ns0:c r="A58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Smoothing</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D58" s="0">
-        <ns0:v>8</ns0:v>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D58" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="59">
-      <ns0:c r="A59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Critical Third Person Distribution</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+      <ns0:c r="A59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Dismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="60">
       <ns0:c r="A60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Dismember Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>60%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="61">
-      <ns0:c r="A61" t="inlineStr" s="2">
+      <ns0:c r="A61" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Dismember Time Scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.30x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2344,7 +2344,7 @@
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Chance</ns0:t>
+          <ns0:t>Dismember Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C62" t="inlineStr" s="0">
@@ -2354,22 +2354,22 @@
       </ns0:c>
       <ns0:c r="D62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>60%</ns0:t>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2381,7 +2381,7 @@
       </ns0:c>
       <ns0:c r="B63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Time Scale</ns0:t>
+          <ns0:t>Dismember Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C63" t="inlineStr" s="0">
@@ -2391,22 +2391,22 @@
       </ns0:c>
       <ns0:c r="D63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.30x</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2418,7 +2418,7 @@
       </ns0:c>
       <ns0:c r="B64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Duration</ns0:t>
+          <ns0:t>Dismember Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C64" t="inlineStr" s="0">
@@ -2426,24 +2426,22 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D64" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1.5s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D64" s="0">
+        <ns0:v>8</ns0:v>
       </ns0:c>
       <ns0:c r="E64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2455,7 +2453,7 @@
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Cooldown</ns0:t>
+          <ns0:t>Dismember Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="0">
@@ -2465,168 +2463,170 @@
       </ns0:c>
       <ns0:c r="D65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="66">
       <ns0:c r="A66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Smoothing</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D66" s="0">
-        <ns0:v>8</ns0:v>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="67">
-      <ns0:c r="A67" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B67" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Dismember Third Person Distribution</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C67" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D67" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E67" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F67" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G67" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+      <ns0:c r="A67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="68">
       <ns0:c r="A68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Decapitation Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>90%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="69">
-      <ns0:c r="A69" t="inlineStr" s="2">
+      <ns0:c r="A69" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B69" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C69" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D69" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E69" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F69" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G69" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Decapitation Time Scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.20x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2638,7 +2638,7 @@
       </ns0:c>
       <ns0:c r="B70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Chance</ns0:t>
+          <ns0:t>Decapitation Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C70" t="inlineStr" s="0">
@@ -2648,22 +2648,22 @@
       </ns0:c>
       <ns0:c r="D70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>90%</ns0:t>
+          <ns0:t>2.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2675,7 +2675,7 @@
       </ns0:c>
       <ns0:c r="B71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Time Scale</ns0:t>
+          <ns0:t>Decapitation Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C71" t="inlineStr" s="0">
@@ -2685,22 +2685,22 @@
       </ns0:c>
       <ns0:c r="D71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.20x</ns0:t>
+          <ns0:t>4.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2712,7 +2712,7 @@
       </ns0:c>
       <ns0:c r="B72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Duration</ns0:t>
+          <ns0:t>Decapitation Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C72" t="inlineStr" s="0">
@@ -2720,24 +2720,22 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D72" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2.0s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D72" s="0">
+        <ns0:v>6</ns0:v>
       </ns0:c>
       <ns0:c r="E72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2749,7 +2747,7 @@
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Cooldown</ns0:t>
+          <ns0:t>Decapitation Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C73" t="inlineStr" s="0">
@@ -2759,168 +2757,170 @@
       </ns0:c>
       <ns0:c r="D73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4.0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="74">
       <ns0:c r="A74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Smoothing</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D74" s="0">
-        <ns0:v>6</ns0:v>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D74" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="75">
-      <ns0:c r="A75" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B75" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Decapitation Third Person Distribution</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C75" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D75" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E75" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F75" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G75" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+      <ns0:c r="A75" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B75" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C75" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D75" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E75" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F75" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G75" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="76">
       <ns0:c r="A76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Last Enemy Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="77">
-      <ns0:c r="A77" t="inlineStr" s="2">
+      <ns0:c r="A77" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B77" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C77" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D77" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E77" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F77" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G77" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B77" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Enemy Time Scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C77" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D77" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.20x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E77" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F77" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G77" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2932,7 +2932,7 @@
       </ns0:c>
       <ns0:c r="B78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Chance</ns0:t>
+          <ns0:t>Last Enemy Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C78" t="inlineStr" s="0">
@@ -2942,22 +2942,22 @@
       </ns0:c>
       <ns0:c r="D78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>100%</ns0:t>
+          <ns0:t>3.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2969,7 +2969,7 @@
       </ns0:c>
       <ns0:c r="B79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Time Scale</ns0:t>
+          <ns0:t>Last Enemy Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C79" t="inlineStr" s="0">
@@ -2979,22 +2979,22 @@
       </ns0:c>
       <ns0:c r="D79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.20x</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3006,7 +3006,7 @@
       </ns0:c>
       <ns0:c r="B80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Duration</ns0:t>
+          <ns0:t>Last Enemy Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C80" t="inlineStr" s="0">
@@ -3014,24 +3014,22 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>3.0s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D80" s="0">
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="E80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3043,7 +3041,7 @@
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Cooldown</ns0:t>
+          <ns0:t>Last Enemy Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="0">
@@ -3053,168 +3051,170 @@
       </ns0:c>
       <ns0:c r="D81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="82">
       <ns0:c r="A82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Smoothing</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D82" s="0">
-        <ns0:v>4</ns0:v>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D82" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="83">
-      <ns0:c r="A83" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B83" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Enemy Third Person Distribution</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C83" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D83" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E83" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F83" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G83" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+      <ns0:c r="A83" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B83" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C83" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D83" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E83" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F83" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G83" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="84">
       <ns0:c r="A84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Last Stand Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.15x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="85">
-      <ns0:c r="A85" t="inlineStr" s="2">
+      <ns0:c r="A85" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Stand Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>5.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomDurationProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3226,7 +3226,7 @@
       </ns0:c>
       <ns0:c r="B86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Time Scale</ns0:t>
+          <ns0:t>Last Stand Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C86" t="inlineStr" s="0">
@@ -3236,22 +3236,22 @@
       </ns0:c>
       <ns0:c r="D86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.15x</ns0:t>
+          <ns0:t>45.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3263,7 +3263,7 @@
       </ns0:c>
       <ns0:c r="B87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Duration</ns0:t>
+          <ns0:t>Last Stand Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C87" t="inlineStr" s="0">
@@ -3271,170 +3271,170 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D87" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>5.0s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D87" s="0">
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="E87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="88">
       <ns0:c r="A88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Cooldown</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>45.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
-      <ns0:c r="A89" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B89" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Stand Smoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C89" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D89" s="0">
-        <ns0:v>4</ns0:v>
-      </ns0:c>
-      <ns0:c r="E89" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F89" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G89" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+      <ns0:c r="A89" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B89" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C89" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D89" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E89" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F89" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G89" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="90">
       <ns0:c r="A90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Parry Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>50%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="91">
-      <ns0:c r="A91" t="inlineStr" s="2">
+      <ns0:c r="A91" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B91" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C91" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D91" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E91" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F91" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G91" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Parry Time Scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.30x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3446,7 +3446,7 @@
       </ns0:c>
       <ns0:c r="B92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Chance</ns0:t>
+          <ns0:t>Parry Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C92" t="inlineStr" s="0">
@@ -3456,22 +3456,22 @@
       </ns0:c>
       <ns0:c r="D92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>50%</ns0:t>
+          <ns0:t>1.2s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3483,7 +3483,7 @@
       </ns0:c>
       <ns0:c r="B93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Time Scale</ns0:t>
+          <ns0:t>Parry Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C93" t="inlineStr" s="0">
@@ -3493,22 +3493,22 @@
       </ns0:c>
       <ns0:c r="D93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.30x</ns0:t>
+          <ns0:t>7.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3520,7 +3520,7 @@
       </ns0:c>
       <ns0:c r="B94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Duration</ns0:t>
+          <ns0:t>Parry Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C94" t="inlineStr" s="0">
@@ -3528,118 +3528,118 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D94" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1.2s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D94" s="0">
+        <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="E94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="95">
       <ns0:c r="A95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Cooldown</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>7.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="96">
-      <ns0:c r="A96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Parry Smoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D96" s="0">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+      <ns0:c r="A96" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B96" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C96" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D96" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E96" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F96" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G96" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="97">
       <ns0:c r="A97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CSM Advanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Debug Logging</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E97" t="inlineStr" s="0">
@@ -3653,80 +3653,6 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="G97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="98">
-      <ns0:c r="A98" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B98" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C98" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D98" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E98" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F98" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G98" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="99">
-      <ns0:c r="A99" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B99" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Debug Logging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C99" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D99" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E99" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F99" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G99" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>

</xml_diff>

<commit_message>
Streamline presets, optional overrides, and killcam settings
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -308,7 +308,7 @@
     <ns0:row r="7">
       <ns0:c r="A7" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>Preset Settings</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B7" t="inlineStr" s="2">
@@ -345,7 +345,7 @@
     <ns0:row r="8">
       <ns0:c r="A8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Settings</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B8" t="inlineStr" s="0">
@@ -375,19 +375,19 @@
       </ns0:c>
       <ns0:c r="G8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Controls how often third-person killcam appears when Camera Mode is Default.</ns0:t>
+          <ns0:t>Controls how often third-person killcam appears.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="9">
       <ns0:c r="A9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Settings</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera Mode</ns0:t>
+          <ns0:t>Intensity Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C9" t="inlineStr" s="0">
@@ -397,34 +397,34 @@
       </ns0:c>
       <ns0:c r="D9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Default (Preset)</ns0:t>
+          <ns0:t>Standard</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Default (Preset) | First Person Only | Third Person Only</ns0:t>
+          <ns0:t>Subtle | Standard | Dramatic | Cinematic | Epic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CameraModeProvider</ns0:t>
+          <ns0:t>PresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Default = Third Person Distribution decides. First Person only disables killcam. Third Person only forces third-person killcam when eligible.</ns0:t>
+          <ns0:t>Intensity profile. Subtle = brief, Standard = default, Dramatic = stronger, Cinematic = dramatic, Epic = extreme</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="10">
       <ns0:c r="A10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Settings</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Intensity Preset</ns0:t>
+          <ns0:t>Chance Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C10" t="inlineStr" s="0">
@@ -434,34 +434,34 @@
       </ns0:c>
       <ns0:c r="D10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Balanced</ns0:t>
+          <ns0:t>Off (Cooldown Only)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Subtle | Balanced | Dramatic | Cinematic | Epic</ns0:t>
+          <ns0:t>Off (Cooldown Only) | Rare | Standard | Frequent</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>PresetProvider</ns0:t>
+          <ns0:t>ChancePresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Intensity profile. Subtle = brief, Balanced = default, Dramatic = stronger, Cinematic = dramatic, Epic = extreme</ns0:t>
+          <ns0:t>Sets per-trigger chance values. Off means chance is ignored (cooldown only).</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="11">
       <ns0:c r="A11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Settings</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance Preset</ns0:t>
+          <ns0:t>Cooldown Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C11" t="inlineStr" s="0">
@@ -471,34 +471,34 @@
       </ns0:c>
       <ns0:c r="D11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (Cooldown Only)</ns0:t>
+          <ns0:t>Standard</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (Cooldown Only) | Rare | Balanced | Frequent</ns0:t>
+          <ns0:t>Off (No Cooldown) | Short | Standard | Long | Extended</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ChancePresetProvider</ns0:t>
+          <ns0:t>CooldownPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger chance values. Off means chance is ignored (cooldown only).</ns0:t>
+          <ns0:t>Sets per-trigger cooldown values. Off disables cooldown.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="12">
       <ns0:c r="A12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Settings</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown Preset</ns0:t>
+          <ns0:t>Duration Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C12" t="inlineStr" s="0">
@@ -508,34 +508,34 @@
       </ns0:c>
       <ns0:c r="D12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Balanced</ns0:t>
+          <ns0:t>Standard</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (No Cooldown) | Short | Balanced | Long | Extended</ns0:t>
+          <ns0:t>Short | Standard | Long | Extended</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CooldownPresetProvider</ns0:t>
+          <ns0:t>DurationPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger cooldown values. Off disables cooldown.</ns0:t>
+          <ns0:t>Sets per-trigger duration values.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="13">
       <ns0:c r="A13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Settings</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration Preset</ns0:t>
+          <ns0:t>Smoothness Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C13" t="inlineStr" s="0">
@@ -545,34 +545,34 @@
       </ns0:c>
       <ns0:c r="D13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Balanced</ns0:t>
+          <ns0:t>Standard</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Short | Balanced | Long | Extended</ns0:t>
+          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Cinematic | Ultra Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>DurationPresetProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger duration values.</ns0:t>
+          <ns0:t>Sets per-trigger transition speed values (lower = smoother).</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="14">
       <ns0:c r="A14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Settings</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smoothness Preset</ns0:t>
+          <ns0:t>Trigger Profile</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C14" t="inlineStr" s="0">
@@ -582,145 +582,145 @@
       </ns0:c>
       <ns0:c r="D14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Balanced</ns0:t>
+          <ns0:t>All Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Very Snappy | Snappy | Balanced | Smooth | Cinematic | Ultra Smooth</ns0:t>
+          <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger transition speed values (lower = smoother).</ns0:t>
+          <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="15">
       <ns0:c r="A15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Settings</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger Profile</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>All Triggers</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerProfileProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="16">
-      <ns0:c r="A16" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B16" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C16" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D16" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E16" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F16" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G16" t="inlineStr" s="0">
+      <ns0:c r="A16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Optional Overrides</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G16" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="17">
-      <ns0:c r="A17" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Global Overrides</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B17" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C17" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D17" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E17" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F17" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G17" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Optional Overrides</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Global Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CooldownProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="18">
       <ns0:c r="A18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Overrides</ns0:t>
+          <ns0:t>Optional Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Cooldown</ns0:t>
+          <ns0:t>Global Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="0">
@@ -730,34 +730,34 @@
       </ns0:c>
       <ns0:c r="D18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3s</ns0:t>
+          <ns0:t>Per Trigger</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
+          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CooldownProvider</ns0:t>
+          <ns0:t>GlobalSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
+          <ns0:t>Override transition speed for all triggers. Per Trigger uses per-trigger smoothing (plus Smoothness Preset).</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Overrides</ns0:t>
+          <ns0:t>Optional Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Smoothing</ns0:t>
+          <ns0:t>Haptic Feedback</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="0">
@@ -767,34 +767,34 @@
       </ns0:c>
       <ns0:c r="D19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
+          <ns0:t>Off | Light | Medium | Strong</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>GlobalSmoothingProvider</ns0:t>
+          <ns0:t>HapticIntensityProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Override transition speed for all triggers. Per Trigger uses per-trigger smoothing (plus Smoothness Preset).</ns0:t>
+          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Overrides</ns0:t>
+          <ns0:t>Optional Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Haptic Feedback</ns0:t>
+          <ns0:t>Dynamic Intensity</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="0">
@@ -804,133 +804,133 @@
       </ns0:c>
       <ns0:c r="D20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Medium</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t>Off | Low Sensitivity | Medium Sensitivity | High Sensitivity</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>HapticIntensityProvider</ns0:t>
+          <ns0:t>DynamicIntensityPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
+          <ns0:t>Scale slowdown based on damage. Low = dampened, High = can reach near-instant slow-mo.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
       <ns0:c r="A21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Overrides</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dynamic Intensity</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C21" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="22">
+      <ns0:c r="A22" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CSM Triggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B22" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C22" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D22" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E22" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F22" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G22" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="23">
+      <ns0:c r="A23" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Triggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B23" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C23" t="inlineStr" s="0">
+        <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D21" t="inlineStr" s="0">
+      <ns0:c r="D23" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Scale intensity based on damage dealt</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="22">
-      <ns0:c r="A22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="23">
-      <ns0:c r="A23" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B23" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C23" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D23" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E23" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F23" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G23" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="E23" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F23" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G23" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -942,7 +942,7 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Kill</ns0:t>
+          <ns0:t>Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C24" t="inlineStr" s="0">
@@ -967,7 +967,7 @@
       </ns0:c>
       <ns0:c r="G24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -979,7 +979,7 @@
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Kill</ns0:t>
+          <ns0:t>Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C25" t="inlineStr" s="0">
@@ -1004,7 +1004,7 @@
       </ns0:c>
       <ns0:c r="G25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1016,7 +1016,7 @@
       </ns0:c>
       <ns0:c r="B26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismemberment</ns0:t>
+          <ns0:t>Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C26" t="inlineStr" s="0">
@@ -1041,7 +1041,7 @@
       </ns0:c>
       <ns0:c r="G26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1053,7 +1053,7 @@
       </ns0:c>
       <ns0:c r="B27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation</ns0:t>
+          <ns0:t>Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C27" t="inlineStr" s="0">
@@ -1078,7 +1078,7 @@
       </ns0:c>
       <ns0:c r="G27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1090,7 +1090,7 @@
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy</ns0:t>
+          <ns0:t>Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C28" t="inlineStr" s="0">
@@ -1115,7 +1115,7 @@
       </ns0:c>
       <ns0:c r="G28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1127,32 +1127,32 @@
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand</ns0:t>
+          <ns0:t>Last Stand Threshold</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>15%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1164,54 +1164,54 @@
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Threshold</ns0:t>
+          <ns0:t>Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
+          <ns0:t>Trigger on successful weapon deflections</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="31">
       <ns0:c r="A31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E31" t="inlineStr" s="0">
@@ -1226,81 +1226,81 @@
       </ns0:c>
       <ns0:c r="G31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on successful weapon deflections</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="32">
-      <ns0:c r="A32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G32" t="inlineStr" s="0">
+      <ns0:c r="A32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CSM Killcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G32" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="33">
-      <ns0:c r="A33" t="inlineStr" s="2">
+      <ns0:c r="A33" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B33" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C33" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D33" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E33" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F33" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G33" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Camera Distance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>3m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1312,32 +1312,32 @@
       </ns0:c>
       <ns0:c r="B34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Enable Killcam</ns0:t>
+          <ns0:t>Camera Height</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>1.5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>WARNING: May cause VR motion sickness</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1349,7 +1349,7 @@
       </ns0:c>
       <ns0:c r="B35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera Distance</ns0:t>
+          <ns0:t>Orbit Speed</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C35" t="inlineStr" s="0">
@@ -1359,404 +1359,402 @@
       </ns0:c>
       <ns0:c r="D35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3m</ns0:t>
+          <ns0:t>Slow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
+          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="36">
       <ns0:c r="A36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera Height</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="37">
-      <ns0:c r="A37" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B37" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Orbit Speed</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C37" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D37" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E37" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F37" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G37" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
+      <ns0:c r="A37" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B37" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C37" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D37" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E37" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F37" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G37" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="38">
       <ns0:c r="A38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On Decapitation</ns0:t>
+          <ns0:t>Basic Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>25%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger killcam on decapitation kills</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="39">
       <ns0:c r="A39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On Critical Kill</ns0:t>
+          <ns0:t>Basic Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>0.35x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G39" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger killcam on critical (head/neck) kills</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="40">
       <ns0:c r="A40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On Last Enemy</ns0:t>
+          <ns0:t>Basic Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>1.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger killcam when killing the last enemy</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="41">
       <ns0:c r="A41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Show Player Body</ns0:t>
+          <ns0:t>Basic Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Show player body during killcam (third-person view)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="42">
       <ns0:c r="A42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Basic Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D42" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D42" s="0">
+        <ns0:v>8</ns0:v>
       </ns0:c>
       <ns0:c r="E42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="43">
-      <ns0:c r="A43" t="inlineStr" s="2">
+      <ns0:c r="A43" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B43" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C43" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D43" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E43" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F43" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G43" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Basic Third Person Distribution</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="44">
       <ns0:c r="A44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Chance</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>25%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="45">
-      <ns0:c r="A45" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B45" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Basic Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C45" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D45" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.35x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E45" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F45" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G45" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="A45" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Critical Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B45" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C45" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D45" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E45" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F45" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G45" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="46">
       <ns0:c r="A46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Duration</ns0:t>
+          <ns0:t>Critical Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C46" t="inlineStr" s="0">
@@ -1766,34 +1764,34 @@
       </ns0:c>
       <ns0:c r="D46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.0s</ns0:t>
+          <ns0:t>75%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="47">
       <ns0:c r="A47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Cooldown</ns0:t>
+          <ns0:t>Critical Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C47" t="inlineStr" s="0">
@@ -1803,34 +1801,34 @@
       </ns0:c>
       <ns0:c r="D47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>0.25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="48">
       <ns0:c r="A48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Smoothing</ns0:t>
+          <ns0:t>Critical Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C48" t="inlineStr" s="0">
@@ -1838,34 +1836,36 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D48" s="0">
-        <ns0:v>8</ns0:v>
+      <ns0:c r="D48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.5s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="49">
       <ns0:c r="A49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Third Person Distribution</ns0:t>
+          <ns0:t>Critical Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C49" t="inlineStr" s="0">
@@ -1875,182 +1875,180 @@
       </ns0:c>
       <ns0:c r="D49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="50">
       <ns0:c r="A50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Critical Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D50" s="0">
+        <ns0:v>8</ns0:v>
       </ns0:c>
       <ns0:c r="E50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="51">
-      <ns0:c r="A51" t="inlineStr" s="2">
+      <ns0:c r="A51" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Critical Third Person Distribution</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="52">
       <ns0:c r="A52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Chance</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>75%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="53">
-      <ns0:c r="A53" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B53" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Critical Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C53" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D53" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.25x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E53" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F53" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G53" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="A53" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Dismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B53" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C53" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D53" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E53" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F53" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G53" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="54">
       <ns0:c r="A54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Duration</ns0:t>
+          <ns0:t>Dismember Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C54" t="inlineStr" s="0">
@@ -2060,34 +2058,34 @@
       </ns0:c>
       <ns0:c r="D54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>60%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="55">
       <ns0:c r="A55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Cooldown</ns0:t>
+          <ns0:t>Dismember Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C55" t="inlineStr" s="0">
@@ -2097,34 +2095,34 @@
       </ns0:c>
       <ns0:c r="D55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>0.30x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="56">
       <ns0:c r="A56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Smoothing</ns0:t>
+          <ns0:t>Dismember Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C56" t="inlineStr" s="0">
@@ -2132,34 +2130,36 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D56" s="0">
-        <ns0:v>8</ns0:v>
+      <ns0:c r="D56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.5s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="57">
       <ns0:c r="A57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Third Person Distribution</ns0:t>
+          <ns0:t>Dismember Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C57" t="inlineStr" s="0">
@@ -2169,182 +2169,180 @@
       </ns0:c>
       <ns0:c r="D57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="58">
       <ns0:c r="A58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Dismember Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D58" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D58" s="0">
+        <ns0:v>8</ns0:v>
       </ns0:c>
       <ns0:c r="E58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="59">
-      <ns0:c r="A59" t="inlineStr" s="2">
+      <ns0:c r="A59" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B59" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C59" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D59" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E59" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F59" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G59" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Dismember Third Person Distribution</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="60">
       <ns0:c r="A60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Chance</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>60%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="61">
-      <ns0:c r="A61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Dismember Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.30x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="A61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="62">
       <ns0:c r="A62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Duration</ns0:t>
+          <ns0:t>Decapitation Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C62" t="inlineStr" s="0">
@@ -2354,34 +2352,34 @@
       </ns0:c>
       <ns0:c r="D62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>90%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="63">
       <ns0:c r="A63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Cooldown</ns0:t>
+          <ns0:t>Decapitation Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C63" t="inlineStr" s="0">
@@ -2391,34 +2389,34 @@
       </ns0:c>
       <ns0:c r="D63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="64">
       <ns0:c r="A64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Smoothing</ns0:t>
+          <ns0:t>Decapitation Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C64" t="inlineStr" s="0">
@@ -2426,34 +2424,36 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D64" s="0">
-        <ns0:v>8</ns0:v>
+      <ns0:c r="D64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2.0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="65">
       <ns0:c r="A65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Third Person Distribution</ns0:t>
+          <ns0:t>Decapitation Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="0">
@@ -2463,182 +2463,180 @@
       </ns0:c>
       <ns0:c r="D65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>4.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="66">
       <ns0:c r="A66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Decapitation Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D66" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D66" s="0">
+        <ns0:v>6</ns0:v>
       </ns0:c>
       <ns0:c r="E66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="67">
-      <ns0:c r="A67" t="inlineStr" s="2">
+      <ns0:c r="A67" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B67" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C67" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D67" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E67" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F67" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G67" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B67" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Decapitation Third Person Distribution</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C67" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D67" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E67" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F67" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G67" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="68">
       <ns0:c r="A68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Chance</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>90%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="69">
-      <ns0:c r="A69" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B69" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Decapitation Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C69" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D69" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.20x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E69" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F69" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G69" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="A69" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B69" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C69" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D69" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E69" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F69" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G69" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="70">
       <ns0:c r="A70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Duration</ns0:t>
+          <ns0:t>Last Enemy Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C70" t="inlineStr" s="0">
@@ -2648,34 +2646,34 @@
       </ns0:c>
       <ns0:c r="D70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.0s</ns0:t>
+          <ns0:t>100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="71">
       <ns0:c r="A71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Cooldown</ns0:t>
+          <ns0:t>Last Enemy Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C71" t="inlineStr" s="0">
@@ -2685,34 +2683,34 @@
       </ns0:c>
       <ns0:c r="D71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4.0s</ns0:t>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="72">
       <ns0:c r="A72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Smoothing</ns0:t>
+          <ns0:t>Last Enemy Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C72" t="inlineStr" s="0">
@@ -2720,34 +2718,36 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D72" s="0">
-        <ns0:v>6</ns0:v>
+      <ns0:c r="D72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>3.0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="73">
       <ns0:c r="A73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Third Person Distribution</ns0:t>
+          <ns0:t>Last Enemy Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C73" t="inlineStr" s="0">
@@ -2757,182 +2757,180 @@
       </ns0:c>
       <ns0:c r="D73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="74">
       <ns0:c r="A74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Last Enemy Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D74" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D74" s="0">
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="E74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="75">
-      <ns0:c r="A75" t="inlineStr" s="2">
+      <ns0:c r="A75" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B75" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C75" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D75" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E75" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F75" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G75" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B75" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Enemy Third Person Distribution</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C75" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D75" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E75" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F75" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G75" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="76">
       <ns0:c r="A76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Chance</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="77">
-      <ns0:c r="A77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Enemy Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.20x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="A77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="78">
       <ns0:c r="A78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Duration</ns0:t>
+          <ns0:t>Last Stand Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C78" t="inlineStr" s="0">
@@ -2942,34 +2940,34 @@
       </ns0:c>
       <ns0:c r="D78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.0s</ns0:t>
+          <ns0:t>0.15x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="79">
       <ns0:c r="A79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Cooldown</ns0:t>
+          <ns0:t>Last Stand Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C79" t="inlineStr" s="0">
@@ -2979,34 +2977,34 @@
       </ns0:c>
       <ns0:c r="D79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="80">
       <ns0:c r="A80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Smoothing</ns0:t>
+          <ns0:t>Last Stand Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C80" t="inlineStr" s="0">
@@ -3014,34 +3012,36 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D80" s="0">
-        <ns0:v>4</ns0:v>
+      <ns0:c r="D80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>45.0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="81">
       <ns0:c r="A81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Third Person Distribution</ns0:t>
+          <ns0:t>Last Stand Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="0">
@@ -3049,24 +3049,22 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D81" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D81" s="0">
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="E81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3110,7 +3108,7 @@
     <ns0:row r="83">
       <ns0:c r="A83" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="2">
@@ -3147,12 +3145,12 @@
     <ns0:row r="84">
       <ns0:c r="A84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Time Scale</ns0:t>
+          <ns0:t>Parry Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C84" t="inlineStr" s="0">
@@ -3162,34 +3160,34 @@
       </ns0:c>
       <ns0:c r="D84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.15x</ns0:t>
+          <ns0:t>50%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="85">
       <ns0:c r="A85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Duration</ns0:t>
+          <ns0:t>Parry Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C85" t="inlineStr" s="0">
@@ -3199,34 +3197,34 @@
       </ns0:c>
       <ns0:c r="D85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>0.30x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="86">
       <ns0:c r="A86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Cooldown</ns0:t>
+          <ns0:t>Parry Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C86" t="inlineStr" s="0">
@@ -3236,34 +3234,34 @@
       </ns0:c>
       <ns0:c r="D86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>45.0s</ns0:t>
+          <ns0:t>1.2s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="87">
       <ns0:c r="A87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Smoothing</ns0:t>
+          <ns0:t>Parry Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C87" t="inlineStr" s="0">
@@ -3271,388 +3269,168 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D87" s="0">
-        <ns0:v>4</ns0:v>
+      <ns0:c r="D87" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>7.0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="88">
       <ns0:c r="A88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Parry Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D88" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D88" s="0">
+        <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
-      <ns0:c r="A89" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B89" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C89" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D89" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E89" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F89" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G89" t="inlineStr" s="2">
+      <ns0:c r="A89" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B89" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C89" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D89" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E89" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F89" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G89" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="90">
-      <ns0:c r="A90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Parry Chance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>50%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+      <ns0:c r="A90" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B90" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C90" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D90" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E90" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F90" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G90" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="91">
       <ns0:c r="A91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>CSM Advanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Time Scale</ns0:t>
+          <ns0:t>Debug Logging</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.30x</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="92">
-      <ns0:c r="A92" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B92" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Parry Duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C92" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D92" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1.2s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E92" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F92" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G92" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="93">
-      <ns0:c r="A93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Parry Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>7.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="94">
-      <ns0:c r="A94" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B94" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Parry Smoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C94" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D94" s="0">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E94" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F94" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G94" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="95">
-      <ns0:c r="A95" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B95" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C95" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D95" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E95" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F95" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G95" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="96">
-      <ns0:c r="A96" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B96" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C96" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D96" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E96" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F96" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G96" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="97">
-      <ns0:c r="A97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Debug Logging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G97" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
@@ -3720,156 +3498,156 @@
     <ns0:row r="5">
       <ns0:c r="A5" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CameraModeProvider</ns0:t>
+          <ns0:t>ChancePresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B5" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Default (Preset) | First Person Only | Third Person Only</ns0:t>
+          <ns0:t>Off (Cooldown Only) | Rare | Standard | Frequent</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="6">
       <ns0:c r="A6" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ChancePresetProvider</ns0:t>
+          <ns0:t>ChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B6" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (Cooldown Only) | Rare | Balanced | Frequent</ns0:t>
+          <ns0:t>10% | 20% | 30% | 50% | 75% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="7">
       <ns0:c r="A7" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ChanceProvider</ns0:t>
+          <ns0:t>CooldownPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B7" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10% | 20% | 30% | 50% | 75% | 100%</ns0:t>
+          <ns0:t>Off (No Cooldown) | Short | Standard | Long | Extended</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="8">
       <ns0:c r="A8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CooldownPresetProvider</ns0:t>
+          <ns0:t>CooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (No Cooldown) | Short | Balanced | Long | Extended</ns0:t>
+          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="9">
       <ns0:c r="A9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CooldownProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="10">
       <ns0:c r="A10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="11">
       <ns0:c r="A11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="12">
       <ns0:c r="A12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="13">
       <ns0:c r="A13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="14">
       <ns0:c r="A14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="15">
       <ns0:c r="A15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>DurationPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>Short | Standard | Long | Extended</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="16">
       <ns0:c r="A16" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>DurationPresetProvider</ns0:t>
+          <ns0:t>DurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B16" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Short | Balanced | Long | Extended</ns0:t>
+          <ns0:t>0.5s | 1.0s | 1.5s | 2.0s | 2.5s | 3.0s | 4.0s | 5.0s | 8.0s</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="17">
       <ns0:c r="A17" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>DurationProvider</ns0:t>
+          <ns0:t>DynamicIntensityPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B17" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 1.0s | 1.5s | 2.0s | 2.5s | 3.0s | 4.0s | 5.0s | 8.0s</ns0:t>
+          <ns0:t>Off | Low Sensitivity | Medium Sensitivity | High Sensitivity</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3953,7 +3731,7 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Subtle | Balanced | Dramatic | Cinematic | Epic</ns0:t>
+          <ns0:t>Subtle | Standard | Dramatic | Cinematic | Epic</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3977,7 +3755,7 @@
       </ns0:c>
       <ns0:c r="B26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Very Snappy | Snappy | Balanced | Smooth | Cinematic | Ultra Smooth</ns0:t>
+          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Cinematic | Ultra Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Adjust dynamic intensity start speed and reorder options
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -197,7 +197,7 @@
     <ns0:row r="4">
       <ns0:c r="A4" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>Presets</ns0:t>
+          <ns0:t>Uncategorized</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B4" t="inlineStr" s="2">
@@ -234,7 +234,7 @@
     <ns0:row r="5">
       <ns0:c r="A5" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Presets</ns0:t>
+          <ns0:t>Uncategorized</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B5" t="inlineStr" s="0">
@@ -641,7 +641,7 @@
     <ns0:row r="16">
       <ns0:c r="A16" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B16" t="inlineStr" s="2">
@@ -678,170 +678,170 @@
     <ns0:row r="17">
       <ns0:c r="A17" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B17" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Cooldown</ns0:t>
+          <ns0:t>Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C17" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D17" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E17" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F17" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CooldownProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G17" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="18">
       <ns0:c r="A18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Smoothing</ns0:t>
+          <ns0:t>Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>GlobalSmoothingProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Override transition speed for all triggers. Per Trigger uses per-trigger smoothing (plus Smoothness Preset).</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Haptic Feedback</ns0:t>
+          <ns0:t>Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>HapticIntensityProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dynamic Intensity</ns0:t>
+          <ns0:t>Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Low Sensitivity | Medium Sensitivity | High Sensitivity</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>DynamicIntensityPresetProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Scale slowdown based on damage. Low = dampened, High = can reach near-instant slow-mo.</ns0:t>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
       <ns0:c r="A21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E21" t="inlineStr" s="0">
@@ -856,44 +856,44 @@
       </ns0:c>
       <ns0:c r="G21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
-      <ns0:c r="A22" t="inlineStr" s="2">
+      <ns0:c r="A22" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B22" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C22" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D22" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E22" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F22" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G22" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -905,32 +905,32 @@
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Kill</ns0:t>
+          <ns0:t>Last Stand Threshold</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>15%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -942,7 +942,7 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Kill</ns0:t>
+          <ns0:t>Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C24" t="inlineStr" s="0">
@@ -967,29 +967,29 @@
       </ns0:c>
       <ns0:c r="G24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Trigger on successful weapon deflections</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismemberment</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E25" t="inlineStr" s="0">
@@ -1004,130 +1004,130 @@
       </ns0:c>
       <ns0:c r="G25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="26">
-      <ns0:c r="A26" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B26" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C26" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D26" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E26" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F26" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G26" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
+      <ns0:c r="A26" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Optional Overrides</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B26" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C26" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D26" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E26" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F26" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G26" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="27">
       <ns0:c r="A27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>Optional Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy</ns0:t>
+          <ns0:t>Global Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="28">
       <ns0:c r="A28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>Optional Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand</ns0:t>
+          <ns0:t>Global Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Per Trigger</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>GlobalSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Override transition speed for all triggers. Per Trigger uses per-trigger smoothing (plus Smoothness Preset).</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="29">
       <ns0:c r="A29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>Optional Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Threshold</ns0:t>
+          <ns0:t>Haptic Feedback</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C29" t="inlineStr" s="0">
@@ -1137,59 +1137,59 @@
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t>Off | Light | Medium | Strong</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t>HapticIntensityProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
+          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="30">
       <ns0:c r="A30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>Optional Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry</ns0:t>
+          <ns0:t>Dynamic Intensity</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off | Low Sensitivity | Medium Sensitivity | High Sensitivity</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>DynamicIntensityPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on successful weapon deflections</ns0:t>
+          <ns0:t>Scale slow-mo start speed based on damage. Low = dampened, High = can reach near-instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Add killcam randomization toggles and smoothing units
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -560,7 +560,7 @@
       </ns0:c>
       <ns0:c r="G13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger transition speed values (lower = smoother).</ns0:t>
+          <ns0:t>Sets per-trigger transition speed multipliers (x). Lower = smoother.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1312,32 +1312,32 @@
       </ns0:c>
       <ns0:c r="B34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera Height</ns0:t>
+          <ns0:t>Randomize Distance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Randomize distance per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1349,7 +1349,7 @@
       </ns0:c>
       <ns0:c r="B35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Orbit Speed</ns0:t>
+          <ns0:t>Camera Height</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C35" t="inlineStr" s="0">
@@ -1359,44 +1359,44 @@
       </ns0:c>
       <ns0:c r="D35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slow</ns0:t>
+          <ns0:t>1.5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="36">
       <ns0:c r="A36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Randomize Height</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E36" t="inlineStr" s="0">
@@ -1411,118 +1411,118 @@
       </ns0:c>
       <ns0:c r="G36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Randomize height per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="37">
-      <ns0:c r="A37" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B37" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C37" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D37" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E37" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F37" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G37" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Killcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Orbit Speed</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="38">
       <ns0:c r="A38" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="39">
+      <ns0:c r="A39" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B38" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Basic Chance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C38" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D38" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>25%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E38" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F38" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G38" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="39">
-      <ns0:c r="A39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Basic Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.35x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="B39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1534,7 +1534,7 @@
       </ns0:c>
       <ns0:c r="B40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Duration</ns0:t>
+          <ns0:t>Basic Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C40" t="inlineStr" s="0">
@@ -1544,22 +1544,22 @@
       </ns0:c>
       <ns0:c r="D40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.0s</ns0:t>
+          <ns0:t>25%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1571,7 +1571,7 @@
       </ns0:c>
       <ns0:c r="B41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Cooldown</ns0:t>
+          <ns0:t>Basic Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C41" t="inlineStr" s="0">
@@ -1581,22 +1581,22 @@
       </ns0:c>
       <ns0:c r="D41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>0.35x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1608,7 +1608,7 @@
       </ns0:c>
       <ns0:c r="B42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Smoothing</ns0:t>
+          <ns0:t>Basic Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C42" t="inlineStr" s="0">
@@ -1616,22 +1616,24 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D42" s="0">
-        <ns0:v>8</ns0:v>
+      <ns0:c r="D42" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1643,7 +1645,7 @@
       </ns0:c>
       <ns0:c r="B43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Third Person Distribution</ns0:t>
+          <ns0:t>Basic Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C43" t="inlineStr" s="0">
@@ -1653,170 +1655,170 @@
       </ns0:c>
       <ns0:c r="D43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="44">
       <ns0:c r="A44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Basic Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>8x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="45">
-      <ns0:c r="A45" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B45" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C45" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D45" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E45" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F45" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G45" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Basic Third Person Distribution</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="46">
       <ns0:c r="A46" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B46" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C46" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D46" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E46" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F46" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G46" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="47">
+      <ns0:c r="A47" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B46" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Critical Chance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C46" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D46" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>75%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E46" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F46" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G46" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="47">
-      <ns0:c r="A47" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B47" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Critical Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C47" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D47" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.25x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E47" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F47" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G47" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="B47" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C47" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D47" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E47" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F47" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G47" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1828,7 +1830,7 @@
       </ns0:c>
       <ns0:c r="B48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Duration</ns0:t>
+          <ns0:t>Critical Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C48" t="inlineStr" s="0">
@@ -1838,22 +1840,22 @@
       </ns0:c>
       <ns0:c r="D48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>75%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1865,7 +1867,7 @@
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Cooldown</ns0:t>
+          <ns0:t>Critical Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C49" t="inlineStr" s="0">
@@ -1875,22 +1877,22 @@
       </ns0:c>
       <ns0:c r="D49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>0.25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1902,7 +1904,7 @@
       </ns0:c>
       <ns0:c r="B50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Smoothing</ns0:t>
+          <ns0:t>Critical Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C50" t="inlineStr" s="0">
@@ -1910,22 +1912,24 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D50" s="0">
-        <ns0:v>8</ns0:v>
+      <ns0:c r="D50" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.5s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1937,7 +1941,7 @@
       </ns0:c>
       <ns0:c r="B51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Third Person Distribution</ns0:t>
+          <ns0:t>Critical Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C51" t="inlineStr" s="0">
@@ -1947,170 +1951,170 @@
       </ns0:c>
       <ns0:c r="D51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="52">
       <ns0:c r="A52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Critical Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>8x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="53">
-      <ns0:c r="A53" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B53" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C53" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D53" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E53" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F53" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G53" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Critical Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Critical Third Person Distribution</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="54">
       <ns0:c r="A54" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="55">
+      <ns0:c r="A55" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B54" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Dismember Chance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C54" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D54" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>60%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E54" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F54" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G54" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="55">
-      <ns0:c r="A55" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B55" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Dismember Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C55" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D55" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.30x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E55" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F55" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G55" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="B55" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C55" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D55" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E55" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F55" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G55" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2122,7 +2126,7 @@
       </ns0:c>
       <ns0:c r="B56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Duration</ns0:t>
+          <ns0:t>Dismember Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C56" t="inlineStr" s="0">
@@ -2132,22 +2136,22 @@
       </ns0:c>
       <ns0:c r="D56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>60%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2159,7 +2163,7 @@
       </ns0:c>
       <ns0:c r="B57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Cooldown</ns0:t>
+          <ns0:t>Dismember Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C57" t="inlineStr" s="0">
@@ -2169,22 +2173,22 @@
       </ns0:c>
       <ns0:c r="D57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>0.30x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2196,7 +2200,7 @@
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Smoothing</ns0:t>
+          <ns0:t>Dismember Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C58" t="inlineStr" s="0">
@@ -2204,22 +2208,24 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D58" s="0">
-        <ns0:v>8</ns0:v>
+      <ns0:c r="D58" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.5s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2231,7 +2237,7 @@
       </ns0:c>
       <ns0:c r="B59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Third Person Distribution</ns0:t>
+          <ns0:t>Dismember Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C59" t="inlineStr" s="0">
@@ -2241,170 +2247,170 @@
       </ns0:c>
       <ns0:c r="D59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="60">
       <ns0:c r="A60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Dismember Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>8x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="61">
-      <ns0:c r="A61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Dismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Dismember Third Person Distribution</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="62">
       <ns0:c r="A62" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B62" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C62" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D62" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E62" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F62" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G62" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="63">
+      <ns0:c r="A63" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B62" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Decapitation Chance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C62" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D62" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>90%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E62" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F62" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G62" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="63">
-      <ns0:c r="A63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Decapitation Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.20x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="B63" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C63" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D63" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E63" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F63" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G63" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2416,7 +2422,7 @@
       </ns0:c>
       <ns0:c r="B64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Duration</ns0:t>
+          <ns0:t>Decapitation Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C64" t="inlineStr" s="0">
@@ -2426,22 +2432,22 @@
       </ns0:c>
       <ns0:c r="D64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.0s</ns0:t>
+          <ns0:t>90%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2453,7 +2459,7 @@
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Cooldown</ns0:t>
+          <ns0:t>Decapitation Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="0">
@@ -2463,22 +2469,22 @@
       </ns0:c>
       <ns0:c r="D65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4.0s</ns0:t>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2490,7 +2496,7 @@
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Smoothing</ns0:t>
+          <ns0:t>Decapitation Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="0">
@@ -2498,22 +2504,24 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D66" s="0">
-        <ns0:v>6</ns0:v>
+      <ns0:c r="D66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2.0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2525,7 +2533,7 @@
       </ns0:c>
       <ns0:c r="B67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Third Person Distribution</ns0:t>
+          <ns0:t>Decapitation Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C67" t="inlineStr" s="0">
@@ -2535,170 +2543,170 @@
       </ns0:c>
       <ns0:c r="D67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>4.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="68">
       <ns0:c r="A68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Decapitation Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>6x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="69">
-      <ns0:c r="A69" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B69" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C69" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D69" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E69" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F69" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G69" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Decapitation Third Person Distribution</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="70">
       <ns0:c r="A70" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="71">
+      <ns0:c r="A71" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B70" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Enemy Chance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C70" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D70" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E70" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F70" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G70" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="71">
-      <ns0:c r="A71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Enemy Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.20x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="B71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2710,7 +2718,7 @@
       </ns0:c>
       <ns0:c r="B72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Duration</ns0:t>
+          <ns0:t>Last Enemy Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C72" t="inlineStr" s="0">
@@ -2720,22 +2728,22 @@
       </ns0:c>
       <ns0:c r="D72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.0s</ns0:t>
+          <ns0:t>100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2747,7 +2755,7 @@
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Cooldown</ns0:t>
+          <ns0:t>Last Enemy Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C73" t="inlineStr" s="0">
@@ -2757,22 +2765,22 @@
       </ns0:c>
       <ns0:c r="D73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2784,7 +2792,7 @@
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Smoothing</ns0:t>
+          <ns0:t>Last Enemy Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C74" t="inlineStr" s="0">
@@ -2792,22 +2800,24 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D74" s="0">
-        <ns0:v>4</ns0:v>
+      <ns0:c r="D74" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>3.0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2819,7 +2829,7 @@
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Third Person Distribution</ns0:t>
+          <ns0:t>Last Enemy Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="0">
@@ -2829,170 +2839,170 @@
       </ns0:c>
       <ns0:c r="D75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="76">
       <ns0:c r="A76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Last Enemy Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>4x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="77">
-      <ns0:c r="A77" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B77" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C77" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D77" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E77" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F77" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G77" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A77" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B77" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Enemy Third Person Distribution</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C77" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D77" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E77" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F77" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G77" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="78">
       <ns0:c r="A78" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B78" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C78" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D78" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E78" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F78" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G78" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="79">
+      <ns0:c r="A79" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B78" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Stand Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C78" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D78" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.15x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E78" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F78" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G78" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="79">
-      <ns0:c r="A79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Stand Duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>5.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
+      <ns0:c r="B79" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C79" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D79" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E79" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F79" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G79" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3004,7 +3014,7 @@
       </ns0:c>
       <ns0:c r="B80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Cooldown</ns0:t>
+          <ns0:t>Last Stand Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C80" t="inlineStr" s="0">
@@ -3014,22 +3024,22 @@
       </ns0:c>
       <ns0:c r="D80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>45.0s</ns0:t>
+          <ns0:t>0.15x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3041,7 +3051,7 @@
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Smoothing</ns0:t>
+          <ns0:t>Last Stand Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="0">
@@ -3049,170 +3059,172 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D81" s="0">
-        <ns0:v>4</ns0:v>
+      <ns0:c r="D81" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>5.0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="82">
       <ns0:c r="A82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Last Stand Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>45.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="83">
-      <ns0:c r="A83" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B83" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C83" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D83" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E83" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F83" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G83" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A83" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B83" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Stand Smoothing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C83" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D83" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>4x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E83" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F83" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G83" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="84">
       <ns0:c r="A84" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="85">
+      <ns0:c r="A85" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Parry Chance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>50%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="85">
-      <ns0:c r="A85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Parry Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.30x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="B85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3224,7 +3236,7 @@
       </ns0:c>
       <ns0:c r="B86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Duration</ns0:t>
+          <ns0:t>Parry Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C86" t="inlineStr" s="0">
@@ -3234,22 +3246,22 @@
       </ns0:c>
       <ns0:c r="D86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.2s</ns0:t>
+          <ns0:t>50%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3261,7 +3273,7 @@
       </ns0:c>
       <ns0:c r="B87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Cooldown</ns0:t>
+          <ns0:t>Parry Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C87" t="inlineStr" s="0">
@@ -3271,22 +3283,22 @@
       </ns0:c>
       <ns0:c r="D87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>7.0s</ns0:t>
+          <ns0:t>0.30x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3298,7 +3310,7 @@
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Smoothing</ns0:t>
+          <ns0:t>Parry Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="0">
@@ -3306,131 +3318,207 @@
           <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D88" s="0">
-        <ns0:v>10</ns0:v>
+      <ns0:c r="D88" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.2s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
       <ns0:c r="A89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Parry Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Select</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>7.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="90">
-      <ns0:c r="A90" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B90" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C90" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D90" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E90" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F90" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G90" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Parry Smoothing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Select</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>10x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="91">
       <ns0:c r="A91" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="92">
+      <ns0:c r="A92" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CSM Advanced</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B91" t="inlineStr" s="0">
+      <ns0:c r="B92" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C92" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D92" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E92" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F92" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G92" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="93">
+      <ns0:c r="A93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B93" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Debug Logging</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C91" t="inlineStr" s="0">
+      <ns0:c r="C93" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D91" t="inlineStr" s="0">
+      <ns0:c r="D93" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G91" t="inlineStr" s="0">
+      <ns0:c r="E93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G93" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
@@ -3587,7 +3675,7 @@
       </ns0:c>
       <ns0:c r="B12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2 | 3 | 4 | 4.5 | 5 | 6 | 7.5 | 8 | 10 | 12.5</ns0:t>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Switch preset selectors to arrows and align menu ordering
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -197,7 +197,7 @@
     <ns0:row r="4">
       <ns0:c r="A4" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>Uncategorized</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B4" t="inlineStr" s="2">
@@ -234,7 +234,7 @@
     <ns0:row r="5">
       <ns0:c r="A5" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Uncategorized</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B5" t="inlineStr" s="0">
@@ -308,7 +308,7 @@
     <ns0:row r="7">
       <ns0:c r="A7" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CSM Advanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B7" t="inlineStr" s="2">
@@ -345,281 +345,281 @@
     <ns0:row r="8">
       <ns0:c r="A8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CSM Advanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third Person Distribution</ns0:t>
+          <ns0:t>Debug Logging</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>First Person Only</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>First Person Only | Mixed (Rare Third Person) | Mixed | Mostly Third Person | Third Person Only</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CameraDistributionProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Controls how often third-person killcam appears.</ns0:t>
+          <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="9">
       <ns0:c r="A9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Intensity Preset</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Standard</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Subtle | Standard | Dramatic | Cinematic | Epic</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>PresetProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Intensity profile. Subtle = brief, Standard = default, Dramatic = stronger, Cinematic = dramatic, Epic = extreme</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="10">
-      <ns0:c r="A10" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B10" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance Preset</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C10" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D10" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (Cooldown Only)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E10" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (Cooldown Only) | Rare | Standard | Frequent</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F10" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>ChancePresetProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G10" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Sets per-trigger chance values. Off means chance is ignored (cooldown only).</ns0:t>
+      <ns0:c r="A10" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CSM Killcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B10" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C10" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D10" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E10" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F10" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G10" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="11">
       <ns0:c r="A11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown Preset</ns0:t>
+          <ns0:t>Camera Distance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Standard</ns0:t>
+          <ns0:t>3m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (No Cooldown) | Short | Standard | Long | Extended</ns0:t>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CooldownPresetProvider</ns0:t>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger cooldown values. Off disables cooldown.</ns0:t>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="12">
       <ns0:c r="A12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration Preset</ns0:t>
+          <ns0:t>Camera Height</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Standard</ns0:t>
+          <ns0:t>1.5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Short | Standard | Long | Extended</ns0:t>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>DurationPresetProvider</ns0:t>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger duration values.</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="13">
       <ns0:c r="A13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smoothness Preset</ns0:t>
+          <ns0:t>Orbit Speed</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Standard</ns0:t>
+          <ns0:t>Slow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Cinematic | Ultra Smooth</ns0:t>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger transition speed multipliers (x). Lower = smoother.</ns0:t>
+          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="14">
       <ns0:c r="A14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger Profile</ns0:t>
+          <ns0:t>Randomize Distance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>All Triggers</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerProfileProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
+          <ns0:t>Randomize distance per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="15">
       <ns0:c r="A15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Randomize Height</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E15" t="inlineStr" s="0">
@@ -634,81 +634,81 @@
       </ns0:c>
       <ns0:c r="G15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Randomize height per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="16">
-      <ns0:c r="A16" t="inlineStr" s="2">
+      <ns0:c r="A16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="17">
+      <ns0:c r="A17" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B16" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C16" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D16" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E16" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F16" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G16" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="17">
-      <ns0:c r="A17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
+      <ns0:c r="B17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -720,7 +720,7 @@
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Kill</ns0:t>
+          <ns0:t>Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="0">
@@ -745,7 +745,7 @@
       </ns0:c>
       <ns0:c r="G18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -757,7 +757,7 @@
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismemberment</ns0:t>
+          <ns0:t>Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="0">
@@ -782,7 +782,7 @@
       </ns0:c>
       <ns0:c r="G19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -831,7 +831,7 @@
       </ns0:c>
       <ns0:c r="B21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy</ns0:t>
+          <ns0:t>Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C21" t="inlineStr" s="0">
@@ -856,7 +856,7 @@
       </ns0:c>
       <ns0:c r="G21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -868,7 +868,7 @@
       </ns0:c>
       <ns0:c r="B22" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand</ns0:t>
+          <ns0:t>Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C22" t="inlineStr" s="0">
@@ -893,7 +893,7 @@
       </ns0:c>
       <ns0:c r="G22" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -905,32 +905,32 @@
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Threshold</ns0:t>
+          <ns0:t>Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -942,54 +942,54 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry</ns0:t>
+          <ns0:t>Last Stand Threshold</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>15%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on successful weapon deflections</ns0:t>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E25" t="inlineStr" s="0">
@@ -1004,325 +1004,325 @@
       </ns0:c>
       <ns0:c r="G25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Trigger on successful weapon deflections</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="26">
-      <ns0:c r="A26" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B26" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C26" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D26" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E26" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F26" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G26" t="inlineStr" s="2">
+      <ns0:c r="A26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G26" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="27">
-      <ns0:c r="A27" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B27" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Global Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C27" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D27" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E27" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F27" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G27" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
+      <ns0:c r="A27" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B27" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C27" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D27" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E27" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F27" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G27" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="28">
       <ns0:c r="A28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Smoothing</ns0:t>
+          <ns0:t>Basic Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger</ns0:t>
+          <ns0:t>25%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>GlobalSmoothingProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Override transition speed for all triggers. Per Trigger uses per-trigger smoothing (plus Smoothness Preset).</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="29">
       <ns0:c r="A29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Haptic Feedback</ns0:t>
+          <ns0:t>Basic Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>HapticIntensityProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="30">
       <ns0:c r="A30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dynamic Intensity</ns0:t>
+          <ns0:t>Basic Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>1.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Low Sensitivity | Medium Sensitivity | High Sensitivity</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>DynamicIntensityPresetProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Scale slow-mo start speed based on damage. Low = dampened, High = can reach near-instant.</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="31">
       <ns0:c r="A31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Basic Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>8x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="32">
-      <ns0:c r="A32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Basic Third Person Distribution</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="33">
       <ns0:c r="A33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera Distance</ns0:t>
+          <ns0:t>Basic Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3m</ns0:t>
+          <ns0:t>0.35x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="34">
       <ns0:c r="A34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize Distance</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E34" t="inlineStr" s="0">
@@ -1337,251 +1337,251 @@
       </ns0:c>
       <ns0:c r="G34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize distance per killcam</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="35">
-      <ns0:c r="A35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Camera Height</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1.5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+      <ns0:c r="A35" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Critical Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B35" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C35" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D35" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E35" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F35" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G35" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="36">
       <ns0:c r="A36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize Height</ns0:t>
+          <ns0:t>Critical Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>75%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize height per killcam</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="37">
       <ns0:c r="A37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Orbit Speed</ns0:t>
+          <ns0:t>Critical Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slow</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="38">
       <ns0:c r="A38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Critical Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="39">
-      <ns0:c r="A39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Critical Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Critical Smoothing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>8x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="40">
       <ns0:c r="A40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Chance</ns0:t>
+          <ns0:t>Critical Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>25%</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="41">
       <ns0:c r="A41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Time Scale</ns0:t>
+          <ns0:t>Critical Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.35x</ns0:t>
+          <ns0:t>0.25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E41" t="inlineStr" s="0">
@@ -1603,281 +1603,281 @@
     <ns0:row r="42">
       <ns0:c r="A42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="43">
-      <ns0:c r="A43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Basic Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>5.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+      <ns0:c r="A43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="44">
       <ns0:c r="A44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Smoothing</ns0:t>
+          <ns0:t>Decapitation Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>8x</ns0:t>
+          <ns0:t>90%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="45">
       <ns0:c r="A45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Third Person Distribution</ns0:t>
+          <ns0:t>Decapitation Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>4.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="46">
       <ns0:c r="A46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Decapitation Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="47">
-      <ns0:c r="A47" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B47" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C47" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D47" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E47" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F47" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G47" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Decapitation Smoothing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>6x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="48">
       <ns0:c r="A48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Chance</ns0:t>
+          <ns0:t>Decapitation Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>75%</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="49">
       <ns0:c r="A49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Time Scale</ns0:t>
+          <ns0:t>Decapitation Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.25x</ns0:t>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E49" t="inlineStr" s="0">
@@ -1899,222 +1899,222 @@
     <ns0:row r="50">
       <ns0:c r="A50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="51">
-      <ns0:c r="A51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Critical Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>5.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+      <ns0:c r="A51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Dismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="52">
       <ns0:c r="A52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Smoothing</ns0:t>
+          <ns0:t>Dismember Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>8x</ns0:t>
+          <ns0:t>60%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="53">
       <ns0:c r="A53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Third Person Distribution</ns0:t>
+          <ns0:t>Dismember Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="54">
       <ns0:c r="A54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Dismember Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="55">
-      <ns0:c r="A55" t="inlineStr" s="2">
+      <ns0:c r="A55" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B55" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C55" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D55" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E55" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F55" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G55" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Dismember Smoothing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>8x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2126,32 +2126,32 @@
       </ns0:c>
       <ns0:c r="B56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Chance</ns0:t>
+          <ns0:t>Dismember Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>60%</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2168,7 +2168,7 @@
       </ns0:c>
       <ns0:c r="C57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D57" t="inlineStr" s="0">
@@ -2195,276 +2195,276 @@
     <ns0:row r="58">
       <ns0:c r="A58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="59">
-      <ns0:c r="A59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Dismember Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>5.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+      <ns0:c r="A59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="60">
       <ns0:c r="A60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Smoothing</ns0:t>
+          <ns0:t>Last Enemy Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>8x</ns0:t>
+          <ns0:t>100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="61">
       <ns0:c r="A61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Third Person Distribution</ns0:t>
+          <ns0:t>Last Enemy Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="62">
       <ns0:c r="A62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Last Enemy Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>3.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="63">
-      <ns0:c r="A63" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B63" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C63" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D63" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E63" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F63" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G63" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Enemy Smoothing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>4x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="64">
       <ns0:c r="A64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Chance</ns0:t>
+          <ns0:t>Last Enemy Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>90%</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="65">
       <ns0:c r="A65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Time Scale</ns0:t>
+          <ns0:t>Last Enemy Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D65" t="inlineStr" s="0">
@@ -2491,355 +2491,355 @@
     <ns0:row r="66">
       <ns0:c r="A66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="67">
-      <ns0:c r="A67" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B67" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Decapitation Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C67" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D67" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>4.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E67" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F67" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G67" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+      <ns0:c r="A67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="68">
       <ns0:c r="A68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Smoothing</ns0:t>
+          <ns0:t>Last Stand Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>6x</ns0:t>
+          <ns0:t>45.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="69">
       <ns0:c r="A69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Third Person Distribution</ns0:t>
+          <ns0:t>Last Stand Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="70">
       <ns0:c r="A70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Last Stand Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>4x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="71">
-      <ns0:c r="A71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Stand Time Scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.15x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="72">
       <ns0:c r="A72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Chance</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="73">
-      <ns0:c r="A73" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B73" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Enemy Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C73" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D73" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.20x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E73" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F73" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G73" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="A73" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B73" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C73" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D73" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E73" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F73" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G73" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="74">
       <ns0:c r="A74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Duration</ns0:t>
+          <ns0:t>Parry Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.0s</ns0:t>
+          <ns0:t>50%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="75">
       <ns0:c r="A75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Cooldown</ns0:t>
+          <ns0:t>Parry Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>7.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E75" t="inlineStr" s="0">
@@ -2861,666 +2861,666 @@
     <ns0:row r="76">
       <ns0:c r="A76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Smoothing</ns0:t>
+          <ns0:t>Parry Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4x</ns0:t>
+          <ns0:t>1.2s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="77">
       <ns0:c r="A77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Third Person Distribution</ns0:t>
+          <ns0:t>Parry Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>10x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="78">
       <ns0:c r="A78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Parry Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.30x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="79">
-      <ns0:c r="A79" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B79" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C79" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D79" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E79" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F79" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G79" t="inlineStr" s="2">
+      <ns0:c r="A79" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B79" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C79" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D79" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E79" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F79" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G79" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="80">
-      <ns0:c r="A80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Stand Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.15x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="A80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Optional Overrides</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="81">
       <ns0:c r="A81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>Optional Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Duration</ns0:t>
+          <ns0:t>Dynamic Intensity</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>Off | Low Sensitivity | Medium Sensitivity | High Sensitivity</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>DynamicIntensityPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Scale slow-mo start speed based on damage. Low = dampened, High = can reach near-instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="82">
       <ns0:c r="A82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>Optional Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Cooldown</ns0:t>
+          <ns0:t>Global Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>45.0s</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="83">
       <ns0:c r="A83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>Optional Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Smoothing</ns0:t>
+          <ns0:t>Global Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4x</ns0:t>
+          <ns0:t>Per Trigger</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>GlobalSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Override transition speed for all triggers. Per Trigger uses per-trigger smoothing (plus Smoothness Preset).</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="84">
       <ns0:c r="A84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Optional Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Haptic Feedback</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off | Light | Medium | Strong</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>HapticIntensityProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="85">
-      <ns0:c r="A85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G85" t="inlineStr" s="2">
+      <ns0:c r="A85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G85" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="86">
-      <ns0:c r="A86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Parry Chance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Select</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>50%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+      <ns0:c r="A86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Preset Selection</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="87">
       <ns0:c r="A87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Time Scale</ns0:t>
+          <ns0:t>Chance Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.30x</ns0:t>
+          <ns0:t>Off (Cooldown Only)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>Off (Cooldown Only) | Rare | Standard | Frequent</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>ChancePresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Sets per-trigger chance values. Off means chance is ignored (cooldown only).</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="88">
       <ns0:c r="A88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Duration</ns0:t>
+          <ns0:t>Cooldown Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.2s</ns0:t>
+          <ns0:t>Standard</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>Off (No Cooldown) | Short | Standard | Long | Extended</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CooldownPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Sets per-trigger cooldown values. Off disables cooldown.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
       <ns0:c r="A89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Cooldown</ns0:t>
+          <ns0:t>Duration Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>7.0s</ns0:t>
+          <ns0:t>Standard</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>Short | Standard | Long | Extended</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>DurationPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Sets per-trigger duration values.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="90">
       <ns0:c r="A90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Smoothing</ns0:t>
+          <ns0:t>Intensity Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Select</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10x</ns0:t>
+          <ns0:t>Standard</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>Subtle | Standard | Dramatic | Cinematic | Epic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>PresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Intensity profile. Subtle = brief, Standard = default, Dramatic = stronger, Cinematic = dramatic, Epic = extreme</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="91">
       <ns0:c r="A91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Smoothness Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Standard</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Cinematic | Ultra Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Sets per-trigger transition speed multipliers (x). Lower = smoother.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="92">
-      <ns0:c r="A92" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B92" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C92" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D92" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E92" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F92" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G92" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A92" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Preset Selection</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B92" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Third Person Distribution</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C92" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D92" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>First Person Only</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E92" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>First Person Only | Mixed (Rare Third Person) | Mixed | Mostly Third Person | Third Person Only</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F92" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CameraDistributionProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G92" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Controls how often third-person killcam appears.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="93">
       <ns0:c r="A93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Debug Logging</ns0:t>
+          <ns0:t>Trigger Profile</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>All Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Enable verbose debug logging</ns0:t>
+          <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Reorder menu and refresh mock/builds
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -308,7 +308,7 @@
     <ns0:row r="7">
       <ns0:c r="A7" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B7" t="inlineStr" s="2">
@@ -345,281 +345,281 @@
     <ns0:row r="8">
       <ns0:c r="A8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Debug Logging</ns0:t>
+          <ns0:t>Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>First Person Only</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>First Person Only | Mixed (Rare Third Person) | Mixed | Mostly Third Person | Third Person Only</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CameraDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Enable verbose debug logging</ns0:t>
+          <ns0:t>Controls how often third-person killcam appears.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="9">
       <ns0:c r="A9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Intensity Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Standard</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Subtle | Standard | Dramatic | Cinematic | Epic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>PresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Intensity profile. Subtle = brief, Standard = default, Dramatic = stronger, Cinematic = dramatic, Epic = extreme</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="10">
-      <ns0:c r="A10" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B10" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C10" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D10" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E10" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F10" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G10" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A10" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Preset Selection</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B10" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Chance Preset</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C10" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D10" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (Cooldown Only)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E10" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (Cooldown Only) | Rare | Standard | Frequent</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F10" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>ChancePresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G10" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Sets per-trigger chance values. Off means chance is ignored (cooldown only).</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="11">
       <ns0:c r="A11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera Distance</ns0:t>
+          <ns0:t>Cooldown Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3m</ns0:t>
+          <ns0:t>Standard</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>Off (No Cooldown) | Short | Standard | Long | Extended</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t>CooldownPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
+          <ns0:t>Sets per-trigger cooldown values. Off disables cooldown.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="12">
       <ns0:c r="A12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera Height</ns0:t>
+          <ns0:t>Duration Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
+          <ns0:t>Standard</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>Short | Standard | Long | Extended</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t>DurationPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Sets per-trigger duration values.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="13">
       <ns0:c r="A13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Orbit Speed</ns0:t>
+          <ns0:t>Smoothness Preset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slow</ns0:t>
+          <ns0:t>Standard</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Cinematic | Ultra Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
+          <ns0:t>Sets per-trigger transition speed multipliers (x). Lower = smoother.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="14">
       <ns0:c r="A14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>Preset Selection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize Distance</ns0:t>
+          <ns0:t>Trigger Profile</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>All Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize distance per killcam</ns0:t>
+          <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="15">
       <ns0:c r="A15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize Height</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E15" t="inlineStr" s="0">
@@ -634,266 +634,266 @@
       </ns0:c>
       <ns0:c r="G15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize height per killcam</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="16">
-      <ns0:c r="A16" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B16" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C16" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D16" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E16" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F16" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G16" t="inlineStr" s="0">
+      <ns0:c r="A16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Optional Overrides</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G16" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="17">
-      <ns0:c r="A17" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B17" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C17" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D17" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E17" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F17" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G17" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Optional Overrides</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Global Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CooldownProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="18">
       <ns0:c r="A18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>Optional Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Kill</ns0:t>
+          <ns0:t>Global Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Per Trigger</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>GlobalSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
+          <ns0:t>Override transition speed for all triggers. Per Trigger uses per-trigger smoothing (plus Smoothness Preset).</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>Optional Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Kill</ns0:t>
+          <ns0:t>Haptic Feedback</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off | Light | Medium | Strong</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>HapticIntensityProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>Optional Overrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation</ns0:t>
+          <ns0:t>Dynamic Intensity</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off | Low Sensitivity | Medium Sensitivity | High Sensitivity</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>DynamicIntensityPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
+          <ns0:t>Scale slow-mo start speed based on damage. Low = dampened, High = can reach near-instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
       <ns0:c r="A21" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="22">
+      <ns0:c r="A22" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Dismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="22">
-      <ns0:c r="A22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+      <ns0:c r="B22" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C22" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D22" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E22" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F22" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G22" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -905,7 +905,7 @@
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand</ns0:t>
+          <ns0:t>Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C23" t="inlineStr" s="0">
@@ -930,7 +930,7 @@
       </ns0:c>
       <ns0:c r="G23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -942,32 +942,32 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Threshold</ns0:t>
+          <ns0:t>Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -979,7 +979,7 @@
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry</ns0:t>
+          <ns0:t>Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C25" t="inlineStr" s="0">
@@ -1004,29 +1004,29 @@
       </ns0:c>
       <ns0:c r="G25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on successful weapon deflections</ns0:t>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="26">
       <ns0:c r="A26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E26" t="inlineStr" s="0">
@@ -1041,93 +1041,93 @@
       </ns0:c>
       <ns0:c r="G26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="27">
-      <ns0:c r="A27" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B27" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C27" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D27" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E27" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F27" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G27" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A27" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Triggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B27" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C27" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D27" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E27" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F27" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G27" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="28">
       <ns0:c r="A28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Chance</ns0:t>
+          <ns0:t>Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>25%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="29">
       <ns0:c r="A29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Cooldown</ns0:t>
+          <ns0:t>Last Stand Threshold</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C29" t="inlineStr" s="0">
@@ -1137,145 +1137,145 @@
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>15%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="30">
       <ns0:c r="A30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>CSM Triggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Duration</ns0:t>
+          <ns0:t>Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.0s</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Trigger on successful weapon deflections</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="31">
       <ns0:c r="A31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Smoothing</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>8x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="32">
-      <ns0:c r="A32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Basic Third Person Distribution</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+      <ns0:c r="A32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CSM Killcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="33">
       <ns0:c r="A33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Time Scale</ns0:t>
+          <ns0:t>Camera Distance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C33" t="inlineStr" s="0">
@@ -1285,44 +1285,44 @@
       </ns0:c>
       <ns0:c r="D33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.35x</ns0:t>
+          <ns0:t>3m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G33" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="34">
       <ns0:c r="A34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Randomize Distance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E34" t="inlineStr" s="0">
@@ -1337,93 +1337,93 @@
       </ns0:c>
       <ns0:c r="G34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Randomize distance per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="35">
-      <ns0:c r="A35" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B35" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C35" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D35" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E35" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F35" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G35" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Killcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Camera Height</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>KillcamHeightProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="36">
       <ns0:c r="A36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Chance</ns0:t>
+          <ns0:t>Randomize Height</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>75%</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Randomize height per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="37">
       <ns0:c r="A37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>CSM Killcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Cooldown</ns0:t>
+          <ns0:t>Orbit Speed</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C37" t="inlineStr" s="0">
@@ -1433,108 +1433,108 @@
       </ns0:c>
       <ns0:c r="D37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>Slow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="38">
       <ns0:c r="A38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="39">
-      <ns0:c r="A39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Critical Smoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>8x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+      <ns0:c r="A39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="40">
       <ns0:c r="A40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Third Person Distribution</ns0:t>
+          <ns0:t>Basic Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C40" t="inlineStr" s="0">
@@ -1544,34 +1544,34 @@
       </ns0:c>
       <ns0:c r="D40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>25%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="41">
       <ns0:c r="A41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Time Scale</ns0:t>
+          <ns0:t>Basic Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C41" t="inlineStr" s="0">
@@ -1581,7 +1581,7 @@
       </ns0:c>
       <ns0:c r="D41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.25x</ns0:t>
+          <ns0:t>0.35x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E41" t="inlineStr" s="0">
@@ -1603,86 +1603,86 @@
     <ns0:row r="42">
       <ns0:c r="A42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Basic Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="43">
-      <ns0:c r="A43" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B43" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C43" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D43" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E43" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F43" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G43" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Basic Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>5.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomCooldownProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="44">
       <ns0:c r="A44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Chance</ns0:t>
+          <ns0:t>Basic Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="0">
@@ -1692,34 +1692,34 @@
       </ns0:c>
       <ns0:c r="D44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>90%</ns0:t>
+          <ns0:t>8x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="45">
       <ns0:c r="A45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Cooldown</ns0:t>
+          <ns0:t>Basic Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C45" t="inlineStr" s="0">
@@ -1729,108 +1729,108 @@
       </ns0:c>
       <ns0:c r="D45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4.0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="46">
       <ns0:c r="A46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="47">
-      <ns0:c r="A47" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B47" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Decapitation Smoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C47" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D47" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>6x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E47" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F47" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G47" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+      <ns0:c r="A47" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Critical Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B47" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C47" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D47" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E47" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F47" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G47" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="48">
       <ns0:c r="A48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Third Person Distribution</ns0:t>
+          <ns0:t>Critical Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C48" t="inlineStr" s="0">
@@ -1840,34 +1840,34 @@
       </ns0:c>
       <ns0:c r="D48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>75%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="49">
       <ns0:c r="A49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Time Scale</ns0:t>
+          <ns0:t>Critical Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C49" t="inlineStr" s="0">
@@ -1877,7 +1877,7 @@
       </ns0:c>
       <ns0:c r="D49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.20x</ns0:t>
+          <ns0:t>0.25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E49" t="inlineStr" s="0">
@@ -1899,86 +1899,86 @@
     <ns0:row r="50">
       <ns0:c r="A50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Critical Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="51">
-      <ns0:c r="A51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Critical Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Critical Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>5.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomCooldownProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="52">
       <ns0:c r="A52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Chance</ns0:t>
+          <ns0:t>Critical Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C52" t="inlineStr" s="0">
@@ -1988,34 +1988,34 @@
       </ns0:c>
       <ns0:c r="D52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>60%</ns0:t>
+          <ns0:t>8x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="53">
       <ns0:c r="A53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>Custom: Critical Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Cooldown</ns0:t>
+          <ns0:t>Critical Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C53" t="inlineStr" s="0">
@@ -2025,96 +2025,96 @@
       </ns0:c>
       <ns0:c r="D53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="54">
       <ns0:c r="A54" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="55">
+      <ns0:c r="A55" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B54" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Dismember Duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C54" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D54" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E54" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F54" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G54" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="55">
-      <ns0:c r="A55" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B55" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Dismember Smoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C55" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D55" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>8x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E55" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F55" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G55" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+      <ns0:c r="B55" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C55" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D55" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E55" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F55" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G55" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2126,7 +2126,7 @@
       </ns0:c>
       <ns0:c r="B56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Third Person Distribution</ns0:t>
+          <ns0:t>Dismember Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C56" t="inlineStr" s="0">
@@ -2136,22 +2136,22 @@
       </ns0:c>
       <ns0:c r="D56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>60%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2195,86 +2195,86 @@
     <ns0:row r="58">
       <ns0:c r="A58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Dismember Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="59">
-      <ns0:c r="A59" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B59" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C59" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D59" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E59" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F59" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G59" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Dismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Dismember Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>5.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomCooldownProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="60">
       <ns0:c r="A60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Chance</ns0:t>
+          <ns0:t>Dismember Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C60" t="inlineStr" s="0">
@@ -2284,34 +2284,34 @@
       </ns0:c>
       <ns0:c r="D60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>100%</ns0:t>
+          <ns0:t>8x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="61">
       <ns0:c r="A61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Dismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Cooldown</ns0:t>
+          <ns0:t>Dismember Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C61" t="inlineStr" s="0">
@@ -2321,108 +2321,108 @@
       </ns0:c>
       <ns0:c r="D61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="62">
       <ns0:c r="A62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="63">
-      <ns0:c r="A63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Enemy Smoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>4x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+      <ns0:c r="A63" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B63" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C63" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D63" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E63" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F63" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G63" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="64">
       <ns0:c r="A64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Third Person Distribution</ns0:t>
+          <ns0:t>Decapitation Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C64" t="inlineStr" s="0">
@@ -2432,34 +2432,34 @@
       </ns0:c>
       <ns0:c r="D64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>90%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="65">
       <ns0:c r="A65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Time Scale</ns0:t>
+          <ns0:t>Decapitation Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="0">
@@ -2491,86 +2491,86 @@
     <ns0:row r="66">
       <ns0:c r="A66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Decapitation Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="67">
-      <ns0:c r="A67" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B67" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C67" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D67" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E67" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F67" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G67" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A67" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B67" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Decapitation Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C67" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D67" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>4.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E67" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F67" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomCooldownProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G67" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="68">
       <ns0:c r="A68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Cooldown</ns0:t>
+          <ns0:t>Decapitation Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C68" t="inlineStr" s="0">
@@ -2580,34 +2580,34 @@
       </ns0:c>
       <ns0:c r="D68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>45.0s</ns0:t>
+          <ns0:t>6x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="69">
       <ns0:c r="A69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>Custom: Decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Duration</ns0:t>
+          <ns0:t>Decapitation Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C69" t="inlineStr" s="0">
@@ -2617,182 +2617,182 @@
       </ns0:c>
       <ns0:c r="D69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="70">
       <ns0:c r="A70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Smoothing</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="71">
-      <ns0:c r="A71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Stand Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.15x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="A71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="72">
       <ns0:c r="A72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Last Enemy Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="73">
-      <ns0:c r="A73" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B73" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C73" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D73" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E73" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F73" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G73" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A73" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B73" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Enemy Time Scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C73" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D73" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.20x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E73" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F73" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G73" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="74">
       <ns0:c r="A74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Chance</ns0:t>
+          <ns0:t>Last Enemy Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C74" t="inlineStr" s="0">
@@ -2802,34 +2802,34 @@
       </ns0:c>
       <ns0:c r="D74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>50%</ns0:t>
+          <ns0:t>3.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="75">
       <ns0:c r="A75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Cooldown</ns0:t>
+          <ns0:t>Last Enemy Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="0">
@@ -2839,7 +2839,7 @@
       </ns0:c>
       <ns0:c r="D75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>7.0s</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E75" t="inlineStr" s="0">
@@ -2861,12 +2861,12 @@
     <ns0:row r="76">
       <ns0:c r="A76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Duration</ns0:t>
+          <ns0:t>Last Enemy Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C76" t="inlineStr" s="0">
@@ -2876,34 +2876,34 @@
       </ns0:c>
       <ns0:c r="D76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.2s</ns0:t>
+          <ns0:t>4x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="77">
       <ns0:c r="A77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>Custom: Last Enemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Smoothing</ns0:t>
+          <ns0:t>Last Enemy Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C77" t="inlineStr" s="0">
@@ -2913,182 +2913,182 @@
       </ns0:c>
       <ns0:c r="D77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10x</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="78">
       <ns0:c r="A78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Time Scale</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.30x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E78" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F78" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G78" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="79">
+      <ns0:c r="A79" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B79" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C79" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D79" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E79" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F79" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G79" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="80">
+      <ns0:c r="A80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Stand Time Scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.15x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E80" t="inlineStr" s="0">
+        <ns0:is>
           <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F78" t="inlineStr" s="0">
+      <ns0:c r="F80" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="G78" t="inlineStr" s="0">
+      <ns0:c r="G80" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="79">
-      <ns0:c r="A79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="80">
-      <ns0:c r="A80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="81">
       <ns0:c r="A81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dynamic Intensity</ns0:t>
+          <ns0:t>Last Stand Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Low Sensitivity | Medium Sensitivity | High Sensitivity</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>DynamicIntensityPresetProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Scale slow-mo start speed based on damage. Low = dampened, High = can reach near-instant.</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="82">
       <ns0:c r="A82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Cooldown</ns0:t>
+          <ns0:t>Last Stand Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="0">
@@ -3098,34 +3098,34 @@
       </ns0:c>
       <ns0:c r="D82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>45.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CooldownProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="83">
       <ns0:c r="A83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>Custom: Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Smoothing</ns0:t>
+          <ns0:t>Last Stand Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="0">
@@ -3135,392 +3135,392 @@
       </ns0:c>
       <ns0:c r="D83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger</ns0:t>
+          <ns0:t>4x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>GlobalSmoothingProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Override transition speed for all triggers. Per Trigger uses per-trigger smoothing (plus Smoothness Preset).</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="84">
       <ns0:c r="A84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Haptic Feedback</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>HapticIntensityProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="85">
-      <ns0:c r="A85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F85" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G85" t="inlineStr" s="0">
+      <ns0:c r="A85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>Custom: Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F85" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G85" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="86">
-      <ns0:c r="A86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Custom: Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Parry Chance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>50%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomChanceProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="87">
       <ns0:c r="A87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance Preset</ns0:t>
+          <ns0:t>Parry Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (Cooldown Only)</ns0:t>
+          <ns0:t>0.30x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (Cooldown Only) | Rare | Standard | Frequent</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ChancePresetProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger chance values. Off means chance is ignored (cooldown only).</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="88">
       <ns0:c r="A88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown Preset</ns0:t>
+          <ns0:t>Parry Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Standard</ns0:t>
+          <ns0:t>1.2s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (No Cooldown) | Short | Standard | Long | Extended</ns0:t>
+          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CooldownPresetProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger cooldown values. Off disables cooldown.</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
       <ns0:c r="A89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration Preset</ns0:t>
+          <ns0:t>Parry Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Standard</ns0:t>
+          <ns0:t>7.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Short | Standard | Long | Extended</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>DurationPresetProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger duration values.</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="90">
       <ns0:c r="A90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>Custom: Parry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Intensity Preset</ns0:t>
+          <ns0:t>Parry Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Standard</ns0:t>
+          <ns0:t>10x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Subtle | Standard | Dramatic | Cinematic | Epic</ns0:t>
+          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>PresetProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Intensity profile. Subtle = brief, Standard = default, Dramatic = stronger, Cinematic = dramatic, Epic = extreme</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="91">
       <ns0:c r="A91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smoothness Preset</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Standard</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Cinematic | Ultra Smooth</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger transition speed multipliers (x). Lower = smoother.</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="92">
-      <ns0:c r="A92" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B92" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Third Person Distribution</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C92" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D92" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>First Person Only</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E92" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>First Person Only | Mixed (Rare Third Person) | Mixed | Mostly Third Person | Third Person Only</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F92" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CameraDistributionProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G92" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Controls how often third-person killcam appears.</ns0:t>
+      <ns0:c r="A92" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B92" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C92" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D92" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E92" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F92" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G92" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="93">
       <ns0:c r="A93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CSM Advanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger Profile</ns0:t>
+          <ns0:t>Debug Logging</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>All Triggers</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerProfileProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
+          <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Add debug diagnostics and quick test controls
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -3524,6 +3524,450 @@
         </ns0:is>
       </ns0:c>
     </ns0:row>
+    <ns0:row r="94">
+      <ns0:c r="A94" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B94" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Show Effective Values</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C94" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D94" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E94" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F94" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G94" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Show effective per-trigger values after presets and overrides</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="95">
+      <ns0:c r="A95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Trigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>None</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>LastTriggerProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last trigger attempt</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="96">
+      <ns0:c r="A96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Trigger Reason</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>None</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>LastTriggerReasonProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Why the last trigger did or didn't fire</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="97">
+      <ns0:c r="A97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Quick Test Trigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Basic Kill | Critical Kill | Dismemberment | Decapitation | Parry | Last Enemy | Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Which trigger to simulate</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="98">
+      <ns0:c r="A98" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B98" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Quick Test Now</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C98" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D98" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E98" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F98" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G98" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle to fire the selected trigger once</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="99">
+      <ns0:c r="A99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Effective: Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>EffectiveBasicProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Effective values for Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="100">
+      <ns0:c r="A100" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B100" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Effective: Critical Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C100" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D100" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E100" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F100" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>EffectiveCriticalProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G100" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Effective values for Critical Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="101">
+      <ns0:c r="A101" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B101" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Effective: Dismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C101" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D101" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E101" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F101" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>EffectiveDismembermentProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G101" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Effective values for Dismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="102">
+      <ns0:c r="A102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Effective: Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>EffectiveDecapitationProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Effective values for Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="103">
+      <ns0:c r="A103" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B103" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Effective: Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C103" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D103" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E103" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F103" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>EffectiveParryProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G103" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Effective values for Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="104">
+      <ns0:c r="A104" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B104" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Effective: Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C104" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D104" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E104" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F104" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>EffectiveLastEnemyProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G104" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Effective values for Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="105">
+      <ns0:c r="A105" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CSM Advanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B105" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Effective: Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C105" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D105" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E105" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F105" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>EffectiveLastStandProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G105" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Effective values for Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
   </ns0:sheetData>
 </ns0:worksheet>
 </file>
@@ -3742,142 +4186,262 @@
     <ns0:row r="18">
       <ns0:c r="A18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>GlobalSmoothingProvider</ns0:t>
+          <ns0:t>EffectiveBasicProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>HapticIntensityProvider</ns0:t>
+          <ns0:t>EffectiveCriticalProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t>EffectiveDecapitationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
       <ns0:c r="A21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t>EffectiveDismembermentProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
       <ns0:c r="A22" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t>EffectiveLastEnemyProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B22" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="23">
       <ns0:c r="A23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>MinEnemyGroupProvider</ns0:t>
+          <ns0:t>EffectiveLastStandProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="24">
       <ns0:c r="A24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>PresetProvider</ns0:t>
+          <ns0:t>EffectiveParryProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Subtle | Standard | Dramatic | Cinematic | Epic</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothingSpeedProvider</ns0:t>
+          <ns0:t>GlobalSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Instant | Fast | Medium | Slow</ns0:t>
+          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="26">
       <ns0:c r="A26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>HapticIntensityProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Cinematic | Ultra Smooth</ns0:t>
+          <ns0:t>Off | Light | Medium | Strong</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="27">
       <ns0:c r="A27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="28">
       <ns0:c r="A28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TimeScaleProvider</ns0:t>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="29">
       <ns0:c r="A29" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B29" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="30">
+      <ns0:c r="A30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>LastTriggerProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="31">
+      <ns0:c r="A31" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>LastTriggerReasonProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B31" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="32">
+      <ns0:c r="A32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>MinEnemyGroupProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="33">
+      <ns0:c r="A33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>PresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Subtle | Standard | Dramatic | Cinematic | Epic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="34">
+      <ns0:c r="A34" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B34" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Basic Kill | Critical Kill | Dismemberment | Decapitation | Parry | Last Enemy | Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="35">
+      <ns0:c r="A35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>SmoothingSpeedProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Instant | Fast | Medium | Slow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="36">
+      <ns0:c r="A36" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B36" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Cinematic | Ultra Smooth</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="37">
+      <ns0:c r="A37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>ThresholdProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="38">
+      <ns0:c r="A38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>TimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="39">
+      <ns0:c r="A39" t="inlineStr" s="0">
+        <ns0:is>
           <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B29" t="inlineStr" s="0">
+      <ns0:c r="B39" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only</ns0:t>
         </ns0:is>

</xml_diff>

<commit_message>
Fix preset sync and menu ordering
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -757,12 +757,12 @@
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Haptic Feedback</ns0:t>
+          <ns0:t>Dynamic Intensity</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D19" t="inlineStr" s="0">
@@ -772,17 +772,17 @@
       </ns0:c>
       <ns0:c r="E19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t>Off | Low Sensitivity | Medium Sensitivity | High Sensitivity</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>HapticIntensityProvider</ns0:t>
+          <ns0:t>DynamicIntensityPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
+          <ns0:t>Scale slow-mo start speed based on damage. Low = dampened, High = can reach near-instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -794,12 +794,12 @@
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dynamic Intensity</ns0:t>
+          <ns0:t>Haptic Feedback</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D20" t="inlineStr" s="0">
@@ -809,17 +809,17 @@
       </ns0:c>
       <ns0:c r="E20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Low Sensitivity | Medium Sensitivity | High Sensitivity</ns0:t>
+          <ns0:t>Off | Light | Medium | Strong</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>DynamicIntensityPresetProvider</ns0:t>
+          <ns0:t>HapticIntensityProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Scale slow-mo start speed based on damage. Low = dampened, High = can reach near-instant.</ns0:t>
+          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Tie effective values to debug logging and trim advanced UI
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -3532,32 +3532,32 @@
       </ns0:c>
       <ns0:c r="B94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Show Effective Values</ns0:t>
+          <ns0:t>Quick Test Trigger</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>Basic Kill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Basic Kill | Critical Kill | Dismemberment | Decapitation | Parry | Last Enemy | Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Show effective per-trigger values after presets and overrides</ns0:t>
+          <ns0:t>Which trigger to simulate</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3569,17 +3569,17 @@
       </ns0:c>
       <ns0:c r="B95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Trigger</ns0:t>
+          <ns0:t>Quick Test Now</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>None</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E95" t="inlineStr" s="0">
@@ -3589,382 +3589,12 @@
       </ns0:c>
       <ns0:c r="F95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>LastTriggerProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last trigger attempt</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="96">
-      <ns0:c r="A96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Last Trigger Reason</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>None</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>LastTriggerReasonProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Why the last trigger did or didn't fire</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="97">
-      <ns0:c r="A97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Quick Test Trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Basic Kill | Critical Kill | Dismemberment | Decapitation | Parry | Last Enemy | Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>QuickTestTriggerProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Which trigger to simulate</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="98">
-      <ns0:c r="A98" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B98" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Quick Test Now</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C98" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D98" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E98" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F98" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G98" t="inlineStr" s="0">
-        <ns0:is>
           <ns0:t>Toggle to fire the selected trigger once</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="99">
-      <ns0:c r="A99" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B99" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Effective: Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C99" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D99" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E99" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F99" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>EffectiveBasicProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G99" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Effective values for Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="100">
-      <ns0:c r="A100" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B100" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Effective: Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C100" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D100" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E100" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F100" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>EffectiveCriticalProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G100" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Effective values for Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="101">
-      <ns0:c r="A101" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B101" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Effective: Dismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C101" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D101" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E101" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F101" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>EffectiveDismembermentProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G101" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Effective values for Dismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="102">
-      <ns0:c r="A102" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B102" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Effective: Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C102" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D102" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E102" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F102" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>EffectiveDecapitationProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G102" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Effective values for Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="103">
-      <ns0:c r="A103" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B103" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Effective: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C103" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D103" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E103" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F103" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>EffectiveParryProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G103" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Effective values for Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="104">
-      <ns0:c r="A104" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B104" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Effective: Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C104" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D104" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E104" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F104" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>EffectiveLastEnemyProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G104" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Effective values for Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="105">
-      <ns0:c r="A105" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B105" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Effective: Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C105" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D105" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E105" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F105" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>EffectiveLastStandProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G105" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Effective values for Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -4186,262 +3816,154 @@
     <ns0:row r="18">
       <ns0:c r="A18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>EffectiveBasicProvider</ns0:t>
+          <ns0:t>GlobalSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>EffectiveCriticalProvider</ns0:t>
+          <ns0:t>HapticIntensityProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off | Light | Medium | Strong</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>EffectiveDecapitationProvider</ns0:t>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
       <ns0:c r="A21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>EffectiveDismembermentProvider</ns0:t>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
       <ns0:c r="A22" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>EffectiveLastEnemyProvider</ns0:t>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B22" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="23">
       <ns0:c r="A23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>EffectiveLastStandProvider</ns0:t>
+          <ns0:t>MinEnemyGroupProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="24">
       <ns0:c r="A24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>EffectiveParryProvider</ns0:t>
+          <ns0:t>PresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Subtle | Standard | Dramatic | Cinematic | Epic</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>GlobalSmoothingProvider</ns0:t>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
+          <ns0:t>Basic Kill | Critical Kill | Dismemberment | Decapitation | Parry | Last Enemy | Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="26">
       <ns0:c r="A26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>HapticIntensityProvider</ns0:t>
+          <ns0:t>SmoothingSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t>Instant | Fast | Medium | Slow</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="27">
       <ns0:c r="A27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Cinematic | Ultra Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="28">
       <ns0:c r="A28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="29">
       <ns0:c r="A29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t>TimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="30">
       <ns0:c r="A30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>LastTriggerProvider</ns0:t>
+          <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="31">
-      <ns0:c r="A31" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>LastTriggerReasonProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B31" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="32">
-      <ns0:c r="A32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>MinEnemyGroupProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="33">
-      <ns0:c r="A33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>PresetProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Subtle | Standard | Dramatic | Cinematic | Epic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="34">
-      <ns0:c r="A34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>QuickTestTriggerProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Basic Kill | Critical Kill | Dismemberment | Decapitation | Parry | Last Enemy | Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="35">
-      <ns0:c r="A35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>SmoothingSpeedProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B35" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Instant | Fast | Medium | Slow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="36">
-      <ns0:c r="A36" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B36" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Cinematic | Ultra Smooth</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="37">
-      <ns0:c r="A37" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B37" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="38">
-      <ns0:c r="A38" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>TimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B38" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="39">
-      <ns0:c r="A39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>TriggerProfileProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B39" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only</ns0:t>
         </ns0:is>

</xml_diff>

<commit_message>
Expand preset ranges and shorten mod name
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -1618,12 +1618,12 @@
       </ns0:c>
       <ns0:c r="D42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.0s</ns0:t>
+          <ns0:t>0.75s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F42" t="inlineStr" s="0">
@@ -1655,12 +1655,12 @@
       </ns0:c>
       <ns0:c r="D43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>4.9s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F43" t="inlineStr" s="0">
@@ -1692,12 +1692,12 @@
       </ns0:c>
       <ns0:c r="D44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>8x</ns0:t>
+          <ns0:t>5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="0">
@@ -1914,12 +1914,12 @@
       </ns0:c>
       <ns0:c r="D50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>1.2s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F50" t="inlineStr" s="0">
@@ -1951,12 +1951,12 @@
       </ns0:c>
       <ns0:c r="D51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>4.9s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F51" t="inlineStr" s="0">
@@ -1988,12 +1988,12 @@
       </ns0:c>
       <ns0:c r="D52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>8x</ns0:t>
+          <ns0:t>5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="0">
@@ -2210,12 +2210,12 @@
       </ns0:c>
       <ns0:c r="D58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>1.2s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="0">
@@ -2247,12 +2247,12 @@
       </ns0:c>
       <ns0:c r="D59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>4.9s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F59" t="inlineStr" s="0">
@@ -2284,12 +2284,12 @@
       </ns0:c>
       <ns0:c r="D60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>8x</ns0:t>
+          <ns0:t>5x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="0">
@@ -2506,12 +2506,12 @@
       </ns0:c>
       <ns0:c r="D66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.0s</ns0:t>
+          <ns0:t>1.8s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="0">
@@ -2543,12 +2543,12 @@
       </ns0:c>
       <ns0:c r="D67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4.0s</ns0:t>
+          <ns0:t>3.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F67" t="inlineStr" s="0">
@@ -2580,12 +2580,12 @@
       </ns0:c>
       <ns0:c r="D68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>6x</ns0:t>
+          <ns0:t>4x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="0">
@@ -2802,12 +2802,12 @@
       </ns0:c>
       <ns0:c r="D74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.0s</ns0:t>
+          <ns0:t>2.25s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="0">
@@ -2844,7 +2844,7 @@
       </ns0:c>
       <ns0:c r="E75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F75" t="inlineStr" s="0">
@@ -2876,12 +2876,12 @@
       </ns0:c>
       <ns0:c r="D76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4x</ns0:t>
+          <ns0:t>2.4x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="0">
@@ -3061,12 +3061,12 @@
       </ns0:c>
       <ns0:c r="D81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>3.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="0">
@@ -3098,12 +3098,12 @@
       </ns0:c>
       <ns0:c r="D82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>45.0s</ns0:t>
+          <ns0:t>10.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="0">
@@ -3135,12 +3135,12 @@
       </ns0:c>
       <ns0:c r="D83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4x</ns0:t>
+          <ns0:t>2.4x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="0">
@@ -3320,12 +3320,12 @@
       </ns0:c>
       <ns0:c r="D88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.2s</ns0:t>
+          <ns0:t>1.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="0">
@@ -3357,12 +3357,12 @@
       </ns0:c>
       <ns0:c r="D89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>7.0s</ns0:t>
+          <ns0:t>6.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="0">
@@ -3394,12 +3394,12 @@
       </ns0:c>
       <ns0:c r="D90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10x</ns0:t>
+          <ns0:t>6x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F90" t="inlineStr" s="0">
@@ -3725,7 +3725,7 @@
       </ns0:c>
       <ns0:c r="B10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 10.5s | 18.0s | 31.5s | 45.0s | 67.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3737,7 +3737,7 @@
       </ns0:c>
       <ns0:c r="B11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.5s | 3.0s | 3.75s | 4.5s | 5.0s | 6.25s | 7.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3749,7 +3749,7 @@
       </ns0:c>
       <ns0:c r="B12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x | 3x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 10x | 12.5x</ns0:t>
+          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Adjust preset gaps and expand custom value ranges
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -1618,12 +1618,12 @@
       </ns0:c>
       <ns0:c r="D42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.75s</ns0:t>
+          <ns0:t>0.72s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F42" t="inlineStr" s="0">
@@ -1655,12 +1655,12 @@
       </ns0:c>
       <ns0:c r="D43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4.9s</ns0:t>
+          <ns0:t>3.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F43" t="inlineStr" s="0">
@@ -1692,12 +1692,12 @@
       </ns0:c>
       <ns0:c r="D44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5x</ns0:t>
+          <ns0:t>3.6x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="0">
@@ -1914,12 +1914,12 @@
       </ns0:c>
       <ns0:c r="D50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.2s</ns0:t>
+          <ns0:t>1.125s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F50" t="inlineStr" s="0">
@@ -1951,12 +1951,12 @@
       </ns0:c>
       <ns0:c r="D51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4.9s</ns0:t>
+          <ns0:t>3.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F51" t="inlineStr" s="0">
@@ -1988,12 +1988,12 @@
       </ns0:c>
       <ns0:c r="D52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5x</ns0:t>
+          <ns0:t>3.6x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="0">
@@ -2210,12 +2210,12 @@
       </ns0:c>
       <ns0:c r="D58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.2s</ns0:t>
+          <ns0:t>1.125s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="0">
@@ -2247,12 +2247,12 @@
       </ns0:c>
       <ns0:c r="D59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4.9s</ns0:t>
+          <ns0:t>3.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F59" t="inlineStr" s="0">
@@ -2284,12 +2284,12 @@
       </ns0:c>
       <ns0:c r="D60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5x</ns0:t>
+          <ns0:t>3.6x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="0">
@@ -2506,12 +2506,12 @@
       </ns0:c>
       <ns0:c r="D66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.8s</ns0:t>
+          <ns0:t>1.4s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="0">
@@ -2543,12 +2543,12 @@
       </ns0:c>
       <ns0:c r="D67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.5s</ns0:t>
+          <ns0:t>2.8s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F67" t="inlineStr" s="0">
@@ -2580,12 +2580,12 @@
       </ns0:c>
       <ns0:c r="D68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4x</ns0:t>
+          <ns0:t>3x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="0">
@@ -2802,12 +2802,12 @@
       </ns0:c>
       <ns0:c r="D74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.25s</ns0:t>
+          <ns0:t>1.8s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="0">
@@ -2844,7 +2844,7 @@
       </ns0:c>
       <ns0:c r="E75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F75" t="inlineStr" s="0">
@@ -2876,12 +2876,12 @@
       </ns0:c>
       <ns0:c r="D76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.4x</ns0:t>
+          <ns0:t>2x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="0">
@@ -3061,12 +3061,12 @@
       </ns0:c>
       <ns0:c r="D81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.0s</ns0:t>
+          <ns0:t>2.1s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="0">
@@ -3098,12 +3098,12 @@
       </ns0:c>
       <ns0:c r="D82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10.5s</ns0:t>
+          <ns0:t>7.2s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="0">
@@ -3135,12 +3135,12 @@
       </ns0:c>
       <ns0:c r="D83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.4x</ns0:t>
+          <ns0:t>2x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="0">
@@ -3320,12 +3320,12 @@
       </ns0:c>
       <ns0:c r="D88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.0s</ns0:t>
+          <ns0:t>0.90s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="0">
@@ -3357,12 +3357,12 @@
       </ns0:c>
       <ns0:c r="D89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>6.0s</ns0:t>
+          <ns0:t>4.2s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="0">
@@ -3394,12 +3394,12 @@
       </ns0:c>
       <ns0:c r="D90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>6x</ns0:t>
+          <ns0:t>4x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F90" t="inlineStr" s="0">
@@ -3725,7 +3725,7 @@
       </ns0:c>
       <ns0:c r="B10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.5s | 2.8s | 3.5s | 4.0s | 4.9s | 5.0s | 6.0s | 7.0s | 7.5s | 8.0s | 10.0s | 10.5s | 14.0s | 17.5s | 18.0s | 22.5s | 24.5s | 28.0s | 31.5s | 45.0s | 67.5s | 90.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3737,7 +3737,7 @@
       </ns0:c>
       <ns0:c r="B11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.5s | 1.8s | 1.875s | 2.0s | 2.25s | 2.4s | 2.5s | 3.0s | 3.75s | 4.0s | 4.5s | 5.0s | 6.0s | 6.25s | 7.5s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3749,7 +3749,7 @@
       </ns0:c>
       <ns0:c r="B12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 2x | 2.4x | 3x | 3.2x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 20x | 25x</ns0:t>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Normalize preset option counts and add Parry Only profile
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -439,7 +439,7 @@
       </ns0:c>
       <ns0:c r="E10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (Cooldown Only) | Rare | Standard | Frequent</ns0:t>
+          <ns0:t>Off (Cooldown Only) | Very Rare | Rare | Standard | Frequent</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F10" t="inlineStr" s="0">
@@ -513,7 +513,7 @@
       </ns0:c>
       <ns0:c r="E12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Short | Standard | Long | Extended</ns0:t>
+          <ns0:t>Very Short | Short | Standard | Long | Extended</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F12" t="inlineStr" s="0">
@@ -550,7 +550,7 @@
       </ns0:c>
       <ns0:c r="E13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Cinematic | Ultra Smooth</ns0:t>
+          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Ultra Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F13" t="inlineStr" s="0">
@@ -587,7 +587,7 @@
       </ns0:c>
       <ns0:c r="E14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only</ns0:t>
+          <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only | Parry Only</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F14" t="inlineStr" s="0">
@@ -1549,7 +1549,7 @@
       </ns0:c>
       <ns0:c r="E40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F40" t="inlineStr" s="0">
@@ -1618,7 +1618,7 @@
       </ns0:c>
       <ns0:c r="D42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.72s</ns0:t>
+          <ns0:t>1.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E42" t="inlineStr" s="0">
@@ -1655,7 +1655,7 @@
       </ns0:c>
       <ns0:c r="D43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.5s</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E43" t="inlineStr" s="0">
@@ -1692,7 +1692,7 @@
       </ns0:c>
       <ns0:c r="D44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.6x</ns0:t>
+          <ns0:t>8x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E44" t="inlineStr" s="0">
@@ -1845,7 +1845,7 @@
       </ns0:c>
       <ns0:c r="E48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F48" t="inlineStr" s="0">
@@ -1914,7 +1914,7 @@
       </ns0:c>
       <ns0:c r="D50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.125s</ns0:t>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E50" t="inlineStr" s="0">
@@ -1951,7 +1951,7 @@
       </ns0:c>
       <ns0:c r="D51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.5s</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E51" t="inlineStr" s="0">
@@ -1988,7 +1988,7 @@
       </ns0:c>
       <ns0:c r="D52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.6x</ns0:t>
+          <ns0:t>8x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E52" t="inlineStr" s="0">
@@ -2141,7 +2141,7 @@
       </ns0:c>
       <ns0:c r="E56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F56" t="inlineStr" s="0">
@@ -2210,7 +2210,7 @@
       </ns0:c>
       <ns0:c r="D58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.125s</ns0:t>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E58" t="inlineStr" s="0">
@@ -2247,7 +2247,7 @@
       </ns0:c>
       <ns0:c r="D59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.5s</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E59" t="inlineStr" s="0">
@@ -2284,7 +2284,7 @@
       </ns0:c>
       <ns0:c r="D60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.6x</ns0:t>
+          <ns0:t>8x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E60" t="inlineStr" s="0">
@@ -2437,7 +2437,7 @@
       </ns0:c>
       <ns0:c r="E64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F64" t="inlineStr" s="0">
@@ -2506,7 +2506,7 @@
       </ns0:c>
       <ns0:c r="D66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.4s</ns0:t>
+          <ns0:t>2.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E66" t="inlineStr" s="0">
@@ -2543,7 +2543,7 @@
       </ns0:c>
       <ns0:c r="D67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.8s</ns0:t>
+          <ns0:t>4.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E67" t="inlineStr" s="0">
@@ -2580,7 +2580,7 @@
       </ns0:c>
       <ns0:c r="D68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3x</ns0:t>
+          <ns0:t>6x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E68" t="inlineStr" s="0">
@@ -2733,7 +2733,7 @@
       </ns0:c>
       <ns0:c r="E72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F72" t="inlineStr" s="0">
@@ -2802,7 +2802,7 @@
       </ns0:c>
       <ns0:c r="D74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.8s</ns0:t>
+          <ns0:t>3.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E74" t="inlineStr" s="0">
@@ -2876,7 +2876,7 @@
       </ns0:c>
       <ns0:c r="D76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x</ns0:t>
+          <ns0:t>4x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E76" t="inlineStr" s="0">
@@ -3061,7 +3061,7 @@
       </ns0:c>
       <ns0:c r="D81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.1s</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E81" t="inlineStr" s="0">
@@ -3098,7 +3098,7 @@
       </ns0:c>
       <ns0:c r="D82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>7.2s</ns0:t>
+          <ns0:t>45.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E82" t="inlineStr" s="0">
@@ -3135,7 +3135,7 @@
       </ns0:c>
       <ns0:c r="D83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2x</ns0:t>
+          <ns0:t>4x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E83" t="inlineStr" s="0">
@@ -3251,7 +3251,7 @@
       </ns0:c>
       <ns0:c r="E86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F86" t="inlineStr" s="0">
@@ -3320,7 +3320,7 @@
       </ns0:c>
       <ns0:c r="D88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.90s</ns0:t>
+          <ns0:t>1.2s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
@@ -3357,7 +3357,7 @@
       </ns0:c>
       <ns0:c r="D89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4.2s</ns0:t>
+          <ns0:t>7.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E89" t="inlineStr" s="0">
@@ -3394,7 +3394,7 @@
       </ns0:c>
       <ns0:c r="D90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4x</ns0:t>
+          <ns0:t>10x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E90" t="inlineStr" s="0">
@@ -3665,7 +3665,7 @@
       </ns0:c>
       <ns0:c r="B5" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (Cooldown Only) | Rare | Standard | Frequent</ns0:t>
+          <ns0:t>Off (Cooldown Only) | Very Rare | Rare | Standard | Frequent</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3713,7 +3713,7 @@
       </ns0:c>
       <ns0:c r="B9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15% | 25% | 30% | 35% | 36% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3785,7 +3785,7 @@
       </ns0:c>
       <ns0:c r="B15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Short | Standard | Long | Extended</ns0:t>
+          <ns0:t>Very Short | Short | Standard | Long | Extended</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3929,7 +3929,7 @@
       </ns0:c>
       <ns0:c r="B27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Cinematic | Ultra Smooth</ns0:t>
+          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Ultra Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3965,7 +3965,7 @@
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only</ns0:t>
+          <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only | Parry Only</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Fix cooldown preset sync and custom labels
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -75,7 +75,7 @@
 <ns0:worksheet xmlns:ns0="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <ns0:cols>
     <ns0:col min="1" max="1" width="23.00" customWidth="1"/>
-    <ns0:col min="2" max="2" width="40.00" customWidth="1"/>
+    <ns0:col min="2" max="2" width="27.00" customWidth="1"/>
     <ns0:col min="3" max="3" width="9.00" customWidth="1"/>
     <ns0:col min="4" max="4" width="21.00" customWidth="1"/>
     <ns0:col min="5" max="5" width="60.00" customWidth="1"/>
@@ -1534,7 +1534,7 @@
       </ns0:c>
       <ns0:c r="B40" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Chance</ns0:t>
+          <ns0:t>Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C40" t="inlineStr" s="0">
@@ -1571,7 +1571,7 @@
       </ns0:c>
       <ns0:c r="B41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Time Scale</ns0:t>
+          <ns0:t>Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C41" t="inlineStr" s="0">
@@ -1608,7 +1608,7 @@
       </ns0:c>
       <ns0:c r="B42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Duration</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C42" t="inlineStr" s="0">
@@ -1645,7 +1645,7 @@
       </ns0:c>
       <ns0:c r="B43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Cooldown</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C43" t="inlineStr" s="0">
@@ -1682,7 +1682,7 @@
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Smoothing</ns0:t>
+          <ns0:t>Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="0">
@@ -1719,7 +1719,7 @@
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Third Person Distribution</ns0:t>
+          <ns0:t>Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C45" t="inlineStr" s="0">
@@ -1830,7 +1830,7 @@
       </ns0:c>
       <ns0:c r="B48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Chance</ns0:t>
+          <ns0:t>Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C48" t="inlineStr" s="0">
@@ -1867,7 +1867,7 @@
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Time Scale</ns0:t>
+          <ns0:t>Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C49" t="inlineStr" s="0">
@@ -1904,7 +1904,7 @@
       </ns0:c>
       <ns0:c r="B50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Duration</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C50" t="inlineStr" s="0">
@@ -1941,7 +1941,7 @@
       </ns0:c>
       <ns0:c r="B51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Cooldown</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C51" t="inlineStr" s="0">
@@ -1978,7 +1978,7 @@
       </ns0:c>
       <ns0:c r="B52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Smoothing</ns0:t>
+          <ns0:t>Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C52" t="inlineStr" s="0">
@@ -2015,7 +2015,7 @@
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Third Person Distribution</ns0:t>
+          <ns0:t>Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C53" t="inlineStr" s="0">
@@ -2126,7 +2126,7 @@
       </ns0:c>
       <ns0:c r="B56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Chance</ns0:t>
+          <ns0:t>Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C56" t="inlineStr" s="0">
@@ -2163,7 +2163,7 @@
       </ns0:c>
       <ns0:c r="B57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Time Scale</ns0:t>
+          <ns0:t>Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C57" t="inlineStr" s="0">
@@ -2200,7 +2200,7 @@
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Duration</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C58" t="inlineStr" s="0">
@@ -2237,7 +2237,7 @@
       </ns0:c>
       <ns0:c r="B59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Cooldown</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C59" t="inlineStr" s="0">
@@ -2274,7 +2274,7 @@
       </ns0:c>
       <ns0:c r="B60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Smoothing</ns0:t>
+          <ns0:t>Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C60" t="inlineStr" s="0">
@@ -2311,7 +2311,7 @@
       </ns0:c>
       <ns0:c r="B61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismember Third Person Distribution</ns0:t>
+          <ns0:t>Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C61" t="inlineStr" s="0">
@@ -2422,7 +2422,7 @@
       </ns0:c>
       <ns0:c r="B64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Chance</ns0:t>
+          <ns0:t>Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C64" t="inlineStr" s="0">
@@ -2459,7 +2459,7 @@
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Time Scale</ns0:t>
+          <ns0:t>Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="0">
@@ -2496,7 +2496,7 @@
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Duration</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="0">
@@ -2533,7 +2533,7 @@
       </ns0:c>
       <ns0:c r="B67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Cooldown</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C67" t="inlineStr" s="0">
@@ -2570,7 +2570,7 @@
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Smoothing</ns0:t>
+          <ns0:t>Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C68" t="inlineStr" s="0">
@@ -2607,7 +2607,7 @@
       </ns0:c>
       <ns0:c r="B69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation Third Person Distribution</ns0:t>
+          <ns0:t>Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C69" t="inlineStr" s="0">
@@ -2718,7 +2718,7 @@
       </ns0:c>
       <ns0:c r="B72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Chance</ns0:t>
+          <ns0:t>Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C72" t="inlineStr" s="0">
@@ -2755,7 +2755,7 @@
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Time Scale</ns0:t>
+          <ns0:t>Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C73" t="inlineStr" s="0">
@@ -2792,7 +2792,7 @@
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Duration</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C74" t="inlineStr" s="0">
@@ -2829,7 +2829,7 @@
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Cooldown</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="0">
@@ -2866,7 +2866,7 @@
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Smoothing</ns0:t>
+          <ns0:t>Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C76" t="inlineStr" s="0">
@@ -2903,7 +2903,7 @@
       </ns0:c>
       <ns0:c r="B77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy Third Person Distribution</ns0:t>
+          <ns0:t>Third Person Distribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C77" t="inlineStr" s="0">
@@ -3014,7 +3014,7 @@
       </ns0:c>
       <ns0:c r="B80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Time Scale</ns0:t>
+          <ns0:t>Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C80" t="inlineStr" s="0">
@@ -3051,7 +3051,7 @@
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Duration</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="0">
@@ -3088,7 +3088,7 @@
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Cooldown</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="0">
@@ -3125,7 +3125,7 @@
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Smoothing</ns0:t>
+          <ns0:t>Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="0">
@@ -3236,7 +3236,7 @@
       </ns0:c>
       <ns0:c r="B86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Chance</ns0:t>
+          <ns0:t>Chance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C86" t="inlineStr" s="0">
@@ -3273,7 +3273,7 @@
       </ns0:c>
       <ns0:c r="B87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Time Scale</ns0:t>
+          <ns0:t>Time Scale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C87" t="inlineStr" s="0">
@@ -3310,7 +3310,7 @@
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Duration</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="0">
@@ -3347,7 +3347,7 @@
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Cooldown</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C89" t="inlineStr" s="0">
@@ -3384,7 +3384,7 @@
       </ns0:c>
       <ns0:c r="B90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry Smoothing</ns0:t>
+          <ns0:t>Smoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C90" t="inlineStr" s="0">

</xml_diff>

<commit_message>
Add thrown impact kill toggle and detection
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -74,10 +74,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <ns0:worksheet xmlns:ns0="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <ns0:cols>
-    <ns0:col min="1" max="1" width="23.00" customWidth="1"/>
-    <ns0:col min="2" max="2" width="27.00" customWidth="1"/>
+    <ns0:col min="1" max="1" width="29.00" customWidth="1"/>
+    <ns0:col min="2" max="2" width="31.00" customWidth="1"/>
     <ns0:col min="3" max="3" width="9.00" customWidth="1"/>
-    <ns0:col min="4" max="4" width="21.00" customWidth="1"/>
+    <ns0:col min="4" max="4" width="19.00" customWidth="1"/>
     <ns0:col min="5" max="5" width="60.00" customWidth="1"/>
     <ns0:col min="6" max="6" width="39.00" customWidth="1"/>
     <ns0:col min="7" max="7" width="60.00" customWidth="1"/>
@@ -239,7 +239,7 @@
       </ns0:c>
       <ns0:c r="B5" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Enable Mod</ns0:t>
+          <ns0:t>OptionEnableMod</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C5" t="inlineStr" s="0">
@@ -308,7 +308,7 @@
     <ns0:row r="7">
       <ns0:c r="A7" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CategoryPresetSelection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B7" t="inlineStr" s="2">
@@ -345,12 +345,12 @@
     <ns0:row r="8">
       <ns0:c r="A8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CategoryPresetSelection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third Person Distribution</ns0:t>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C8" t="inlineStr" s="0">
@@ -365,7 +365,7 @@
       </ns0:c>
       <ns0:c r="E8" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>First Person Only | Mixed (Rare Third Person) | Mixed | Mostly Third Person | Third Person Only</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F8" t="inlineStr" s="0">
@@ -382,12 +382,12 @@
     <ns0:row r="9">
       <ns0:c r="A9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CategoryPresetSelection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Intensity Preset</ns0:t>
+          <ns0:t>OptionIntensityPreset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C9" t="inlineStr" s="0">
@@ -402,7 +402,7 @@
       </ns0:c>
       <ns0:c r="E9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Subtle | Standard | Dramatic | Cinematic | Epic</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F9" t="inlineStr" s="0">
@@ -419,12 +419,12 @@
     <ns0:row r="10">
       <ns0:c r="A10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CategoryPresetSelection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance Preset</ns0:t>
+          <ns0:t>OptionChancePreset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C10" t="inlineStr" s="0">
@@ -434,12 +434,12 @@
       </ns0:c>
       <ns0:c r="D10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (Cooldown Only)</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (Cooldown Only) | Very Rare | Rare | Standard | Frequent</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F10" t="inlineStr" s="0">
@@ -456,12 +456,12 @@
     <ns0:row r="11">
       <ns0:c r="A11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CategoryPresetSelection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown Preset</ns0:t>
+          <ns0:t>OptionCooldownPreset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C11" t="inlineStr" s="0">
@@ -476,7 +476,7 @@
       </ns0:c>
       <ns0:c r="E11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (No Cooldown) | Short | Standard | Long | Extended</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F11" t="inlineStr" s="0">
@@ -493,12 +493,12 @@
     <ns0:row r="12">
       <ns0:c r="A12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CategoryPresetSelection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration Preset</ns0:t>
+          <ns0:t>OptionDurationPreset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C12" t="inlineStr" s="0">
@@ -513,7 +513,7 @@
       </ns0:c>
       <ns0:c r="E12" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Very Short | Short | Standard | Long | Extended</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F12" t="inlineStr" s="0">
@@ -530,12 +530,12 @@
     <ns0:row r="13">
       <ns0:c r="A13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CategoryPresetSelection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smoothness Preset</ns0:t>
+          <ns0:t>OptionSmoothnessPreset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C13" t="inlineStr" s="0">
@@ -550,7 +550,7 @@
       </ns0:c>
       <ns0:c r="E13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Ultra Smooth</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F13" t="inlineStr" s="0">
@@ -567,12 +567,12 @@
     <ns0:row r="14">
       <ns0:c r="A14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Preset Selection</ns0:t>
+          <ns0:t>CategoryPresetSelection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger Profile</ns0:t>
+          <ns0:t>OptionTriggerProfile</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C14" t="inlineStr" s="0">
@@ -582,12 +582,12 @@
       </ns0:c>
       <ns0:c r="D14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>All Triggers</ns0:t>
+          <ns0:t>All</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only | Parry Only</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F14" t="inlineStr" s="0">
@@ -641,7 +641,7 @@
     <ns0:row r="16">
       <ns0:c r="A16" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>CategoryOptionalOverrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B16" t="inlineStr" s="2">
@@ -678,12 +678,12 @@
     <ns0:row r="17">
       <ns0:c r="A17" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>CategoryOptionalOverrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B17" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Cooldown</ns0:t>
+          <ns0:t>OptionGlobalCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C17" t="inlineStr" s="0">
@@ -715,12 +715,12 @@
     <ns0:row r="18">
       <ns0:c r="A18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>CategoryOptionalOverrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Global Smoothing</ns0:t>
+          <ns0:t>OptionGlobalSmoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="0">
@@ -752,12 +752,12 @@
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>CategoryOptionalOverrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dynamic Intensity</ns0:t>
+          <ns0:t>OptionDynamicIntensity</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="0">
@@ -772,7 +772,7 @@
       </ns0:c>
       <ns0:c r="E19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Low Sensitivity | Medium Sensitivity | High Sensitivity</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="0">
@@ -789,12 +789,12 @@
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Optional Overrides</ns0:t>
+          <ns0:t>CategoryOptionalOverrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Haptic Feedback</ns0:t>
+          <ns0:t>OptionHapticFeedback</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="0">
@@ -863,7 +863,7 @@
     <ns0:row r="22">
       <ns0:c r="A22" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B22" t="inlineStr" s="2">
@@ -900,12 +900,12 @@
     <ns0:row r="23">
       <ns0:c r="A23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Kill</ns0:t>
+          <ns0:t>TriggerBasicKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C23" t="inlineStr" s="0">
@@ -937,12 +937,12 @@
     <ns0:row r="24">
       <ns0:c r="A24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Critical Kill</ns0:t>
+          <ns0:t>TriggerThrownImpactKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C24" t="inlineStr" s="0">
@@ -952,7 +952,7 @@
       </ns0:c>
       <ns0:c r="D24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E24" t="inlineStr" s="0">
@@ -967,19 +967,19 @@
       </ns0:c>
       <ns0:c r="G24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Dismemberment</ns0:t>
+          <ns0:t>TriggerCriticalKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C25" t="inlineStr" s="0">
@@ -1004,19 +1004,19 @@
       </ns0:c>
       <ns0:c r="G25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="26">
       <ns0:c r="A26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Decapitation</ns0:t>
+          <ns0:t>TriggerDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C26" t="inlineStr" s="0">
@@ -1041,19 +1041,19 @@
       </ns0:c>
       <ns0:c r="G26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="27">
       <ns0:c r="A27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Enemy</ns0:t>
+          <ns0:t>TriggerDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C27" t="inlineStr" s="0">
@@ -1078,19 +1078,19 @@
       </ns0:c>
       <ns0:c r="G27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="28">
       <ns0:c r="A28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand</ns0:t>
+          <ns0:t>TriggerLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C28" t="inlineStr" s="0">
@@ -1115,103 +1115,103 @@
       </ns0:c>
       <ns0:c r="G28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="29">
       <ns0:c r="A29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Last Stand Threshold</ns0:t>
+          <ns0:t>TriggerLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="30">
       <ns0:c r="A30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Triggers</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Parry</ns0:t>
+          <ns0:t>OptionLastStandThreshold</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>15%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on successful weapon deflections</ns0:t>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="31">
       <ns0:c r="A31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>TriggerParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E31" t="inlineStr" s="0">
@@ -1226,352 +1226,352 @@
       </ns0:c>
       <ns0:c r="G31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Trigger on successful weapon deflections</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="32">
-      <ns0:c r="A32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G32" t="inlineStr" s="2">
+      <ns0:c r="A32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G32" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="33">
-      <ns0:c r="A33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Camera Distance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>3m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
+      <ns0:c r="A33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="34">
       <ns0:c r="A34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize Distance</ns0:t>
+          <ns0:t>OptionCameraDistance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>3m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize distance per killcam</ns0:t>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="35">
       <ns0:c r="A35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera Height</ns0:t>
+          <ns0:t>OptionRandomizeDistance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Randomize distance per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="36">
       <ns0:c r="A36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize Height</ns0:t>
+          <ns0:t>OptionCameraHeight</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>1.5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize height per killcam</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="37">
       <ns0:c r="A37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Killcam</ns0:t>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Orbit Speed</ns0:t>
+          <ns0:t>OptionRandomizeHeight</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slow</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
+          <ns0:t>Randomize height per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="38">
       <ns0:c r="A38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionOrbitSpeed</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="39">
-      <ns0:c r="A39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G39" t="inlineStr" s="2">
+      <ns0:c r="A39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G39" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="40">
-      <ns0:c r="A40" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B40" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C40" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D40" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>25%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E40" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F40" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G40" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+      <ns0:c r="A40" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B40" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C40" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D40" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E40" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F40" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G40" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="41">
       <ns0:c r="A41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time Scale</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C41" t="inlineStr" s="0">
@@ -1581,34 +1581,34 @@
       </ns0:c>
       <ns0:c r="D41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.35x</ns0:t>
+          <ns0:t>25%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="42">
       <ns0:c r="A42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C42" t="inlineStr" s="0">
@@ -1618,34 +1618,34 @@
       </ns0:c>
       <ns0:c r="D42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.0s</ns0:t>
+          <ns0:t>0.35x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="43">
       <ns0:c r="A43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C43" t="inlineStr" s="0">
@@ -1655,34 +1655,34 @@
       </ns0:c>
       <ns0:c r="D43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>1.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="44">
       <ns0:c r="A44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smoothing</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="0">
@@ -1692,34 +1692,34 @@
       </ns0:c>
       <ns0:c r="D44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>8x</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="45">
       <ns0:c r="A45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Basic Kill</ns0:t>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third Person Distribution</ns0:t>
+          <ns0:t>OptionSmoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C45" t="inlineStr" s="0">
@@ -1729,145 +1729,145 @@
       </ns0:c>
       <ns0:c r="D45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>8x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="46">
       <ns0:c r="A46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="47">
-      <ns0:c r="A47" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B47" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C47" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D47" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E47" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F47" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G47" t="inlineStr" s="2">
+      <ns0:c r="A47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G47" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="48">
-      <ns0:c r="A48" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B48" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C48" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D48" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>75%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E48" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F48" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G48" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+      <ns0:c r="A48" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B48" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C48" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D48" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E48" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F48" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G48" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="49">
       <ns0:c r="A49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time Scale</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C49" t="inlineStr" s="0">
@@ -1877,34 +1877,34 @@
       </ns0:c>
       <ns0:c r="D49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.25x</ns0:t>
+          <ns0:t>75%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="50">
       <ns0:c r="A50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C50" t="inlineStr" s="0">
@@ -1914,34 +1914,34 @@
       </ns0:c>
       <ns0:c r="D50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>0.25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G50" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="51">
       <ns0:c r="A51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C51" t="inlineStr" s="0">
@@ -1951,34 +1951,34 @@
       </ns0:c>
       <ns0:c r="D51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="52">
       <ns0:c r="A52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smoothing</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C52" t="inlineStr" s="0">
@@ -1988,34 +1988,34 @@
       </ns0:c>
       <ns0:c r="D52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>8x</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="53">
       <ns0:c r="A53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Critical Kill</ns0:t>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third Person Distribution</ns0:t>
+          <ns0:t>OptionSmoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C53" t="inlineStr" s="0">
@@ -2025,145 +2025,145 @@
       </ns0:c>
       <ns0:c r="D53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>8x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="54">
       <ns0:c r="A54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="55">
-      <ns0:c r="A55" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B55" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C55" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D55" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E55" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F55" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G55" t="inlineStr" s="2">
+      <ns0:c r="A55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G55" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="56">
-      <ns0:c r="A56" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B56" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C56" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D56" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>60%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E56" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F56" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G56" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+      <ns0:c r="A56" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B56" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C56" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D56" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E56" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F56" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G56" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="57">
       <ns0:c r="A57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time Scale</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C57" t="inlineStr" s="0">
@@ -2173,34 +2173,34 @@
       </ns0:c>
       <ns0:c r="D57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.30x</ns0:t>
+          <ns0:t>60%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="58">
       <ns0:c r="A58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C58" t="inlineStr" s="0">
@@ -2210,34 +2210,34 @@
       </ns0:c>
       <ns0:c r="D58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>0.30x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="59">
       <ns0:c r="A59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C59" t="inlineStr" s="0">
@@ -2247,34 +2247,34 @@
       </ns0:c>
       <ns0:c r="D59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="60">
       <ns0:c r="A60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smoothing</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C60" t="inlineStr" s="0">
@@ -2284,34 +2284,34 @@
       </ns0:c>
       <ns0:c r="D60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>8x</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="61">
       <ns0:c r="A61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Dismemberment</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third Person Distribution</ns0:t>
+          <ns0:t>OptionSmoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C61" t="inlineStr" s="0">
@@ -2321,145 +2321,145 @@
       </ns0:c>
       <ns0:c r="D61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>8x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="62">
       <ns0:c r="A62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="63">
-      <ns0:c r="A63" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B63" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C63" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D63" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E63" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F63" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G63" t="inlineStr" s="2">
+      <ns0:c r="A63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G63" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="64">
-      <ns0:c r="A64" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B64" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C64" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D64" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>90%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E64" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F64" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G64" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+      <ns0:c r="A64" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B64" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C64" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D64" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E64" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F64" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G64" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="65">
       <ns0:c r="A65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time Scale</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="0">
@@ -2469,34 +2469,34 @@
       </ns0:c>
       <ns0:c r="D65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.20x</ns0:t>
+          <ns0:t>90%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="66">
       <ns0:c r="A66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="0">
@@ -2506,34 +2506,34 @@
       </ns0:c>
       <ns0:c r="D66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.0s</ns0:t>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="67">
       <ns0:c r="A67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C67" t="inlineStr" s="0">
@@ -2543,34 +2543,34 @@
       </ns0:c>
       <ns0:c r="D67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4.0s</ns0:t>
+          <ns0:t>2.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="68">
       <ns0:c r="A68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smoothing</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C68" t="inlineStr" s="0">
@@ -2580,34 +2580,34 @@
       </ns0:c>
       <ns0:c r="D68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>6x</ns0:t>
+          <ns0:t>4.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="69">
       <ns0:c r="A69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Decapitation</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third Person Distribution</ns0:t>
+          <ns0:t>OptionSmoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C69" t="inlineStr" s="0">
@@ -2617,145 +2617,145 @@
       </ns0:c>
       <ns0:c r="D69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>6x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="70">
       <ns0:c r="A70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="71">
-      <ns0:c r="A71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G71" t="inlineStr" s="2">
+      <ns0:c r="A71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G71" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="72">
-      <ns0:c r="A72" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B72" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C72" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D72" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E72" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F72" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G72" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+      <ns0:c r="A72" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B72" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C72" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D72" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E72" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F72" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G72" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="73">
       <ns0:c r="A73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time Scale</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C73" t="inlineStr" s="0">
@@ -2765,34 +2765,34 @@
       </ns0:c>
       <ns0:c r="D73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.20x</ns0:t>
+          <ns0:t>100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="74">
       <ns0:c r="A74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C74" t="inlineStr" s="0">
@@ -2802,34 +2802,34 @@
       </ns0:c>
       <ns0:c r="D74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.0s</ns0:t>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="75">
       <ns0:c r="A75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="0">
@@ -2839,34 +2839,34 @@
       </ns0:c>
       <ns0:c r="D75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>3.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="76">
       <ns0:c r="A76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smoothing</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C76" t="inlineStr" s="0">
@@ -2876,34 +2876,34 @@
       </ns0:c>
       <ns0:c r="D76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4x</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="77">
       <ns0:c r="A77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Enemy</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third Person Distribution</ns0:t>
+          <ns0:t>OptionSmoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C77" t="inlineStr" s="0">
@@ -2913,145 +2913,145 @@
       </ns0:c>
       <ns0:c r="D77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>4x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="78">
       <ns0:c r="A78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="79">
-      <ns0:c r="A79" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B79" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C79" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D79" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E79" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F79" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G79" t="inlineStr" s="2">
+      <ns0:c r="A79" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B79" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C79" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D79" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E79" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F79" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G79" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="80">
-      <ns0:c r="A80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time Scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.15x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="A80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="81">
       <ns0:c r="A81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="0">
@@ -3061,34 +3061,34 @@
       </ns0:c>
       <ns0:c r="D81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>0.15x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="82">
       <ns0:c r="A82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="0">
@@ -3098,34 +3098,34 @@
       </ns0:c>
       <ns0:c r="D82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>45.0s</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="83">
       <ns0:c r="A83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Last Stand</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smoothing</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="0">
@@ -3135,145 +3135,145 @@
       </ns0:c>
       <ns0:c r="D83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4x</ns0:t>
+          <ns0:t>45.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="84">
       <ns0:c r="A84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionSmoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>4x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="85">
-      <ns0:c r="A85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F85" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G85" t="inlineStr" s="2">
+      <ns0:c r="A85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F85" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G85" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="86">
-      <ns0:c r="A86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>50%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+      <ns0:c r="A86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="87">
       <ns0:c r="A87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time Scale</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C87" t="inlineStr" s="0">
@@ -3283,34 +3283,34 @@
       </ns0:c>
       <ns0:c r="D87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.30x</ns0:t>
+          <ns0:t>50%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="88">
       <ns0:c r="A88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="0">
@@ -3320,34 +3320,34 @@
       </ns0:c>
       <ns0:c r="D88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.2s</ns0:t>
+          <ns0:t>0.30x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
       <ns0:c r="A89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C89" t="inlineStr" s="0">
@@ -3357,34 +3357,34 @@
       </ns0:c>
       <ns0:c r="D89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>7.0s</ns0:t>
+          <ns0:t>1.2s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="90">
       <ns0:c r="A90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Custom: Parry</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smoothing</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C90" t="inlineStr" s="0">
@@ -3394,205 +3394,242 @@
       </ns0:c>
       <ns0:c r="D90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10x</ns0:t>
+          <ns0:t>7.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="91">
       <ns0:c r="A91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionSmoothing</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>10x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G91" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition speed</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="92">
-      <ns0:c r="A92" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B92" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C92" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D92" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E92" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F92" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G92" t="inlineStr" s="2">
+      <ns0:c r="A92" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B92" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C92" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D92" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E92" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F92" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G92" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="93">
-      <ns0:c r="A93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Debug Logging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Enable verbose debug logging</ns0:t>
+      <ns0:c r="A93" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B93" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C93" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D93" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E93" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F93" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G93" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="94">
       <ns0:c r="A94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Quick Test Trigger</ns0:t>
+          <ns0:t>OptionDebugLogging</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Kill</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Kill | Critical Kill | Dismemberment | Decapitation | Parry | Last Enemy | Last Stand</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>QuickTestTriggerProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Which trigger to simulate</ns0:t>
+          <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="95">
       <ns0:c r="A95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CSM Advanced</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Quick Test Now</ns0:t>
+          <ns0:t>OptionQuickTestTrigger</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C95" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G95" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Which trigger to simulate</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="96">
+      <ns0:c r="A96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionQuickTestNow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C96" t="inlineStr" s="0">
+        <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D95" t="inlineStr" s="0">
+      <ns0:c r="D96" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E95" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F95" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G95" t="inlineStr" s="0">
+      <ns0:c r="E96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G96" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Toggle to fire the selected trigger once</ns0:t>
         </ns0:is>
@@ -3653,7 +3690,7 @@
       </ns0:c>
       <ns0:c r="B4" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>First Person Only | Mixed (Rare Third Person) | Mixed | Mostly Third Person | Third Person Only</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3665,7 +3702,7 @@
       </ns0:c>
       <ns0:c r="B5" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (Cooldown Only) | Very Rare | Rare | Standard | Frequent</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3689,7 +3726,7 @@
       </ns0:c>
       <ns0:c r="B7" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (No Cooldown) | Short | Standard | Long | Extended</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3785,7 +3822,7 @@
       </ns0:c>
       <ns0:c r="B15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Very Short | Short | Standard | Long | Extended</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3809,7 +3846,7 @@
       </ns0:c>
       <ns0:c r="B17" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Low Sensitivity | Medium Sensitivity | High Sensitivity</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3893,7 +3930,7 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Subtle | Standard | Dramatic | Cinematic | Epic</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3905,7 +3942,7 @@
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Basic Kill | Critical Kill | Dismemberment | Decapitation | Parry | Last Enemy | Last Stand</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3929,7 +3966,7 @@
       </ns0:c>
       <ns0:c r="B27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Very Snappy | Snappy | Standard | Smooth | Ultra Smooth</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3965,7 +4002,7 @@
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>All Triggers | Kills Only | Highlights | Last Enemy Only | Parry Only</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Replace speed-based smoothing with duration-based smooth-in/out presets
- Add separate Smooth-In and Smooth-Out preset options (% of duration)
- Preset mapping: VerySnappy 10%, Snappy 15%, Smooth 20%, Cinematic 30%, UltraSmooth 40%
- Clamp/rescale when in + out > 100% of duration
- Remove per-trigger smoothing options, GlobalSmoothing, and DynamicIntensity
- Transition now uses time-based easing over computed windows

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -535,7 +535,7 @@
       </ns0:c>
       <ns0:c r="B13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothnessPreset</ns0:t>
+          <ns0:t>OptionSmoothInPreset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C13" t="inlineStr" s="0">
@@ -545,7 +545,7 @@
       </ns0:c>
       <ns0:c r="D13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Standard</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E13" t="inlineStr" s="0">
@@ -560,7 +560,7 @@
       </ns0:c>
       <ns0:c r="G13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Sets per-trigger transition speed multipliers (x). Lower = smoother.</ns0:t>
+          <ns0:t>Smooth-in window as % of duration. Higher = smoother transition in.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -572,7 +572,7 @@
       </ns0:c>
       <ns0:c r="B14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTriggerProfile</ns0:t>
+          <ns0:t>OptionSmoothOutPreset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C14" t="inlineStr" s="0">
@@ -582,7 +582,7 @@
       </ns0:c>
       <ns0:c r="D14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>All</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E14" t="inlineStr" s="0">
@@ -592,34 +592,34 @@
       </ns0:c>
       <ns0:c r="F14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerProfileProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
+          <ns0:t>Smooth-out window as % of duration. Higher = smoother transition out.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="15">
       <ns0:c r="A15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryPresetSelection</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionTriggerProfile</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>All</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E15" t="inlineStr" s="0">
@@ -629,86 +629,86 @@
       </ns0:c>
       <ns0:c r="F15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G15" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="16">
-      <ns0:c r="A16" t="inlineStr" s="2">
+      <ns0:c r="A16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="17">
+      <ns0:c r="A17" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryOptionalOverrides</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B16" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C16" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D16" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E16" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F16" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G16" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="17">
-      <ns0:c r="A17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryOptionalOverrides</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionGlobalCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G17" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
+      <ns0:c r="B17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -720,7 +720,7 @@
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionGlobalSmoothing</ns0:t>
+          <ns0:t>OptionGlobalCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="0">
@@ -730,22 +730,22 @@
       </ns0:c>
       <ns0:c r="D18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
+          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>GlobalSmoothingProvider</ns0:t>
+          <ns0:t>CooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Override transition speed for all triggers. Per Trigger uses per-trigger smoothing (plus Smoothness Preset).</ns0:t>
+          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -757,12 +757,12 @@
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDynamicIntensity</ns0:t>
+          <ns0:t>OptionHapticFeedback</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D19" t="inlineStr" s="0">
@@ -772,128 +772,128 @@
       </ns0:c>
       <ns0:c r="E19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off | Light | Medium | Strong</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>DynamicIntensityPresetProvider</ns0:t>
+          <ns0:t>HapticIntensityProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Scale slow-mo start speed based on damage. Low = dampened, High = can reach near-instant.</ns0:t>
+          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryOptionalOverrides</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionHapticFeedback</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>HapticIntensityProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
-      <ns0:c r="A21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F21" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G21" t="inlineStr" s="0">
+      <ns0:c r="A21" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B21" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C21" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D21" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E21" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F21" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G21" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
-      <ns0:c r="A22" t="inlineStr" s="2">
+      <ns0:c r="A22" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B22" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C22" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D22" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E22" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F22" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G22" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -905,7 +905,7 @@
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
+          <ns0:t>TriggerThrownImpactKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C23" t="inlineStr" s="0">
@@ -915,7 +915,7 @@
       </ns0:c>
       <ns0:c r="D23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E23" t="inlineStr" s="0">
@@ -930,7 +930,7 @@
       </ns0:c>
       <ns0:c r="G23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
+          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -942,7 +942,7 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerThrownImpactKill</ns0:t>
+          <ns0:t>TriggerCriticalKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C24" t="inlineStr" s="0">
@@ -952,7 +952,7 @@
       </ns0:c>
       <ns0:c r="D24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E24" t="inlineStr" s="0">
@@ -967,7 +967,7 @@
       </ns0:c>
       <ns0:c r="G24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -979,7 +979,7 @@
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerCriticalKill</ns0:t>
+          <ns0:t>TriggerDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C25" t="inlineStr" s="0">
@@ -1004,7 +1004,7 @@
       </ns0:c>
       <ns0:c r="G25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1016,7 +1016,7 @@
       </ns0:c>
       <ns0:c r="B26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerDismemberment</ns0:t>
+          <ns0:t>TriggerDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C26" t="inlineStr" s="0">
@@ -1041,7 +1041,7 @@
       </ns0:c>
       <ns0:c r="G26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1053,7 +1053,7 @@
       </ns0:c>
       <ns0:c r="B27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerDecapitation</ns0:t>
+          <ns0:t>TriggerLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C27" t="inlineStr" s="0">
@@ -1078,7 +1078,7 @@
       </ns0:c>
       <ns0:c r="G27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1090,7 +1090,7 @@
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerLastEnemy</ns0:t>
+          <ns0:t>TriggerLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C28" t="inlineStr" s="0">
@@ -1115,7 +1115,7 @@
       </ns0:c>
       <ns0:c r="G28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1127,32 +1127,32 @@
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerLastStand</ns0:t>
+          <ns0:t>OptionLastStandThreshold</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>15%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1164,54 +1164,54 @@
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionLastStandThreshold</ns0:t>
+          <ns0:t>TriggerParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
+          <ns0:t>Trigger on successful weapon deflections</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="31">
       <ns0:c r="A31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerParry</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E31" t="inlineStr" s="0">
@@ -1226,81 +1226,81 @@
       </ns0:c>
       <ns0:c r="G31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on successful weapon deflections</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="32">
-      <ns0:c r="A32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F32" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G32" t="inlineStr" s="0">
+      <ns0:c r="A32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F32" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G32" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="33">
-      <ns0:c r="A33" t="inlineStr" s="2">
+      <ns0:c r="A33" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B33" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C33" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D33" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E33" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F33" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G33" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionCameraDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>3m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1312,32 +1312,32 @@
       </ns0:c>
       <ns0:c r="B34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCameraDistance</ns0:t>
+          <ns0:t>OptionRandomizeDistance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3m</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G34" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
+          <ns0:t>Randomize distance per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1349,32 +1349,32 @@
       </ns0:c>
       <ns0:c r="B35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionRandomizeDistance</ns0:t>
+          <ns0:t>OptionCameraHeight</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>1.5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize distance per killcam</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1386,32 +1386,32 @@
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCameraHeight</ns0:t>
+          <ns0:t>OptionRandomizeHeight</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Randomize height per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1423,143 +1423,143 @@
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionRandomizeHeight</ns0:t>
+          <ns0:t>OptionOrbitSpeed</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>Slow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize height per killcam</ns0:t>
+          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="38">
       <ns0:c r="A38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionOrbitSpeed</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C38" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="39">
+      <ns0:c r="A39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="40">
+      <ns0:c r="A40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C40" t="inlineStr" s="0">
+        <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D38" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E38" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F38" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G38" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="39">
-      <ns0:c r="A39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G39" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="40">
-      <ns0:c r="A40" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B40" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C40" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D40" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E40" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F40" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G40" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="D40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>25%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomChanceProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1571,7 +1571,7 @@
       </ns0:c>
       <ns0:c r="B41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C41" t="inlineStr" s="0">
@@ -1581,22 +1581,22 @@
       </ns0:c>
       <ns0:c r="D41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>25%</ns0:t>
+          <ns0:t>0.35x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G41" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1608,7 +1608,7 @@
       </ns0:c>
       <ns0:c r="B42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C42" t="inlineStr" s="0">
@@ -1618,22 +1618,22 @@
       </ns0:c>
       <ns0:c r="D42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.35x</ns0:t>
+          <ns0:t>1.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1645,7 +1645,7 @@
       </ns0:c>
       <ns0:c r="B43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C43" t="inlineStr" s="0">
@@ -1655,22 +1655,22 @@
       </ns0:c>
       <ns0:c r="D43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.0s</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1682,32 +1682,32 @@
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Smooth-in window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1719,32 +1719,32 @@
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothing</ns0:t>
+          <ns0:t>OptionSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>8x</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Smooth-out window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2015,32 +2015,32 @@
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothing</ns0:t>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>8x</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Smooth-in window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2052,143 +2052,143 @@
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Smooth-out window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="55">
       <ns0:c r="A55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="56">
-      <ns0:c r="A56" t="inlineStr" s="2">
+      <ns0:c r="A56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="57">
+      <ns0:c r="A57" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B56" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C56" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D56" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E56" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F56" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G56" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="57">
-      <ns0:c r="A57" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B57" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C57" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D57" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>60%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E57" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F57" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G57" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+      <ns0:c r="B57" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C57" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D57" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E57" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F57" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G57" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2200,7 +2200,7 @@
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C58" t="inlineStr" s="0">
@@ -2210,22 +2210,22 @@
       </ns0:c>
       <ns0:c r="D58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.30x</ns0:t>
+          <ns0:t>60%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2237,7 +2237,7 @@
       </ns0:c>
       <ns0:c r="B59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C59" t="inlineStr" s="0">
@@ -2247,22 +2247,22 @@
       </ns0:c>
       <ns0:c r="D59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>0.30x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2274,7 +2274,7 @@
       </ns0:c>
       <ns0:c r="B60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C60" t="inlineStr" s="0">
@@ -2284,22 +2284,22 @@
       </ns0:c>
       <ns0:c r="D60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2311,7 +2311,7 @@
       </ns0:c>
       <ns0:c r="B61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothing</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C61" t="inlineStr" s="0">
@@ -2321,22 +2321,22 @@
       </ns0:c>
       <ns0:c r="D61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>8x</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2348,54 +2348,54 @@
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Smooth-in window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="63">
       <ns0:c r="A63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E63" t="inlineStr" s="0">
@@ -2405,123 +2405,123 @@
       </ns0:c>
       <ns0:c r="F63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Smooth-out window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="64">
-      <ns0:c r="A64" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B64" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C64" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D64" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E64" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F64" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G64" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="65">
       <ns0:c r="A65" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B65" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C65" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D65" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E65" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F65" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G65" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="66">
+      <ns0:c r="A66" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B65" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C65" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D65" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>90%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E65" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F65" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G65" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="66">
-      <ns0:c r="A66" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B66" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C66" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D66" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.20x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E66" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F66" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G66" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="B66" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C66" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D66" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E66" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F66" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G66" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2533,7 +2533,7 @@
       </ns0:c>
       <ns0:c r="B67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C67" t="inlineStr" s="0">
@@ -2543,22 +2543,22 @@
       </ns0:c>
       <ns0:c r="D67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.0s</ns0:t>
+          <ns0:t>90%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2570,7 +2570,7 @@
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C68" t="inlineStr" s="0">
@@ -2580,22 +2580,22 @@
       </ns0:c>
       <ns0:c r="D68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4.0s</ns0:t>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2607,7 +2607,7 @@
       </ns0:c>
       <ns0:c r="B69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothing</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C69" t="inlineStr" s="0">
@@ -2617,22 +2617,22 @@
       </ns0:c>
       <ns0:c r="D69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>6x</ns0:t>
+          <ns0:t>2.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2644,7 +2644,7 @@
       </ns0:c>
       <ns0:c r="B70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C70" t="inlineStr" s="0">
@@ -2654,44 +2654,44 @@
       </ns0:c>
       <ns0:c r="D70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>4.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="71">
       <ns0:c r="A71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E71" t="inlineStr" s="0">
@@ -2701,61 +2701,61 @@
       </ns0:c>
       <ns0:c r="F71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Smooth-in window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="72">
-      <ns0:c r="A72" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B72" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C72" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D72" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E72" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F72" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G72" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionSmoothOut</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth-out window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="73">
       <ns0:c r="A73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C73" t="inlineStr" s="0">
@@ -2765,96 +2765,96 @@
       </ns0:c>
       <ns0:c r="D73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>100%</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="74">
       <ns0:c r="A74" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B74" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C74" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D74" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E74" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F74" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G74" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="75">
+      <ns0:c r="A75" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B74" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C74" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D74" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.20x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E74" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F74" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G74" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="75">
-      <ns0:c r="A75" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B75" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C75" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D75" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>3.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E75" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F75" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G75" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
+      <ns0:c r="B75" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C75" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D75" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E75" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F75" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G75" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2866,7 +2866,7 @@
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C76" t="inlineStr" s="0">
@@ -2876,22 +2876,22 @@
       </ns0:c>
       <ns0:c r="D76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2903,7 +2903,7 @@
       </ns0:c>
       <ns0:c r="B77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothing</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C77" t="inlineStr" s="0">
@@ -2913,22 +2913,22 @@
       </ns0:c>
       <ns0:c r="D77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4x</ns0:t>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2940,7 +2940,7 @@
       </ns0:c>
       <ns0:c r="B78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C78" t="inlineStr" s="0">
@@ -2950,145 +2950,145 @@
       </ns0:c>
       <ns0:c r="D78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>3.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="79">
       <ns0:c r="A79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="80">
-      <ns0:c r="A80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionSmoothIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth-in window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="81">
       <ns0:c r="A81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.15x</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Smooth-out window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="82">
       <ns0:c r="A82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="0">
@@ -3098,182 +3098,182 @@
       </ns0:c>
       <ns0:c r="D82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="83">
       <ns0:c r="A83" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B83" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C83" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D83" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E83" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F83" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G83" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="84">
+      <ns0:c r="A84" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B83" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C83" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D83" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>45.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E83" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F83" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G83" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="84">
-      <ns0:c r="A84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionSmoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>4x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G84" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+      <ns0:c r="B84" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C84" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D84" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E84" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F84" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G84" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="85">
       <ns0:c r="A85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.15x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="86">
-      <ns0:c r="A86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionDuration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>5.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomDurationProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G86" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="87">
       <ns0:c r="A87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C87" t="inlineStr" s="0">
@@ -3283,353 +3283,575 @@
       </ns0:c>
       <ns0:c r="D87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>50%</ns0:t>
+          <ns0:t>45.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="88">
       <ns0:c r="A88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.30x</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Smooth-in window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
       <ns0:c r="A89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.2s</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Smooth-out window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="90">
       <ns0:c r="A90" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G90" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="91">
+      <ns0:c r="A91" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>7.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G90" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="91">
-      <ns0:c r="A91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionSmoothing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>10x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G91" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Transition speed</ns0:t>
+      <ns0:c r="B91" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C91" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D91" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E91" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F91" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G91" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="92">
       <ns0:c r="A92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>50%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="93">
-      <ns0:c r="A93" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B93" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C93" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D93" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E93" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F93" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G93" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.30x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G93" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="94">
       <ns0:c r="A94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDebugLogging</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>1.2s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Enable verbose debug logging</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="95">
       <ns0:c r="A95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionQuickTestTrigger</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
+          <ns0:t>7.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>QuickTestTriggerProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Which trigger to simulate</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="96">
       <ns0:c r="A96" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionSmoothIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G96" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth-in window as % of duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="97">
+      <ns0:c r="A97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionSmoothOut</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G97" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth-out window as % of duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="98">
+      <ns0:c r="A98" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B98" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C98" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D98" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E98" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F98" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G98" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="99">
+      <ns0:c r="A99" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B96" t="inlineStr" s="0">
+      <ns0:c r="B99" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C99" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D99" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E99" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F99" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G99" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="100">
+      <ns0:c r="A100" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B100" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionDebugLogging</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C100" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D100" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E100" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F100" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G100" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Enable verbose debug logging</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="101">
+      <ns0:c r="A101" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B101" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionQuickTestTrigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C101" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D101" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E101" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F101" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G101" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Which trigger to simulate</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="102">
+      <ns0:c r="A102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B102" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>OptionQuickTestNow</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C96" t="inlineStr" s="0">
+      <ns0:c r="C102" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D96" t="inlineStr" s="0">
+      <ns0:c r="D102" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G96" t="inlineStr" s="0">
+      <ns0:c r="E102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G102" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Toggle to fire the selected trigger once</ns0:t>
         </ns0:is>

</xml_diff>

<commit_message>
Add easing curves, instant mode, min time scale, and statistics tracking
- Add EasingCurve option (Smoothstep, Linear, EaseIn, EaseOut)
- Add per-trigger Instant Transition checkbox to bypass smoothing
- Add MinTimeScale floor option to prevent extreme slow-mo stutter
- Add statistics tracking (total slow-mo time, trigger counts) with PlayerPrefs
- Add Reset Statistics toggle in CSM Statistics category

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -789,148 +789,148 @@
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryOptionalOverrides</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionEasingCurve</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Smoothstep</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>EasingCurveProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition curve shape. Smoothstep = smooth both ends, Linear = constant speed, EaseIn = slow start, EaseOut = slow end.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
-      <ns0:c r="A21" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B21" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C21" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D21" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E21" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F21" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G21" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryOptionalOverrides</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionMinTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off (0%) | 5% | 8% | 10% | 15% | 20%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>MinTimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G21" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Floor for time scale to prevent extreme slow-mo stutter. 0% = no limit.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
       <ns0:c r="A22" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G22" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="23">
+      <ns0:c r="A23" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G22" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="23">
-      <ns0:c r="A23" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B23" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>TriggerThrownImpactKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C23" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D23" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E23" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F23" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G23" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
+      <ns0:c r="B23" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C23" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D23" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E23" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F23" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G23" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -942,7 +942,7 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerCriticalKill</ns0:t>
+          <ns0:t>TriggerBasicKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C24" t="inlineStr" s="0">
@@ -967,7 +967,7 @@
       </ns0:c>
       <ns0:c r="G24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -979,7 +979,7 @@
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerDismemberment</ns0:t>
+          <ns0:t>TriggerThrownImpactKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C25" t="inlineStr" s="0">
@@ -989,7 +989,7 @@
       </ns0:c>
       <ns0:c r="D25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E25" t="inlineStr" s="0">
@@ -1004,7 +1004,7 @@
       </ns0:c>
       <ns0:c r="G25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1016,7 +1016,7 @@
       </ns0:c>
       <ns0:c r="B26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerDecapitation</ns0:t>
+          <ns0:t>TriggerCriticalKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C26" t="inlineStr" s="0">
@@ -1041,7 +1041,7 @@
       </ns0:c>
       <ns0:c r="G26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1053,7 +1053,7 @@
       </ns0:c>
       <ns0:c r="B27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerLastEnemy</ns0:t>
+          <ns0:t>TriggerDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C27" t="inlineStr" s="0">
@@ -1078,7 +1078,7 @@
       </ns0:c>
       <ns0:c r="G27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1090,7 +1090,7 @@
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerLastStand</ns0:t>
+          <ns0:t>TriggerDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C28" t="inlineStr" s="0">
@@ -1115,7 +1115,7 @@
       </ns0:c>
       <ns0:c r="G28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1127,32 +1127,32 @@
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionLastStandThreshold</ns0:t>
+          <ns0:t>TriggerLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1164,7 +1164,7 @@
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerParry</ns0:t>
+          <ns0:t>TriggerLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C30" t="inlineStr" s="0">
@@ -1189,155 +1189,155 @@
       </ns0:c>
       <ns0:c r="G30" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Trigger on successful weapon deflections</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="31">
       <ns0:c r="A31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionLastStandThreshold</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>15%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G31" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="32">
-      <ns0:c r="A32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G32" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>TriggerParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G32" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Trigger on successful weapon deflections</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="33">
       <ns0:c r="A33" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="34">
+      <ns0:c r="A34" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionCameraDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>3m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G33" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="34">
-      <ns0:c r="A34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionRandomizeDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G34" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Randomize distance per killcam</ns0:t>
+      <ns0:c r="B34" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C34" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D34" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E34" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F34" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G34" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1349,7 +1349,7 @@
       </ns0:c>
       <ns0:c r="B35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCameraHeight</ns0:t>
+          <ns0:t>OptionCameraDistance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C35" t="inlineStr" s="0">
@@ -1359,22 +1359,22 @@
       </ns0:c>
       <ns0:c r="D35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
+          <ns0:t>3m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G35" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1386,7 +1386,7 @@
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionRandomizeHeight</ns0:t>
+          <ns0:t>OptionRandomizeDistance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="0">
@@ -1411,7 +1411,7 @@
       </ns0:c>
       <ns0:c r="G36" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Randomize height per killcam</ns0:t>
+          <ns0:t>Randomize distance per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1423,7 +1423,7 @@
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionOrbitSpeed</ns0:t>
+          <ns0:t>OptionCameraHeight</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C37" t="inlineStr" s="0">
@@ -1433,44 +1433,44 @@
       </ns0:c>
       <ns0:c r="D37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slow</ns0:t>
+          <ns0:t>1.5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G37" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="38">
       <ns0:c r="A38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionRandomizeHeight</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E38" t="inlineStr" s="0">
@@ -1485,118 +1485,118 @@
       </ns0:c>
       <ns0:c r="G38" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Randomize height per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="39">
-      <ns0:c r="A39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G39" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionOrbitSpeed</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G39" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="40">
       <ns0:c r="A40" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G40" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="41">
+      <ns0:c r="A41" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B40" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C40" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D40" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>25%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E40" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F40" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G40" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="41">
-      <ns0:c r="A41" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B41" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C41" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D41" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.35x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E41" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F41" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G41" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="B41" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C41" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D41" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E41" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F41" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G41" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1608,7 +1608,7 @@
       </ns0:c>
       <ns0:c r="B42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C42" t="inlineStr" s="0">
@@ -1618,22 +1618,22 @@
       </ns0:c>
       <ns0:c r="D42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.0s</ns0:t>
+          <ns0:t>25%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1645,7 +1645,7 @@
       </ns0:c>
       <ns0:c r="B43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C43" t="inlineStr" s="0">
@@ -1655,22 +1655,22 @@
       </ns0:c>
       <ns0:c r="D43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>0.35x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1682,32 +1682,32 @@
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>1.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-in window as % of duration</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1719,32 +1719,32 @@
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-out window as % of duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1756,54 +1756,54 @@
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Smooth-in window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="47">
       <ns0:c r="A47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E47" t="inlineStr" s="0">
@@ -1813,61 +1813,61 @@
       </ns0:c>
       <ns0:c r="F47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Smooth-out window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="48">
-      <ns0:c r="A48" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B48" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C48" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D48" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E48" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F48" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G48" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionInstantTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Skip smooth-in/out transitions for instant time scale change</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="49">
       <ns0:c r="A49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C49" t="inlineStr" s="0">
@@ -1877,96 +1877,96 @@
       </ns0:c>
       <ns0:c r="D49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>75%</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="50">
       <ns0:c r="A50" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B50" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C50" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D50" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E50" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F50" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G50" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="51">
+      <ns0:c r="A51" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.25x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="51">
-      <ns0:c r="A51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
+      <ns0:c r="B51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1978,7 +1978,7 @@
       </ns0:c>
       <ns0:c r="B52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C52" t="inlineStr" s="0">
@@ -1988,22 +1988,22 @@
       </ns0:c>
       <ns0:c r="D52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>75%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2015,32 +2015,32 @@
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>0.25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-in window as % of duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2052,32 +2052,32 @@
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-out window as % of duration</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2089,7 +2089,7 @@
       </ns0:c>
       <ns0:c r="B55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C55" t="inlineStr" s="0">
@@ -2099,44 +2099,44 @@
       </ns0:c>
       <ns0:c r="D55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="56">
       <ns0:c r="A56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E56" t="inlineStr" s="0">
@@ -2146,98 +2146,98 @@
       </ns0:c>
       <ns0:c r="F56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Smooth-in window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="57">
-      <ns0:c r="A57" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B57" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C57" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D57" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E57" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F57" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G57" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A57" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B57" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionSmoothOut</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C57" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D57" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E57" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F57" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G57" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth-out window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="58">
       <ns0:c r="A58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionInstantTransition</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>60%</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Skip smooth-in/out transitions for instant time scale change</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="59">
       <ns0:c r="A59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C59" t="inlineStr" s="0">
@@ -2247,96 +2247,96 @@
       </ns0:c>
       <ns0:c r="D59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.30x</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G59" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="60">
       <ns0:c r="A60" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="61">
+      <ns0:c r="A61" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B60" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C60" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D60" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E60" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F60" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G60" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="61">
-      <ns0:c r="A61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>5.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+      <ns0:c r="B61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2348,32 +2348,32 @@
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>60%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-in window as % of duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2385,32 +2385,32 @@
       </ns0:c>
       <ns0:c r="B63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>0.30x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-out window as % of duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2422,7 +2422,7 @@
       </ns0:c>
       <ns0:c r="B64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C64" t="inlineStr" s="0">
@@ -2432,182 +2432,182 @@
       </ns0:c>
       <ns0:c r="D64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="65">
       <ns0:c r="A65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="66">
-      <ns0:c r="A66" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B66" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C66" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D66" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E66" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F66" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G66" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionSmoothIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth-in window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="67">
       <ns0:c r="A67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>90%</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Smooth-out window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="68">
       <ns0:c r="A68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionInstantTransition</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.20x</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G68" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Skip smooth-in/out transitions for instant time scale change</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="69">
       <ns0:c r="A69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C69" t="inlineStr" s="0">
@@ -2617,96 +2617,96 @@
       </ns0:c>
       <ns0:c r="D69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="70">
       <ns0:c r="A70" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="71">
+      <ns0:c r="A71" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B70" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C70" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D70" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>4.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E70" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F70" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G70" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="71">
-      <ns0:c r="A71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Smooth</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Smooth-in window as % of duration</ns0:t>
+      <ns0:c r="B71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G71" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2718,32 +2718,32 @@
       </ns0:c>
       <ns0:c r="B72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>90%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-out window as % of duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2755,7 +2755,7 @@
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C73" t="inlineStr" s="0">
@@ -2765,219 +2765,219 @@
       </ns0:c>
       <ns0:c r="D73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="74">
       <ns0:c r="A74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>2.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="75">
-      <ns0:c r="A75" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B75" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C75" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D75" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E75" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F75" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G75" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A75" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B75" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C75" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D75" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>4.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E75" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F75" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomCooldownProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G75" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="76">
       <ns0:c r="A76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>100%</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Smooth-in window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="77">
       <ns0:c r="A77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.20x</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G77" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Smooth-out window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="78">
       <ns0:c r="A78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionInstantTransition</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.0s</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Skip smooth-in/out transitions for instant time scale change</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="79">
       <ns0:c r="A79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C79" t="inlineStr" s="0">
@@ -2987,96 +2987,96 @@
       </ns0:c>
       <ns0:c r="D79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="80">
       <ns0:c r="A80" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G80" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="81">
+      <ns0:c r="A81" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Smooth</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Smooth-in window as % of duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="81">
-      <ns0:c r="A81" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B81" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C81" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D81" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Smooth</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E81" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F81" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G81" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Smooth-out window as % of duration</ns0:t>
+      <ns0:c r="B81" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C81" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D81" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E81" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F81" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G81" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3088,7 +3088,7 @@
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="0">
@@ -3098,108 +3098,108 @@
       </ns0:c>
       <ns0:c r="D82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="83">
       <ns0:c r="A83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="84">
-      <ns0:c r="A84" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B84" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C84" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D84" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E84" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F84" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G84" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="A84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionDuration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>3.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomDurationProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G84" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="85">
       <ns0:c r="A85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C85" t="inlineStr" s="0">
@@ -3209,118 +3209,118 @@
       </ns0:c>
       <ns0:c r="D85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.15x</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="86">
       <ns0:c r="A86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G86" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Smooth-in window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="87">
       <ns0:c r="A87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>45.0s</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Smooth-out window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="88">
       <ns0:c r="A88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionInstantTransition</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
@@ -3330,49 +3330,49 @@
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-in window as % of duration</ns0:t>
+          <ns0:t>Skip smooth-in/out transitions for instant time scale change</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
       <ns0:c r="A89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-out window as % of duration</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3416,7 +3416,7 @@
     <ns0:row r="91">
       <ns0:c r="A91" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B91" t="inlineStr" s="2">
@@ -3453,12 +3453,12 @@
     <ns0:row r="92">
       <ns0:c r="A92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C92" t="inlineStr" s="0">
@@ -3468,34 +3468,34 @@
       </ns0:c>
       <ns0:c r="D92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>50%</ns0:t>
+          <ns0:t>0.15x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="93">
       <ns0:c r="A93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C93" t="inlineStr" s="0">
@@ -3505,34 +3505,34 @@
       </ns0:c>
       <ns0:c r="D93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.30x</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G93" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="94">
       <ns0:c r="A94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C94" t="inlineStr" s="0">
@@ -3542,71 +3542,71 @@
       </ns0:c>
       <ns0:c r="D94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.2s</ns0:t>
+          <ns0:t>45.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="95">
       <ns0:c r="A95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>7.0s</ns0:t>
+          <ns0:t>Smooth</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Smooth-in window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="96">
       <ns0:c r="A96" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B96" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C96" t="inlineStr" s="0">
@@ -3631,29 +3631,29 @@
       </ns0:c>
       <ns0:c r="G96" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-in window as % of duration</ns0:t>
+          <ns0:t>Smooth-out window as % of duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="97">
       <ns0:c r="A97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionInstantTransition</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E97" t="inlineStr" s="0">
@@ -3663,12 +3663,12 @@
       </ns0:c>
       <ns0:c r="F97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-out window as % of duration</ns0:t>
+          <ns0:t>Skip smooth-in/out transitions for instant time scale change</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3712,7 +3712,7 @@
     <ns0:row r="99">
       <ns0:c r="A99" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B99" t="inlineStr" s="2">
@@ -3749,111 +3749,555 @@
     <ns0:row r="100">
       <ns0:c r="A100" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B100" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDebugLogging</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C100" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D100" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>50%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E100" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F100" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G100" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Enable verbose debug logging</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="101">
       <ns0:c r="A101" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B101" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionQuickTestTrigger</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C101" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D101" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
+          <ns0:t>0.30x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E101" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F101" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>QuickTestTriggerProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G101" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Which trigger to simulate</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="102">
       <ns0:c r="A102" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionDuration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.2s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomDurationProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G102" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="103">
+      <ns0:c r="A103" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B103" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C103" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D103" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>7.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E103" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F103" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomCooldownProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G103" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="104">
+      <ns0:c r="A104" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B104" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionSmoothIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C104" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D104" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E104" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F104" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G104" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth-in window as % of duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="105">
+      <ns0:c r="A105" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B105" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionSmoothOut</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C105" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D105" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E105" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F105" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G105" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Smooth-out window as % of duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="106">
+      <ns0:c r="A106" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B106" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionInstantTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C106" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D106" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E106" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F106" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G106" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Skip smooth-in/out transitions for instant time scale change</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="107">
+      <ns0:c r="A107" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B107" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C107" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D107" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E107" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F107" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G107" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="108">
+      <ns0:c r="A108" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B102" t="inlineStr" s="0">
+      <ns0:c r="B108" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C108" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D108" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E108" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F108" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G108" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="109">
+      <ns0:c r="A109" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B109" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionDebugLogging</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C109" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D109" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E109" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F109" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G109" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Enable verbose debug logging</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="110">
+      <ns0:c r="A110" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B110" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionQuickTestTrigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C110" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D110" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E110" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F110" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G110" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Which trigger to simulate</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="111">
+      <ns0:c r="A111" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B111" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>OptionQuickTestNow</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C102" t="inlineStr" s="0">
+      <ns0:c r="C111" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D102" t="inlineStr" s="0">
+      <ns0:c r="D111" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E102" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F102" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G102" t="inlineStr" s="0">
+      <ns0:c r="E111" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F111" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G111" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Toggle to fire the selected trigger once</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="112">
+      <ns0:c r="A112" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B112" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C112" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D112" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E112" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F112" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G112" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="113">
+      <ns0:c r="A113" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryStatistics</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B113" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C113" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D113" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E113" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F113" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G113" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="114">
+      <ns0:c r="A114" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryStatistics</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B114" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionResetStats</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C114" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D114" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E114" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F114" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G114" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Toggle to reset all statistics</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -4075,115 +4519,115 @@
     <ns0:row r="18">
       <ns0:c r="A18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>GlobalSmoothingProvider</ns0:t>
+          <ns0:t>EasingCurveProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
+          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>HapticIntensityProvider</ns0:t>
+          <ns0:t>GlobalSmoothingProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t>HapticIntensityProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>Off | Light | Medium | Strong</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
       <ns0:c r="A21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B21" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
       <ns0:c r="A22" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B22" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="23">
       <ns0:c r="A23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>MinEnemyGroupProvider</ns0:t>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="24">
       <ns0:c r="A24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>PresetProvider</ns0:t>
+          <ns0:t>MinEnemyGroupProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>QuickTestTriggerProvider</ns0:t>
+          <ns0:t>MinTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%) | 5% | 8% | 10% | 15% | 20%</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="26">
       <ns0:c r="A26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothingSpeedProvider</ns0:t>
+          <ns0:t>PresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B26" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Instant | Fast | Medium | Slow</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="27">
       <ns0:c r="A27" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B27" t="inlineStr" s="0">
@@ -4195,34 +4639,58 @@
     <ns0:row r="28">
       <ns0:c r="A28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t>SmoothingSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t>Instant | Fast | Medium | Slow</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="29">
       <ns0:c r="A29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>TimeScaleProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="30">
       <ns0:c r="A30" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t>ThresholdProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="31">
+      <ns0:c r="A31" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>TimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B31" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="32">
+      <ns0:c r="A32" t="inlineStr" s="0">
+        <ns0:is>
           <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B30" t="inlineStr" s="0">
+      <ns0:c r="B32" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t/>
         </ns0:is>

</xml_diff>

<commit_message>
Simplify fade presets and make Default (10%) the default selection
- Rename smoothing options from "Smooth-In/Out" to "Fade In/Out"
- Add Instant (0%) preset for immediate time scale changes
- Add Default (10%) preset with natural feel, selected by default
- Rename presets: Quick Fade (15%), Medium Fade (20%), Long Fade (30%), Very Long Fade (40%)
- Remove redundant per-trigger "Instant Transition" checkboxes
- Remove legacy preset mappings
- Update tooltips for clarity

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -545,7 +545,7 @@
       </ns0:c>
       <ns0:c r="D13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E13" t="inlineStr" s="0">
@@ -560,7 +560,7 @@
       </ns0:c>
       <ns0:c r="G13" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-in window as % of duration. Higher = smoother transition in.</ns0:t>
+          <ns0:t>Transition into slow motion. Instant = immediate. Default = natural feel.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -582,7 +582,7 @@
       </ns0:c>
       <ns0:c r="D14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E14" t="inlineStr" s="0">
@@ -597,7 +597,7 @@
       </ns0:c>
       <ns0:c r="G14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-out window as % of duration. Higher = smoother transition out.</ns0:t>
+          <ns0:t>Transition out of slow motion. Instant = immediate. Default = natural feel.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1766,7 +1766,7 @@
       </ns0:c>
       <ns0:c r="D46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E46" t="inlineStr" s="0">
@@ -1781,7 +1781,7 @@
       </ns0:c>
       <ns0:c r="G46" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-in window as % of duration</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1803,7 +1803,7 @@
       </ns0:c>
       <ns0:c r="D47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E47" t="inlineStr" s="0">
@@ -1818,7 +1818,7 @@
       </ns0:c>
       <ns0:c r="G47" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-out window as % of duration</ns0:t>
+          <ns0:t>Transition out of slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1830,143 +1830,143 @@
       </ns0:c>
       <ns0:c r="B48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionInstantTransition</ns0:t>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G48" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Skip smooth-in/out transitions for instant time scale change</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="49">
       <ns0:c r="A49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C49" t="inlineStr" s="0">
         <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D49" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E49" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F49" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G49" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="50">
+      <ns0:c r="A50" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B50" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C50" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D50" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E50" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F50" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G50" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="51">
+      <ns0:c r="A51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C51" t="inlineStr" s="0">
+        <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D49" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E49" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F49" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G49" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="50">
-      <ns0:c r="A50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G50" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="51">
-      <ns0:c r="A51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G51" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="D51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>75%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomChanceProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1978,7 +1978,7 @@
       </ns0:c>
       <ns0:c r="B52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C52" t="inlineStr" s="0">
@@ -1988,22 +1988,22 @@
       </ns0:c>
       <ns0:c r="D52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>75%</ns0:t>
+          <ns0:t>0.25x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2015,7 +2015,7 @@
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C53" t="inlineStr" s="0">
@@ -2025,22 +2025,22 @@
       </ns0:c>
       <ns0:c r="D53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.25x</ns0:t>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2052,7 +2052,7 @@
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C54" t="inlineStr" s="0">
@@ -2062,22 +2062,22 @@
       </ns0:c>
       <ns0:c r="D54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2089,32 +2089,32 @@
       </ns0:c>
       <ns0:c r="B55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G55" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2126,7 +2126,7 @@
       </ns0:c>
       <ns0:c r="B56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C56" t="inlineStr" s="0">
@@ -2136,7 +2136,7 @@
       </ns0:c>
       <ns0:c r="D56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E56" t="inlineStr" s="0">
@@ -2151,7 +2151,7 @@
       </ns0:c>
       <ns0:c r="G56" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-in window as % of duration</ns0:t>
+          <ns0:t>Transition out of slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2163,54 +2163,54 @@
       </ns0:c>
       <ns0:c r="B57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G57" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-out window as % of duration</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="58">
       <ns0:c r="A58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionInstantTransition</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E58" t="inlineStr" s="0">
@@ -2225,118 +2225,118 @@
       </ns0:c>
       <ns0:c r="G58" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Skip smooth-in/out transitions for instant time scale change</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="59">
-      <ns0:c r="A59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G59" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+      <ns0:c r="A59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="60">
       <ns0:c r="A60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>60%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="61">
-      <ns0:c r="A61" t="inlineStr" s="2">
+      <ns0:c r="A61" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G61" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.30x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2348,7 +2348,7 @@
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C62" t="inlineStr" s="0">
@@ -2358,22 +2358,22 @@
       </ns0:c>
       <ns0:c r="D62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>60%</ns0:t>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2385,7 +2385,7 @@
       </ns0:c>
       <ns0:c r="B63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C63" t="inlineStr" s="0">
@@ -2395,22 +2395,22 @@
       </ns0:c>
       <ns0:c r="D63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.30x</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2422,32 +2422,32 @@
       </ns0:c>
       <ns0:c r="B64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G64" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2459,32 +2459,32 @@
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G65" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition out of slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2496,54 +2496,54 @@
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G66" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-in window as % of duration</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="67">
       <ns0:c r="A67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E67" t="inlineStr" s="0">
@@ -2553,61 +2553,61 @@
       </ns0:c>
       <ns0:c r="F67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G67" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-out window as % of duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="68">
-      <ns0:c r="A68" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B68" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionInstantTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C68" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D68" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E68" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F68" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G68" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Skip smooth-in/out transitions for instant time scale change</ns0:t>
+      <ns0:c r="A68" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B68" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C68" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D68" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E68" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F68" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G68" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="69">
       <ns0:c r="A69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C69" t="inlineStr" s="0">
@@ -2617,96 +2617,96 @@
       </ns0:c>
       <ns0:c r="D69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>90%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="70">
       <ns0:c r="A70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="71">
-      <ns0:c r="A71" t="inlineStr" s="2">
+      <ns0:c r="A71" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G71" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionDuration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomDurationProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2718,7 +2718,7 @@
       </ns0:c>
       <ns0:c r="B72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C72" t="inlineStr" s="0">
@@ -2728,22 +2728,22 @@
       </ns0:c>
       <ns0:c r="D72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>90%</ns0:t>
+          <ns0:t>4.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2755,32 +2755,32 @@
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.20x</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G73" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2792,32 +2792,32 @@
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.0s</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G74" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Transition out of slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2829,7 +2829,7 @@
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="0">
@@ -2839,44 +2839,44 @@
       </ns0:c>
       <ns0:c r="D75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4.0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G75" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="76">
       <ns0:c r="A76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E76" t="inlineStr" s="0">
@@ -2886,98 +2886,98 @@
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G76" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-in window as % of duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="77">
-      <ns0:c r="A77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Smooth</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G77" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Smooth-out window as % of duration</ns0:t>
+      <ns0:c r="A77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G77" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="78">
       <ns0:c r="A78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionInstantTransition</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Skip smooth-in/out transitions for instant time scale change</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="79">
       <ns0:c r="A79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C79" t="inlineStr" s="0">
@@ -2987,96 +2987,96 @@
       </ns0:c>
       <ns0:c r="D79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>0.20x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="80">
       <ns0:c r="A80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>3.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="81">
-      <ns0:c r="A81" t="inlineStr" s="2">
+      <ns0:c r="A81" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B81" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C81" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D81" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E81" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F81" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G81" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B81" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C81" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D81" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E81" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F81" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>CustomCooldownProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G81" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3088,32 +3088,32 @@
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>100%</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G82" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3125,32 +3125,32 @@
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.20x</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G83" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Transition out of slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3162,7 +3162,7 @@
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionThirdPersonDistribution</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C84" t="inlineStr" s="0">
@@ -3172,182 +3172,182 @@
       </ns0:c>
       <ns0:c r="D84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.0s</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G84" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="85">
       <ns0:c r="A85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G85" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="86">
-      <ns0:c r="A86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Smooth</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G86" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Smooth-in window as % of duration</ns0:t>
+      <ns0:c r="A86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="87">
       <ns0:c r="A87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>0.15x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-out window as % of duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="88">
       <ns0:c r="A88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionInstantTransition</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Skip smooth-in/out transitions for instant time scale change</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
       <ns0:c r="A89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C89" t="inlineStr" s="0">
@@ -3357,44 +3357,44 @@
       </ns0:c>
       <ns0:c r="D89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>45.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="90">
       <ns0:c r="A90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E90" t="inlineStr" s="0">
@@ -3404,135 +3404,135 @@
       </ns0:c>
       <ns0:c r="F90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G90" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="91">
-      <ns0:c r="A91" t="inlineStr" s="2">
+      <ns0:c r="A91" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B91" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C91" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D91" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E91" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F91" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G91" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionSmoothOut</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Default</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G91" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Transition out of slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="92">
       <ns0:c r="A92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.15x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G92" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="93">
-      <ns0:c r="A93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>5.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G93" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
+      <ns0:c r="A93" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B93" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C93" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D93" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E93" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F93" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G93" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="94">
       <ns0:c r="A94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C94" t="inlineStr" s="0">
@@ -3542,155 +3542,155 @@
       </ns0:c>
       <ns0:c r="D94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>45.0s</ns0:t>
+          <ns0:t>50%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>CustomChanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="95">
       <ns0:c r="A95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>0.30x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-in window as % of duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="96">
       <ns0:c r="A96" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B96" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C96" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D96" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>1.2s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E96" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F96" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G96" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-out window as % of duration</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="97">
       <ns0:c r="A97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionInstantTransition</ns0:t>
+          <ns0:t>OptionCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>7.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CustomCooldownProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Skip smooth-in/out transitions for instant time scale change</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="98">
       <ns0:c r="A98" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B98" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C98" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D98" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E98" t="inlineStr" s="0">
@@ -3700,219 +3700,219 @@
       </ns0:c>
       <ns0:c r="F98" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G98" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="99">
-      <ns0:c r="A99" t="inlineStr" s="2">
+      <ns0:c r="A99" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B99" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C99" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D99" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E99" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F99" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G99" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
+      <ns0:c r="B99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>OptionSmoothOut</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Arrow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Default</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>SmoothnessPresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G99" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Transition out of slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="100">
       <ns0:c r="A100" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B100" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C100" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D100" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>50%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E100" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F100" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomChanceProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G100" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="101">
-      <ns0:c r="A101" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B101" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C101" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D101" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.30x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E101" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F101" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G101" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="A101" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B101" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C101" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D101" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E101" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F101" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G101" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="102">
       <ns0:c r="A102" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B102" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionDebugLogging</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C102" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D102" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.2s</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E102" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F102" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G102" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="103">
       <ns0:c r="A103" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B103" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionQuickTestTrigger</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C103" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>Arrow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D103" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>7.0s</ns0:t>
+          <ns0:t>TriggerBasicKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E103" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F103" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CustomCooldownProvider</ns0:t>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G103" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Which trigger to simulate</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="104">
       <ns0:c r="A104" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B104" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionQuickTestNow</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C104" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D104" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E104" t="inlineStr" s="0">
@@ -3922,34 +3922,34 @@
       </ns0:c>
       <ns0:c r="F104" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G104" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-in window as % of duration</ns0:t>
+          <ns0:t>Toggle to fire the selected trigger once</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="105">
       <ns0:c r="A105" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B105" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C105" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Arrow</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D105" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E105" t="inlineStr" s="0">
@@ -3959,71 +3959,71 @@
       </ns0:c>
       <ns0:c r="F105" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="G105" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>Smooth-out window as % of duration</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="106">
-      <ns0:c r="A106" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B106" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionInstantTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C106" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D106" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E106" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F106" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G106" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Skip smooth-in/out transitions for instant time scale change</ns0:t>
+      <ns0:c r="A106" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryStatistics</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B106" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C106" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D106" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E106" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F106" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="G106" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="107">
       <ns0:c r="A107" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B107" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>OptionResetStats</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C107" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D107" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t/>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E107" t="inlineStr" s="0">
@@ -4037,265 +4037,6 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="G107" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="108">
-      <ns0:c r="A108" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B108" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C108" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D108" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E108" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F108" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G108" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="109">
-      <ns0:c r="A109" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B109" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionDebugLogging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C109" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D109" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E109" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F109" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G109" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Enable verbose debug logging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="110">
-      <ns0:c r="A110" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B110" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionQuickTestTrigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C110" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Arrow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D110" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E110" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F110" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>QuickTestTriggerProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G110" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Which trigger to simulate</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="111">
-      <ns0:c r="A111" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B111" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionQuickTestNow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C111" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D111" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E111" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F111" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G111" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle to fire the selected trigger once</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="112">
-      <ns0:c r="A112" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B112" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C112" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D112" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E112" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F112" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G112" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="113">
-      <ns0:c r="A113" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryStatistics</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B113" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C113" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D113" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E113" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F113" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G113" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="114">
-      <ns0:c r="A114" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>CategoryStatistics</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B114" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>OptionResetStats</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C114" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D114" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E114" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F114" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t/>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="G114" t="inlineStr" s="0">
         <ns0:is>
           <ns0:t>Toggle to reset all statistics</ns0:t>
         </ns0:is>

</xml_diff>

<commit_message>
Update duration system with new base values and multipliers
Base durations (Standard preset):
- Basic Kill: 2.5s
- Parry: 1.5s
- Dismemberment: 2.0s
- Critical: 3.0s
- Decapitation: 3.25s
- Last Enemy: 2.75s
- Last Stand: 3.5s

Duration multipliers:
- Very Short: x0.5
- Short: x0.7
- Standard: x1.0
- Long: x1.3
- Extended: x1.5

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -1692,12 +1692,12 @@
       </ns0:c>
       <ns0:c r="D44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.0s</ns0:t>
+          <ns0:t>2.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="0">
@@ -2025,12 +2025,12 @@
       </ns0:c>
       <ns0:c r="D53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>3.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="0">
@@ -2358,12 +2358,12 @@
       </ns0:c>
       <ns0:c r="D62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.5s</ns0:t>
+          <ns0:t>2.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="0">
@@ -2691,12 +2691,12 @@
       </ns0:c>
       <ns0:c r="D71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>2.0s</ns0:t>
+          <ns0:t>3.25s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F71" t="inlineStr" s="0">
@@ -3024,12 +3024,12 @@
       </ns0:c>
       <ns0:c r="D80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>3.0s</ns0:t>
+          <ns0:t>2.75s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F80" t="inlineStr" s="0">
@@ -3320,12 +3320,12 @@
       </ns0:c>
       <ns0:c r="D88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>3.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="0">
@@ -3616,12 +3616,12 @@
       </ns0:c>
       <ns0:c r="D96" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>1.2s</ns0:t>
+          <ns0:t>1.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E96" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F96" t="inlineStr" s="0">
@@ -4181,7 +4181,7 @@
       </ns0:c>
       <ns0:c r="B11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.8s | 3.0s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Update intensity (time scale) system with per-trigger Standard preset values
Adds distinct time scale values for each trigger based on significance:
- Parry: 34%, Dismemberment: 30%, Basic Kill: 28%, Last Enemy: 26%
- Critical: 25%, Decapitation: 23%, Last Stand: 21%

Intensity presets scale from these base values:
- Subtle: +12%, Standard: baseline, Dramatic: -5%, Cinematic: -10%, Epic: -15%

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -1655,12 +1655,12 @@
       </ns0:c>
       <ns0:c r="D43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.35x</ns0:t>
+          <ns0:t>0.28x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F43" t="inlineStr" s="0">
@@ -1993,7 +1993,7 @@
       </ns0:c>
       <ns0:c r="E52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="0">
@@ -2326,7 +2326,7 @@
       </ns0:c>
       <ns0:c r="E61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F61" t="inlineStr" s="0">
@@ -2654,12 +2654,12 @@
       </ns0:c>
       <ns0:c r="D70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.20x</ns0:t>
+          <ns0:t>0.23x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F70" t="inlineStr" s="0">
@@ -2987,12 +2987,12 @@
       </ns0:c>
       <ns0:c r="D79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.20x</ns0:t>
+          <ns0:t>0.26x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F79" t="inlineStr" s="0">
@@ -3283,12 +3283,12 @@
       </ns0:c>
       <ns0:c r="D87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.15x</ns0:t>
+          <ns0:t>0.21x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F87" t="inlineStr" s="0">
@@ -3579,12 +3579,12 @@
       </ns0:c>
       <ns0:c r="D95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.30x</ns0:t>
+          <ns0:t>0.34x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F95" t="inlineStr" s="0">
@@ -4217,7 +4217,7 @@
       </ns0:c>
       <ns0:c r="B14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.25x | 0.30x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Update standard cooldown values for all triggers
New cooldowns: Basic Kill 10s, Parry 5s, Dismemberment 10s, Critical 10s,
Decapitation 10s, Last Enemy 20s (was 0), Last Stand 60s (was 45s).

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -1729,12 +1729,12 @@
       </ns0:c>
       <ns0:c r="D45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="0">
@@ -2062,12 +2062,12 @@
       </ns0:c>
       <ns0:c r="D54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="0">
@@ -2395,12 +2395,12 @@
       </ns0:c>
       <ns0:c r="D63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>5.0s</ns0:t>
+          <ns0:t>10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F63" t="inlineStr" s="0">
@@ -2728,12 +2728,12 @@
       </ns0:c>
       <ns0:c r="D72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>4.0s</ns0:t>
+          <ns0:t>10.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F72" t="inlineStr" s="0">
@@ -3061,12 +3061,12 @@
       </ns0:c>
       <ns0:c r="D81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>20.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="0">
@@ -3357,12 +3357,12 @@
       </ns0:c>
       <ns0:c r="D89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>45.0s</ns0:t>
+          <ns0:t>60.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="0">
@@ -3653,12 +3653,12 @@
       </ns0:c>
       <ns0:c r="D97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>7.0s</ns0:t>
+          <ns0:t>5.0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F97" t="inlineStr" s="0">
@@ -4169,7 +4169,7 @@
       </ns0:c>
       <ns0:c r="B10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 19.6s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Add Preset Reference sheet to MENU_MOCK.xlsx
New sheet documents all preset systems:
- Intensity: per-trigger time scale values for all 5 presets
- Duration: base values per trigger + multipliers (0.5x-1.5x)
- Cooldown: base values per trigger + multipliers (0x-3.0x)
- Chance: base values per trigger + multipliers (0.5x-1.4x)
- Fade: smoothing percentages (0%-40%)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -3,7 +3,8 @@
 <ns0:workbook xmlns:ns0="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ns1="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ns1:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <ns0:sheets>
     <ns0:sheet name="Menu Mock" sheetId="1" ns1:id="rId1"/>
-    <ns0:sheet name="Providers" sheetId="2" ns1:id="rId2"/>
+    <ns0:sheet name="Preset Reference" sheetId="2" ns1:id="rId2"/>
+    <ns0:sheet name="Providers" sheetId="3" ns1:id="rId3"/>
   </ns0:sheets>
 </ns0:workbook>
 </file>
@@ -4049,6 +4050,2389 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <ns0:worksheet xmlns:ns0="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <ns0:cols>
+    <ns0:col min="1" max="1" width="42.00" customWidth="1"/>
+    <ns0:col min="2" max="2" width="24.00" customWidth="1"/>
+    <ns0:col min="3" max="3" width="26.00" customWidth="1"/>
+    <ns0:col min="4" max="4" width="10.00" customWidth="1"/>
+    <ns0:col min="5" max="5" width="11.00" customWidth="1"/>
+    <ns0:col min="6" max="6" width="8.00" customWidth="1"/>
+  </ns0:cols>
+  <ns0:sheetData>
+    <ns0:row r="1">
+      <ns0:c r="A1" t="inlineStr" s="1">
+        <ns0:is>
+          <ns0:t>Preset Reference</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B1" t="inlineStr" s="1">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C1" t="inlineStr" s="1">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D1" t="inlineStr" s="1">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E1" t="inlineStr" s="1">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F1" t="inlineStr" s="1">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="2">
+      <ns0:c r="A2" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B2" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C2" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D2" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E2" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F2" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="3">
+      <ns0:c r="A3" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>INTENSITY PRESET - Time Scale Values</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B3" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C3" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D3" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E3" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F3" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="4">
+      <ns0:c r="A4" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B4" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Subtle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C4" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Standard</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D4" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Dramatic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E4" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cinematic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F4" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Epic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="5">
+      <ns0:c r="A5" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B5" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>46%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C5" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>34%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D5" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>29%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E5" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>24%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F5" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>19%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="6">
+      <ns0:c r="A6" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Dismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B6" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>42%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C6" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>30%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D6" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>25%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E6" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>20%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F6" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>15%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="7">
+      <ns0:c r="A7" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B7" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>40%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C7" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>28%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D7" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>23%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E7" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>18%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F7" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>13%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="8">
+      <ns0:c r="A8" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B8" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>38%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C8" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>26%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D8" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>21%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E8" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>16%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F8" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>11%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="9">
+      <ns0:c r="A9" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Critical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B9" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>37%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C9" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>25%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D9" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>20%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E9" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>15%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F9" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>10%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="10">
+      <ns0:c r="A10" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B10" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>35%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C10" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>23%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D10" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>18%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E10" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>13%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F10" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>8%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="11">
+      <ns0:c r="A11" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B11" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>33%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C11" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>21%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D11" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>16%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E11" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>11%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F11" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>8%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="12">
+      <ns0:c r="A12" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B12" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C12" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D12" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E12" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F12" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="13">
+      <ns0:c r="A13" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>DURATION PRESET - Multipliers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B13" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C13" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D13" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E13" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F13" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="14">
+      <ns0:c r="A14" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Preset</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B14" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Multiplier</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C14" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D14" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E14" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F14" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="15">
+      <ns0:c r="A15" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Very Short</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B15" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.5x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C15" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D15" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E15" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F15" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="16">
+      <ns0:c r="A16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Short</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.7x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F16" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="17">
+      <ns0:c r="A17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Standard</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.0x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F17" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="18">
+      <ns0:c r="A18" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Long</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B18" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.3x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C18" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D18" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E18" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F18" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="19">
+      <ns0:c r="A19" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Extended</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B19" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.5x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C19" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D19" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E19" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F19" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="20">
+      <ns0:c r="A20" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B20" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C20" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D20" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E20" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F20" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="21">
+      <ns0:c r="A21" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>DURATION PRESET - Base Values (Standard)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B21" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C21" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D21" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E21" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F21" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="22">
+      <ns0:c r="A22" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B22" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Base Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C22" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D22" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E22" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F22" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="23">
+      <ns0:c r="A23" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B23" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C23" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D23" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E23" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F23" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="24">
+      <ns0:c r="A24" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Dismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B24" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C24" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D24" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E24" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F24" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="25">
+      <ns0:c r="A25" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B25" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C25" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D25" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E25" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F25" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="26">
+      <ns0:c r="A26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2.75s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F26" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="27">
+      <ns0:c r="A27" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Critical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B27" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>3.0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C27" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D27" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E27" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F27" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="28">
+      <ns0:c r="A28" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B28" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>3.25s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C28" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D28" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E28" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F28" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="29">
+      <ns0:c r="A29" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B29" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>3.5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C29" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D29" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E29" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F29" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="30">
+      <ns0:c r="A30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F30" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="31">
+      <ns0:c r="A31" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>COOLDOWN PRESET - Multipliers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B31" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C31" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D31" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E31" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F31" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="32">
+      <ns0:c r="A32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Preset</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Multiplier</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="33">
+      <ns0:c r="A33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0x (disabled)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F33" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="34">
+      <ns0:c r="A34" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Short</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B34" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.6x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C34" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D34" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E34" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F34" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="35">
+      <ns0:c r="A35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Standard</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.0x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F35" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="36">
+      <ns0:c r="A36" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Long</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B36" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>2.0x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C36" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D36" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E36" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F36" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="37">
+      <ns0:c r="A37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Extended</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>3.0x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F37" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="38">
+      <ns0:c r="A38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F38" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="39">
+      <ns0:c r="A39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>COOLDOWN PRESET - Base Values (Standard)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F39" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="40">
+      <ns0:c r="A40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Base Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="41">
+      <ns0:c r="A41" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B41" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>5s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C41" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D41" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E41" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F41" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="42">
+      <ns0:c r="A42" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B42" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>10s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C42" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D42" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E42" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F42" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="43">
+      <ns0:c r="A43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Dismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>10s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F43" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="44">
+      <ns0:c r="A44" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Critical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B44" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>10s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C44" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D44" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E44" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F44" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="45">
+      <ns0:c r="A45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>10s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F45" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="46">
+      <ns0:c r="A46" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B46" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>20s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C46" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D46" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E46" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F46" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="47">
+      <ns0:c r="A47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>60s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F47" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="48">
+      <ns0:c r="A48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F48" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="49">
+      <ns0:c r="A49" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CHANCE PRESET - Multipliers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B49" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C49" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D49" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E49" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F49" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="50">
+      <ns0:c r="A50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Preset</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Multiplier</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="51">
+      <ns0:c r="A51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>100% (always triggers)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F51" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="52">
+      <ns0:c r="A52" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Very Rare</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B52" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.5x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C52" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D52" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E52" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F52" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="53">
+      <ns0:c r="A53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Rare</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0.6x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F53" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="54">
+      <ns0:c r="A54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Standard</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.0x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F54" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="55">
+      <ns0:c r="A55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Frequent</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>1.4x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F55" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="56">
+      <ns0:c r="A56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F56" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="57">
+      <ns0:c r="A57" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CHANCE PRESET - Base Values (Standard)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B57" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C57" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D57" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E57" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F57" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="58">
+      <ns0:c r="A58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Base Chance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="59">
+      <ns0:c r="A59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Basic Kill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>25%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F59" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="60">
+      <ns0:c r="A60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Parry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>50%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F60" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="61">
+      <ns0:c r="A61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Dismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>60%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F61" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="62">
+      <ns0:c r="A62" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Critical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B62" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>75%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C62" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D62" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E62" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F62" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="63">
+      <ns0:c r="A63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Decapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>90%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F63" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="64">
+      <ns0:c r="A64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Enemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>100%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F64" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="65">
+      <ns0:c r="A65" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B65" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>100%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C65" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D65" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E65" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F65" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="66">
+      <ns0:c r="A66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F66" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="67">
+      <ns0:c r="A67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>FADE PRESETS - Smoothing Percentages</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="68">
+      <ns0:c r="A68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Preset</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothing %</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Description</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="69">
+      <ns0:c r="A69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Instant</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>0%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>No transition, immediate</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F69" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="70">
+      <ns0:c r="A70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Default</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>10%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Natural B&amp;S feel</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F70" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="71">
+      <ns0:c r="A71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Quick Fade</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>15%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Quick transition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F71" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="72">
+      <ns0:c r="A72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Medium Fade</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>20%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Moderate transition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F72" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="73">
+      <ns0:c r="A73" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Long Fade</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B73" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>30%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C73" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Slow transition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D73" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E73" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F73" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="74">
+      <ns0:c r="A74" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Very Long Fade</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B74" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>40%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C74" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t>Very gradual transition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D74" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E74" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F74" t="inlineStr" s="0">
+        <ns0:is>
+          <ns0:t/>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+  </ns0:sheetData>
+</ns0:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<ns0:worksheet xmlns:ns0="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <ns0:cols>
     <ns0:col min="1" max="1" width="39.00" customWidth="1"/>
     <ns0:col min="2" max="2" width="60.00" customWidth="1"/>
   </ns0:cols>

</xml_diff>

<commit_message>
Expand dropdown providers with comprehensive value ranges
- TimeScale: 0.05-0.50 in 0.01 increments (46 values)
- Duration: 0.5-10s in 0.25s increments (39 values)
- Cooldown: 0-180s with variable increments (52 values)
- Chance: 5-100% in 5% increments (20 values)

Fixes preset sync issues where calculated values had no matching
dropdown option, causing all triggers to show the same value.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -1617,14 +1617,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D42" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>25%</ns0:t>
-        </ns0:is>
+      <ns0:c r="D42" s="0">
+        <ns0:v>0.25</ns0:v>
       </ns0:c>
       <ns0:c r="E42" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F42" t="inlineStr" s="0">
@@ -1654,14 +1652,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D43" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.28x</ns0:t>
-        </ns0:is>
+      <ns0:c r="D43" s="0">
+        <ns0:v>0.28</ns0:v>
       </ns0:c>
       <ns0:c r="E43" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F43" t="inlineStr" s="0">
@@ -1691,14 +1687,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D44" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2.5s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D44" s="0">
+        <ns0:v>2.5</ns0:v>
       </ns0:c>
       <ns0:c r="E44" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="0">
@@ -1728,14 +1722,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D45" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>10.0s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D45" s="0">
+        <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="E45" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="0">
@@ -1950,14 +1942,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D51" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>75%</ns0:t>
-        </ns0:is>
+      <ns0:c r="D51" s="0">
+        <ns0:v>0.75</ns0:v>
       </ns0:c>
       <ns0:c r="E51" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F51" t="inlineStr" s="0">
@@ -1987,14 +1977,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D52" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.25x</ns0:t>
-        </ns0:is>
+      <ns0:c r="D52" s="0">
+        <ns0:v>0.25</ns0:v>
       </ns0:c>
       <ns0:c r="E52" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="0">
@@ -2024,14 +2012,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D53" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>3.0s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D53" s="0">
+        <ns0:v>3.0</ns0:v>
       </ns0:c>
       <ns0:c r="E53" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="0">
@@ -2061,14 +2047,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D54" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>10.0s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D54" s="0">
+        <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="E54" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="0">
@@ -2283,14 +2267,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D60" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>60%</ns0:t>
-        </ns0:is>
+      <ns0:c r="D60" s="0">
+        <ns0:v>0.6</ns0:v>
       </ns0:c>
       <ns0:c r="E60" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="0">
@@ -2320,14 +2302,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D61" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.30x</ns0:t>
-        </ns0:is>
+      <ns0:c r="D61" s="0">
+        <ns0:v>0.3</ns0:v>
       </ns0:c>
       <ns0:c r="E61" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F61" t="inlineStr" s="0">
@@ -2357,14 +2337,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D62" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2.0s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D62" s="0">
+        <ns0:v>2.0</ns0:v>
       </ns0:c>
       <ns0:c r="E62" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="0">
@@ -2394,14 +2372,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D63" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>10.0s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D63" s="0">
+        <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="E63" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F63" t="inlineStr" s="0">
@@ -2616,14 +2592,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D69" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>90%</ns0:t>
-        </ns0:is>
+      <ns0:c r="D69" s="0">
+        <ns0:v>0.9</ns0:v>
       </ns0:c>
       <ns0:c r="E69" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F69" t="inlineStr" s="0">
@@ -2653,14 +2627,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D70" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.23x</ns0:t>
-        </ns0:is>
+      <ns0:c r="D70" s="0">
+        <ns0:v>0.23</ns0:v>
       </ns0:c>
       <ns0:c r="E70" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F70" t="inlineStr" s="0">
@@ -2690,14 +2662,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D71" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>3.25s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D71" s="0">
+        <ns0:v>3.25</ns0:v>
       </ns0:c>
       <ns0:c r="E71" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F71" t="inlineStr" s="0">
@@ -2727,14 +2697,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D72" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>10.0s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D72" s="0">
+        <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="E72" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F72" t="inlineStr" s="0">
@@ -2949,14 +2917,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D78" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>100%</ns0:t>
-        </ns0:is>
+      <ns0:c r="D78" s="0">
+        <ns0:v>1.0</ns0:v>
       </ns0:c>
       <ns0:c r="E78" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F78" t="inlineStr" s="0">
@@ -2986,14 +2952,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D79" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.26x</ns0:t>
-        </ns0:is>
+      <ns0:c r="D79" s="0">
+        <ns0:v>0.26</ns0:v>
       </ns0:c>
       <ns0:c r="E79" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F79" t="inlineStr" s="0">
@@ -3023,14 +2987,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D80" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>2.75s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D80" s="0">
+        <ns0:v>2.75</ns0:v>
       </ns0:c>
       <ns0:c r="E80" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F80" t="inlineStr" s="0">
@@ -3060,14 +3022,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D81" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>20.0s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D81" s="0">
+        <ns0:v>20</ns0:v>
       </ns0:c>
       <ns0:c r="E81" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="0">
@@ -3282,14 +3242,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D87" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.21x</ns0:t>
-        </ns0:is>
+      <ns0:c r="D87" s="0">
+        <ns0:v>0.21</ns0:v>
       </ns0:c>
       <ns0:c r="E87" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F87" t="inlineStr" s="0">
@@ -3319,14 +3277,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D88" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>3.5s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D88" s="0">
+        <ns0:v>3.5</ns0:v>
       </ns0:c>
       <ns0:c r="E88" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="0">
@@ -3356,14 +3312,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D89" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>60.0s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D89" s="0">
+        <ns0:v>60</ns0:v>
       </ns0:c>
       <ns0:c r="E89" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="0">
@@ -3541,14 +3495,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D94" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>50%</ns0:t>
-        </ns0:is>
+      <ns0:c r="D94" s="0">
+        <ns0:v>0.5</ns0:v>
       </ns0:c>
       <ns0:c r="E94" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F94" t="inlineStr" s="0">
@@ -3578,14 +3530,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D95" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>0.34x</ns0:t>
-        </ns0:is>
+      <ns0:c r="D95" s="0">
+        <ns0:v>0.34</ns0:v>
       </ns0:c>
       <ns0:c r="E95" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F95" t="inlineStr" s="0">
@@ -3615,14 +3565,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D96" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>1.5s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D96" s="0">
+        <ns0:v>1.5</ns0:v>
       </ns0:c>
       <ns0:c r="E96" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F96" t="inlineStr" s="0">
@@ -3652,14 +3600,12 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D97" t="inlineStr" s="0">
-        <ns0:is>
-          <ns0:t>5.0s</ns0:t>
-        </ns0:is>
+      <ns0:c r="D97" s="0">
+        <ns0:v>5</ns0:v>
       </ns0:c>
       <ns0:c r="E97" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F97" t="inlineStr" s="0">
@@ -6541,7 +6487,7 @@
       </ns0:c>
       <ns0:c r="B9" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>12.5% | 15% | 25% | 30% | 35% | 36% | 37.5% | 45% | 50% | 54% | 60% | 70% | 75% | 84% | 90% | 100%</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -6553,7 +6499,7 @@
       </ns0:c>
       <ns0:c r="B10" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0s | 1.6s | 2.0s | 2.4s | 2.5s | 2.8s | 3.0s | 3.5s | 4.0s | 4.2s | 4.9s | 5.0s | 6.0s | 7.0s | 7.2s | 7.5s | 8.0s | 9.0s | 10.0s | 10.5s | 11.2s | 12.6s | 14.0s | 17.5s | 18.0s | 20.0s | 22.5s | 24.5s | 27.0s | 28.0s | 31.5s | 45.0s | 60.0s | 67.5s | 81.0s | 90.0s | 126.0s | 157.5s</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -6565,7 +6511,7 @@
       </ns0:c>
       <ns0:c r="B11" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.5s | 0.6s | 0.72s | 0.75s | 0.90s | 1.0s | 1.125s | 1.2s | 1.25s | 1.4s | 1.5s | 1.68s | 1.8s | 1.875s | 2.0s | 2.1s | 2.16s | 2.25s | 2.4s | 2.5s | 2.7s | 2.75s | 2.8s | 3.0s | 3.25s | 3.5s | 3.6s | 3.75s | 4.0s | 4.2s | 4.5s | 5.0s | 5.4s | 6.0s | 6.25s | 7.0s | 7.5s | 9.0s | 10.0s</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -6601,7 +6547,7 @@
       </ns0:c>
       <ns0:c r="B14" t="inlineStr" s="0">
         <ns0:is>
-          <ns0:t>0.08x | 0.10x | 0.12x | 0.15x | 0.20x | 0.21x | 0.23x | 0.25x | 0.26x | 0.28x | 0.30x | 0.34x | 0.35x | 0.40x | 0.45x | 0.50x</ns0:t>
+          <ns0:t/>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
fix: unique ModOption names to prevent B&S storage key collision
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -1092,7 +1092,7 @@
       </ns0:c>
       <ns0:c r="B42" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionBasicChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C42" t="inlineStr" s="7">
@@ -1117,7 +1117,7 @@
       </ns0:c>
       <ns0:c r="B43" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionBasicTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C43" t="inlineStr" s="7">
@@ -1142,7 +1142,7 @@
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionBasicDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="7">
@@ -1167,7 +1167,7 @@
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionBasicCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C45" t="inlineStr" s="7">
@@ -1197,7 +1197,7 @@
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionBasicSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C46" t="inlineStr" s="8">
@@ -1224,7 +1224,7 @@
       </ns0:c>
       <ns0:c r="B47" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionBasicSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C47" t="inlineStr" s="8">
@@ -1251,7 +1251,7 @@
       </ns0:c>
       <ns0:c r="B48" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionBasicThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C48" t="inlineStr" s="7">
@@ -1291,7 +1291,7 @@
       </ns0:c>
       <ns0:c r="B51" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionCriticalChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C51" t="inlineStr" s="7">
@@ -1316,7 +1316,7 @@
       </ns0:c>
       <ns0:c r="B52" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionCriticalTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C52" t="inlineStr" s="7">
@@ -1341,7 +1341,7 @@
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionCriticalDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C53" t="inlineStr" s="7">
@@ -1366,7 +1366,7 @@
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionCriticalCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C54" t="inlineStr" s="7">
@@ -1396,7 +1396,7 @@
       </ns0:c>
       <ns0:c r="B55" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionCriticalSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C55" t="inlineStr" s="8">
@@ -1423,7 +1423,7 @@
       </ns0:c>
       <ns0:c r="B56" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionCriticalSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C56" t="inlineStr" s="8">
@@ -1450,7 +1450,7 @@
       </ns0:c>
       <ns0:c r="B57" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionCriticalThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C57" t="inlineStr" s="7">
@@ -1490,7 +1490,7 @@
       </ns0:c>
       <ns0:c r="B60" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionDismemberChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C60" t="inlineStr" s="7">
@@ -1515,7 +1515,7 @@
       </ns0:c>
       <ns0:c r="B61" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionDismemberTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C61" t="inlineStr" s="7">
@@ -1540,7 +1540,7 @@
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionDismemberDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C62" t="inlineStr" s="7">
@@ -1565,7 +1565,7 @@
       </ns0:c>
       <ns0:c r="B63" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionDismemberCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C63" t="inlineStr" s="7">
@@ -1595,7 +1595,7 @@
       </ns0:c>
       <ns0:c r="B64" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionDismemberSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C64" t="inlineStr" s="8">
@@ -1622,7 +1622,7 @@
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionDismemberSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="8">
@@ -1649,7 +1649,7 @@
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionDismemberThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="7">
@@ -1689,7 +1689,7 @@
       </ns0:c>
       <ns0:c r="B69" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionDecapChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C69" t="inlineStr" s="7">
@@ -1714,7 +1714,7 @@
       </ns0:c>
       <ns0:c r="B70" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionDecapTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C70" t="inlineStr" s="7">
@@ -1739,7 +1739,7 @@
       </ns0:c>
       <ns0:c r="B71" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionDecapDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C71" t="inlineStr" s="7">
@@ -1764,7 +1764,7 @@
       </ns0:c>
       <ns0:c r="B72" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionDecapCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C72" t="inlineStr" s="7">
@@ -1794,7 +1794,7 @@
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionDecapSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C73" t="inlineStr" s="8">
@@ -1821,7 +1821,7 @@
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionDecapSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C74" t="inlineStr" s="8">
@@ -1848,7 +1848,7 @@
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionDecapThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="7">
@@ -1888,7 +1888,7 @@
       </ns0:c>
       <ns0:c r="B78" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionLastEnemyChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C78" t="inlineStr" s="7">
@@ -1913,7 +1913,7 @@
       </ns0:c>
       <ns0:c r="B79" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C79" t="inlineStr" s="7">
@@ -1938,7 +1938,7 @@
       </ns0:c>
       <ns0:c r="B80" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionLastEnemyDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C80" t="inlineStr" s="7">
@@ -1963,7 +1963,7 @@
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionLastEnemyCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="7">
@@ -1993,7 +1993,7 @@
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionLastEnemySmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="8">
@@ -2020,7 +2020,7 @@
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionLastEnemySmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="8">
@@ -2047,7 +2047,7 @@
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionThirdPersonDistribution</ns0:t>
+          <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C84" t="inlineStr" s="7">
@@ -2087,7 +2087,7 @@
       </ns0:c>
       <ns0:c r="B87" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionLastStandTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C87" t="inlineStr" s="7">
@@ -2112,7 +2112,7 @@
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionLastStandDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="7">
@@ -2137,7 +2137,7 @@
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionLastStandCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C89" t="inlineStr" s="7">
@@ -2167,7 +2167,7 @@
       </ns0:c>
       <ns0:c r="B90" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionLastStandSmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C90" t="inlineStr" s="8">
@@ -2194,7 +2194,7 @@
       </ns0:c>
       <ns0:c r="B91" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionLastStandSmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C91" t="inlineStr" s="8">
@@ -2229,7 +2229,7 @@
       </ns0:c>
       <ns0:c r="B94" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionChance</ns0:t>
+          <ns0:t>OptionParryChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C94" t="inlineStr" s="7">
@@ -2254,7 +2254,7 @@
       </ns0:c>
       <ns0:c r="B95" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionTimeScale</ns0:t>
+          <ns0:t>OptionParryTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C95" t="inlineStr" s="7">
@@ -2279,7 +2279,7 @@
       </ns0:c>
       <ns0:c r="B96" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDuration</ns0:t>
+          <ns0:t>OptionParryDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C96" t="inlineStr" s="7">
@@ -2304,7 +2304,7 @@
       </ns0:c>
       <ns0:c r="B97" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCooldown</ns0:t>
+          <ns0:t>OptionParryCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C97" t="inlineStr" s="7">
@@ -2334,7 +2334,7 @@
       </ns0:c>
       <ns0:c r="B98" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothIn</ns0:t>
+          <ns0:t>OptionParrySmoothIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C98" t="inlineStr" s="8">
@@ -2361,7 +2361,7 @@
       </ns0:c>
       <ns0:c r="B99" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothOut</ns0:t>
+          <ns0:t>OptionParrySmoothOut</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C99" t="inlineStr" s="8">

</xml_diff>

<commit_message>
refactor: remove DelayOut, simplify Delay to additive time
- Remove DelayOut option from presets and all per-trigger settings
- Change Delay from percentage-of-duration to fixed additive time
- Slow motion now ends instantly (no transition out)
- Simplify delay-related methods and remove unused code

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -453,7 +453,7 @@
       </ns0:c>
       <ns0:c r="B13" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothInPreset</ns0:t>
+          <ns0:t>OptionDelayInPreset</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C13" t="inlineStr" s="8">
@@ -480,7 +480,7 @@
       </ns0:c>
       <ns0:c r="B14" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionSmoothOutPreset</ns0:t>
+          <ns0:t>OptionTriggerProfile</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C14" t="inlineStr" s="8">
@@ -490,47 +490,52 @@
       </ns0:c>
       <ns0:c r="D14" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Default</ns0:t>
+          <ns0:t>All</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F14" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition out of slow motion. Instant = immediate. Default = natural feel.</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="15">
-      <ns0:c r="A15" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryPresetSelection</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B15" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionTriggerProfile</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C15" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D15" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>All</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F15" t="inlineStr" s="4">
-        <ns0:is>
           <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="16"/>
+    <ns0:row r="15"/>
+    <ns0:row r="16">
+      <ns0:c r="A16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryOptionalOverrides</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="17">
-      <ns0:c r="A17" t="inlineStr" s="2">
+      <ns0:c r="A17" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryOptionalOverrides</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B17" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionGlobalCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C17" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D17" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E17" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F17" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -542,7 +547,7 @@
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionGlobalCooldown</ns0:t>
+          <ns0:t>OptionHapticFeedback</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="7">
@@ -552,17 +557,17 @@
       </ns0:c>
       <ns0:c r="D18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
+          <ns0:t>Off | Light | Medium | Strong</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
+          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -574,27 +579,27 @@
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionHapticFeedback</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C19" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionEasingCurve</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C19" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>Smoothstep</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
+          <ns0:t>Transition curve shape. Smoothstep = smooth both ends, Linear = constant speed, EaseIn = slow start, EaseOut = slow end.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -606,67 +611,62 @@
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionEasingCurve</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C20" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
+          <ns0:t>OptionMinTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C20" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>Off (0%) | 5% | 8% | 10% | 15% | 20%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape. Smoothstep = smooth both ends, Linear = constant speed, EaseIn = slow start, EaseOut = slow end.</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="21">
-      <ns0:c r="A21" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryOptionalOverrides</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B21" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionMinTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C21" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D21" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E21" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | 5% | 8% | 10% | 15% | 20%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F21" t="inlineStr" s="4">
-        <ns0:is>
           <ns0:t>Floor for time scale to prevent extreme slow-mo stutter. 0% = no limit.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="22"/>
+    <ns0:row r="21"/>
+    <ns0:row r="22">
+      <ns0:c r="A22" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="23">
-      <ns0:c r="A23" t="inlineStr" s="2">
+      <ns0:c r="A23" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B23" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C23" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D23" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F23" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -678,7 +678,7 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
+          <ns0:t>TriggerThrownImpactKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C24" t="inlineStr" s="6">
@@ -688,12 +688,12 @@
       </ns0:c>
       <ns0:c r="D24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
+          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -705,7 +705,7 @@
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerThrownImpactKill</ns0:t>
+          <ns0:t>TriggerCriticalKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C25" t="inlineStr" s="6">
@@ -715,12 +715,12 @@
       </ns0:c>
       <ns0:c r="D25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -732,7 +732,7 @@
       </ns0:c>
       <ns0:c r="B26" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerCriticalKill</ns0:t>
+          <ns0:t>TriggerDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C26" t="inlineStr" s="6">
@@ -747,7 +747,7 @@
       </ns0:c>
       <ns0:c r="F26" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -759,7 +759,7 @@
       </ns0:c>
       <ns0:c r="B27" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDismemberment</ns0:t>
+          <ns0:t>TriggerDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C27" t="inlineStr" s="6">
@@ -774,7 +774,7 @@
       </ns0:c>
       <ns0:c r="F27" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -786,7 +786,7 @@
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDecapitation</ns0:t>
+          <ns0:t>TriggerLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C28" t="inlineStr" s="6">
@@ -801,7 +801,7 @@
       </ns0:c>
       <ns0:c r="F28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -813,7 +813,7 @@
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastEnemy</ns0:t>
+          <ns0:t>TriggerLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C29" t="inlineStr" s="6">
@@ -828,7 +828,7 @@
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -840,22 +840,27 @@
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C30" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionLastStandThreshold</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C30" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>15%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E30" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -867,62 +872,62 @@
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandThreshold</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C31" t="inlineStr" s="7">
+          <ns0:t>TriggerParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C31" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D31" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F31" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger on successful weapon deflections</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="32"/>
+    <ns0:row r="33">
+      <ns0:c r="A33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="34">
+      <ns0:c r="A34" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B34" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCameraDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C34" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D31" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>15%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E31" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F31" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="32">
-      <ns0:c r="A32" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B32" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C32" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D32" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F32" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Trigger on successful weapon deflections</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="33"/>
-    <ns0:row r="34">
-      <ns0:c r="A34" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
+      <ns0:c r="D34" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>3m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E34" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F34" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -934,27 +939,22 @@
       </ns0:c>
       <ns0:c r="B35" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCameraDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C35" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionRandomizeDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C35" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D35" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>3m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E35" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F35" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
+          <ns0:t>Randomize distance per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -966,22 +966,27 @@
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C36" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionCameraHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C36" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>1.5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E36" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize distance per killcam</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -993,27 +998,22 @@
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCameraHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C37" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionRandomizeHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C37" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E37" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Randomize height per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1025,62 +1025,60 @@
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C38" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionOrbitSpeed</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C38" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>Slow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E38" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize height per killcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="39">
-      <ns0:c r="A39" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B39" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionOrbitSpeed</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C39" t="inlineStr" s="7">
+          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="39"/>
+    <ns0:row r="40">
+      <ns0:c r="A40" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="41">
+      <ns0:c r="A41" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B41" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionBasicChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C41" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D39" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Slow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E39" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F39" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="40"/>
-    <ns0:row r="41">
-      <ns0:c r="A41" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
+      <ns0:c r="D41" s="4">
+        <ns0:v>0.25</ns0:v>
+      </ns0:c>
+      <ns0:c r="F41" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1092,7 +1090,7 @@
       </ns0:c>
       <ns0:c r="B42" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicChance</ns0:t>
+          <ns0:t>OptionBasicTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C42" t="inlineStr" s="7">
@@ -1101,11 +1099,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D42" s="4">
-        <ns0:v>0.25</ns0:v>
+        <ns0:v>0.28</ns0:v>
       </ns0:c>
       <ns0:c r="F42" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1117,7 +1115,7 @@
       </ns0:c>
       <ns0:c r="B43" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicTimeScale</ns0:t>
+          <ns0:t>OptionBasicDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C43" t="inlineStr" s="7">
@@ -1126,11 +1124,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D43" s="4">
-        <ns0:v>0.28</ns0:v>
+        <ns0:v>2.5</ns0:v>
       </ns0:c>
       <ns0:c r="F43" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1142,7 +1140,7 @@
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicDuration</ns0:t>
+          <ns0:t>OptionBasicCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="7">
@@ -1151,11 +1149,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D44" s="4">
-        <ns0:v>2.5</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E44" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1167,25 +1170,22 @@
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C45" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D45" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E45" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>OptionBasicDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C45" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D45" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1197,89 +1197,85 @@
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicSmoothIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C46" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
+          <ns0:t>OptionBasicThirdPerson</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C46" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Default</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E46" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="47">
-      <ns0:c r="A47" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B47" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionBasicSmoothOut</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C47" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D47" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F47" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition out of slow motion</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="47"/>
     <ns0:row r="48">
-      <ns0:c r="A48" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B48" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionBasicThirdPerson</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C48" t="inlineStr" s="7">
+      <ns0:c r="A48" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="49">
+      <ns0:c r="A49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCriticalChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C49" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D48" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E48" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F48" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="49"/>
+      <ns0:c r="D49" s="4">
+        <ns0:v>0.75</ns0:v>
+      </ns0:c>
+      <ns0:c r="F49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="50">
-      <ns0:c r="A50" t="inlineStr" s="2">
+      <ns0:c r="A50" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCriticalTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C50" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D50" s="4">
+        <ns0:v>0.25</ns0:v>
+      </ns0:c>
+      <ns0:c r="F50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1291,7 +1287,7 @@
       </ns0:c>
       <ns0:c r="B51" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalChance</ns0:t>
+          <ns0:t>OptionCriticalDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C51" t="inlineStr" s="7">
@@ -1300,11 +1296,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D51" s="4">
-        <ns0:v>0.75</ns0:v>
+        <ns0:v>3.0</ns0:v>
       </ns0:c>
       <ns0:c r="F51" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1316,7 +1312,7 @@
       </ns0:c>
       <ns0:c r="B52" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalTimeScale</ns0:t>
+          <ns0:t>OptionCriticalCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C52" t="inlineStr" s="7">
@@ -1325,11 +1321,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D52" s="4">
-        <ns0:v>0.25</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E52" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1341,20 +1342,22 @@
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C53" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D53" s="4">
-        <ns0:v>3.0</ns0:v>
+          <ns0:t>OptionCriticalDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C53" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D53" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Default</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1366,7 +1369,7 @@
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalCooldown</ns0:t>
+          <ns0:t>OptionCriticalThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C54" t="inlineStr" s="7">
@@ -1374,83 +1377,39 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D54" s="4">
-        <ns0:v>10</ns0:v>
+      <ns0:c r="D54" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="55">
-      <ns0:c r="A55" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B55" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCriticalSmoothIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C55" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D55" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F55" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="55"/>
     <ns0:row r="56">
-      <ns0:c r="A56" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B56" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCriticalSmoothOut</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C56" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D56" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F56" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition out of slow motion</ns0:t>
+      <ns0:c r="A56" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="57">
       <ns0:c r="A57" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B57" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalThirdPerson</ns0:t>
+          <ns0:t>OptionDismemberChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C57" t="inlineStr" s="7">
@@ -1458,27 +1417,62 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D57" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E57" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D57" s="4">
+        <ns0:v>0.3</ns0:v>
       </ns0:c>
       <ns0:c r="F57" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="58"/>
+          <ns0:t>Chance to trigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="58">
+      <ns0:c r="A58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDismemberTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C58" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D58" s="4">
+        <ns0:v>0.3</ns0:v>
+      </ns0:c>
+      <ns0:c r="F58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="59">
-      <ns0:c r="A59" t="inlineStr" s="2">
+      <ns0:c r="A59" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B59" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDismemberDuration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C59" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D59" s="4">
+        <ns0:v>2.0</ns0:v>
+      </ns0:c>
+      <ns0:c r="F59" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1490,7 +1484,7 @@
       </ns0:c>
       <ns0:c r="B60" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberChance</ns0:t>
+          <ns0:t>OptionDismemberCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C60" t="inlineStr" s="7">
@@ -1499,11 +1493,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D60" s="4">
-        <ns0:v>0.3</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E60" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1515,20 +1514,22 @@
       </ns0:c>
       <ns0:c r="B61" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C61" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D61" s="4">
-        <ns0:v>0.3</ns0:v>
+          <ns0:t>OptionDismemberDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C61" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D61" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Default</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F61" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1540,7 +1541,7 @@
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberDuration</ns0:t>
+          <ns0:t>OptionDismemberThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C62" t="inlineStr" s="7">
@@ -1548,108 +1549,64 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D62" s="4">
-        <ns0:v>2.0</ns0:v>
+      <ns0:c r="D62" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E62" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="63">
-      <ns0:c r="A63" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B63" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDismemberCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C63" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D63" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E63" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F63" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="63"/>
     <ns0:row r="64">
-      <ns0:c r="A64" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B64" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDismemberSmoothIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C64" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D64" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F64" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+      <ns0:c r="A64" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="65">
       <ns0:c r="A65" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberSmoothOut</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C65" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D65" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionDecapChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C65" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D65" s="4">
+        <ns0:v>0.9</ns0:v>
       </ns0:c>
       <ns0:c r="F65" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition out of slow motion</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="66">
       <ns0:c r="A66" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberThirdPerson</ns0:t>
+          <ns0:t>OptionDecapTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="7">
@@ -1657,27 +1614,67 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D66" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E66" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D66" s="4">
+        <ns0:v>0.23</ns0:v>
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="67"/>
+          <ns0:t>Time scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="67">
+      <ns0:c r="A67" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B67" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDecapDuration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C67" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D67" s="4">
+        <ns0:v>3.25</ns0:v>
+      </ns0:c>
+      <ns0:c r="F67" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="68">
-      <ns0:c r="A68" t="inlineStr" s="2">
+      <ns0:c r="A68" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDecapCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C68" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D68" s="4">
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1689,20 +1686,22 @@
       </ns0:c>
       <ns0:c r="B69" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C69" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D69" s="4">
-        <ns0:v>0.9</ns0:v>
+          <ns0:t>OptionDecapDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C69" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D69" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Default</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F69" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1714,7 +1713,7 @@
       </ns0:c>
       <ns0:c r="B70" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapTimeScale</ns0:t>
+          <ns0:t>OptionDecapThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C70" t="inlineStr" s="7">
@@ -1722,133 +1721,89 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D70" s="4">
-        <ns0:v>0.23</ns0:v>
+      <ns0:c r="D70" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E70" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F70" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="71">
-      <ns0:c r="A71" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B71" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDecapDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C71" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D71" s="4">
-        <ns0:v>3.25</ns0:v>
-      </ns0:c>
-      <ns0:c r="F71" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="71"/>
     <ns0:row r="72">
-      <ns0:c r="A72" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B72" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDecapCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C72" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D72" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E72" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F72" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+      <ns0:c r="A72" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="73">
       <ns0:c r="A73" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapSmoothIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C73" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D73" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionLastEnemyChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C73" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D73" s="4">
+        <ns0:v>1.0</ns0:v>
       </ns0:c>
       <ns0:c r="F73" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="74">
       <ns0:c r="A74" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapSmoothOut</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C74" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D74" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C74" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D74" s="4">
+        <ns0:v>0.26</ns0:v>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition out of slow motion</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="75">
       <ns0:c r="A75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapThirdPerson</ns0:t>
+          <ns0:t>OptionLastEnemyDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="7">
@@ -1856,27 +1811,69 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D75" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E75" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D75" s="4">
+        <ns0:v>2.75</ns0:v>
       </ns0:c>
       <ns0:c r="F75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="76"/>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="76">
+      <ns0:c r="A76" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B76" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastEnemyCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C76" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D76" s="4">
+        <ns0:v>30</ns0:v>
+      </ns0:c>
+      <ns0:c r="E76" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F76" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="77">
-      <ns0:c r="A77" t="inlineStr" s="2">
+      <ns0:c r="A77" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B77" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastEnemyDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C77" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D77" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Default</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F77" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1888,7 +1885,7 @@
       </ns0:c>
       <ns0:c r="B78" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyChance</ns0:t>
+          <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C78" t="inlineStr" s="7">
@@ -1896,74 +1893,39 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D78" s="4">
-        <ns0:v>1.0</ns0:v>
+      <ns0:c r="D78" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E78" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F78" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="79">
-      <ns0:c r="A79" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B79" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C79" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D79" s="4">
-        <ns0:v>0.26</ns0:v>
-      </ns0:c>
-      <ns0:c r="F79" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="79"/>
     <ns0:row r="80">
-      <ns0:c r="A80" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B80" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastEnemyDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C80" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D80" s="4">
-        <ns0:v>2.75</ns0:v>
-      </ns0:c>
-      <ns0:c r="F80" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
+      <ns0:c r="A80" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="81">
       <ns0:c r="A81" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyCooldown</ns0:t>
+          <ns0:t>OptionLastStandTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="7">
@@ -1972,102 +1934,93 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D81" s="4">
-        <ns0:v>30</ns0:v>
-      </ns0:c>
-      <ns0:c r="E81" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.30</ns0:v>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="82">
       <ns0:c r="A82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemySmoothIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C82" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D82" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionLastStandDuration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C82" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D82" s="4">
+        <ns0:v>4.0</ns0:v>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="83">
       <ns0:c r="A83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemySmoothOut</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C83" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D83" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
+          <ns0:t>OptionLastStandCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C83" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D83" s="4">
+        <ns0:v>90</ns0:v>
+      </ns0:c>
+      <ns0:c r="E83" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition out of slow motion</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="84">
       <ns0:c r="A84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C84" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionLastStandDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C84" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E84" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2075,19 +2028,19 @@
     <ns0:row r="86">
       <ns0:c r="A86" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="87">
       <ns0:c r="A87" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B87" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandTimeScale</ns0:t>
+          <ns0:t>OptionParryChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C87" t="inlineStr" s="7">
@@ -2096,23 +2049,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D87" s="4">
-        <ns0:v>0.30</ns0:v>
+        <ns0:v>0.5</ns0:v>
       </ns0:c>
       <ns0:c r="F87" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="88">
       <ns0:c r="A88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandDuration</ns0:t>
+          <ns0:t>OptionParryTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="7">
@@ -2121,23 +2074,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D88" s="4">
-        <ns0:v>4.0</ns0:v>
+        <ns0:v>0.34</ns0:v>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
       <ns0:c r="A89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandCooldown</ns0:t>
+          <ns0:t>OptionParryDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C89" t="inlineStr" s="7">
@@ -2146,55 +2099,53 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D89" s="4">
-        <ns0:v>90</ns0:v>
-      </ns0:c>
-      <ns0:c r="E89" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>1.5</ns0:v>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="90">
       <ns0:c r="A90" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B90" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandSmoothIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C90" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D90" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
+          <ns0:t>OptionParryCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C90" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D90" s="4">
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="E90" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F90" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="91">
       <ns0:c r="A91" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B91" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandSmoothOut</ns0:t>
+          <ns0:t>OptionParryDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C91" t="inlineStr" s="8">
@@ -2209,7 +2160,7 @@
       </ns0:c>
       <ns0:c r="F91" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition out of slow motion</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2217,288 +2168,121 @@
     <ns0:row r="93">
       <ns0:c r="A93" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="94">
       <ns0:c r="A94" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B94" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C94" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D94" s="4">
-        <ns0:v>0.5</ns0:v>
+          <ns0:t>OptionDebugLogging</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C94" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D94" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F94" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="95">
       <ns0:c r="A95" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B95" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C95" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D95" s="4">
-        <ns0:v>0.34</ns0:v>
+          <ns0:t>OptionQuickTestTrigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C95" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D95" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F95" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Which trigger to simulate</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="96">
       <ns0:c r="A96" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B96" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C96" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D96" s="4">
-        <ns0:v>1.5</ns0:v>
+          <ns0:t>OptionQuickTestNow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C96" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D96" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F96" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="97">
-      <ns0:c r="A97" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B97" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionParryCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C97" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D97" s="4">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="E97" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F97" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Toggle to fire the selected trigger once</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="97"/>
     <ns0:row r="98">
-      <ns0:c r="A98" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B98" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionParrySmoothIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C98" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D98" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F98" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+      <ns0:c r="A98" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="99">
       <ns0:c r="A99" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B99" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParrySmoothOut</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C99" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
+          <ns0:t>OptionResetStats</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C99" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D99" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Default</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F99" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition out of slow motion</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="100"/>
-    <ns0:row r="101">
-      <ns0:c r="A101" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="102">
-      <ns0:c r="A102" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B102" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDebugLogging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C102" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D102" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F102" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Enable verbose debug logging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="103">
-      <ns0:c r="A103" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B103" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionQuickTestTrigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C103" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D103" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F103" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Which trigger to simulate</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="104">
-      <ns0:c r="A104" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B104" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionQuickTestNow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C104" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D104" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F104" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Toggle to fire the selected trigger once</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="105"/>
-    <ns0:row r="106">
-      <ns0:c r="A106" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryStatistics</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="107">
-      <ns0:c r="A107" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryStatistics</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B107" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionResetStats</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C107" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D107" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F107" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Toggle to reset all statistics</ns0:t>
         </ns0:is>
@@ -3873,26 +3657,26 @@
     <ns0:row r="11">
       <ns0:c r="A11" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomDelayIngProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B11" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>22</ns0:v>
+      </ns0:c>
+      <ns0:c r="C11" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="12">
       <ns0:c r="A12" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CustomSmoothingProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B12" s="4">
-        <ns0:v>22</ns0:v>
-      </ns0:c>
-      <ns0:c r="C12" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="13">
@@ -3923,32 +3707,32 @@
     <ns0:row r="15">
       <ns0:c r="A15" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>DurationPresetProvider</ns0:t>
+          <ns0:t>DelayIngSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B15" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>4</ns0:v>
+      </ns0:c>
+      <ns0:c r="C15" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Instant | Fast | Medium | Slow</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="16">
       <ns0:c r="A16" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>DurationProvider</ns0:t>
+          <ns0:t>DelayPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B16" s="4">
-        <ns0:v>9</ns0:v>
-      </ns0:c>
-      <ns0:c r="C16" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0.5s | 1.0s | 1.5s | 2.0s | 2.5s | 3.0s | 4.0s | 5.0s | 8.0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="17">
       <ns0:c r="A17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>DynamicIntensityPresetProvider</ns0:t>
+          <ns0:t>DurationPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B17" s="4">
@@ -3958,37 +3742,32 @@
     <ns0:row r="18">
       <ns0:c r="A18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>EasingCurveProvider</ns0:t>
+          <ns0:t>DurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" s="4">
-        <ns0:v>4</ns0:v>
+        <ns0:v>9</ns0:v>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>0.5s | 1.0s | 1.5s | 2.0s | 2.5s | 3.0s | 4.0s | 5.0s | 8.0s</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>GlobalSmoothingProvider</ns0:t>
+          <ns0:t>DynamicIntensityPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" s="4">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C19" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>HapticIntensityProvider</ns0:t>
+          <ns0:t>EasingCurveProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" s="4">
@@ -3996,44 +3775,44 @@
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
       <ns0:c r="A21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t>GlobalDelayIngProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B21" s="4">
-        <ns0:v>4</ns0:v>
+        <ns0:v>5</ns0:v>
       </ns0:c>
       <ns0:c r="C21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
       <ns0:c r="A22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t>HapticIntensityProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B22" s="4">
-        <ns0:v>3</ns0:v>
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="C22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>Off | Light | Medium | Strong</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="23">
       <ns0:c r="A23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B23" s="4">
@@ -4041,79 +3820,84 @@
       </ns0:c>
       <ns0:c r="C23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="24">
       <ns0:c r="A24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>MinEnemyGroupProvider</ns0:t>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B24" s="4">
-        <ns0:v>4</ns0:v>
+        <ns0:v>3</ns0:v>
       </ns0:c>
       <ns0:c r="C24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>MinTimeScaleProvider</ns0:t>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B25" s="4">
-        <ns0:v>6</ns0:v>
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="C25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off (0%) | 5% | 8% | 10% | 15% | 20%</ns0:t>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="26">
       <ns0:c r="A26" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>PresetProvider</ns0:t>
+          <ns0:t>MinEnemyGroupProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B26" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>4</ns0:v>
+      </ns0:c>
+      <ns0:c r="C26" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="27">
       <ns0:c r="A27" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>QuickTestTriggerProvider</ns0:t>
+          <ns0:t>MinTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B27" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>6</ns0:v>
+      </ns0:c>
+      <ns0:c r="C27" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | 5% | 8% | 10% | 15% | 20%</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="28">
       <ns0:c r="A28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>SmoothingSpeedProvider</ns0:t>
+          <ns0:t>PresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B28" s="4">
-        <ns0:v>4</ns0:v>
-      </ns0:c>
-      <ns0:c r="C28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Instant | Fast | Medium | Slow</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="29">
       <ns0:c r="A29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>SmoothnessPresetProvider</ns0:t>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B29" s="4">

</xml_diff>

<commit_message>
refactor: convert per-trigger Delay to float slider, remove dead code
- Convert per-trigger Delay from dropdown preset to 0-1s float slider
- Remove DynamicIntensity (unused deprecated feature)
- Remove GlobalDelayIng and related dead code
- Clean up deprecated comments
- Global Delay preset still applies to all triggers via conversion

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -1173,15 +1173,13 @@
           <ns0:t>OptionBasicDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C45" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D45" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
+      <ns0:c r="C45" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D45" s="4">
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="4">
         <ns0:is>
@@ -1345,15 +1343,13 @@
           <ns0:t>OptionCriticalDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C53" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D53" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
+      <ns0:c r="C53" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D53" s="4">
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="4">
         <ns0:is>
@@ -1517,15 +1513,13 @@
           <ns0:t>OptionDismemberDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C61" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D61" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
+      <ns0:c r="C61" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D61" s="4">
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F61" t="inlineStr" s="4">
         <ns0:is>
@@ -1689,15 +1683,13 @@
           <ns0:t>OptionDecapDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C69" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D69" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
+      <ns0:c r="C69" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D69" s="4">
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F69" t="inlineStr" s="4">
         <ns0:is>
@@ -1861,15 +1853,13 @@
           <ns0:t>OptionLastEnemyDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C77" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D77" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
+      <ns0:c r="C77" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D77" s="4">
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F77" t="inlineStr" s="4">
         <ns0:is>
@@ -2008,15 +1998,13 @@
           <ns0:t>OptionLastStandDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C84" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D84" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
+      <ns0:c r="C84" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D84" s="4">
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F84" t="inlineStr" s="4">
         <ns0:is>
@@ -2148,15 +2136,13 @@
           <ns0:t>OptionParryDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C91" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D91" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Default</ns0:t>
-        </ns0:is>
+      <ns0:c r="C91" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D91" s="4">
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F91" t="inlineStr" s="4">
         <ns0:is>
@@ -3657,16 +3643,11 @@
     <ns0:row r="11">
       <ns0:c r="A11" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CustomDelayIngProvider</ns0:t>
+          <ns0:t>CustomDelayProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B11" s="4">
-        <ns0:v>22</ns0:v>
-      </ns0:c>
-      <ns0:c r="C11" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1.6x | 1.8x | 2x | 2.4x | 2.7x | 3x | 3.2x | 3.6x | 4x | 4.5x | 5x | 6x | 7.5x | 8x | 9x | 10x | 12x | 12.5x | 15x | 16x | 20x | 25x</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="12">
@@ -3707,22 +3688,17 @@
     <ns0:row r="15">
       <ns0:c r="A15" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>DelayIngSpeedProvider</ns0:t>
+          <ns0:t>DelayPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B15" s="4">
-        <ns0:v>4</ns0:v>
-      </ns0:c>
-      <ns0:c r="C15" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Instant | Fast | Medium | Slow</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="16">
       <ns0:c r="A16" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>DelayPresetProvider</ns0:t>
+          <ns0:t>DurationPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B16" s="4">
@@ -3732,42 +3708,52 @@
     <ns0:row r="17">
       <ns0:c r="A17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>DurationPresetProvider</ns0:t>
+          <ns0:t>DurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B17" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C17" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0.5s | 1.0s | 1.5s | 2.0s | 2.5s | 3.0s | 4.0s | 5.0s | 8.0s</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="18">
       <ns0:c r="A18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>DurationProvider</ns0:t>
+          <ns0:t>EasingCurveProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" s="4">
-        <ns0:v>9</ns0:v>
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>0.5s | 1.0s | 1.5s | 2.0s | 2.5s | 3.0s | 4.0s | 5.0s | 8.0s</ns0:t>
+          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>DynamicIntensityPresetProvider</ns0:t>
+          <ns0:t>HapticIntensityProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>4</ns0:v>
+      </ns0:c>
+      <ns0:c r="C19" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>EasingCurveProvider</ns0:t>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" s="4">
@@ -3775,29 +3761,29 @@
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
       <ns0:c r="A21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>GlobalDelayIngProvider</ns0:t>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B21" s="4">
-        <ns0:v>5</ns0:v>
+        <ns0:v>3</ns0:v>
       </ns0:c>
       <ns0:c r="C21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Per Trigger | Instant | Fast | Medium | Slow</ns0:t>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
       <ns0:c r="A22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>HapticIntensityProvider</ns0:t>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B22" s="4">
@@ -3805,14 +3791,14 @@
       </ns0:c>
       <ns0:c r="C22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="23">
       <ns0:c r="A23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t>MinEnemyGroupProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B23" s="4">
@@ -3820,127 +3806,82 @@
       </ns0:c>
       <ns0:c r="C23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="24">
       <ns0:c r="A24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t>MinTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B24" s="4">
-        <ns0:v>3</ns0:v>
+        <ns0:v>6</ns0:v>
       </ns0:c>
       <ns0:c r="C24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>Off (0%) | 5% | 8% | 10% | 15% | 20%</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t>PresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B25" s="4">
-        <ns0:v>4</ns0:v>
-      </ns0:c>
-      <ns0:c r="C25" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="26">
       <ns0:c r="A26" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>MinEnemyGroupProvider</ns0:t>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B26" s="4">
-        <ns0:v>4</ns0:v>
-      </ns0:c>
-      <ns0:c r="C26" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="27">
       <ns0:c r="A27" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>MinTimeScaleProvider</ns0:t>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B27" s="4">
-        <ns0:v>6</ns0:v>
+        <ns0:v>5</ns0:v>
       </ns0:c>
       <ns0:c r="C27" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off (0%) | 5% | 8% | 10% | 15% | 20%</ns0:t>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="28">
       <ns0:c r="A28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>PresetProvider</ns0:t>
+          <ns0:t>TimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B28" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="C28" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="29">
       <ns0:c r="A29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>QuickTestTriggerProvider</ns0:t>
+          <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B29" s="4">
-        <ns0:v>0</ns0:v>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="30">
-      <ns0:c r="A30" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B30" s="4">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C30" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="31">
-      <ns0:c r="A31" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B31" s="4">
-        <ns0:v>8</ns0:v>
-      </ns0:c>
-      <ns0:c r="C31" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="32">
-      <ns0:c r="A32" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerProfileProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B32" s="4">
         <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
refactor: remove Optional category, use duration for easing
- Remove GlobalCooldown, HapticFeedback, MinTimeScale settings
- Move EasingCurve to Preset Selection category
- Change easing to use 15% of duration (min 0.1s) instead of delay
- Easing now cuts into duration time as expected

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -499,147 +499,178 @@
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="15"/>
-    <ns0:row r="16">
-      <ns0:c r="A16" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryOptionalOverrides</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+    <ns0:row r="15">
+      <ns0:c r="A15" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryPresetSelection</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B15" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionEasingCurve</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C15" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D15" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E15" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F15" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition curve shape. Smoothstep = smooth both ends, Linear = constant speed, EaseIn = slow start, EaseOut = slow end.</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="16"/>
     <ns0:row r="17">
-      <ns0:c r="A17" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryOptionalOverrides</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B17" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionGlobalCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C17" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D17" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E17" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s | 2s | 3s | 5s | 10s | 30s | 60s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F17" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Minimum time between any slow motion triggers</ns0:t>
+      <ns0:c r="A17" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="18">
       <ns0:c r="A18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryOptionalOverrides</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionHapticFeedback</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C18" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C18" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E18" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Controller vibration when slow motion triggers</ns0:t>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryOptionalOverrides</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionEasingCurve</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C19" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
+          <ns0:t>TriggerThrownImpactKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C19" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E19" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape. Smoothstep = smooth both ends, Linear = constant speed, EaseIn = slow start, EaseOut = slow end.</ns0:t>
+          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryOptionalOverrides</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionMinTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C20" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>TriggerCriticalKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C20" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E20" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | 5% | 8% | 10% | 15% | 20%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Floor for time scale to prevent extreme slow-mo stutter. 0% = no limit.</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="21"/>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="21">
+      <ns0:c r="A21" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B21" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C21" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D21" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F21" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger when severing limbs</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="22">
-      <ns0:c r="A22" t="inlineStr" s="2">
+      <ns0:c r="A22" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B22" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C22" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D22" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F22" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -651,7 +682,7 @@
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
+          <ns0:t>TriggerLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C23" t="inlineStr" s="6">
@@ -666,7 +697,7 @@
       </ns0:c>
       <ns0:c r="F23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -678,7 +709,7 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerThrownImpactKill</ns0:t>
+          <ns0:t>TriggerLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C24" t="inlineStr" s="6">
@@ -688,12 +719,12 @@
       </ns0:c>
       <ns0:c r="D24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -705,22 +736,27 @@
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerCriticalKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C25" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionLastStandThreshold</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C25" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>15%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E25" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -732,7 +768,7 @@
       </ns0:c>
       <ns0:c r="B26" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDismemberment</ns0:t>
+          <ns0:t>TriggerParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C26" t="inlineStr" s="6">
@@ -747,226 +783,185 @@
       </ns0:c>
       <ns0:c r="F26" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="27">
-      <ns0:c r="A27" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B27" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C27" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D27" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F27" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Trigger on successful weapon deflections</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="27"/>
     <ns0:row r="28">
-      <ns0:c r="A28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C28" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+      <ns0:c r="A28" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="29">
       <ns0:c r="A29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C29" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionCameraDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C29" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>3m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E29" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="30">
       <ns0:c r="A30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandThreshold</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C30" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionRandomizeDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C30" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E30" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
+          <ns0:t>Randomize distance per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="31">
       <ns0:c r="A31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C31" t="inlineStr" s="6">
+          <ns0:t>OptionCameraHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C31" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D31" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1.5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E31" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F31" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Height offset</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="32">
+      <ns0:c r="A32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionRandomizeHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C32" t="inlineStr" s="6">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D31" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F31" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Trigger on successful weapon deflections</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="32"/>
+      <ns0:c r="D32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Randomize height per killcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="33">
-      <ns0:c r="A33" t="inlineStr" s="2">
+      <ns0:c r="A33" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
-    </ns0:row>
-    <ns0:row r="34">
-      <ns0:c r="A34" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B34" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCameraDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C34" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D34" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>3m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E34" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F34" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+      <ns0:c r="B33" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionOrbitSpeed</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C33" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D33" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Slow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E33" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F33" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="34"/>
     <ns0:row r="35">
-      <ns0:c r="A35" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B35" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionRandomizeDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C35" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D35" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F35" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Randomize distance per killcam</ns0:t>
+      <ns0:c r="A35" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="36">
       <ns0:c r="A36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCameraHeight</ns0:t>
+          <ns0:t>OptionBasicChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="7">
@@ -974,58 +969,49 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D36" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1.5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E36" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
-        </ns0:is>
+      <ns0:c r="D36" s="4">
+        <ns0:v>0.25</ns0:v>
       </ns0:c>
       <ns0:c r="F36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="37">
       <ns0:c r="A37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C37" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D37" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionBasicTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C37" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D37" s="4">
+        <ns0:v>0.28</ns0:v>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize height per killcam</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="38">
       <ns0:c r="A38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionOrbitSpeed</ns0:t>
+          <ns0:t>OptionBasicDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C38" t="inlineStr" s="7">
@@ -1033,27 +1019,67 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D38" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Slow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E38" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
-        </ns0:is>
+      <ns0:c r="D38" s="4">
+        <ns0:v>2.5</ns0:v>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="39"/>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="39">
+      <ns0:c r="A39" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B39" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionBasicCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C39" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D39" s="4">
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E39" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F39" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="40">
-      <ns0:c r="A40" t="inlineStr" s="2">
+      <ns0:c r="A40" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionBasicDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C40" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D40" s="4">
+        <ns0:v>0.10</ns0:v>
+      </ns0:c>
+      <ns0:c r="F40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1065,7 +1091,7 @@
       </ns0:c>
       <ns0:c r="B41" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicChance</ns0:t>
+          <ns0:t>OptionBasicThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C41" t="inlineStr" s="7">
@@ -1073,74 +1099,39 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D41" s="4">
-        <ns0:v>0.25</ns0:v>
+      <ns0:c r="D41" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E41" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F41" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="42">
-      <ns0:c r="A42" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B42" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionBasicTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C42" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D42" s="4">
-        <ns0:v>0.28</ns0:v>
-      </ns0:c>
-      <ns0:c r="F42" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="42"/>
     <ns0:row r="43">
-      <ns0:c r="A43" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B43" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionBasicDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C43" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D43" s="4">
-        <ns0:v>2.5</ns0:v>
-      </ns0:c>
-      <ns0:c r="F43" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
+      <ns0:c r="A43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="44">
       <ns0:c r="A44" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicCooldown</ns0:t>
+          <ns0:t>OptionCriticalChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="7">
@@ -1149,28 +1140,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D44" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E44" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.75</ns0:v>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="45">
       <ns0:c r="A45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicDelayIn</ns0:t>
+          <ns0:t>OptionCriticalTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C45" t="inlineStr" s="7">
@@ -1179,23 +1165,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D45" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>0.25</ns0:v>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="46">
       <ns0:c r="A46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicThirdPerson</ns0:t>
+          <ns0:t>OptionCriticalDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C46" t="inlineStr" s="7">
@@ -1203,27 +1189,67 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D46" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E46" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D46" s="4">
+        <ns0:v>3.0</ns0:v>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="47"/>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="47">
+      <ns0:c r="A47" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B47" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCriticalCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C47" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D47" s="4">
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E47" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F47" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="48">
-      <ns0:c r="A48" t="inlineStr" s="2">
+      <ns0:c r="A48" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B48" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCriticalDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C48" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D48" s="4">
+        <ns0:v>0.10</ns0:v>
+      </ns0:c>
+      <ns0:c r="F48" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1235,7 +1261,7 @@
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalChance</ns0:t>
+          <ns0:t>OptionCriticalThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C49" t="inlineStr" s="7">
@@ -1243,74 +1269,39 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D49" s="4">
-        <ns0:v>0.75</ns0:v>
+      <ns0:c r="D49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F49" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="50">
-      <ns0:c r="A50" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B50" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCriticalTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C50" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D50" s="4">
-        <ns0:v>0.25</ns0:v>
-      </ns0:c>
-      <ns0:c r="F50" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="50"/>
     <ns0:row r="51">
-      <ns0:c r="A51" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B51" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCriticalDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C51" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D51" s="4">
-        <ns0:v>3.0</ns0:v>
-      </ns0:c>
-      <ns0:c r="F51" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
+      <ns0:c r="A51" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="52">
       <ns0:c r="A52" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B52" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalCooldown</ns0:t>
+          <ns0:t>OptionDismemberChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C52" t="inlineStr" s="7">
@@ -1319,28 +1310,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D52" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E52" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.3</ns0:v>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="53">
       <ns0:c r="A53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalDelayIn</ns0:t>
+          <ns0:t>OptionDismemberTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C53" t="inlineStr" s="7">
@@ -1349,23 +1335,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D53" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>0.3</ns0:v>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="54">
       <ns0:c r="A54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalThirdPerson</ns0:t>
+          <ns0:t>OptionDismemberDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C54" t="inlineStr" s="7">
@@ -1373,27 +1359,67 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D54" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E54" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D54" s="4">
+        <ns0:v>2.0</ns0:v>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="55"/>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="55">
+      <ns0:c r="A55" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B55" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDismemberCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C55" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D55" s="4">
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E55" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F55" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="56">
-      <ns0:c r="A56" t="inlineStr" s="2">
+      <ns0:c r="A56" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B56" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDismemberDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C56" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D56" s="4">
+        <ns0:v>0.10</ns0:v>
+      </ns0:c>
+      <ns0:c r="F56" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1405,7 +1431,7 @@
       </ns0:c>
       <ns0:c r="B57" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberChance</ns0:t>
+          <ns0:t>OptionDismemberThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C57" t="inlineStr" s="7">
@@ -1413,74 +1439,39 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D57" s="4">
-        <ns0:v>0.3</ns0:v>
+      <ns0:c r="D57" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E57" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F57" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="58">
-      <ns0:c r="A58" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B58" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDismemberTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C58" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D58" s="4">
-        <ns0:v>0.3</ns0:v>
-      </ns0:c>
-      <ns0:c r="F58" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="58"/>
     <ns0:row r="59">
-      <ns0:c r="A59" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B59" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDismemberDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C59" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D59" s="4">
-        <ns0:v>2.0</ns0:v>
-      </ns0:c>
-      <ns0:c r="F59" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
+      <ns0:c r="A59" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="60">
       <ns0:c r="A60" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B60" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberCooldown</ns0:t>
+          <ns0:t>OptionDecapChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C60" t="inlineStr" s="7">
@@ -1489,28 +1480,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D60" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E60" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.9</ns0:v>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="61">
       <ns0:c r="A61" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B61" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberDelayIn</ns0:t>
+          <ns0:t>OptionDecapTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C61" t="inlineStr" s="7">
@@ -1519,23 +1505,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D61" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>0.23</ns0:v>
       </ns0:c>
       <ns0:c r="F61" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="62">
       <ns0:c r="A62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberThirdPerson</ns0:t>
+          <ns0:t>OptionDecapDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C62" t="inlineStr" s="7">
@@ -1543,27 +1529,67 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D62" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E62" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D62" s="4">
+        <ns0:v>3.25</ns0:v>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="63"/>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="63">
+      <ns0:c r="A63" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B63" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDecapCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C63" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D63" s="4">
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E63" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F63" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="64">
-      <ns0:c r="A64" t="inlineStr" s="2">
+      <ns0:c r="A64" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B64" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDecapDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C64" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D64" s="4">
+        <ns0:v>0.10</ns0:v>
+      </ns0:c>
+      <ns0:c r="F64" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1575,7 +1601,7 @@
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapChance</ns0:t>
+          <ns0:t>OptionDecapThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="7">
@@ -1583,74 +1609,39 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D65" s="4">
-        <ns0:v>0.9</ns0:v>
+      <ns0:c r="D65" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E65" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F65" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="66">
-      <ns0:c r="A66" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B66" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDecapTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C66" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D66" s="4">
-        <ns0:v>0.23</ns0:v>
-      </ns0:c>
-      <ns0:c r="F66" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="66"/>
     <ns0:row r="67">
-      <ns0:c r="A67" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B67" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDecapDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C67" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D67" s="4">
-        <ns0:v>3.25</ns0:v>
-      </ns0:c>
-      <ns0:c r="F67" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
+      <ns0:c r="A67" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="68">
       <ns0:c r="A68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapCooldown</ns0:t>
+          <ns0:t>OptionLastEnemyChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C68" t="inlineStr" s="7">
@@ -1659,28 +1650,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D68" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E68" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>1.0</ns0:v>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="69">
       <ns0:c r="A69" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B69" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapDelayIn</ns0:t>
+          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C69" t="inlineStr" s="7">
@@ -1689,23 +1675,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D69" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>0.26</ns0:v>
       </ns0:c>
       <ns0:c r="F69" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="70">
       <ns0:c r="A70" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B70" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapThirdPerson</ns0:t>
+          <ns0:t>OptionLastEnemyDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C70" t="inlineStr" s="7">
@@ -1713,27 +1699,67 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D70" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E70" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D70" s="4">
+        <ns0:v>2.75</ns0:v>
       </ns0:c>
       <ns0:c r="F70" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="71"/>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="71">
+      <ns0:c r="A71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastEnemyCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C71" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D71" s="4">
+        <ns0:v>30</ns0:v>
+      </ns0:c>
+      <ns0:c r="E71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="72">
-      <ns0:c r="A72" t="inlineStr" s="2">
+      <ns0:c r="A72" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B72" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastEnemyDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C72" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D72" s="4">
+        <ns0:v>0.10</ns0:v>
+      </ns0:c>
+      <ns0:c r="F72" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1745,7 +1771,7 @@
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyChance</ns0:t>
+          <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C73" t="inlineStr" s="7">
@@ -1753,74 +1779,39 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D73" s="4">
-        <ns0:v>1.0</ns0:v>
+      <ns0:c r="D73" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E73" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F73" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="74">
-      <ns0:c r="A74" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B74" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C74" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D74" s="4">
-        <ns0:v>0.26</ns0:v>
-      </ns0:c>
-      <ns0:c r="F74" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="74"/>
     <ns0:row r="75">
-      <ns0:c r="A75" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B75" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastEnemyDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C75" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D75" s="4">
-        <ns0:v>2.75</ns0:v>
-      </ns0:c>
-      <ns0:c r="F75" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
+      <ns0:c r="A75" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="76">
       <ns0:c r="A76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyCooldown</ns0:t>
+          <ns0:t>OptionLastStandTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C76" t="inlineStr" s="7">
@@ -1829,28 +1820,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D76" s="4">
-        <ns0:v>30</ns0:v>
-      </ns0:c>
-      <ns0:c r="E76" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.30</ns0:v>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="77">
       <ns0:c r="A77" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B77" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyDelayIn</ns0:t>
+          <ns0:t>OptionLastStandDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C77" t="inlineStr" s="7">
@@ -1859,23 +1845,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D77" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>4.0</ns0:v>
       </ns0:c>
       <ns0:c r="F77" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="78">
       <ns0:c r="A78" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B78" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
+          <ns0:t>OptionLastStandCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C78" t="inlineStr" s="7">
@@ -1883,64 +1869,62 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D78" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D78" s="4">
+        <ns0:v>90</ns0:v>
       </ns0:c>
       <ns0:c r="E78" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F78" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="79"/>
-    <ns0:row r="80">
-      <ns0:c r="A80" t="inlineStr" s="2">
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="79">
+      <ns0:c r="A79" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
-    </ns0:row>
+      <ns0:c r="B79" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastStandDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C79" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D79" s="4">
+        <ns0:v>0.10</ns0:v>
+      </ns0:c>
+      <ns0:c r="F79" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition into slow motion</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="80"/>
     <ns0:row r="81">
-      <ns0:c r="A81" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B81" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastStandTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C81" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D81" s="4">
-        <ns0:v>0.30</ns0:v>
-      </ns0:c>
-      <ns0:c r="F81" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="A81" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="82">
       <ns0:c r="A82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandDuration</ns0:t>
+          <ns0:t>OptionParryChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="7">
@@ -1949,23 +1933,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D82" s="4">
-        <ns0:v>4.0</ns0:v>
+        <ns0:v>0.5</ns0:v>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="83">
       <ns0:c r="A83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandCooldown</ns0:t>
+          <ns0:t>OptionParryTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="7">
@@ -1974,28 +1958,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D83" s="4">
-        <ns0:v>90</ns0:v>
-      </ns0:c>
-      <ns0:c r="E83" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.34</ns0:v>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="84">
       <ns0:c r="A84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandDelayIn</ns0:t>
+          <ns0:t>OptionParryDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C84" t="inlineStr" s="7">
@@ -2004,149 +1983,155 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D84" s="4">
+        <ns0:v>1.5</ns0:v>
+      </ns0:c>
+      <ns0:c r="F84" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="85">
+      <ns0:c r="A85" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B85" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionParryCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C85" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D85" s="4">
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="E85" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F85" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="86">
+      <ns0:c r="A86" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B86" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionParryDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C86" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D86" s="4">
         <ns0:v>0.10</ns0:v>
       </ns0:c>
-      <ns0:c r="F84" t="inlineStr" s="4">
+      <ns0:c r="F86" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="85"/>
-    <ns0:row r="86">
-      <ns0:c r="A86" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="87">
-      <ns0:c r="A87" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B87" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionParryChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C87" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D87" s="4">
-        <ns0:v>0.5</ns0:v>
-      </ns0:c>
-      <ns0:c r="F87" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+    <ns0:row r="87"/>
     <ns0:row r="88">
-      <ns0:c r="A88" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B88" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionParryTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C88" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D88" s="4">
-        <ns0:v>0.34</ns0:v>
-      </ns0:c>
-      <ns0:c r="F88" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+      <ns0:c r="A88" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
       <ns0:c r="A89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C89" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D89" s="4">
-        <ns0:v>1.5</ns0:v>
+          <ns0:t>OptionDebugLogging</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C89" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D89" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="90">
       <ns0:c r="A90" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B90" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C90" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D90" s="4">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="E90" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>OptionQuickTestTrigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C90" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D90" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F90" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Which trigger to simulate</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="91">
       <ns0:c r="A91" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B91" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryDelayIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C91" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D91" s="4">
-        <ns0:v>0.10</ns0:v>
+          <ns0:t>OptionQuickTestNow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C91" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D91" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F91" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Toggle to fire the selected trigger once</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2154,19 +2139,19 @@
     <ns0:row r="93">
       <ns0:c r="A93" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
+          <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="94">
       <ns0:c r="A94" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
+          <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B94" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDebugLogging</ns0:t>
+          <ns0:t>OptionResetStats</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C94" t="inlineStr" s="6">
@@ -2180,95 +2165,6 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="F94" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Enable verbose debug logging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="95">
-      <ns0:c r="A95" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B95" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionQuickTestTrigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C95" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D95" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F95" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Which trigger to simulate</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="96">
-      <ns0:c r="A96" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B96" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionQuickTestNow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C96" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D96" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F96" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Toggle to fire the selected trigger once</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="97"/>
-    <ns0:row r="98">
-      <ns0:c r="A98" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryStatistics</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="99">
-      <ns0:c r="A99" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryStatistics</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B99" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionResetStats</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C99" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D99" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F99" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Toggle to reset all statistics</ns0:t>
         </ns0:is>
@@ -3738,7 +3634,7 @@
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>HapticIntensityProvider</ns0:t>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" s="4">
@@ -3746,44 +3642,44 @@
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Light | Medium | Strong</ns0:t>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" s="4">
-        <ns0:v>4</ns0:v>
+        <ns0:v>3</ns0:v>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
       <ns0:c r="A21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B21" s="4">
-        <ns0:v>3</ns0:v>
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="C21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
       <ns0:c r="A22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t>MinEnemyGroupProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B22" s="4">
@@ -3791,97 +3687,67 @@
       </ns0:c>
       <ns0:c r="C22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="23">
       <ns0:c r="A23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>MinEnemyGroupProvider</ns0:t>
+          <ns0:t>PresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B23" s="4">
-        <ns0:v>4</ns0:v>
-      </ns0:c>
-      <ns0:c r="C23" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="24">
       <ns0:c r="A24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>MinTimeScaleProvider</ns0:t>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B24" s="4">
-        <ns0:v>6</ns0:v>
-      </ns0:c>
-      <ns0:c r="C24" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | 5% | 8% | 10% | 15% | 20%</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>PresetProvider</ns0:t>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B25" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="C25" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="26">
       <ns0:c r="A26" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>QuickTestTriggerProvider</ns0:t>
+          <ns0:t>TimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B26" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="C26" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="27">
       <ns0:c r="A27" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B27" s="4">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C27" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="28">
-      <ns0:c r="A28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B28" s="4">
-        <ns0:v>8</ns0:v>
-      </ns0:c>
-      <ns0:c r="C28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="29">
-      <ns0:c r="A29" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerProfileProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B29" s="4">
         <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Add per-trigger easing options to each collapsible section
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -499,43 +499,38 @@
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="15">
-      <ns0:c r="A15" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryPresetSelection</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B15" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionEasingCurve</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C15" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D15" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E15" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F15" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition curve shape. Smoothstep = smooth both ends, Linear = constant speed, EaseIn = slow start, EaseOut = slow end.</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="16"/>
+    <ns0:row r="15"/>
+    <ns0:row r="16">
+      <ns0:c r="A16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="17">
-      <ns0:c r="A17" t="inlineStr" s="2">
+      <ns0:c r="A17" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B17" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C17" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D17" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F17" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -547,7 +542,7 @@
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
+          <ns0:t>TriggerThrownImpactKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="6">
@@ -557,12 +552,12 @@
       </ns0:c>
       <ns0:c r="D18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
+          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -574,7 +569,7 @@
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerThrownImpactKill</ns0:t>
+          <ns0:t>TriggerCriticalKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="6">
@@ -584,12 +579,12 @@
       </ns0:c>
       <ns0:c r="D19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -601,7 +596,7 @@
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerCriticalKill</ns0:t>
+          <ns0:t>TriggerDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="6">
@@ -616,7 +611,7 @@
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -628,7 +623,7 @@
       </ns0:c>
       <ns0:c r="B21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDismemberment</ns0:t>
+          <ns0:t>TriggerDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C21" t="inlineStr" s="6">
@@ -643,7 +638,7 @@
       </ns0:c>
       <ns0:c r="F21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -655,7 +650,7 @@
       </ns0:c>
       <ns0:c r="B22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDecapitation</ns0:t>
+          <ns0:t>TriggerLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C22" t="inlineStr" s="6">
@@ -670,7 +665,7 @@
       </ns0:c>
       <ns0:c r="F22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -682,7 +677,7 @@
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastEnemy</ns0:t>
+          <ns0:t>TriggerLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C23" t="inlineStr" s="6">
@@ -697,7 +692,7 @@
       </ns0:c>
       <ns0:c r="F23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -709,22 +704,27 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C24" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionLastStandThreshold</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C24" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>15%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E24" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -736,62 +736,62 @@
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandThreshold</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C25" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>TriggerParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C25" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E25" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="26">
-      <ns0:c r="A26" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B26" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C26" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D26" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F26" t="inlineStr" s="4">
-        <ns0:is>
           <ns0:t>Trigger on successful weapon deflections</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="27"/>
+    <ns0:row r="26"/>
+    <ns0:row r="27">
+      <ns0:c r="A27" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="28">
-      <ns0:c r="A28" t="inlineStr" s="2">
+      <ns0:c r="A28" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B28" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCameraDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C28" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D28" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>3m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E28" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F28" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -803,27 +803,22 @@
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCameraDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C29" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionRandomizeDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C29" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>3m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E29" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
+          <ns0:t>Randomize distance per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -835,22 +830,27 @@
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C30" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionCameraHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C30" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>1.5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E30" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize distance per killcam</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -862,27 +862,22 @@
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCameraHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C31" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionRandomizeHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C31" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E31" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Randomize height per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -894,62 +889,60 @@
       </ns0:c>
       <ns0:c r="B32" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C32" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionOrbitSpeed</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C32" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D32" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>Slow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F32" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize height per killcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="33">
-      <ns0:c r="A33" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B33" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionOrbitSpeed</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C33" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D33" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Slow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E33" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F33" t="inlineStr" s="4">
-        <ns0:is>
           <ns0:t>Camera rotation speed (0 for static)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="34"/>
+    <ns0:row r="33"/>
+    <ns0:row r="34">
+      <ns0:c r="A34" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="35">
-      <ns0:c r="A35" t="inlineStr" s="2">
+      <ns0:c r="A35" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B35" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionBasicChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C35" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D35" s="4">
+        <ns0:v>0.25</ns0:v>
+      </ns0:c>
+      <ns0:c r="F35" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -961,7 +954,7 @@
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicChance</ns0:t>
+          <ns0:t>OptionBasicTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="7">
@@ -970,11 +963,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D36" s="4">
-        <ns0:v>0.25</ns0:v>
+        <ns0:v>0.28</ns0:v>
       </ns0:c>
       <ns0:c r="F36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -986,7 +979,7 @@
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicTimeScale</ns0:t>
+          <ns0:t>OptionBasicDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C37" t="inlineStr" s="7">
@@ -995,11 +988,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D37" s="4">
-        <ns0:v>0.28</ns0:v>
+        <ns0:v>2.5</ns0:v>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1011,7 +1004,7 @@
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicDuration</ns0:t>
+          <ns0:t>OptionBasicCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C38" t="inlineStr" s="7">
@@ -1020,11 +1013,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D38" s="4">
-        <ns0:v>2.5</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E38" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1036,7 +1034,7 @@
       </ns0:c>
       <ns0:c r="B39" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicCooldown</ns0:t>
+          <ns0:t>OptionBasicDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C39" t="inlineStr" s="7">
@@ -1045,16 +1043,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D39" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E39" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F39" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1066,20 +1059,27 @@
       </ns0:c>
       <ns0:c r="B40" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicDelayIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C40" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D40" s="4">
-        <ns0:v>0.10</ns0:v>
+          <ns0:t>OptionBasicEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C40" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F40" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Transition curve shape</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1261,60 +1261,67 @@
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionCriticalEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C49" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition curve shape</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="50">
+      <ns0:c r="A50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B50" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionCriticalThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C49" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D49" t="inlineStr" s="4">
+      <ns0:c r="C50" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D50" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E49" t="inlineStr" s="4">
+      <ns0:c r="E50" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F49" t="inlineStr" s="4">
+      <ns0:c r="F50" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="50"/>
-    <ns0:row r="51">
-      <ns0:c r="A51" t="inlineStr" s="2">
+    <ns0:row r="51"/>
+    <ns0:row r="52">
+      <ns0:c r="A52" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="52">
-      <ns0:c r="A52" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B52" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDismemberChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C52" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D52" s="4">
-        <ns0:v>0.3</ns0:v>
-      </ns0:c>
-      <ns0:c r="F52" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1326,7 +1333,7 @@
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberTimeScale</ns0:t>
+          <ns0:t>OptionDismemberChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C53" t="inlineStr" s="7">
@@ -1339,7 +1346,7 @@
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1351,7 +1358,7 @@
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberDuration</ns0:t>
+          <ns0:t>OptionDismemberTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C54" t="inlineStr" s="7">
@@ -1360,11 +1367,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D54" s="4">
-        <ns0:v>2.0</ns0:v>
+        <ns0:v>0.3</ns0:v>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1376,7 +1383,7 @@
       </ns0:c>
       <ns0:c r="B55" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberCooldown</ns0:t>
+          <ns0:t>OptionDismemberDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C55" t="inlineStr" s="7">
@@ -1385,16 +1392,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D55" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E55" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>2.0</ns0:v>
       </ns0:c>
       <ns0:c r="F55" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1406,7 +1408,7 @@
       </ns0:c>
       <ns0:c r="B56" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberDelayIn</ns0:t>
+          <ns0:t>OptionDismemberCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C56" t="inlineStr" s="7">
@@ -1415,11 +1417,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D56" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E56" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F56" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1431,85 +1438,92 @@
       </ns0:c>
       <ns0:c r="B57" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionDismemberDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C57" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D57" s="4">
+        <ns0:v>0.10</ns0:v>
+      </ns0:c>
+      <ns0:c r="F57" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition into slow motion</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="58">
+      <ns0:c r="A58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDismemberEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C58" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition curve shape</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="59">
+      <ns0:c r="A59" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B59" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionDismemberThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C57" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D57" t="inlineStr" s="4">
+      <ns0:c r="C59" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D59" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E57" t="inlineStr" s="4">
+      <ns0:c r="E59" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F57" t="inlineStr" s="4">
+      <ns0:c r="F59" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="58"/>
-    <ns0:row r="59">
-      <ns0:c r="A59" t="inlineStr" s="2">
+    <ns0:row r="60"/>
+    <ns0:row r="61">
+      <ns0:c r="A61" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="60">
-      <ns0:c r="A60" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B60" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDecapChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C60" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D60" s="4">
-        <ns0:v>0.9</ns0:v>
-      </ns0:c>
-      <ns0:c r="F60" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="61">
-      <ns0:c r="A61" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B61" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDecapTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C61" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D61" s="4">
-        <ns0:v>0.23</ns0:v>
-      </ns0:c>
-      <ns0:c r="F61" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1521,7 +1535,7 @@
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapDuration</ns0:t>
+          <ns0:t>OptionDecapChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C62" t="inlineStr" s="7">
@@ -1530,11 +1544,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D62" s="4">
-        <ns0:v>3.25</ns0:v>
+        <ns0:v>0.9</ns0:v>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1546,7 +1560,7 @@
       </ns0:c>
       <ns0:c r="B63" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapCooldown</ns0:t>
+          <ns0:t>OptionDecapTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C63" t="inlineStr" s="7">
@@ -1555,16 +1569,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D63" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E63" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.23</ns0:v>
       </ns0:c>
       <ns0:c r="F63" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1576,7 +1585,7 @@
       </ns0:c>
       <ns0:c r="B64" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapDelayIn</ns0:t>
+          <ns0:t>OptionDecapDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C64" t="inlineStr" s="7">
@@ -1585,11 +1594,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D64" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>3.25</ns0:v>
       </ns0:c>
       <ns0:c r="F64" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1601,7 +1610,7 @@
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapThirdPerson</ns0:t>
+          <ns0:t>OptionDecapCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="7">
@@ -1609,102 +1618,114 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D65" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D65" s="4">
+        <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="E65" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F65" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="66"/>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="66">
+      <ns0:c r="A66" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B66" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDecapDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C66" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D66" s="4">
+        <ns0:v>0.10</ns0:v>
+      </ns0:c>
+      <ns0:c r="F66" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition into slow motion</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="67">
-      <ns0:c r="A67" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+      <ns0:c r="A67" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B67" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDecapEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C67" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D67" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E67" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F67" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition curve shape</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="68">
       <ns0:c r="A68" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDecapThirdPerson</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C68" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="69"/>
+    <ns0:row r="70">
+      <ns0:c r="A70" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B68" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastEnemyChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C68" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D68" s="4">
-        <ns0:v>1.0</ns0:v>
-      </ns0:c>
-      <ns0:c r="F68" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="69">
-      <ns0:c r="A69" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B69" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C69" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D69" s="4">
-        <ns0:v>0.26</ns0:v>
-      </ns0:c>
-      <ns0:c r="F69" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="70">
-      <ns0:c r="A70" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B70" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastEnemyDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C70" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D70" s="4">
-        <ns0:v>2.75</ns0:v>
-      </ns0:c>
-      <ns0:c r="F70" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1716,7 +1737,7 @@
       </ns0:c>
       <ns0:c r="B71" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyCooldown</ns0:t>
+          <ns0:t>OptionLastEnemyChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C71" t="inlineStr" s="7">
@@ -1725,16 +1746,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D71" s="4">
-        <ns0:v>30</ns0:v>
-      </ns0:c>
-      <ns0:c r="E71" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>1.0</ns0:v>
       </ns0:c>
       <ns0:c r="F71" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1746,7 +1762,7 @@
       </ns0:c>
       <ns0:c r="B72" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyDelayIn</ns0:t>
+          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C72" t="inlineStr" s="7">
@@ -1755,11 +1771,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D72" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>0.26</ns0:v>
       </ns0:c>
       <ns0:c r="F72" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1771,7 +1787,7 @@
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
+          <ns0:t>OptionLastEnemyDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C73" t="inlineStr" s="7">
@@ -1779,152 +1795,201 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D73" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E73" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D73" s="4">
+        <ns0:v>2.75</ns0:v>
       </ns0:c>
       <ns0:c r="F73" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="74"/>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="74">
+      <ns0:c r="A74" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B74" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastEnemyCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C74" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D74" s="4">
+        <ns0:v>30</ns0:v>
+      </ns0:c>
+      <ns0:c r="E74" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F74" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="75">
-      <ns0:c r="A75" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+      <ns0:c r="A75" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B75" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastEnemyDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C75" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D75" s="4">
+        <ns0:v>0.10</ns0:v>
+      </ns0:c>
+      <ns0:c r="F75" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="76">
       <ns0:c r="A76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C76" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D76" s="4">
-        <ns0:v>0.30</ns0:v>
+          <ns0:t>OptionLastEnemyEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C76" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D76" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E76" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Transition curve shape</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="77">
       <ns0:c r="A77" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B77" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C77" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D77" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E77" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F77" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="78"/>
+    <ns0:row r="79">
+      <ns0:c r="A79" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B77" t="inlineStr" s="4">
+    </ns0:row>
+    <ns0:row r="80">
+      <ns0:c r="A80" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B80" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastStandTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C80" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D80" s="4">
+        <ns0:v>0.30</ns0:v>
+      </ns0:c>
+      <ns0:c r="F80" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="81">
+      <ns0:c r="A81" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B81" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>OptionLastStandDuration</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C77" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D77" s="4">
+      <ns0:c r="C81" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D81" s="4">
         <ns0:v>4.0</ns0:v>
       </ns0:c>
-      <ns0:c r="F77" t="inlineStr" s="4">
+      <ns0:c r="F81" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="78">
-      <ns0:c r="A78" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B78" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastStandCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C78" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D78" s="4">
-        <ns0:v>90</ns0:v>
-      </ns0:c>
-      <ns0:c r="E78" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F78" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="79">
-      <ns0:c r="A79" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B79" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastStandDelayIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C79" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D79" s="4">
-        <ns0:v>0.10</ns0:v>
-      </ns0:c>
-      <ns0:c r="F79" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="80"/>
-    <ns0:row r="81">
-      <ns0:c r="A81" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="82">
       <ns0:c r="A82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryChance</ns0:t>
+          <ns0:t>OptionLastStandCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="7">
@@ -1933,23 +1998,28 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D82" s="4">
-        <ns0:v>0.5</ns0:v>
+        <ns0:v>90</ns0:v>
+      </ns0:c>
+      <ns0:c r="E82" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="83">
       <ns0:c r="A83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryTimeScale</ns0:t>
+          <ns0:t>OptionLastStandDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="7">
@@ -1958,213 +2028,335 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D83" s="4">
-        <ns0:v>0.34</ns0:v>
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="84">
       <ns0:c r="A84" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B84" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastStandEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C84" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D84" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E84" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F84" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition curve shape</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="85"/>
+    <ns0:row r="86">
+      <ns0:c r="A86" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B84" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionParryDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C84" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D84" s="4">
-        <ns0:v>1.5</ns0:v>
-      </ns0:c>
-      <ns0:c r="F84" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="85">
-      <ns0:c r="A85" t="inlineStr" s="4">
+    </ns0:row>
+    <ns0:row r="87">
+      <ns0:c r="A87" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B85" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionParryCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C85" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D85" s="4">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="E85" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F85" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="86">
-      <ns0:c r="A86" t="inlineStr" s="4">
+      <ns0:c r="B87" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionParryChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C87" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D87" s="4">
+        <ns0:v>0.5</ns0:v>
+      </ns0:c>
+      <ns0:c r="F87" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="88">
+      <ns0:c r="A88" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B86" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionParryDelayIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C86" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D86" s="4">
-        <ns0:v>0.10</ns0:v>
-      </ns0:c>
-      <ns0:c r="F86" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="87"/>
-    <ns0:row r="88">
-      <ns0:c r="A88" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
+      <ns0:c r="B88" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionParryTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C88" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D88" s="4">
+        <ns0:v>0.34</ns0:v>
+      </ns0:c>
+      <ns0:c r="F88" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
       <ns0:c r="A89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDebugLogging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C89" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D89" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionParryDuration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C89" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D89" s="4">
+        <ns0:v>1.5</ns0:v>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Enable verbose debug logging</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="90">
       <ns0:c r="A90" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B90" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionQuickTestTrigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C90" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D90" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
+          <ns0:t>OptionParryCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C90" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D90" s="4">
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="E90" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F90" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Which trigger to simulate</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="91">
       <ns0:c r="A91" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B91" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionParryDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C91" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D91" s="4">
+        <ns0:v>0.10</ns0:v>
+      </ns0:c>
+      <ns0:c r="F91" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition into slow motion</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="92">
+      <ns0:c r="A92" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B92" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionParryEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C92" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D92" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E92" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F92" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition curve shape</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="93"/>
+    <ns0:row r="94">
+      <ns0:c r="A94" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B91" t="inlineStr" s="4">
+    </ns0:row>
+    <ns0:row r="95">
+      <ns0:c r="A95" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B95" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDebugLogging</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C95" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D95" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F95" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Enable verbose debug logging</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="96">
+      <ns0:c r="A96" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B96" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionQuickTestTrigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C96" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D96" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F96" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Which trigger to simulate</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="97">
+      <ns0:c r="A97" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B97" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>OptionQuickTestNow</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C91" t="inlineStr" s="6">
+      <ns0:c r="C97" t="inlineStr" s="6">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D91" t="inlineStr" s="4">
+      <ns0:c r="D97" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F91" t="inlineStr" s="4">
+      <ns0:c r="F97" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Toggle to fire the selected trigger once</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="92"/>
-    <ns0:row r="93">
-      <ns0:c r="A93" t="inlineStr" s="2">
+    <ns0:row r="98"/>
+    <ns0:row r="99">
+      <ns0:c r="A99" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="94">
-      <ns0:c r="A94" t="inlineStr" s="4">
+    <ns0:row r="100">
+      <ns0:c r="A100" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B94" t="inlineStr" s="4">
+      <ns0:c r="B100" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>OptionResetStats</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C94" t="inlineStr" s="6">
+      <ns0:c r="C100" t="inlineStr" s="6">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D94" t="inlineStr" s="4">
+      <ns0:c r="D100" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F94" t="inlineStr" s="4">
+      <ns0:c r="F100" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Toggle to reset all statistics</ns0:t>
         </ns0:is>

</xml_diff>

<commit_message>
Easing improvements: add Off mode (default), easing out support, configurable percentage (0-50%)
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -480,57 +480,62 @@
       </ns0:c>
       <ns0:c r="B14" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionEasingPercent</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C14" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D14" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>25%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E14" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0% | 5% | 10% | 15% | 20% | 25% | 30% | 35% | 40% | 45% | 50%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F14" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Percentage of duration used for easing in/out transitions (0% = instant, 50% = half duration is transition)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="15">
+      <ns0:c r="A15" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryPresetSelection</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B15" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionTriggerProfile</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C14" t="inlineStr" s="8">
+      <ns0:c r="C15" t="inlineStr" s="8">
         <ns0:is>
           <ns0:t>Dropdown</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D14" t="inlineStr" s="4">
+      <ns0:c r="D15" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>All</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F14" t="inlineStr" s="4">
+      <ns0:c r="F15" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="15"/>
-    <ns0:row r="16">
-      <ns0:c r="A16" t="inlineStr" s="2">
+    <ns0:row r="16"/>
+    <ns0:row r="17">
+      <ns0:c r="A17" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="17">
-      <ns0:c r="A17" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B17" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C17" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D17" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F17" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -542,7 +547,7 @@
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerThrownImpactKill</ns0:t>
+          <ns0:t>TriggerBasicKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="6">
@@ -552,12 +557,12 @@
       </ns0:c>
       <ns0:c r="D18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -569,7 +574,7 @@
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerCriticalKill</ns0:t>
+          <ns0:t>TriggerThrownImpactKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="6">
@@ -579,12 +584,12 @@
       </ns0:c>
       <ns0:c r="D19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -596,7 +601,7 @@
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDismemberment</ns0:t>
+          <ns0:t>TriggerCriticalKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="6">
@@ -611,7 +616,7 @@
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -623,7 +628,7 @@
       </ns0:c>
       <ns0:c r="B21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDecapitation</ns0:t>
+          <ns0:t>TriggerDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C21" t="inlineStr" s="6">
@@ -638,7 +643,7 @@
       </ns0:c>
       <ns0:c r="F21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -650,7 +655,7 @@
       </ns0:c>
       <ns0:c r="B22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastEnemy</ns0:t>
+          <ns0:t>TriggerDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C22" t="inlineStr" s="6">
@@ -665,7 +670,7 @@
       </ns0:c>
       <ns0:c r="F22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -677,7 +682,7 @@
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastStand</ns0:t>
+          <ns0:t>TriggerLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C23" t="inlineStr" s="6">
@@ -692,7 +697,7 @@
       </ns0:c>
       <ns0:c r="F23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -704,27 +709,22 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandThreshold</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C24" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>TriggerLastStand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C24" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E24" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -736,62 +736,62 @@
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionLastStandThreshold</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C25" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D25" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>15%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E25" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F25" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="26">
+      <ns0:c r="A26" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B26" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>TriggerParry</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C25" t="inlineStr" s="6">
+      <ns0:c r="C26" t="inlineStr" s="6">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D25" t="inlineStr" s="4">
+      <ns0:c r="D26" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F25" t="inlineStr" s="4">
+      <ns0:c r="F26" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Trigger on successful weapon deflections</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="26"/>
-    <ns0:row r="27">
-      <ns0:c r="A27" t="inlineStr" s="2">
+    <ns0:row r="27"/>
+    <ns0:row r="28">
+      <ns0:c r="A28" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="28">
-      <ns0:c r="A28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCameraDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C28" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>3m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -803,22 +803,27 @@
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C29" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionCameraDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C29" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>3m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E29" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize distance per killcam</ns0:t>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -830,27 +835,22 @@
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCameraHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C30" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionRandomizeDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C30" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E30" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Randomize distance per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -862,22 +862,27 @@
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C31" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionCameraHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C31" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>1.5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E31" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize height per killcam</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -889,60 +894,62 @@
       </ns0:c>
       <ns0:c r="B32" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionRandomizeHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C32" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Randomize height per killcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="33">
+      <ns0:c r="A33" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B33" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionOrbitSpeed</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C32" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D32" t="inlineStr" s="4">
+      <ns0:c r="C33" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D33" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Slow</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E32" t="inlineStr" s="4">
+      <ns0:c r="E33" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F32" t="inlineStr" s="4">
+      <ns0:c r="F33" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Camera rotation speed (0 for static)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="33"/>
-    <ns0:row r="34">
-      <ns0:c r="A34" t="inlineStr" s="2">
+    <ns0:row r="34"/>
+    <ns0:row r="35">
+      <ns0:c r="A35" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="35">
-      <ns0:c r="A35" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B35" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionBasicChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C35" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D35" s="4">
-        <ns0:v>0.25</ns0:v>
-      </ns0:c>
-      <ns0:c r="F35" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -954,7 +961,7 @@
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicTimeScale</ns0:t>
+          <ns0:t>OptionBasicChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="7">
@@ -963,11 +970,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D36" s="4">
-        <ns0:v>0.28</ns0:v>
+        <ns0:v>0.25</ns0:v>
       </ns0:c>
       <ns0:c r="F36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -979,7 +986,7 @@
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicDuration</ns0:t>
+          <ns0:t>OptionBasicTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C37" t="inlineStr" s="7">
@@ -988,11 +995,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D37" s="4">
-        <ns0:v>2.5</ns0:v>
+        <ns0:v>0.28</ns0:v>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1004,7 +1011,7 @@
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicCooldown</ns0:t>
+          <ns0:t>OptionBasicDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C38" t="inlineStr" s="7">
@@ -1013,16 +1020,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D38" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E38" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>2.5</ns0:v>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1034,7 +1036,7 @@
       </ns0:c>
       <ns0:c r="B39" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicDelayIn</ns0:t>
+          <ns0:t>OptionBasicCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C39" t="inlineStr" s="7">
@@ -1043,11 +1045,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D39" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E39" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F39" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1059,27 +1066,20 @@
       </ns0:c>
       <ns0:c r="B40" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicEasing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C40" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D40" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E40" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionBasicDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C40" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D40" s="4">
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F40" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1091,60 +1091,67 @@
       </ns0:c>
       <ns0:c r="B41" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionBasicEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C41" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D41" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E41" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F41" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition curve shape</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="42">
+      <ns0:c r="A42" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B42" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionBasicThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C41" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D41" t="inlineStr" s="4">
+      <ns0:c r="C42" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D42" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E41" t="inlineStr" s="4">
+      <ns0:c r="E42" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F41" t="inlineStr" s="4">
+      <ns0:c r="F42" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="42"/>
-    <ns0:row r="43">
-      <ns0:c r="A43" t="inlineStr" s="2">
+    <ns0:row r="43"/>
+    <ns0:row r="44">
+      <ns0:c r="A44" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="44">
-      <ns0:c r="A44" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B44" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCriticalChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C44" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D44" s="4">
-        <ns0:v>0.75</ns0:v>
-      </ns0:c>
-      <ns0:c r="F44" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1156,7 +1163,7 @@
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalTimeScale</ns0:t>
+          <ns0:t>OptionCriticalChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C45" t="inlineStr" s="7">
@@ -1165,11 +1172,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D45" s="4">
-        <ns0:v>0.25</ns0:v>
+        <ns0:v>0.75</ns0:v>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1181,7 +1188,7 @@
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalDuration</ns0:t>
+          <ns0:t>OptionCriticalTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C46" t="inlineStr" s="7">
@@ -1190,11 +1197,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D46" s="4">
-        <ns0:v>3.0</ns0:v>
+        <ns0:v>0.25</ns0:v>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1206,7 +1213,7 @@
       </ns0:c>
       <ns0:c r="B47" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalCooldown</ns0:t>
+          <ns0:t>OptionCriticalDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C47" t="inlineStr" s="7">
@@ -1215,16 +1222,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D47" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E47" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>3.0</ns0:v>
       </ns0:c>
       <ns0:c r="F47" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1236,7 +1238,7 @@
       </ns0:c>
       <ns0:c r="B48" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalDelayIn</ns0:t>
+          <ns0:t>OptionCriticalCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C48" t="inlineStr" s="7">
@@ -1245,11 +1247,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D48" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E48" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F48" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1261,27 +1268,20 @@
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalEasing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C49" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D49" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E49" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionCriticalDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C49" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D49" s="4">
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F49" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1293,60 +1293,67 @@
       </ns0:c>
       <ns0:c r="B50" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionCriticalEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C50" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition curve shape</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="51">
+      <ns0:c r="A51" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B51" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionCriticalThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C50" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D50" t="inlineStr" s="4">
+      <ns0:c r="C51" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D51" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E50" t="inlineStr" s="4">
+      <ns0:c r="E51" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F50" t="inlineStr" s="4">
+      <ns0:c r="F51" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="51"/>
-    <ns0:row r="52">
-      <ns0:c r="A52" t="inlineStr" s="2">
+    <ns0:row r="52"/>
+    <ns0:row r="53">
+      <ns0:c r="A53" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="53">
-      <ns0:c r="A53" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B53" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDismemberChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C53" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D53" s="4">
-        <ns0:v>0.3</ns0:v>
-      </ns0:c>
-      <ns0:c r="F53" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1358,7 +1365,7 @@
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberTimeScale</ns0:t>
+          <ns0:t>OptionDismemberChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C54" t="inlineStr" s="7">
@@ -1371,7 +1378,7 @@
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1383,7 +1390,7 @@
       </ns0:c>
       <ns0:c r="B55" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberDuration</ns0:t>
+          <ns0:t>OptionDismemberTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C55" t="inlineStr" s="7">
@@ -1392,11 +1399,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D55" s="4">
-        <ns0:v>2.0</ns0:v>
+        <ns0:v>0.3</ns0:v>
       </ns0:c>
       <ns0:c r="F55" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1408,7 +1415,7 @@
       </ns0:c>
       <ns0:c r="B56" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberCooldown</ns0:t>
+          <ns0:t>OptionDismemberDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C56" t="inlineStr" s="7">
@@ -1417,16 +1424,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D56" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E56" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>2.0</ns0:v>
       </ns0:c>
       <ns0:c r="F56" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1438,7 +1440,7 @@
       </ns0:c>
       <ns0:c r="B57" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberDelayIn</ns0:t>
+          <ns0:t>OptionDismemberCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C57" t="inlineStr" s="7">
@@ -1447,11 +1449,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D57" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E57" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F57" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1463,27 +1470,20 @@
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberEasing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C58" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D58" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E58" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionDismemberDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C58" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D58" s="4">
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1495,60 +1495,67 @@
       </ns0:c>
       <ns0:c r="B59" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionDismemberEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C59" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D59" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E59" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F59" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition curve shape</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="60">
+      <ns0:c r="A60" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B60" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionDismemberThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C59" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D59" t="inlineStr" s="4">
+      <ns0:c r="C60" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D60" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E59" t="inlineStr" s="4">
+      <ns0:c r="E60" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F59" t="inlineStr" s="4">
+      <ns0:c r="F60" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="60"/>
-    <ns0:row r="61">
-      <ns0:c r="A61" t="inlineStr" s="2">
+    <ns0:row r="61"/>
+    <ns0:row r="62">
+      <ns0:c r="A62" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="62">
-      <ns0:c r="A62" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B62" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDecapChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C62" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D62" s="4">
-        <ns0:v>0.9</ns0:v>
-      </ns0:c>
-      <ns0:c r="F62" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1560,7 +1567,7 @@
       </ns0:c>
       <ns0:c r="B63" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapTimeScale</ns0:t>
+          <ns0:t>OptionDecapChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C63" t="inlineStr" s="7">
@@ -1569,11 +1576,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D63" s="4">
-        <ns0:v>0.23</ns0:v>
+        <ns0:v>0.9</ns0:v>
       </ns0:c>
       <ns0:c r="F63" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1585,7 +1592,7 @@
       </ns0:c>
       <ns0:c r="B64" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapDuration</ns0:t>
+          <ns0:t>OptionDecapTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C64" t="inlineStr" s="7">
@@ -1594,11 +1601,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D64" s="4">
-        <ns0:v>3.25</ns0:v>
+        <ns0:v>0.23</ns0:v>
       </ns0:c>
       <ns0:c r="F64" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1610,7 +1617,7 @@
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapCooldown</ns0:t>
+          <ns0:t>OptionDecapDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="7">
@@ -1619,16 +1626,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D65" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E65" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>3.25</ns0:v>
       </ns0:c>
       <ns0:c r="F65" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1640,7 +1642,7 @@
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapDelayIn</ns0:t>
+          <ns0:t>OptionDecapCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="7">
@@ -1649,11 +1651,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D66" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E66" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1665,27 +1672,20 @@
       </ns0:c>
       <ns0:c r="B67" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapEasing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C67" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D67" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E67" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionDecapDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C67" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D67" s="4">
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F67" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1697,60 +1697,67 @@
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionDecapEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C68" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F68" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition curve shape</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="69">
+      <ns0:c r="A69" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B69" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionDecapThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C68" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D68" t="inlineStr" s="4">
+      <ns0:c r="C69" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D69" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E68" t="inlineStr" s="4">
+      <ns0:c r="E69" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F68" t="inlineStr" s="4">
+      <ns0:c r="F69" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="69"/>
-    <ns0:row r="70">
-      <ns0:c r="A70" t="inlineStr" s="2">
+    <ns0:row r="70"/>
+    <ns0:row r="71">
+      <ns0:c r="A71" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="71">
-      <ns0:c r="A71" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B71" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastEnemyChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C71" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D71" s="4">
-        <ns0:v>1.0</ns0:v>
-      </ns0:c>
-      <ns0:c r="F71" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1762,7 +1769,7 @@
       </ns0:c>
       <ns0:c r="B72" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
+          <ns0:t>OptionLastEnemyChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C72" t="inlineStr" s="7">
@@ -1771,11 +1778,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D72" s="4">
-        <ns0:v>0.26</ns0:v>
+        <ns0:v>1.0</ns0:v>
       </ns0:c>
       <ns0:c r="F72" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1787,7 +1794,7 @@
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyDuration</ns0:t>
+          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C73" t="inlineStr" s="7">
@@ -1796,11 +1803,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D73" s="4">
-        <ns0:v>2.75</ns0:v>
+        <ns0:v>0.26</ns0:v>
       </ns0:c>
       <ns0:c r="F73" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1812,7 +1819,7 @@
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyCooldown</ns0:t>
+          <ns0:t>OptionLastEnemyDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C74" t="inlineStr" s="7">
@@ -1821,16 +1828,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D74" s="4">
-        <ns0:v>30</ns0:v>
-      </ns0:c>
-      <ns0:c r="E74" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>2.75</ns0:v>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1842,7 +1844,7 @@
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyDelayIn</ns0:t>
+          <ns0:t>OptionLastEnemyCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="7">
@@ -1851,11 +1853,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D75" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>30</ns0:v>
+      </ns0:c>
+      <ns0:c r="E75" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1867,27 +1874,20 @@
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyEasing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C76" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D76" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E76" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionLastEnemyDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C76" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D76" s="4">
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1899,60 +1899,67 @@
       </ns0:c>
       <ns0:c r="B77" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionLastEnemyEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C77" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D77" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E77" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F77" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition curve shape</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="78">
+      <ns0:c r="A78" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B78" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C77" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D77" t="inlineStr" s="4">
+      <ns0:c r="C78" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D78" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E77" t="inlineStr" s="4">
+      <ns0:c r="E78" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F77" t="inlineStr" s="4">
+      <ns0:c r="F78" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="78"/>
-    <ns0:row r="79">
-      <ns0:c r="A79" t="inlineStr" s="2">
+    <ns0:row r="79"/>
+    <ns0:row r="80">
+      <ns0:c r="A80" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="80">
-      <ns0:c r="A80" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B80" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastStandTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C80" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D80" s="4">
-        <ns0:v>0.30</ns0:v>
-      </ns0:c>
-      <ns0:c r="F80" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1964,7 +1971,7 @@
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandDuration</ns0:t>
+          <ns0:t>OptionLastStandTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="7">
@@ -1973,11 +1980,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D81" s="4">
-        <ns0:v>4.0</ns0:v>
+        <ns0:v>0.30</ns0:v>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1989,7 +1996,7 @@
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandCooldown</ns0:t>
+          <ns0:t>OptionLastStandDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="7">
@@ -1998,16 +2005,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D82" s="4">
-        <ns0:v>90</ns0:v>
-      </ns0:c>
-      <ns0:c r="E82" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>4.0</ns0:v>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2019,7 +2021,7 @@
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandDelayIn</ns0:t>
+          <ns0:t>OptionLastStandCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="7">
@@ -2028,11 +2030,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D83" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>90</ns0:v>
+      </ns0:c>
+      <ns0:c r="E83" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2044,60 +2051,60 @@
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionLastStandDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C84" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D84" s="4">
+        <ns0:v>0.10</ns0:v>
+      </ns0:c>
+      <ns0:c r="F84" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition into slow motion</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="85">
+      <ns0:c r="A85" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B85" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionLastStandEasing</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C84" t="inlineStr" s="8">
+      <ns0:c r="C85" t="inlineStr" s="8">
         <ns0:is>
           <ns0:t>Dropdown</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D84" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E84" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F84" t="inlineStr" s="4">
+      <ns0:c r="D85" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E85" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F85" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Transition curve shape</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="85"/>
-    <ns0:row r="86">
-      <ns0:c r="A86" t="inlineStr" s="2">
+    <ns0:row r="86"/>
+    <ns0:row r="87">
+      <ns0:c r="A87" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="87">
-      <ns0:c r="A87" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B87" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionParryChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C87" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D87" s="4">
-        <ns0:v>0.5</ns0:v>
-      </ns0:c>
-      <ns0:c r="F87" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2109,7 +2116,7 @@
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryTimeScale</ns0:t>
+          <ns0:t>OptionParryChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="7">
@@ -2118,11 +2125,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D88" s="4">
-        <ns0:v>0.34</ns0:v>
+        <ns0:v>0.5</ns0:v>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2134,7 +2141,7 @@
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryDuration</ns0:t>
+          <ns0:t>OptionParryTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C89" t="inlineStr" s="7">
@@ -2143,11 +2150,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D89" s="4">
-        <ns0:v>1.5</ns0:v>
+        <ns0:v>0.34</ns0:v>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2159,7 +2166,7 @@
       </ns0:c>
       <ns0:c r="B90" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryCooldown</ns0:t>
+          <ns0:t>OptionParryDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C90" t="inlineStr" s="7">
@@ -2168,16 +2175,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D90" s="4">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="E90" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>1.5</ns0:v>
       </ns0:c>
       <ns0:c r="F90" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2189,7 +2191,7 @@
       </ns0:c>
       <ns0:c r="B91" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryDelayIn</ns0:t>
+          <ns0:t>OptionParryCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C91" t="inlineStr" s="7">
@@ -2198,11 +2200,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D91" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="E91" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F91" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2214,62 +2221,60 @@
       </ns0:c>
       <ns0:c r="B92" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionParryDelayIn</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C92" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D92" s="4">
+        <ns0:v>0.10</ns0:v>
+      </ns0:c>
+      <ns0:c r="F92" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition into slow motion</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="93">
+      <ns0:c r="A93" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B93" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionParryEasing</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C92" t="inlineStr" s="8">
+      <ns0:c r="C93" t="inlineStr" s="8">
         <ns0:is>
           <ns0:t>Dropdown</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D92" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E92" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F92" t="inlineStr" s="4">
+      <ns0:c r="D93" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E93" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F93" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Transition curve shape</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="93"/>
-    <ns0:row r="94">
-      <ns0:c r="A94" t="inlineStr" s="2">
+    <ns0:row r="94"/>
+    <ns0:row r="95">
+      <ns0:c r="A95" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="95">
-      <ns0:c r="A95" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B95" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDebugLogging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C95" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D95" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F95" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2281,22 +2286,22 @@
       </ns0:c>
       <ns0:c r="B96" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionQuickTestTrigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C96" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
+          <ns0:t>OptionDebugLogging</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C96" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D96" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F96" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Which trigger to simulate</ns0:t>
+          <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2308,55 +2313,82 @@
       </ns0:c>
       <ns0:c r="B97" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionQuickTestTrigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C97" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D97" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F97" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Which trigger to simulate</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="98">
+      <ns0:c r="A98" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B98" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionQuickTestNow</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C97" t="inlineStr" s="6">
+      <ns0:c r="C98" t="inlineStr" s="6">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D97" t="inlineStr" s="4">
+      <ns0:c r="D98" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F97" t="inlineStr" s="4">
+      <ns0:c r="F98" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Toggle to fire the selected trigger once</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="98"/>
-    <ns0:row r="99">
-      <ns0:c r="A99" t="inlineStr" s="2">
+    <ns0:row r="99"/>
+    <ns0:row r="100">
+      <ns0:c r="A100" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="100">
-      <ns0:c r="A100" t="inlineStr" s="4">
+    <ns0:row r="101">
+      <ns0:c r="A101" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B100" t="inlineStr" s="4">
+      <ns0:c r="B101" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>OptionResetStats</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C100" t="inlineStr" s="6">
+      <ns0:c r="C101" t="inlineStr" s="6">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D100" t="inlineStr" s="4">
+      <ns0:c r="D101" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F100" t="inlineStr" s="4">
+      <ns0:c r="F101" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Toggle to reset all statistics</ns0:t>
         </ns0:is>
@@ -3815,63 +3847,63 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" s="4">
-        <ns0:v>4</ns0:v>
+        <ns0:v>5</ns0:v>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t>EasingPercentProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" s="4">
-        <ns0:v>4</ns0:v>
+        <ns0:v>11</ns0:v>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>0% | 5% | 10% | 15% | 20% | 25% | 30% | 35% | 40% | 45% | 50%</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" s="4">
-        <ns0:v>3</ns0:v>
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
       <ns0:c r="A21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B21" s="4">
-        <ns0:v>4</ns0:v>
+        <ns0:v>3</ns0:v>
       </ns0:c>
       <ns0:c r="C21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
       <ns0:c r="A22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>MinEnemyGroupProvider</ns0:t>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B22" s="4">
@@ -3879,24 +3911,29 @@
       </ns0:c>
       <ns0:c r="C22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="23">
       <ns0:c r="A23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>PresetProvider</ns0:t>
+          <ns0:t>MinEnemyGroupProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B23" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>4</ns0:v>
+      </ns0:c>
+      <ns0:c r="C23" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="24">
       <ns0:c r="A24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>QuickTestTriggerProvider</ns0:t>
+          <ns0:t>PresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B24" s="4">
@@ -3906,40 +3943,50 @@
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B25" s="4">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C25" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="26">
       <ns0:c r="A26" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TimeScaleProvider</ns0:t>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B26" s="4">
-        <ns0:v>8</ns0:v>
+        <ns0:v>5</ns0:v>
       </ns0:c>
       <ns0:c r="C26" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="27">
       <ns0:c r="A27" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>TimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B27" s="4">
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="C27" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="28">
+      <ns0:c r="A28" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B27" s="4">
+      <ns0:c r="B28" s="4">
         <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
refactor: per-trigger easing with Delay controlling transition time
- Add per-trigger Easing dropdown to each collapsible (Smoothstep default)
- Change Delay setting to control easing transition duration (in seconds)
- If Easing is Off, transition is instant regardless of Delay
- Remove global EasingPercent setting (per-trigger Delay replaces it)
- Easing curve options: Off, Smoothstep, Linear, Ease In, Ease Out

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -480,62 +480,57 @@
       </ns0:c>
       <ns0:c r="B14" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionEasingPercent</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C14" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionTriggerProfile</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C14" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D14" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>25%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E14" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0% | 5% | 10% | 15% | 20% | 25% | 30% | 35% | 40% | 45% | 50%</ns0:t>
+          <ns0:t>All</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F14" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Percentage of duration used for easing in/out transitions (0% = instant, 50% = half duration is transition)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="15">
-      <ns0:c r="A15" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryPresetSelection</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B15" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionTriggerProfile</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C15" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D15" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>All</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F15" t="inlineStr" s="4">
-        <ns0:is>
           <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="16"/>
+    <ns0:row r="15"/>
+    <ns0:row r="16">
+      <ns0:c r="A16" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="17">
-      <ns0:c r="A17" t="inlineStr" s="2">
+      <ns0:c r="A17" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B17" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C17" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D17" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F17" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -547,7 +542,7 @@
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
+          <ns0:t>TriggerThrownImpactKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="6">
@@ -557,12 +552,12 @@
       </ns0:c>
       <ns0:c r="D18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
+          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -574,7 +569,7 @@
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerThrownImpactKill</ns0:t>
+          <ns0:t>TriggerCriticalKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="6">
@@ -584,12 +579,12 @@
       </ns0:c>
       <ns0:c r="D19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -601,7 +596,7 @@
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerCriticalKill</ns0:t>
+          <ns0:t>TriggerDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="6">
@@ -616,7 +611,7 @@
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -628,7 +623,7 @@
       </ns0:c>
       <ns0:c r="B21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDismemberment</ns0:t>
+          <ns0:t>TriggerDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C21" t="inlineStr" s="6">
@@ -643,7 +638,7 @@
       </ns0:c>
       <ns0:c r="F21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -655,7 +650,7 @@
       </ns0:c>
       <ns0:c r="B22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDecapitation</ns0:t>
+          <ns0:t>TriggerLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C22" t="inlineStr" s="6">
@@ -670,7 +665,7 @@
       </ns0:c>
       <ns0:c r="F22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -682,7 +677,7 @@
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastEnemy</ns0:t>
+          <ns0:t>TriggerLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C23" t="inlineStr" s="6">
@@ -697,7 +692,7 @@
       </ns0:c>
       <ns0:c r="F23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -709,22 +704,27 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C24" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionLastStandThreshold</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C24" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>15%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E24" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -736,62 +736,62 @@
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandThreshold</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C25" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>TriggerParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C25" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E25" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="26">
-      <ns0:c r="A26" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B26" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C26" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D26" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F26" t="inlineStr" s="4">
-        <ns0:is>
           <ns0:t>Trigger on successful weapon deflections</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="27"/>
+    <ns0:row r="26"/>
+    <ns0:row r="27">
+      <ns0:c r="A27" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="28">
-      <ns0:c r="A28" t="inlineStr" s="2">
+      <ns0:c r="A28" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B28" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCameraDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C28" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D28" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>3m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E28" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F28" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -803,27 +803,22 @@
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCameraDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C29" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionRandomizeDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C29" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>3m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E29" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
+          <ns0:t>Randomize distance per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -835,22 +830,27 @@
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C30" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionCameraHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C30" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>1.5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E30" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize distance per killcam</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -862,27 +862,22 @@
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCameraHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C31" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionRandomizeHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C31" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E31" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Randomize height per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -894,62 +889,60 @@
       </ns0:c>
       <ns0:c r="B32" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C32" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionOrbitSpeed</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C32" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D32" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>Slow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F32" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize height per killcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="33">
-      <ns0:c r="A33" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B33" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionOrbitSpeed</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C33" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D33" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Slow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E33" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F33" t="inlineStr" s="4">
-        <ns0:is>
           <ns0:t>Camera rotation speed (0 for static)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="34"/>
+    <ns0:row r="33"/>
+    <ns0:row r="34">
+      <ns0:c r="A34" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="35">
-      <ns0:c r="A35" t="inlineStr" s="2">
+      <ns0:c r="A35" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B35" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionBasicChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C35" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D35" s="4">
+        <ns0:v>0.25</ns0:v>
+      </ns0:c>
+      <ns0:c r="F35" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -961,7 +954,7 @@
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicChance</ns0:t>
+          <ns0:t>OptionBasicTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="7">
@@ -970,11 +963,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D36" s="4">
-        <ns0:v>0.25</ns0:v>
+        <ns0:v>0.28</ns0:v>
       </ns0:c>
       <ns0:c r="F36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -986,7 +979,7 @@
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicTimeScale</ns0:t>
+          <ns0:t>OptionBasicDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C37" t="inlineStr" s="7">
@@ -995,11 +988,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D37" s="4">
-        <ns0:v>0.28</ns0:v>
+        <ns0:v>2.5</ns0:v>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1011,7 +1004,7 @@
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicDuration</ns0:t>
+          <ns0:t>OptionBasicCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C38" t="inlineStr" s="7">
@@ -1020,11 +1013,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D38" s="4">
-        <ns0:v>2.5</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E38" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1036,7 +1034,7 @@
       </ns0:c>
       <ns0:c r="B39" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicCooldown</ns0:t>
+          <ns0:t>OptionBasicDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C39" t="inlineStr" s="7">
@@ -1045,16 +1043,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D39" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E39" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F39" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1066,20 +1059,27 @@
       </ns0:c>
       <ns0:c r="B40" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicDelayIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C40" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D40" s="4">
-        <ns0:v>0.10</ns0:v>
+          <ns0:t>OptionBasicEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C40" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F40" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Transition curve shape</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1091,67 +1091,60 @@
       </ns0:c>
       <ns0:c r="B41" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicEasing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C41" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
+          <ns0:t>OptionBasicThirdPerson</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C41" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D41" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E41" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F41" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="42">
-      <ns0:c r="A42" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B42" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionBasicThirdPerson</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C42" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D42" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E42" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F42" t="inlineStr" s="4">
-        <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="43"/>
+    <ns0:row r="42"/>
+    <ns0:row r="43">
+      <ns0:c r="A43" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="44">
-      <ns0:c r="A44" t="inlineStr" s="2">
+      <ns0:c r="A44" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B44" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCriticalChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C44" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D44" s="4">
+        <ns0:v>0.75</ns0:v>
+      </ns0:c>
+      <ns0:c r="F44" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1163,7 +1156,7 @@
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalChance</ns0:t>
+          <ns0:t>OptionCriticalTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C45" t="inlineStr" s="7">
@@ -1172,11 +1165,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D45" s="4">
-        <ns0:v>0.75</ns0:v>
+        <ns0:v>0.25</ns0:v>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1188,7 +1181,7 @@
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalTimeScale</ns0:t>
+          <ns0:t>OptionCriticalDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C46" t="inlineStr" s="7">
@@ -1197,11 +1190,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D46" s="4">
-        <ns0:v>0.25</ns0:v>
+        <ns0:v>3.0</ns0:v>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1213,7 +1206,7 @@
       </ns0:c>
       <ns0:c r="B47" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalDuration</ns0:t>
+          <ns0:t>OptionCriticalCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C47" t="inlineStr" s="7">
@@ -1222,11 +1215,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D47" s="4">
-        <ns0:v>3.0</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E47" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F47" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1238,7 +1236,7 @@
       </ns0:c>
       <ns0:c r="B48" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalCooldown</ns0:t>
+          <ns0:t>OptionCriticalDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C48" t="inlineStr" s="7">
@@ -1247,16 +1245,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D48" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E48" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F48" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1268,20 +1261,27 @@
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalDelayIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C49" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D49" s="4">
-        <ns0:v>0.10</ns0:v>
+          <ns0:t>OptionCriticalEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C49" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F49" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Transition curve shape</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1293,67 +1293,60 @@
       </ns0:c>
       <ns0:c r="B50" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalEasing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C50" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
+          <ns0:t>OptionCriticalThirdPerson</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C50" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D50" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E50" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F50" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="51">
-      <ns0:c r="A51" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B51" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCriticalThirdPerson</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C51" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D51" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E51" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F51" t="inlineStr" s="4">
-        <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="52"/>
+    <ns0:row r="51"/>
+    <ns0:row r="52">
+      <ns0:c r="A52" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="53">
-      <ns0:c r="A53" t="inlineStr" s="2">
+      <ns0:c r="A53" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B53" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDismemberChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C53" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D53" s="4">
+        <ns0:v>0.3</ns0:v>
+      </ns0:c>
+      <ns0:c r="F53" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1365,7 +1358,7 @@
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberChance</ns0:t>
+          <ns0:t>OptionDismemberTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C54" t="inlineStr" s="7">
@@ -1378,7 +1371,7 @@
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1390,7 +1383,7 @@
       </ns0:c>
       <ns0:c r="B55" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberTimeScale</ns0:t>
+          <ns0:t>OptionDismemberDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C55" t="inlineStr" s="7">
@@ -1399,11 +1392,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D55" s="4">
-        <ns0:v>0.3</ns0:v>
+        <ns0:v>2.0</ns0:v>
       </ns0:c>
       <ns0:c r="F55" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1415,7 +1408,7 @@
       </ns0:c>
       <ns0:c r="B56" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberDuration</ns0:t>
+          <ns0:t>OptionDismemberCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C56" t="inlineStr" s="7">
@@ -1424,11 +1417,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D56" s="4">
-        <ns0:v>2.0</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E56" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F56" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1440,7 +1438,7 @@
       </ns0:c>
       <ns0:c r="B57" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberCooldown</ns0:t>
+          <ns0:t>OptionDismemberDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C57" t="inlineStr" s="7">
@@ -1449,16 +1447,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D57" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E57" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F57" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1470,20 +1463,27 @@
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberDelayIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C58" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D58" s="4">
-        <ns0:v>0.10</ns0:v>
+          <ns0:t>OptionDismemberEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C58" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Transition curve shape</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1495,67 +1495,60 @@
       </ns0:c>
       <ns0:c r="B59" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberEasing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C59" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
+          <ns0:t>OptionDismemberThirdPerson</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C59" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D59" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E59" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F59" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="60">
-      <ns0:c r="A60" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B60" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDismemberThirdPerson</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C60" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D60" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E60" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F60" t="inlineStr" s="4">
-        <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="61"/>
+    <ns0:row r="60"/>
+    <ns0:row r="61">
+      <ns0:c r="A61" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="62">
-      <ns0:c r="A62" t="inlineStr" s="2">
+      <ns0:c r="A62" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B62" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDecapChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C62" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D62" s="4">
+        <ns0:v>0.9</ns0:v>
+      </ns0:c>
+      <ns0:c r="F62" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1567,7 +1560,7 @@
       </ns0:c>
       <ns0:c r="B63" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapChance</ns0:t>
+          <ns0:t>OptionDecapTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C63" t="inlineStr" s="7">
@@ -1576,11 +1569,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D63" s="4">
-        <ns0:v>0.9</ns0:v>
+        <ns0:v>0.23</ns0:v>
       </ns0:c>
       <ns0:c r="F63" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1592,7 +1585,7 @@
       </ns0:c>
       <ns0:c r="B64" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapTimeScale</ns0:t>
+          <ns0:t>OptionDecapDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C64" t="inlineStr" s="7">
@@ -1601,11 +1594,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D64" s="4">
-        <ns0:v>0.23</ns0:v>
+        <ns0:v>3.25</ns0:v>
       </ns0:c>
       <ns0:c r="F64" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1617,7 +1610,7 @@
       </ns0:c>
       <ns0:c r="B65" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapDuration</ns0:t>
+          <ns0:t>OptionDecapCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C65" t="inlineStr" s="7">
@@ -1626,11 +1619,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D65" s="4">
-        <ns0:v>3.25</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E65" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F65" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1642,7 +1640,7 @@
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapCooldown</ns0:t>
+          <ns0:t>OptionDecapDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="7">
@@ -1651,16 +1649,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D66" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E66" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1672,20 +1665,27 @@
       </ns0:c>
       <ns0:c r="B67" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapDelayIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C67" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D67" s="4">
-        <ns0:v>0.10</ns0:v>
+          <ns0:t>OptionDecapEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C67" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D67" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E67" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F67" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Transition curve shape</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1697,67 +1697,60 @@
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapEasing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C68" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
+          <ns0:t>OptionDecapThirdPerson</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C68" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="69">
-      <ns0:c r="A69" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B69" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDecapThirdPerson</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C69" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D69" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E69" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F69" t="inlineStr" s="4">
-        <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="70"/>
+    <ns0:row r="69"/>
+    <ns0:row r="70">
+      <ns0:c r="A70" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="71">
-      <ns0:c r="A71" t="inlineStr" s="2">
+      <ns0:c r="A71" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastEnemyChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C71" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D71" s="4">
+        <ns0:v>1.0</ns0:v>
+      </ns0:c>
+      <ns0:c r="F71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1769,7 +1762,7 @@
       </ns0:c>
       <ns0:c r="B72" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyChance</ns0:t>
+          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C72" t="inlineStr" s="7">
@@ -1778,11 +1771,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D72" s="4">
-        <ns0:v>1.0</ns0:v>
+        <ns0:v>0.26</ns0:v>
       </ns0:c>
       <ns0:c r="F72" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1794,7 +1787,7 @@
       </ns0:c>
       <ns0:c r="B73" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
+          <ns0:t>OptionLastEnemyDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C73" t="inlineStr" s="7">
@@ -1803,11 +1796,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D73" s="4">
-        <ns0:v>0.26</ns0:v>
+        <ns0:v>2.75</ns0:v>
       </ns0:c>
       <ns0:c r="F73" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1819,7 +1812,7 @@
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyDuration</ns0:t>
+          <ns0:t>OptionLastEnemyCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C74" t="inlineStr" s="7">
@@ -1828,11 +1821,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D74" s="4">
-        <ns0:v>2.75</ns0:v>
+        <ns0:v>30</ns0:v>
+      </ns0:c>
+      <ns0:c r="E74" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1844,7 +1842,7 @@
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyCooldown</ns0:t>
+          <ns0:t>OptionLastEnemyDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="7">
@@ -1853,16 +1851,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D75" s="4">
-        <ns0:v>30</ns0:v>
-      </ns0:c>
-      <ns0:c r="E75" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1874,20 +1867,27 @@
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyDelayIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C76" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D76" s="4">
-        <ns0:v>0.10</ns0:v>
+          <ns0:t>OptionLastEnemyEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C76" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D76" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E76" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Transition curve shape</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1899,67 +1899,60 @@
       </ns0:c>
       <ns0:c r="B77" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyEasing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C77" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
+          <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C77" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D77" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E77" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F77" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="78">
-      <ns0:c r="A78" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B78" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C78" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D78" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E78" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F78" t="inlineStr" s="4">
-        <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="79"/>
+    <ns0:row r="78"/>
+    <ns0:row r="79">
+      <ns0:c r="A79" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="80">
-      <ns0:c r="A80" t="inlineStr" s="2">
+      <ns0:c r="A80" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomLastStand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B80" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastStandTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C80" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D80" s="4">
+        <ns0:v>0.30</ns0:v>
+      </ns0:c>
+      <ns0:c r="F80" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1971,7 +1964,7 @@
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandTimeScale</ns0:t>
+          <ns0:t>OptionLastStandDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="7">
@@ -1980,11 +1973,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D81" s="4">
-        <ns0:v>0.30</ns0:v>
+        <ns0:v>4.0</ns0:v>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1996,7 +1989,7 @@
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandDuration</ns0:t>
+          <ns0:t>OptionLastStandCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="7">
@@ -2005,11 +1998,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D82" s="4">
-        <ns0:v>4.0</ns0:v>
+        <ns0:v>90</ns0:v>
+      </ns0:c>
+      <ns0:c r="E82" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2021,7 +2019,7 @@
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandCooldown</ns0:t>
+          <ns0:t>OptionLastStandDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="7">
@@ -2030,16 +2028,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D83" s="4">
-        <ns0:v>90</ns0:v>
-      </ns0:c>
-      <ns0:c r="E83" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2051,60 +2044,60 @@
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandDelayIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C84" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D84" s="4">
-        <ns0:v>0.10</ns0:v>
+          <ns0:t>OptionLastStandEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C84" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D84" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E84" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="85">
-      <ns0:c r="A85" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B85" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastStandEasing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C85" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D85" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E85" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F85" t="inlineStr" s="4">
-        <ns0:is>
           <ns0:t>Transition curve shape</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="86"/>
+    <ns0:row r="85"/>
+    <ns0:row r="86">
+      <ns0:c r="A86" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="87">
-      <ns0:c r="A87" t="inlineStr" s="2">
+      <ns0:c r="A87" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B87" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionParryChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C87" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D87" s="4">
+        <ns0:v>0.5</ns0:v>
+      </ns0:c>
+      <ns0:c r="F87" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2116,7 +2109,7 @@
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryChance</ns0:t>
+          <ns0:t>OptionParryTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C88" t="inlineStr" s="7">
@@ -2125,11 +2118,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D88" s="4">
-        <ns0:v>0.5</ns0:v>
+        <ns0:v>0.34</ns0:v>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2141,7 +2134,7 @@
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryTimeScale</ns0:t>
+          <ns0:t>OptionParryDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C89" t="inlineStr" s="7">
@@ -2150,11 +2143,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D89" s="4">
-        <ns0:v>0.34</ns0:v>
+        <ns0:v>1.5</ns0:v>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2166,7 +2159,7 @@
       </ns0:c>
       <ns0:c r="B90" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryDuration</ns0:t>
+          <ns0:t>OptionParryCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C90" t="inlineStr" s="7">
@@ -2175,11 +2168,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D90" s="4">
-        <ns0:v>1.5</ns0:v>
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="E90" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F90" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2191,7 +2189,7 @@
       </ns0:c>
       <ns0:c r="B91" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryCooldown</ns0:t>
+          <ns0:t>OptionParryDelayIn</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C91" t="inlineStr" s="7">
@@ -2200,16 +2198,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D91" s="4">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="E91" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.10</ns0:v>
       </ns0:c>
       <ns0:c r="F91" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition into slow motion</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2221,60 +2214,62 @@
       </ns0:c>
       <ns0:c r="B92" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryDelayIn</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C92" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D92" s="4">
-        <ns0:v>0.10</ns0:v>
+          <ns0:t>OptionParryEasing</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C92" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D92" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E92" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F92" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="93">
-      <ns0:c r="A93" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B93" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionParryEasing</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C93" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D93" t="inlineStr" s="4">
+          <ns0:t>Transition curve shape</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="93"/>
+    <ns0:row r="94">
+      <ns0:c r="A94" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="95">
+      <ns0:c r="A95" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B95" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDebugLogging</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C95" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D95" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E93" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F93" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="94"/>
-    <ns0:row r="95">
-      <ns0:c r="A95" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
+      <ns0:c r="F95" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2286,22 +2281,22 @@
       </ns0:c>
       <ns0:c r="B96" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDebugLogging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C96" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionQuickTestTrigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C96" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D96" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>TriggerBasicKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F96" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Enable verbose debug logging</ns0:t>
+          <ns0:t>Which trigger to simulate</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2313,82 +2308,55 @@
       </ns0:c>
       <ns0:c r="B97" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionQuickTestTrigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C97" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
+          <ns0:t>OptionQuickTestNow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C97" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D97" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F97" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Which trigger to simulate</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="98">
-      <ns0:c r="A98" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B98" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionQuickTestNow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C98" t="inlineStr" s="6">
+          <ns0:t>Toggle to fire the selected trigger once</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="98"/>
+    <ns0:row r="99">
+      <ns0:c r="A99" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryStatistics</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="100">
+      <ns0:c r="A100" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryStatistics</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B100" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionResetStats</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C100" t="inlineStr" s="6">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D98" t="inlineStr" s="4">
+      <ns0:c r="D100" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F98" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Toggle to fire the selected trigger once</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="99"/>
-    <ns0:row r="100">
-      <ns0:c r="A100" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryStatistics</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="101">
-      <ns0:c r="A101" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryStatistics</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B101" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionResetStats</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C101" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D101" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F101" t="inlineStr" s="4">
+      <ns0:c r="F100" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Toggle to reset all statistics</ns0:t>
         </ns0:is>
@@ -3858,52 +3826,52 @@
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>EasingPercentProvider</ns0:t>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" s="4">
-        <ns0:v>11</ns0:v>
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>0% | 5% | 10% | 15% | 20% | 25% | 30% | 35% | 40% | 45% | 50%</ns0:t>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" s="4">
-        <ns0:v>4</ns0:v>
+        <ns0:v>3</ns0:v>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
       <ns0:c r="A21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B21" s="4">
-        <ns0:v>3</ns0:v>
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="C21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
       <ns0:c r="A22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t>MinEnemyGroupProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B22" s="4">
@@ -3911,29 +3879,24 @@
       </ns0:c>
       <ns0:c r="C22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="23">
       <ns0:c r="A23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>MinEnemyGroupProvider</ns0:t>
+          <ns0:t>PresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B23" s="4">
-        <ns0:v>4</ns0:v>
-      </ns0:c>
-      <ns0:c r="C23" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="24">
       <ns0:c r="A24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>PresetProvider</ns0:t>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B24" s="4">
@@ -3943,50 +3906,40 @@
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>QuickTestTriggerProvider</ns0:t>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B25" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="C25" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="26">
       <ns0:c r="A26" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t>TimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B26" s="4">
-        <ns0:v>5</ns0:v>
+        <ns0:v>8</ns0:v>
       </ns0:c>
       <ns0:c r="C26" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="27">
       <ns0:c r="A27" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TimeScaleProvider</ns0:t>
+          <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B27" s="4">
-        <ns0:v>8</ns0:v>
-      </ns0:c>
-      <ns0:c r="C27" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="28">
-      <ns0:c r="A28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerProfileProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B28" s="4">
         <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
rename: Delay → Ramp Time, Easing → Transition
- "Ramp Time" = duration of transition (seconds)
- "Transition" = curve shape (Off, Smoothstep, Linear, Ease In, Ease Out)
- Updated tooltips for clarity

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -1034,7 +1034,7 @@
       </ns0:c>
       <ns0:c r="B39" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicDelayIn</ns0:t>
+          <ns0:t>OptionBasicRampTime</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C39" t="inlineStr" s="7">
@@ -1047,7 +1047,7 @@
       </ns0:c>
       <ns0:c r="F39" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Duration of transition ramp (seconds)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1059,7 +1059,7 @@
       </ns0:c>
       <ns0:c r="B40" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicEasing</ns0:t>
+          <ns0:t>OptionBasicTransition</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C40" t="inlineStr" s="8">
@@ -1079,7 +1079,7 @@
       </ns0:c>
       <ns0:c r="F40" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1236,7 +1236,7 @@
       </ns0:c>
       <ns0:c r="B48" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalDelayIn</ns0:t>
+          <ns0:t>OptionCriticalRampTime</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C48" t="inlineStr" s="7">
@@ -1249,7 +1249,7 @@
       </ns0:c>
       <ns0:c r="F48" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Duration of transition ramp (seconds)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1261,7 +1261,7 @@
       </ns0:c>
       <ns0:c r="B49" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalEasing</ns0:t>
+          <ns0:t>OptionCriticalTransition</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C49" t="inlineStr" s="8">
@@ -1281,7 +1281,7 @@
       </ns0:c>
       <ns0:c r="F49" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1438,7 +1438,7 @@
       </ns0:c>
       <ns0:c r="B57" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberDelayIn</ns0:t>
+          <ns0:t>OptionDismemberRampTime</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C57" t="inlineStr" s="7">
@@ -1451,7 +1451,7 @@
       </ns0:c>
       <ns0:c r="F57" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Duration of transition ramp (seconds)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1463,7 +1463,7 @@
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberEasing</ns0:t>
+          <ns0:t>OptionDismemberTransition</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C58" t="inlineStr" s="8">
@@ -1483,7 +1483,7 @@
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1640,7 +1640,7 @@
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapDelayIn</ns0:t>
+          <ns0:t>OptionDecapRampTime</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="7">
@@ -1653,7 +1653,7 @@
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Duration of transition ramp (seconds)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1665,7 +1665,7 @@
       </ns0:c>
       <ns0:c r="B67" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapEasing</ns0:t>
+          <ns0:t>OptionDecapTransition</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C67" t="inlineStr" s="8">
@@ -1685,7 +1685,7 @@
       </ns0:c>
       <ns0:c r="F67" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1842,7 +1842,7 @@
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyDelayIn</ns0:t>
+          <ns0:t>OptionLastEnemyRampTime</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="7">
@@ -1855,7 +1855,7 @@
       </ns0:c>
       <ns0:c r="F75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Duration of transition ramp (seconds)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1867,7 +1867,7 @@
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyEasing</ns0:t>
+          <ns0:t>OptionLastEnemyTransition</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C76" t="inlineStr" s="8">
@@ -1887,7 +1887,7 @@
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2019,7 +2019,7 @@
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandDelayIn</ns0:t>
+          <ns0:t>OptionLastStandRampTime</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="7">
@@ -2032,7 +2032,7 @@
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Duration of transition ramp (seconds)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2044,7 +2044,7 @@
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandEasing</ns0:t>
+          <ns0:t>OptionLastStandTransition</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C84" t="inlineStr" s="8">
@@ -2064,7 +2064,7 @@
       </ns0:c>
       <ns0:c r="F84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2189,7 +2189,7 @@
       </ns0:c>
       <ns0:c r="B91" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryDelayIn</ns0:t>
+          <ns0:t>OptionParryRampTime</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C91" t="inlineStr" s="7">
@@ -2202,7 +2202,7 @@
       </ns0:c>
       <ns0:c r="F91" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion</ns0:t>
+          <ns0:t>Duration of transition ramp (seconds)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2214,7 +2214,7 @@
       </ns0:c>
       <ns0:c r="B92" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryEasing</ns0:t>
+          <ns0:t>OptionParryTransition</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C92" t="inlineStr" s="8">
@@ -2234,7 +2234,7 @@
       </ns0:c>
       <ns0:c r="F92" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve shape</ns0:t>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Simplify transitions: remove Ramp Time sliders, use hardcoded 0.25s duration
Transition duration is now fixed at 0.25s when Transition dropdown is not Off.
Removes all delay-related code: CustomDelayProvider, SetTriggerDelay, GetDelayDuration,
Delay field from TriggerCustomValues, and all per-trigger delay variables.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -453,7 +453,7 @@
       </ns0:c>
       <ns0:c r="B13" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDelayInPreset</ns0:t>
+          <ns0:t>OptionTriggerProfile</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C13" t="inlineStr" s="8">
@@ -463,47 +463,47 @@
       </ns0:c>
       <ns0:c r="D13" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Default</ns0:t>
+          <ns0:t>All</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F13" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition into slow motion. Instant = immediate. Default = natural feel.</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="14">
-      <ns0:c r="A14" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryPresetSelection</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B14" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionTriggerProfile</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C14" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D14" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>All</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F14" t="inlineStr" s="4">
-        <ns0:is>
           <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="15"/>
+    <ns0:row r="14"/>
+    <ns0:row r="15">
+      <ns0:c r="A15" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="16">
-      <ns0:c r="A16" t="inlineStr" s="2">
+      <ns0:c r="A16" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B16" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C16" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D16" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F16" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -515,7 +515,7 @@
       </ns0:c>
       <ns0:c r="B17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
+          <ns0:t>TriggerThrownImpactKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C17" t="inlineStr" s="6">
@@ -525,12 +525,12 @@
       </ns0:c>
       <ns0:c r="D17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
+          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -542,7 +542,7 @@
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerThrownImpactKill</ns0:t>
+          <ns0:t>TriggerCriticalKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="6">
@@ -552,12 +552,12 @@
       </ns0:c>
       <ns0:c r="D18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -569,7 +569,7 @@
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerCriticalKill</ns0:t>
+          <ns0:t>TriggerDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="6">
@@ -584,7 +584,7 @@
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -596,7 +596,7 @@
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDismemberment</ns0:t>
+          <ns0:t>TriggerDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="6">
@@ -611,7 +611,7 @@
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -623,7 +623,7 @@
       </ns0:c>
       <ns0:c r="B21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDecapitation</ns0:t>
+          <ns0:t>TriggerLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C21" t="inlineStr" s="6">
@@ -638,7 +638,7 @@
       </ns0:c>
       <ns0:c r="F21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -650,7 +650,7 @@
       </ns0:c>
       <ns0:c r="B22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastEnemy</ns0:t>
+          <ns0:t>TriggerLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C22" t="inlineStr" s="6">
@@ -665,7 +665,7 @@
       </ns0:c>
       <ns0:c r="F22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -677,22 +677,27 @@
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C23" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionLastStandThreshold</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C23" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>15%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E23" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -704,62 +709,62 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandThreshold</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C24" t="inlineStr" s="7">
+          <ns0:t>TriggerParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C24" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D24" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F24" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger on successful weapon deflections</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="25"/>
+    <ns0:row r="26">
+      <ns0:c r="A26" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="27">
+      <ns0:c r="A27" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B27" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCameraDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C27" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D24" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>15%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E24" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F24" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="25">
-      <ns0:c r="A25" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B25" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C25" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D25" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F25" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Trigger on successful weapon deflections</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="26"/>
-    <ns0:row r="27">
-      <ns0:c r="A27" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
+      <ns0:c r="D27" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>3m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E27" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F27" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -771,27 +776,22 @@
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCameraDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C28" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionRandomizeDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C28" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>3m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
+          <ns0:t>Randomize distance per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -803,22 +803,27 @@
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C29" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionCameraHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C29" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>1.5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E29" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize distance per killcam</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -830,27 +835,22 @@
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCameraHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C30" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionRandomizeHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C30" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E30" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Randomize height per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -862,62 +862,60 @@
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C31" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionOrbitSpeed</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C31" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>Slow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E31" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize height per killcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="32">
-      <ns0:c r="A32" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B32" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionOrbitSpeed</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C32" t="inlineStr" s="7">
+          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="32"/>
+    <ns0:row r="33">
+      <ns0:c r="A33" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="34">
+      <ns0:c r="A34" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B34" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionBasicChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C34" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D32" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Slow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E32" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F32" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="33"/>
-    <ns0:row r="34">
-      <ns0:c r="A34" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
+      <ns0:c r="D34" s="4">
+        <ns0:v>0.25</ns0:v>
+      </ns0:c>
+      <ns0:c r="F34" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -929,7 +927,7 @@
       </ns0:c>
       <ns0:c r="B35" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicChance</ns0:t>
+          <ns0:t>OptionBasicTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C35" t="inlineStr" s="7">
@@ -938,11 +936,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D35" s="4">
-        <ns0:v>0.25</ns0:v>
+        <ns0:v>0.28</ns0:v>
       </ns0:c>
       <ns0:c r="F35" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -954,7 +952,7 @@
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicTimeScale</ns0:t>
+          <ns0:t>OptionBasicDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="7">
@@ -963,11 +961,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D36" s="4">
-        <ns0:v>0.28</ns0:v>
+        <ns0:v>2.5</ns0:v>
       </ns0:c>
       <ns0:c r="F36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -979,7 +977,7 @@
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicDuration</ns0:t>
+          <ns0:t>OptionBasicCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C37" t="inlineStr" s="7">
@@ -988,11 +986,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D37" s="4">
-        <ns0:v>2.5</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E37" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1004,25 +1007,27 @@
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C38" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D38" s="4">
-        <ns0:v>10</ns0:v>
+          <ns0:t>OptionBasicTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C38" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D38" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1034,7 +1039,7 @@
       </ns0:c>
       <ns0:c r="B39" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicRampTime</ns0:t>
+          <ns0:t>OptionBasicThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C39" t="inlineStr" s="7">
@@ -1042,84 +1047,77 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D39" s="4">
-        <ns0:v>0.10</ns0:v>
+      <ns0:c r="D39" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E39" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F39" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration of transition ramp (seconds)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="40">
-      <ns0:c r="A40" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B40" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionBasicTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C40" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D40" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E40" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F40" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="40"/>
     <ns0:row r="41">
-      <ns0:c r="A41" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B41" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionBasicThirdPerson</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C41" t="inlineStr" s="7">
+      <ns0:c r="A41" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="42">
+      <ns0:c r="A42" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B42" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCriticalChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C42" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D41" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E41" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F41" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="42"/>
+      <ns0:c r="D42" s="4">
+        <ns0:v>0.75</ns0:v>
+      </ns0:c>
+      <ns0:c r="F42" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="43">
-      <ns0:c r="A43" t="inlineStr" s="2">
+      <ns0:c r="A43" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B43" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCriticalTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C43" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D43" s="4">
+        <ns0:v>0.25</ns0:v>
+      </ns0:c>
+      <ns0:c r="F43" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1131,7 +1129,7 @@
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalChance</ns0:t>
+          <ns0:t>OptionCriticalDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="7">
@@ -1140,11 +1138,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D44" s="4">
-        <ns0:v>0.75</ns0:v>
+        <ns0:v>3.0</ns0:v>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1156,7 +1154,7 @@
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalTimeScale</ns0:t>
+          <ns0:t>OptionCriticalCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C45" t="inlineStr" s="7">
@@ -1165,11 +1163,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D45" s="4">
-        <ns0:v>0.25</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E45" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1181,20 +1184,27 @@
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C46" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D46" s="4">
-        <ns0:v>3.0</ns0:v>
+          <ns0:t>OptionCriticalTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C46" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D46" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E46" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1206,7 +1216,7 @@
       </ns0:c>
       <ns0:c r="B47" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalCooldown</ns0:t>
+          <ns0:t>OptionCriticalThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C47" t="inlineStr" s="7">
@@ -1214,86 +1224,39 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D47" s="4">
-        <ns0:v>10</ns0:v>
+      <ns0:c r="D47" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E47" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F47" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="48">
-      <ns0:c r="A48" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B48" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCriticalRampTime</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C48" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D48" s="4">
-        <ns0:v>0.10</ns0:v>
-      </ns0:c>
-      <ns0:c r="F48" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration of transition ramp (seconds)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="48"/>
     <ns0:row r="49">
-      <ns0:c r="A49" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B49" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCriticalTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C49" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D49" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E49" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F49" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+      <ns0:c r="A49" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="50">
       <ns0:c r="A50" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B50" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalThirdPerson</ns0:t>
+          <ns0:t>OptionDismemberChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C50" t="inlineStr" s="7">
@@ -1301,27 +1264,62 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D50" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E50" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D50" s="4">
+        <ns0:v>0.3</ns0:v>
       </ns0:c>
       <ns0:c r="F50" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="51"/>
+          <ns0:t>Chance to trigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="51">
+      <ns0:c r="A51" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B51" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDismemberTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C51" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D51" s="4">
+        <ns0:v>0.3</ns0:v>
+      </ns0:c>
+      <ns0:c r="F51" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Time scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="52">
-      <ns0:c r="A52" t="inlineStr" s="2">
+      <ns0:c r="A52" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B52" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDismemberDuration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C52" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D52" s="4">
+        <ns0:v>2.0</ns0:v>
+      </ns0:c>
+      <ns0:c r="F52" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1333,7 +1331,7 @@
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberChance</ns0:t>
+          <ns0:t>OptionDismemberCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C53" t="inlineStr" s="7">
@@ -1342,11 +1340,16 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D53" s="4">
-        <ns0:v>0.3</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E53" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1358,20 +1361,27 @@
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C54" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D54" s="4">
-        <ns0:v>0.3</ns0:v>
+          <ns0:t>OptionDismemberTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C54" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D54" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E54" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1383,7 +1393,7 @@
       </ns0:c>
       <ns0:c r="B55" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberDuration</ns0:t>
+          <ns0:t>OptionDismemberThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C55" t="inlineStr" s="7">
@@ -1391,111 +1401,64 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D55" s="4">
-        <ns0:v>2.0</ns0:v>
+      <ns0:c r="D55" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E55" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F55" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="56">
-      <ns0:c r="A56" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B56" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDismemberCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C56" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D56" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E56" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F56" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="56"/>
     <ns0:row r="57">
-      <ns0:c r="A57" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B57" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDismemberRampTime</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C57" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D57" s="4">
-        <ns0:v>0.10</ns0:v>
-      </ns0:c>
-      <ns0:c r="F57" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration of transition ramp (seconds)</ns0:t>
+      <ns0:c r="A57" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="58">
       <ns0:c r="A58" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B58" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C58" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D58" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E58" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionDecapChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C58" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D58" s="4">
+        <ns0:v>0.9</ns0:v>
       </ns0:c>
       <ns0:c r="F58" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="59">
       <ns0:c r="A59" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B59" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberThirdPerson</ns0:t>
+          <ns0:t>OptionDecapTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C59" t="inlineStr" s="7">
@@ -1503,27 +1466,67 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D59" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E59" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D59" s="4">
+        <ns0:v>0.23</ns0:v>
       </ns0:c>
       <ns0:c r="F59" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="60"/>
+          <ns0:t>Time scale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="60">
+      <ns0:c r="A60" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B60" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDecapDuration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C60" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D60" s="4">
+        <ns0:v>3.25</ns0:v>
+      </ns0:c>
+      <ns0:c r="F60" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="61">
-      <ns0:c r="A61" t="inlineStr" s="2">
+      <ns0:c r="A61" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B61" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDecapCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C61" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D61" s="4">
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E61" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F61" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1535,20 +1538,27 @@
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C62" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D62" s="4">
-        <ns0:v>0.9</ns0:v>
+          <ns0:t>OptionDecapTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C62" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D62" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E62" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1560,7 +1570,7 @@
       </ns0:c>
       <ns0:c r="B63" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapTimeScale</ns0:t>
+          <ns0:t>OptionDecapThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C63" t="inlineStr" s="7">
@@ -1568,79 +1578,39 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D63" s="4">
-        <ns0:v>0.23</ns0:v>
+      <ns0:c r="D63" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E63" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F63" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="64">
-      <ns0:c r="A64" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B64" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDecapDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C64" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D64" s="4">
-        <ns0:v>3.25</ns0:v>
-      </ns0:c>
-      <ns0:c r="F64" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="64"/>
     <ns0:row r="65">
-      <ns0:c r="A65" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B65" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDecapCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C65" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D65" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E65" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F65" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+      <ns0:c r="A65" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="66">
       <ns0:c r="A66" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B66" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapRampTime</ns0:t>
+          <ns0:t>OptionLastEnemyChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C66" t="inlineStr" s="7">
@@ -1649,55 +1619,48 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D66" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>1.0</ns0:v>
       </ns0:c>
       <ns0:c r="F66" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration of transition ramp (seconds)</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="67">
       <ns0:c r="A67" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B67" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C67" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D67" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E67" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C67" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D67" s="4">
+        <ns0:v>0.26</ns0:v>
       </ns0:c>
       <ns0:c r="F67" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="68">
       <ns0:c r="A68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapThirdPerson</ns0:t>
+          <ns0:t>OptionLastEnemyDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C68" t="inlineStr" s="7">
@@ -1705,27 +1668,74 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D68" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E68" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D68" s="4">
+        <ns0:v>2.75</ns0:v>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="69"/>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="69">
+      <ns0:c r="A69" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B69" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastEnemyCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C69" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D69" s="4">
+        <ns0:v>30</ns0:v>
+      </ns0:c>
+      <ns0:c r="E69" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F69" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="70">
-      <ns0:c r="A70" t="inlineStr" s="2">
+      <ns0:c r="A70" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B70" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastEnemyTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C70" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D70" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E70" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F70" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1737,7 +1747,7 @@
       </ns0:c>
       <ns0:c r="B71" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyChance</ns0:t>
+          <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C71" t="inlineStr" s="7">
@@ -1745,74 +1755,39 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D71" s="4">
-        <ns0:v>1.0</ns0:v>
+      <ns0:c r="D71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F71" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="72">
-      <ns0:c r="A72" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B72" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C72" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D72" s="4">
-        <ns0:v>0.26</ns0:v>
-      </ns0:c>
-      <ns0:c r="F72" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="72"/>
     <ns0:row r="73">
-      <ns0:c r="A73" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B73" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastEnemyDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C73" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D73" s="4">
-        <ns0:v>2.75</ns0:v>
-      </ns0:c>
-      <ns0:c r="F73" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
+      <ns0:c r="A73" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="74">
       <ns0:c r="A74" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B74" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyCooldown</ns0:t>
+          <ns0:t>OptionLastStandTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C74" t="inlineStr" s="7">
@@ -1821,28 +1796,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D74" s="4">
-        <ns0:v>30</ns0:v>
-      </ns0:c>
-      <ns0:c r="E74" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.30</ns0:v>
       </ns0:c>
       <ns0:c r="F74" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="75">
       <ns0:c r="A75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyRampTime</ns0:t>
+          <ns0:t>OptionLastStandDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="7">
@@ -1851,75 +1821,73 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D75" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>4.0</ns0:v>
       </ns0:c>
       <ns0:c r="F75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration of transition ramp (seconds)</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="76">
       <ns0:c r="A76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C76" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D76" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionLastStandCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C76" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D76" s="4">
+        <ns0:v>90</ns0:v>
       </ns0:c>
       <ns0:c r="E76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="77">
       <ns0:c r="A77" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B77" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C77" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionLastStandTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C77" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D77" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
+          <ns0:t>Smoothstep</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="E77" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F77" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1927,19 +1895,19 @@
     <ns0:row r="79">
       <ns0:c r="A79" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="80">
       <ns0:c r="A80" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B80" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandTimeScale</ns0:t>
+          <ns0:t>OptionParryChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C80" t="inlineStr" s="7">
@@ -1948,23 +1916,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D80" s="4">
-        <ns0:v>0.30</ns0:v>
+        <ns0:v>0.5</ns0:v>
       </ns0:c>
       <ns0:c r="F80" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="81">
       <ns0:c r="A81" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandDuration</ns0:t>
+          <ns0:t>OptionParryTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="7">
@@ -1973,23 +1941,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D81" s="4">
-        <ns0:v>4.0</ns0:v>
+        <ns0:v>0.34</ns0:v>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="82">
       <ns0:c r="A82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandCooldown</ns0:t>
+          <ns0:t>OptionParryDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="7">
@@ -1998,28 +1966,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D82" s="4">
-        <ns0:v>90</ns0:v>
-      </ns0:c>
-      <ns0:c r="E82" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>1.5</ns0:v>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="83">
       <ns0:c r="A83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandRampTime</ns0:t>
+          <ns0:t>OptionParryCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="7">
@@ -2028,23 +1991,28 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D83" s="4">
-        <ns0:v>0.10</ns0:v>
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="E83" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration of transition ramp (seconds)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="84">
       <ns0:c r="A84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandTransition</ns0:t>
+          <ns0:t>OptionParryTransition</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C84" t="inlineStr" s="8">
@@ -2072,291 +2040,121 @@
     <ns0:row r="86">
       <ns0:c r="A86" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="87">
       <ns0:c r="A87" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B87" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C87" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D87" s="4">
-        <ns0:v>0.5</ns0:v>
+          <ns0:t>OptionDebugLogging</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C87" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D87" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F87" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="88">
       <ns0:c r="A88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C88" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D88" s="4">
-        <ns0:v>0.34</ns0:v>
+          <ns0:t>OptionQuickTestTrigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C88" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D88" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Which trigger to simulate</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
       <ns0:c r="A89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C89" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D89" s="4">
-        <ns0:v>1.5</ns0:v>
+          <ns0:t>OptionQuickTestNow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C89" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D89" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="90">
-      <ns0:c r="A90" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B90" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionParryCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C90" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D90" s="4">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="E90" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F90" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
+          <ns0:t>Toggle to fire the selected trigger once</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="90"/>
     <ns0:row r="91">
-      <ns0:c r="A91" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B91" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionParryRampTime</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C91" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D91" s="4">
-        <ns0:v>0.10</ns0:v>
-      </ns0:c>
-      <ns0:c r="F91" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration of transition ramp (seconds)</ns0:t>
+      <ns0:c r="A91" t="inlineStr" s="2">
+        <ns0:is>
+          <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="92">
       <ns0:c r="A92" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B92" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C92" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
+          <ns0:t>OptionResetStats</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C92" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D92" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E92" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F92" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="93"/>
-    <ns0:row r="94">
-      <ns0:c r="A94" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="95">
-      <ns0:c r="A95" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B95" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDebugLogging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C95" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D95" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F95" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Enable verbose debug logging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="96">
-      <ns0:c r="A96" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B96" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionQuickTestTrigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C96" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D96" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F96" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Which trigger to simulate</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="97">
-      <ns0:c r="A97" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B97" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionQuickTestNow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C97" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D97" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F97" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Toggle to fire the selected trigger once</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="98"/>
-    <ns0:row r="99">
-      <ns0:c r="A99" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryStatistics</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="100">
-      <ns0:c r="A100" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryStatistics</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B100" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionResetStats</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C100" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D100" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F100" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Toggle to reset all statistics</ns0:t>
         </ns0:is>
@@ -3731,7 +3529,7 @@
     <ns0:row r="11">
       <ns0:c r="A11" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CustomDelayProvider</ns0:t>
+          <ns0:t>CustomDurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B11" s="4">
@@ -3741,32 +3539,32 @@
     <ns0:row r="12">
       <ns0:c r="A12" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CustomDurationProvider</ns0:t>
+          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B12" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="C12" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="13">
       <ns0:c r="A13" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CustomThirdPersonDistributionProvider</ns0:t>
+          <ns0:t>CustomTimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B13" s="4">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C13" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="14">
       <ns0:c r="A14" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CustomTimeScaleProvider</ns0:t>
+          <ns0:t>DurationPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B14" s="4">
@@ -3776,57 +3574,67 @@
     <ns0:row r="15">
       <ns0:c r="A15" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>DelayPresetProvider</ns0:t>
+          <ns0:t>DurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B15" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>9</ns0:v>
+      </ns0:c>
+      <ns0:c r="C15" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0.5s | 1.0s | 1.5s | 2.0s | 2.5s | 3.0s | 4.0s | 5.0s | 8.0s</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="16">
       <ns0:c r="A16" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>DurationPresetProvider</ns0:t>
+          <ns0:t>EasingCurveProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B16" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="C16" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="17">
       <ns0:c r="A17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>DurationProvider</ns0:t>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B17" s="4">
-        <ns0:v>9</ns0:v>
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="C17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>0.5s | 1.0s | 1.5s | 2.0s | 2.5s | 3.0s | 4.0s | 5.0s | 8.0s</ns0:t>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="18">
       <ns0:c r="A18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>EasingCurveProvider</ns0:t>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" s="4">
-        <ns0:v>5</ns0:v>
+        <ns0:v>3</ns0:v>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" s="4">
@@ -3834,112 +3642,82 @@
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t>MinEnemyGroupProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" s="4">
-        <ns0:v>3</ns0:v>
+        <ns0:v>4</ns0:v>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
       <ns0:c r="A21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t>PresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B21" s="4">
-        <ns0:v>4</ns0:v>
-      </ns0:c>
-      <ns0:c r="C21" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
       <ns0:c r="A22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>MinEnemyGroupProvider</ns0:t>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B22" s="4">
-        <ns0:v>4</ns0:v>
-      </ns0:c>
-      <ns0:c r="C22" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="23">
       <ns0:c r="A23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>PresetProvider</ns0:t>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B23" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="C23" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="24">
       <ns0:c r="A24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>QuickTestTriggerProvider</ns0:t>
+          <ns0:t>TimeScaleProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B24" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="C24" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B25" s="4">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C25" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="26">
-      <ns0:c r="A26" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TimeScaleProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B26" s="4">
-        <ns0:v>8</ns0:v>
-      </ns0:c>
-      <ns0:c r="C26" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="27">
-      <ns0:c r="A27" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerProfileProvider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B27" s="4">
         <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Transition improvements: preset control, percentage-based ramp, simplified curves
- Add Transition Preset dropdown to Preset Selection (controls all triggers)
- Change ramp time from hardcoded 0.25s to 20% of trigger duration
- Remove EaseIn/EaseOut options, keep only Off/Smoothstep/Linear
- Transition Preset syncs to per-trigger Transition dropdowns like other presets

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -453,57 +453,57 @@
       </ns0:c>
       <ns0:c r="B13" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionTransitionPreset</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C13" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D13" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F13" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Sets per-trigger transition curve. Off = instant, Smoothstep = smooth ramp, Linear = constant rate.</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="14">
+      <ns0:c r="A14" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryPresetSelection</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B14" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionTriggerProfile</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C13" t="inlineStr" s="8">
+      <ns0:c r="C14" t="inlineStr" s="8">
         <ns0:is>
           <ns0:t>Dropdown</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D13" t="inlineStr" s="4">
+      <ns0:c r="D14" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>All</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F13" t="inlineStr" s="4">
+      <ns0:c r="F14" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Which triggers are active. Selecting a profile updates the per-trigger toggles.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="14"/>
-    <ns0:row r="15">
-      <ns0:c r="A15" t="inlineStr" s="2">
+    <ns0:row r="15"/>
+    <ns0:row r="16">
+      <ns0:c r="A16" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="16">
-      <ns0:c r="A16" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B16" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C16" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D16" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F16" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -515,7 +515,7 @@
       </ns0:c>
       <ns0:c r="B17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerThrownImpactKill</ns0:t>
+          <ns0:t>TriggerBasicKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C17" t="inlineStr" s="6">
@@ -525,12 +525,12 @@
       </ns0:c>
       <ns0:c r="D17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -542,7 +542,7 @@
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerCriticalKill</ns0:t>
+          <ns0:t>TriggerThrownImpactKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C18" t="inlineStr" s="6">
@@ -552,12 +552,12 @@
       </ns0:c>
       <ns0:c r="D18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -569,7 +569,7 @@
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDismemberment</ns0:t>
+          <ns0:t>TriggerCriticalKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="6">
@@ -584,7 +584,7 @@
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -596,7 +596,7 @@
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDecapitation</ns0:t>
+          <ns0:t>TriggerDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="6">
@@ -611,7 +611,7 @@
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -623,7 +623,7 @@
       </ns0:c>
       <ns0:c r="B21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastEnemy</ns0:t>
+          <ns0:t>TriggerDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C21" t="inlineStr" s="6">
@@ -638,7 +638,7 @@
       </ns0:c>
       <ns0:c r="F21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -650,7 +650,7 @@
       </ns0:c>
       <ns0:c r="B22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastStand</ns0:t>
+          <ns0:t>TriggerLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C22" t="inlineStr" s="6">
@@ -665,7 +665,7 @@
       </ns0:c>
       <ns0:c r="F22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -677,27 +677,22 @@
       </ns0:c>
       <ns0:c r="B23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandThreshold</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C23" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>TriggerLastStand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C23" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E23" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -709,62 +704,62 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionLastStandThreshold</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C24" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D24" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>15%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E24" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F24" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="25">
+      <ns0:c r="A25" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B25" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>TriggerParry</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C24" t="inlineStr" s="6">
+      <ns0:c r="C25" t="inlineStr" s="6">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D24" t="inlineStr" s="4">
+      <ns0:c r="D25" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F24" t="inlineStr" s="4">
+      <ns0:c r="F25" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Trigger on successful weapon deflections</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="25"/>
-    <ns0:row r="26">
-      <ns0:c r="A26" t="inlineStr" s="2">
+    <ns0:row r="26"/>
+    <ns0:row r="27">
+      <ns0:c r="A27" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="27">
-      <ns0:c r="A27" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B27" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCameraDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C27" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D27" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>3m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E27" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F27" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -776,22 +771,27 @@
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C28" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionCameraDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C28" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>3m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E28" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize distance per killcam</ns0:t>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -803,27 +803,22 @@
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCameraHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C29" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionRandomizeDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C29" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E29" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Randomize distance per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -835,22 +830,27 @@
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C30" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionCameraHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C30" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>1.5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E30" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize height per killcam</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -862,60 +862,62 @@
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionRandomizeHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C31" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D31" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F31" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Randomize height per killcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="32">
+      <ns0:c r="A32" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B32" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionOrbitSpeed</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C31" t="inlineStr" s="7">
+      <ns0:c r="C32" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D31" t="inlineStr" s="4">
+      <ns0:c r="D32" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Slow</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E31" t="inlineStr" s="4">
+      <ns0:c r="E32" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>None | Slow | Medium | Fast</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F31" t="inlineStr" s="4">
+      <ns0:c r="F32" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Camera rotation speed (0 for static)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="32"/>
-    <ns0:row r="33">
-      <ns0:c r="A33" t="inlineStr" s="2">
+    <ns0:row r="33"/>
+    <ns0:row r="34">
+      <ns0:c r="A34" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="34">
-      <ns0:c r="A34" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B34" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionBasicChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C34" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D34" s="4">
-        <ns0:v>0.25</ns0:v>
-      </ns0:c>
-      <ns0:c r="F34" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -927,7 +929,7 @@
       </ns0:c>
       <ns0:c r="B35" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicTimeScale</ns0:t>
+          <ns0:t>OptionBasicChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C35" t="inlineStr" s="7">
@@ -936,11 +938,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D35" s="4">
-        <ns0:v>0.28</ns0:v>
+        <ns0:v>0.25</ns0:v>
       </ns0:c>
       <ns0:c r="F35" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -952,7 +954,7 @@
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicDuration</ns0:t>
+          <ns0:t>OptionBasicTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C36" t="inlineStr" s="7">
@@ -961,11 +963,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D36" s="4">
-        <ns0:v>2.5</ns0:v>
+        <ns0:v>0.28</ns0:v>
       </ns0:c>
       <ns0:c r="F36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -977,7 +979,7 @@
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicCooldown</ns0:t>
+          <ns0:t>OptionBasicDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C37" t="inlineStr" s="7">
@@ -986,16 +988,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D37" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E37" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>2.5</ns0:v>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1007,27 +1004,25 @@
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C38" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D38" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionBasicCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C38" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D38" s="4">
+        <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="E38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1039,60 +1034,67 @@
       </ns0:c>
       <ns0:c r="B39" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionBasicTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C39" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D39" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E39" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F39" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="40">
+      <ns0:c r="A40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B40" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionBasicThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C39" t="inlineStr" s="7">
+      <ns0:c r="C40" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D39" t="inlineStr" s="4">
+      <ns0:c r="D40" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E39" t="inlineStr" s="4">
+      <ns0:c r="E40" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F39" t="inlineStr" s="4">
+      <ns0:c r="F40" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="40"/>
-    <ns0:row r="41">
-      <ns0:c r="A41" t="inlineStr" s="2">
+    <ns0:row r="41"/>
+    <ns0:row r="42">
+      <ns0:c r="A42" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="42">
-      <ns0:c r="A42" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B42" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCriticalChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C42" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D42" s="4">
-        <ns0:v>0.75</ns0:v>
-      </ns0:c>
-      <ns0:c r="F42" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1104,7 +1106,7 @@
       </ns0:c>
       <ns0:c r="B43" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalTimeScale</ns0:t>
+          <ns0:t>OptionCriticalChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C43" t="inlineStr" s="7">
@@ -1113,11 +1115,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D43" s="4">
-        <ns0:v>0.25</ns0:v>
+        <ns0:v>0.75</ns0:v>
       </ns0:c>
       <ns0:c r="F43" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1129,7 +1131,7 @@
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalDuration</ns0:t>
+          <ns0:t>OptionCriticalTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="7">
@@ -1138,11 +1140,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D44" s="4">
-        <ns0:v>3.0</ns0:v>
+        <ns0:v>0.25</ns0:v>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1154,7 +1156,7 @@
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalCooldown</ns0:t>
+          <ns0:t>OptionCriticalDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C45" t="inlineStr" s="7">
@@ -1163,16 +1165,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D45" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E45" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>3.0</ns0:v>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1184,27 +1181,25 @@
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C46" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D46" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionCriticalCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C46" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D46" s="4">
+        <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="E46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1216,60 +1211,67 @@
       </ns0:c>
       <ns0:c r="B47" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionCriticalTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C47" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D47" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E47" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F47" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="48">
+      <ns0:c r="A48" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B48" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionCriticalThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C47" t="inlineStr" s="7">
+      <ns0:c r="C48" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D47" t="inlineStr" s="4">
+      <ns0:c r="D48" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E47" t="inlineStr" s="4">
+      <ns0:c r="E48" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F47" t="inlineStr" s="4">
+      <ns0:c r="F48" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="48"/>
-    <ns0:row r="49">
-      <ns0:c r="A49" t="inlineStr" s="2">
+    <ns0:row r="49"/>
+    <ns0:row r="50">
+      <ns0:c r="A50" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="50">
-      <ns0:c r="A50" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B50" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDismemberChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C50" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D50" s="4">
-        <ns0:v>0.3</ns0:v>
-      </ns0:c>
-      <ns0:c r="F50" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1281,7 +1283,7 @@
       </ns0:c>
       <ns0:c r="B51" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberTimeScale</ns0:t>
+          <ns0:t>OptionDismemberChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C51" t="inlineStr" s="7">
@@ -1294,7 +1296,7 @@
       </ns0:c>
       <ns0:c r="F51" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1306,7 +1308,7 @@
       </ns0:c>
       <ns0:c r="B52" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberDuration</ns0:t>
+          <ns0:t>OptionDismemberTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C52" t="inlineStr" s="7">
@@ -1315,11 +1317,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D52" s="4">
-        <ns0:v>2.0</ns0:v>
+        <ns0:v>0.3</ns0:v>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1331,7 +1333,7 @@
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberCooldown</ns0:t>
+          <ns0:t>OptionDismemberDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C53" t="inlineStr" s="7">
@@ -1340,16 +1342,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D53" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E53" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>2.0</ns0:v>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1361,27 +1358,25 @@
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C54" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D54" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionDismemberCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C54" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D54" s="4">
+        <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="E54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1393,60 +1388,67 @@
       </ns0:c>
       <ns0:c r="B55" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionDismemberTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C55" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D55" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E55" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F55" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="56">
+      <ns0:c r="A56" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B56" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionDismemberThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C55" t="inlineStr" s="7">
+      <ns0:c r="C56" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D55" t="inlineStr" s="4">
+      <ns0:c r="D56" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E55" t="inlineStr" s="4">
+      <ns0:c r="E56" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F55" t="inlineStr" s="4">
+      <ns0:c r="F56" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="56"/>
-    <ns0:row r="57">
-      <ns0:c r="A57" t="inlineStr" s="2">
+    <ns0:row r="57"/>
+    <ns0:row r="58">
+      <ns0:c r="A58" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="58">
-      <ns0:c r="A58" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B58" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDecapChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C58" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D58" s="4">
-        <ns0:v>0.9</ns0:v>
-      </ns0:c>
-      <ns0:c r="F58" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1458,7 +1460,7 @@
       </ns0:c>
       <ns0:c r="B59" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapTimeScale</ns0:t>
+          <ns0:t>OptionDecapChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C59" t="inlineStr" s="7">
@@ -1467,11 +1469,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D59" s="4">
-        <ns0:v>0.23</ns0:v>
+        <ns0:v>0.9</ns0:v>
       </ns0:c>
       <ns0:c r="F59" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1483,7 +1485,7 @@
       </ns0:c>
       <ns0:c r="B60" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapDuration</ns0:t>
+          <ns0:t>OptionDecapTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C60" t="inlineStr" s="7">
@@ -1492,11 +1494,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D60" s="4">
-        <ns0:v>3.25</ns0:v>
+        <ns0:v>0.23</ns0:v>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1508,7 +1510,7 @@
       </ns0:c>
       <ns0:c r="B61" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapCooldown</ns0:t>
+          <ns0:t>OptionDecapDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C61" t="inlineStr" s="7">
@@ -1517,16 +1519,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D61" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E61" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>3.25</ns0:v>
       </ns0:c>
       <ns0:c r="F61" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1538,27 +1535,25 @@
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C62" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D62" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionDecapCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C62" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D62" s="4">
+        <ns0:v>10</ns0:v>
       </ns0:c>
       <ns0:c r="E62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1570,60 +1565,67 @@
       </ns0:c>
       <ns0:c r="B63" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionDecapTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C63" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D63" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E63" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F63" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="64">
+      <ns0:c r="A64" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B64" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionDecapThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C63" t="inlineStr" s="7">
+      <ns0:c r="C64" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D63" t="inlineStr" s="4">
+      <ns0:c r="D64" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E63" t="inlineStr" s="4">
+      <ns0:c r="E64" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F63" t="inlineStr" s="4">
+      <ns0:c r="F64" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="64"/>
-    <ns0:row r="65">
-      <ns0:c r="A65" t="inlineStr" s="2">
+    <ns0:row r="65"/>
+    <ns0:row r="66">
+      <ns0:c r="A66" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="66">
-      <ns0:c r="A66" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B66" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastEnemyChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C66" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D66" s="4">
-        <ns0:v>1.0</ns0:v>
-      </ns0:c>
-      <ns0:c r="F66" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1635,7 +1637,7 @@
       </ns0:c>
       <ns0:c r="B67" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
+          <ns0:t>OptionLastEnemyChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C67" t="inlineStr" s="7">
@@ -1644,11 +1646,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D67" s="4">
-        <ns0:v>0.26</ns0:v>
+        <ns0:v>1.0</ns0:v>
       </ns0:c>
       <ns0:c r="F67" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1660,7 +1662,7 @@
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyDuration</ns0:t>
+          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C68" t="inlineStr" s="7">
@@ -1669,11 +1671,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D68" s="4">
-        <ns0:v>2.75</ns0:v>
+        <ns0:v>0.26</ns0:v>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1685,7 +1687,7 @@
       </ns0:c>
       <ns0:c r="B69" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyCooldown</ns0:t>
+          <ns0:t>OptionLastEnemyDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C69" t="inlineStr" s="7">
@@ -1694,16 +1696,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D69" s="4">
-        <ns0:v>30</ns0:v>
-      </ns0:c>
-      <ns0:c r="E69" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>2.75</ns0:v>
       </ns0:c>
       <ns0:c r="F69" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1715,27 +1712,25 @@
       </ns0:c>
       <ns0:c r="B70" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C70" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D70" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionLastEnemyCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C70" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D70" s="4">
+        <ns0:v>30</ns0:v>
       </ns0:c>
       <ns0:c r="E70" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>0s</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F70" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1747,60 +1742,67 @@
       </ns0:c>
       <ns0:c r="B71" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionLastEnemyTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C71" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="72">
+      <ns0:c r="A72" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B72" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C71" t="inlineStr" s="7">
+      <ns0:c r="C72" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D71" t="inlineStr" s="4">
+      <ns0:c r="D72" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E71" t="inlineStr" s="4">
+      <ns0:c r="E72" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F71" t="inlineStr" s="4">
+      <ns0:c r="F72" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="72"/>
-    <ns0:row r="73">
-      <ns0:c r="A73" t="inlineStr" s="2">
+    <ns0:row r="73"/>
+    <ns0:row r="74">
+      <ns0:c r="A74" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="74">
-      <ns0:c r="A74" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B74" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastStandTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C74" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D74" s="4">
-        <ns0:v>0.30</ns0:v>
-      </ns0:c>
-      <ns0:c r="F74" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1812,7 +1814,7 @@
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandDuration</ns0:t>
+          <ns0:t>OptionLastStandTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="7">
@@ -1821,11 +1823,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D75" s="4">
-        <ns0:v>4.0</ns0:v>
+        <ns0:v>0.30</ns0:v>
       </ns0:c>
       <ns0:c r="F75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1837,7 +1839,7 @@
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandCooldown</ns0:t>
+          <ns0:t>OptionLastStandDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C76" t="inlineStr" s="7">
@@ -1846,16 +1848,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D76" s="4">
-        <ns0:v>90</ns0:v>
-      </ns0:c>
-      <ns0:c r="E76" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>4.0</ns0:v>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1867,60 +1864,65 @@
       </ns0:c>
       <ns0:c r="B77" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionLastStandCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C77" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D77" s="4">
+        <ns0:v>90</ns0:v>
+      </ns0:c>
+      <ns0:c r="E77" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F77" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="78">
+      <ns0:c r="A78" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B78" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionLastStandTransition</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C77" t="inlineStr" s="8">
+      <ns0:c r="C78" t="inlineStr" s="8">
         <ns0:is>
           <ns0:t>Dropdown</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D77" t="inlineStr" s="4">
+      <ns0:c r="D78" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Smoothstep</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E77" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F77" t="inlineStr" s="4">
+      <ns0:c r="E78" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F78" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="78"/>
-    <ns0:row r="79">
-      <ns0:c r="A79" t="inlineStr" s="2">
+    <ns0:row r="79"/>
+    <ns0:row r="80">
+      <ns0:c r="A80" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="80">
-      <ns0:c r="A80" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B80" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionParryChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C80" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D80" s="4">
-        <ns0:v>0.5</ns0:v>
-      </ns0:c>
-      <ns0:c r="F80" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1932,7 +1934,7 @@
       </ns0:c>
       <ns0:c r="B81" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryTimeScale</ns0:t>
+          <ns0:t>OptionParryChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C81" t="inlineStr" s="7">
@@ -1941,11 +1943,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D81" s="4">
-        <ns0:v>0.34</ns0:v>
+        <ns0:v>0.5</ns0:v>
       </ns0:c>
       <ns0:c r="F81" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1957,7 +1959,7 @@
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryDuration</ns0:t>
+          <ns0:t>OptionParryTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="7">
@@ -1966,11 +1968,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D82" s="4">
-        <ns0:v>1.5</ns0:v>
+        <ns0:v>0.34</ns0:v>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1982,7 +1984,7 @@
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryCooldown</ns0:t>
+          <ns0:t>OptionParryDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="7">
@@ -1991,16 +1993,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D83" s="4">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="E83" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>1.5</ns0:v>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2012,62 +2009,65 @@
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionParryCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C84" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D84" s="4">
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="E84" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F84" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="85">
+      <ns0:c r="A85" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B85" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionParryTransition</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C84" t="inlineStr" s="8">
+      <ns0:c r="C85" t="inlineStr" s="8">
         <ns0:is>
           <ns0:t>Dropdown</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D84" t="inlineStr" s="4">
+      <ns0:c r="D85" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Smoothstep</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="E84" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F84" t="inlineStr" s="4">
+      <ns0:c r="E85" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F85" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="85"/>
-    <ns0:row r="86">
-      <ns0:c r="A86" t="inlineStr" s="2">
+    <ns0:row r="86"/>
+    <ns0:row r="87">
+      <ns0:c r="A87" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="87">
-      <ns0:c r="A87" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B87" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDebugLogging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C87" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D87" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F87" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2079,22 +2079,22 @@
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionQuickTestTrigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C88" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
+          <ns0:t>OptionDebugLogging</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C88" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Which trigger to simulate</ns0:t>
+          <ns0:t>Enable verbose debug logging</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2106,55 +2106,82 @@
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>OptionQuickTestTrigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C89" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D89" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F89" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Which trigger to simulate</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="90">
+      <ns0:c r="A90" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B90" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>OptionQuickTestNow</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C89" t="inlineStr" s="6">
+      <ns0:c r="C90" t="inlineStr" s="6">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D89" t="inlineStr" s="4">
+      <ns0:c r="D90" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F89" t="inlineStr" s="4">
+      <ns0:c r="F90" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Toggle to fire the selected trigger once</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="90"/>
-    <ns0:row r="91">
-      <ns0:c r="A91" t="inlineStr" s="2">
+    <ns0:row r="91"/>
+    <ns0:row r="92">
+      <ns0:c r="A92" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="92">
-      <ns0:c r="A92" t="inlineStr" s="4">
+    <ns0:row r="93">
+      <ns0:c r="A93" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B92" t="inlineStr" s="4">
+      <ns0:c r="B93" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>OptionResetStats</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C92" t="inlineStr" s="6">
+      <ns0:c r="C93" t="inlineStr" s="6">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D92" t="inlineStr" s="4">
+      <ns0:c r="D93" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F92" t="inlineStr" s="4">
+      <ns0:c r="F93" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Toggle to reset all statistics</ns0:t>
         </ns0:is>
@@ -3593,11 +3620,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="B16" s="4">
-        <ns0:v>5</ns0:v>
+        <ns0:v>3</ns0:v>
       </ns0:c>
       <ns0:c r="C16" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear | Ease In | Ease Out</ns0:t>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -3714,10 +3741,20 @@
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>TransitionPresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B25" s="4">
+        <ns0:v>0</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="26">
+      <ns0:c r="A26" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B25" s="4">
+      <ns0:c r="B26" s="4">
         <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Rename 'Standard' preset option to 'Default' across all presets
Consistent naming: Intensity, Chance, Cooldown, and Duration presets
now use 'Default' instead of 'Standard' for the middle/balanced option.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -355,12 +355,12 @@
       </ns0:c>
       <ns0:c r="D9" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Standard</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F9" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Intensity profile. Subtle = brief, Standard = default, Dramatic = stronger, Cinematic = dramatic, Epic = extreme</ns0:t>
+          <ns0:t>Intensity profile. Subtle = brief, Default = balanced, Dramatic = stronger, Cinematic = dramatic, Epic = extreme</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -409,7 +409,7 @@
       </ns0:c>
       <ns0:c r="D11" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Standard</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F11" t="inlineStr" s="4">
@@ -436,7 +436,7 @@
       </ns0:c>
       <ns0:c r="D12" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Standard</ns0:t>
+          <ns0:t>Default</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F12" t="inlineStr" s="4">

</xml_diff>

<commit_message>
Polish: add instant debug log, clarify transition tooltips
- Add debug log when instant transition applies time scale
- Update per-trigger transition tooltips to mention 20% ramp duration

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -1054,7 +1054,7 @@
       </ns0:c>
       <ns0:c r="F39" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1231,7 +1231,7 @@
       </ns0:c>
       <ns0:c r="F47" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1408,7 +1408,7 @@
       </ns0:c>
       <ns0:c r="F55" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1585,7 +1585,7 @@
       </ns0:c>
       <ns0:c r="F63" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1762,7 +1762,7 @@
       </ns0:c>
       <ns0:c r="F71" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1914,7 +1914,7 @@
       </ns0:c>
       <ns0:c r="F78" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -2059,7 +2059,7 @@
       </ns0:c>
       <ns0:c r="F85" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Curve shape for ramping into slow-mo (Off = instant)</ns0:t>
+          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Add damage type multipliers (Pierce/Slash/Blunt) and intensity scaling
- Add DamageMultipliers category with Pierce, Slash, Blunt multipliers (0.5x-2.0x)
- Add Intensity Scaling toggle and Max Intensity Multiplier option
- Update TriggerSlow to accept DamageType and intensity parameters
- Apply combined multiplier to timeScale (higher mult = lower timeScale = more intense)
- Extract damageType from CollisionInstance.damageStruct
- Calculate intensity from impactVelocity magnitude (normalized 0-1)
- Add debug logging for multiplier values when enabled
- Regenerate MENU_MOCK.xlsx with new options
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -503,100 +503,94 @@
     <ns0:row r="16">
       <ns0:c r="A16" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
+          <ns0:t>CategoryDamageMultipliers</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="17">
       <ns0:c r="A17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
+          <ns0:t>CategoryDamageMultipliers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C17" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D17" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionPierceMultiplier</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C17" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D17" s="4">
+        <ns0:v>1.0</ns0:v>
       </ns0:c>
       <ns0:c r="F17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
+          <ns0:t>Multiplier for piercing damage (stabs). Higher = more intense slow-mo.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="18">
       <ns0:c r="A18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
+          <ns0:t>CategoryDamageMultipliers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerThrownImpactKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C18" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D18" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionSlashMultiplier</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C18" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D18" s="4">
+        <ns0:v>1.0</ns0:v>
       </ns0:c>
       <ns0:c r="F18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
+          <ns0:t>Multiplier for slashing damage (cuts). Higher = more intense slow-mo.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
+          <ns0:t>CategoryDamageMultipliers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerCriticalKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C19" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D19" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionBluntMultiplier</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C19" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D19" s="4">
+        <ns0:v>1.0</ns0:v>
       </ns0:c>
       <ns0:c r="F19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
+          <ns0:t>Multiplier for blunt damage (impacts). Higher = more intense slow-mo.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
+          <ns0:t>CategoryDamageMultipliers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDismemberment</ns0:t>
+          <ns0:t>OptionIntensityScalingEnabled</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="6">
@@ -606,93 +600,45 @@
       </ns0:c>
       <ns0:c r="D20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Scale slow-mo intensity based on impact force. Off by default.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
       <ns0:c r="A21" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryDamageMultipliers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B21" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionIntensityScalingMax</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C21" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D21" s="4">
+        <ns0:v>1.5</ns0:v>
+      </ns0:c>
+      <ns0:c r="F21" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Maximum multiplier at full intensity (min is always 1.0x).</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="22"/>
+    <ns0:row r="23">
+      <ns0:c r="A23" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B21" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerDecapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C21" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D21" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F21" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="22">
-      <ns0:c r="A22" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B22" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerLastEnemy</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C22" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D22" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F22" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="23">
-      <ns0:c r="A23" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B23" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C23" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D23" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F23" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -704,27 +650,22 @@
       </ns0:c>
       <ns0:c r="B24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandThreshold</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C24" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C24" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E24" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -736,7 +677,7 @@
       </ns0:c>
       <ns0:c r="B25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerParry</ns0:t>
+          <ns0:t>TriggerThrownImpactKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C25" t="inlineStr" s="6">
@@ -746,64 +687,105 @@
       </ns0:c>
       <ns0:c r="D25" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F25" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="26">
+      <ns0:c r="A26" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B26" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerCriticalKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C26" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D26" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F25" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Trigger on successful weapon deflections</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="26"/>
+      <ns0:c r="F26" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="27">
-      <ns0:c r="A27" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
+      <ns0:c r="A27" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B27" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C27" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D27" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F27" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="28">
       <ns0:c r="A28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCameraDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C28" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>TriggerDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C28" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>3m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E28" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="29">
       <ns0:c r="A29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeDistance</ns0:t>
+          <ns0:t>TriggerLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C29" t="inlineStr" s="6">
@@ -813,103 +795,98 @@
       </ns0:c>
       <ns0:c r="D29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize distance per killcam</ns0:t>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="30">
       <ns0:c r="A30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCameraHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C30" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>TriggerLastStand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C30" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1.5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E30" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Height offset</ns0:t>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="31">
       <ns0:c r="A31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C31" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionLastStandThreshold</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C31" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>15%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E31" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize height per killcam</ns0:t>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="32">
       <ns0:c r="A32" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
+          <ns0:t>CategoryTriggers</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B32" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionOrbitSpeed</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C32" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>TriggerParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C32" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D32" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Slow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E32" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F32" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
+          <ns0:t>Trigger on successful weapon deflections</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -917,19 +894,19 @@
     <ns0:row r="34">
       <ns0:c r="A34" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="35">
       <ns0:c r="A35" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B35" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicChance</ns0:t>
+          <ns0:t>OptionCameraDistance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C35" t="inlineStr" s="7">
@@ -937,49 +914,58 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D35" s="4">
-        <ns0:v>0.25</ns0:v>
+      <ns0:c r="D35" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>3m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E35" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F35" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="36">
       <ns0:c r="A36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C36" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D36" s="4">
-        <ns0:v>0.28</ns0:v>
+          <ns0:t>OptionRandomizeDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C36" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D36" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F36" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Randomize distance per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="37">
       <ns0:c r="A37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicDuration</ns0:t>
+          <ns0:t>OptionCameraHeight</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C37" t="inlineStr" s="7">
@@ -987,126 +973,123 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D37" s="4">
-        <ns0:v>2.5</ns0:v>
+      <ns0:c r="D37" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1.5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E37" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F37" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="38">
       <ns0:c r="A38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
+          <ns0:t>CategoryKillcam</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C38" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D38" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E38" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>OptionRandomizeHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C38" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D38" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Randomize height per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="39">
       <ns0:c r="A39" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B39" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionOrbitSpeed</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C39" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D39" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Slow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E39" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F39" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="40"/>
+    <ns0:row r="41">
+      <ns0:c r="A41" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B39" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionBasicTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C39" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D39" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E39" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F39" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="40">
-      <ns0:c r="A40" t="inlineStr" s="4">
+    </ns0:row>
+    <ns0:row r="42">
+      <ns0:c r="A42" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B40" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionBasicThirdPerson</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C40" t="inlineStr" s="7">
+      <ns0:c r="B42" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionBasicChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C42" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D40" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E40" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F40" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="41"/>
-    <ns0:row r="42">
-      <ns0:c r="A42" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
+      <ns0:c r="D42" s="4">
+        <ns0:v>0.25</ns0:v>
+      </ns0:c>
+      <ns0:c r="F42" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="43">
       <ns0:c r="A43" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B43" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalChance</ns0:t>
+          <ns0:t>OptionBasicTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C43" t="inlineStr" s="7">
@@ -1115,23 +1098,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D43" s="4">
-        <ns0:v>0.75</ns0:v>
+        <ns0:v>0.28</ns0:v>
       </ns0:c>
       <ns0:c r="F43" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="44">
       <ns0:c r="A44" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B44" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalTimeScale</ns0:t>
+          <ns0:t>OptionBasicDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C44" t="inlineStr" s="7">
@@ -1140,23 +1123,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D44" s="4">
-        <ns0:v>0.25</ns0:v>
+        <ns0:v>2.5</ns0:v>
       </ns0:c>
       <ns0:c r="F44" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="45">
       <ns0:c r="A45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalDuration</ns0:t>
+          <ns0:t>OptionBasicCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C45" t="inlineStr" s="7">
@@ -1165,125 +1148,125 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D45" s="4">
-        <ns0:v>3.0</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E45" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="46">
       <ns0:c r="A46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
+          <ns0:t>CategoryCustomBasic</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C46" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D46" s="4">
-        <ns0:v>10</ns0:v>
+          <ns0:t>OptionBasicTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C46" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D46" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="47">
       <ns0:c r="A47" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B47" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionBasicThirdPerson</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C47" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D47" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E47" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F47" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="48"/>
+    <ns0:row r="49">
+      <ns0:c r="A49" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B47" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCriticalTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C47" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D47" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E47" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F47" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="48">
-      <ns0:c r="A48" t="inlineStr" s="4">
+    </ns0:row>
+    <ns0:row r="50">
+      <ns0:c r="A50" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B48" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCriticalThirdPerson</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C48" t="inlineStr" s="7">
+      <ns0:c r="B50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCriticalChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C50" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D48" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E48" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F48" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="49"/>
-    <ns0:row r="50">
-      <ns0:c r="A50" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+      <ns0:c r="D50" s="4">
+        <ns0:v>0.75</ns0:v>
+      </ns0:c>
+      <ns0:c r="F50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="51">
       <ns0:c r="A51" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B51" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberChance</ns0:t>
+          <ns0:t>OptionCriticalTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C51" t="inlineStr" s="7">
@@ -1292,23 +1275,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D51" s="4">
-        <ns0:v>0.3</ns0:v>
+        <ns0:v>0.25</ns0:v>
       </ns0:c>
       <ns0:c r="F51" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="52">
       <ns0:c r="A52" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B52" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberTimeScale</ns0:t>
+          <ns0:t>OptionCriticalDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C52" t="inlineStr" s="7">
@@ -1317,23 +1300,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D52" s="4">
-        <ns0:v>0.3</ns0:v>
+        <ns0:v>3.0</ns0:v>
       </ns0:c>
       <ns0:c r="F52" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="53">
       <ns0:c r="A53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberDuration</ns0:t>
+          <ns0:t>OptionCriticalCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C53" t="inlineStr" s="7">
@@ -1342,125 +1325,125 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D53" s="4">
-        <ns0:v>2.0</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E53" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="54">
       <ns0:c r="A54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDismemberment</ns0:t>
+          <ns0:t>CategoryCustomCritical</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDismemberCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C54" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D54" s="4">
-        <ns0:v>10</ns0:v>
+          <ns0:t>OptionCriticalTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C54" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D54" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="55">
       <ns0:c r="A55" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B55" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCriticalThirdPerson</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C55" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D55" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E55" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F55" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="56"/>
+    <ns0:row r="57">
+      <ns0:c r="A57" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B55" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDismemberTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C55" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D55" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E55" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F55" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="56">
-      <ns0:c r="A56" t="inlineStr" s="4">
+    </ns0:row>
+    <ns0:row r="58">
+      <ns0:c r="A58" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B56" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDismemberThirdPerson</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C56" t="inlineStr" s="7">
+      <ns0:c r="B58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDismemberChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C58" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D56" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E56" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F56" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="57"/>
-    <ns0:row r="58">
-      <ns0:c r="A58" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+      <ns0:c r="D58" s="4">
+        <ns0:v>0.3</ns0:v>
+      </ns0:c>
+      <ns0:c r="F58" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="59">
       <ns0:c r="A59" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B59" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapChance</ns0:t>
+          <ns0:t>OptionDismemberTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C59" t="inlineStr" s="7">
@@ -1469,23 +1452,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D59" s="4">
-        <ns0:v>0.9</ns0:v>
+        <ns0:v>0.3</ns0:v>
       </ns0:c>
       <ns0:c r="F59" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="60">
       <ns0:c r="A60" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B60" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapTimeScale</ns0:t>
+          <ns0:t>OptionDismemberDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C60" t="inlineStr" s="7">
@@ -1494,23 +1477,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D60" s="4">
-        <ns0:v>0.23</ns0:v>
+        <ns0:v>2.0</ns0:v>
       </ns0:c>
       <ns0:c r="F60" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="61">
       <ns0:c r="A61" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B61" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapDuration</ns0:t>
+          <ns0:t>OptionDismemberCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C61" t="inlineStr" s="7">
@@ -1519,125 +1502,125 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D61" s="4">
-        <ns0:v>3.25</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E61" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F61" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="62">
       <ns0:c r="A62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomDecapitation</ns0:t>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDecapCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C62" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D62" s="4">
-        <ns0:v>10</ns0:v>
+          <ns0:t>OptionDismemberTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C62" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D62" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F62" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="63">
       <ns0:c r="A63" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryCustomDismemberment</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B63" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDismemberThirdPerson</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C63" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D63" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E63" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F63" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="64"/>
+    <ns0:row r="65">
+      <ns0:c r="A65" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B63" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDecapTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C63" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D63" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E63" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F63" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="64">
-      <ns0:c r="A64" t="inlineStr" s="4">
+    </ns0:row>
+    <ns0:row r="66">
+      <ns0:c r="A66" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B64" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionDecapThirdPerson</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C64" t="inlineStr" s="7">
+      <ns0:c r="B66" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDecapChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C66" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D64" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E64" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F64" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="65"/>
-    <ns0:row r="66">
-      <ns0:c r="A66" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+      <ns0:c r="D66" s="4">
+        <ns0:v>0.9</ns0:v>
+      </ns0:c>
+      <ns0:c r="F66" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="67">
       <ns0:c r="A67" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B67" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyChance</ns0:t>
+          <ns0:t>OptionDecapTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C67" t="inlineStr" s="7">
@@ -1646,23 +1629,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D67" s="4">
-        <ns0:v>1.0</ns0:v>
+        <ns0:v>0.23</ns0:v>
       </ns0:c>
       <ns0:c r="F67" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="68">
       <ns0:c r="A68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
+          <ns0:t>OptionDecapDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C68" t="inlineStr" s="7">
@@ -1671,23 +1654,23 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D68" s="4">
-        <ns0:v>0.26</ns0:v>
+        <ns0:v>3.25</ns0:v>
       </ns0:c>
       <ns0:c r="F68" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Time scale</ns0:t>
+          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="69">
       <ns0:c r="A69" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B69" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyDuration</ns0:t>
+          <ns0:t>OptionDecapCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C69" t="inlineStr" s="7">
@@ -1696,125 +1679,125 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D69" s="4">
-        <ns0:v>2.75</ns0:v>
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E69" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="F69" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Duration</ns0:t>
+          <ns0:t>Cooldown</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="70">
       <ns0:c r="A70" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B70" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastEnemyCooldown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C70" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D70" s="4">
-        <ns0:v>30</ns0:v>
+          <ns0:t>OptionDecapTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C70" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D70" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
       </ns0:c>
       <ns0:c r="E70" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>0s</ns0:t>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F70" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="71">
       <ns0:c r="A71" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryCustomDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDecapThirdPerson</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C71" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F71" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="72"/>
+    <ns0:row r="73">
+      <ns0:c r="A73" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B71" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastEnemyTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C71" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D71" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E71" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F71" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="72">
-      <ns0:c r="A72" t="inlineStr" s="4">
+    </ns0:row>
+    <ns0:row r="74">
+      <ns0:c r="A74" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B72" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C72" t="inlineStr" s="7">
+      <ns0:c r="B74" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastEnemyChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C74" t="inlineStr" s="7">
         <ns0:is>
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D72" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E72" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F72" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="73"/>
-    <ns0:row r="74">
-      <ns0:c r="A74" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+      <ns0:c r="D74" s="4">
+        <ns0:v>1.0</ns0:v>
+      </ns0:c>
+      <ns0:c r="F74" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="75">
       <ns0:c r="A75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B75" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandTimeScale</ns0:t>
+          <ns0:t>OptionLastEnemyTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C75" t="inlineStr" s="7">
@@ -1823,7 +1806,7 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D75" s="4">
-        <ns0:v>0.30</ns0:v>
+        <ns0:v>0.26</ns0:v>
       </ns0:c>
       <ns0:c r="F75" t="inlineStr" s="4">
         <ns0:is>
@@ -1834,12 +1817,12 @@
     <ns0:row r="76">
       <ns0:c r="A76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B76" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandDuration</ns0:t>
+          <ns0:t>OptionLastEnemyDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C76" t="inlineStr" s="7">
@@ -1848,7 +1831,7 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D76" s="4">
-        <ns0:v>4.0</ns0:v>
+        <ns0:v>2.75</ns0:v>
       </ns0:c>
       <ns0:c r="F76" t="inlineStr" s="4">
         <ns0:is>
@@ -1859,12 +1842,12 @@
     <ns0:row r="77">
       <ns0:c r="A77" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomLastStand</ns0:t>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B77" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandCooldown</ns0:t>
+          <ns0:t>OptionLastEnemyCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C77" t="inlineStr" s="7">
@@ -1873,7 +1856,7 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D77" s="4">
-        <ns0:v>90</ns0:v>
+        <ns0:v>30</ns0:v>
       </ns0:c>
       <ns0:c r="E77" t="inlineStr" s="4">
         <ns0:is>
@@ -1889,77 +1872,84 @@
     <ns0:row r="78">
       <ns0:c r="A78" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B78" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastEnemyTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C78" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D78" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E78" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F78" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="79">
+      <ns0:c r="A79" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomLastEnemy</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B79" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastEnemyThirdPerson</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C79" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D79" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E79" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F79" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="80"/>
+    <ns0:row r="81">
+      <ns0:c r="A81" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomLastStand</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B78" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionLastStandTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C78" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D78" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E78" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F78" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="79"/>
-    <ns0:row r="80">
-      <ns0:c r="A80" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="81">
-      <ns0:c r="A81" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B81" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionParryChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C81" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D81" s="4">
-        <ns0:v>0.5</ns0:v>
-      </ns0:c>
-      <ns0:c r="F81" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="82">
       <ns0:c r="A82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B82" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryTimeScale</ns0:t>
+          <ns0:t>OptionLastStandTimeScale</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C82" t="inlineStr" s="7">
@@ -1968,7 +1958,7 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D82" s="4">
-        <ns0:v>0.34</ns0:v>
+        <ns0:v>0.30</ns0:v>
       </ns0:c>
       <ns0:c r="F82" t="inlineStr" s="4">
         <ns0:is>
@@ -1979,12 +1969,12 @@
     <ns0:row r="83">
       <ns0:c r="A83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B83" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryDuration</ns0:t>
+          <ns0:t>OptionLastStandDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C83" t="inlineStr" s="7">
@@ -1993,7 +1983,7 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D83" s="4">
-        <ns0:v>1.5</ns0:v>
+        <ns0:v>4.0</ns0:v>
       </ns0:c>
       <ns0:c r="F83" t="inlineStr" s="4">
         <ns0:is>
@@ -2004,12 +1994,12 @@
     <ns0:row r="84">
       <ns0:c r="A84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B84" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryCooldown</ns0:t>
+          <ns0:t>OptionLastStandCooldown</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C84" t="inlineStr" s="7">
@@ -2018,7 +2008,7 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D84" s="4">
-        <ns0:v>5</ns0:v>
+        <ns0:v>90</ns0:v>
       </ns0:c>
       <ns0:c r="E84" t="inlineStr" s="4">
         <ns0:is>
@@ -2034,12 +2024,12 @@
     <ns0:row r="85">
       <ns0:c r="A85" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryCustomParry</ns0:t>
+          <ns0:t>CategoryCustomLastStand</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B85" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionParryTransition</ns0:t>
+          <ns0:t>OptionLastStandTransition</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C85" t="inlineStr" s="8">
@@ -2067,121 +2057,266 @@
     <ns0:row r="87">
       <ns0:c r="A87" t="inlineStr" s="2">
         <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="88">
       <ns0:c r="A88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionDebugLogging</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C88" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D88" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionParryChance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C88" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D88" s="4">
+        <ns0:v>0.5</ns0:v>
       </ns0:c>
       <ns0:c r="F88" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Enable verbose debug logging</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="89">
       <ns0:c r="A89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>CategoryAdvanced</ns0:t>
+          <ns0:t>CategoryCustomParry</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionQuickTestTrigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C89" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D89" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionParryTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C89" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D89" s="4">
+        <ns0:v>0.34</ns0:v>
       </ns0:c>
       <ns0:c r="F89" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Which trigger to simulate</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="90">
       <ns0:c r="A90" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B90" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionParryDuration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C90" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D90" s="4">
+        <ns0:v>1.5</ns0:v>
+      </ns0:c>
+      <ns0:c r="F90" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="91">
+      <ns0:c r="A91" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B91" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionParryCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C91" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D91" s="4">
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="E91" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F91" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="92">
+      <ns0:c r="A92" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B92" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionParryTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C92" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D92" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E92" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F92" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="93"/>
+    <ns0:row r="94">
+      <ns0:c r="A94" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryAdvanced</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B90" t="inlineStr" s="4">
+    </ns0:row>
+    <ns0:row r="95">
+      <ns0:c r="A95" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B95" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionDebugLogging</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C95" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D95" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F95" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Enable verbose debug logging</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="96">
+      <ns0:c r="A96" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B96" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionQuickTestTrigger</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C96" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D96" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerBasicKill</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F96" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Which trigger to simulate</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="97">
+      <ns0:c r="A97" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryAdvanced</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B97" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>OptionQuickTestNow</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C90" t="inlineStr" s="6">
+      <ns0:c r="C97" t="inlineStr" s="6">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D90" t="inlineStr" s="4">
+      <ns0:c r="D97" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F90" t="inlineStr" s="4">
+      <ns0:c r="F97" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Toggle to fire the selected trigger once</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="91"/>
-    <ns0:row r="92">
-      <ns0:c r="A92" t="inlineStr" s="2">
+    <ns0:row r="98"/>
+    <ns0:row r="99">
+      <ns0:c r="A99" t="inlineStr" s="2">
         <ns0:is>
           <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
-    <ns0:row r="93">
-      <ns0:c r="A93" t="inlineStr" s="4">
+    <ns0:row r="100">
+      <ns0:c r="A100" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>CategoryStatistics</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B93" t="inlineStr" s="4">
+      <ns0:c r="B100" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>OptionResetStats</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="C93" t="inlineStr" s="6">
+      <ns0:c r="C100" t="inlineStr" s="6">
         <ns0:is>
           <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D93" t="inlineStr" s="4">
+      <ns0:c r="D100" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="F93" t="inlineStr" s="4">
+      <ns0:c r="F100" t="inlineStr" s="4">
         <ns0:is>
           <ns0:t>Toggle to reset all statistics</ns0:t>
         </ns0:is>
@@ -3591,7 +3726,7 @@
     <ns0:row r="14">
       <ns0:c r="A14" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>DurationPresetProvider</ns0:t>
+          <ns0:t>DamageMultiplierProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B14" s="4">
@@ -3601,67 +3736,57 @@
     <ns0:row r="15">
       <ns0:c r="A15" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>DurationProvider</ns0:t>
+          <ns0:t>DurationPresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B15" s="4">
-        <ns0:v>9</ns0:v>
-      </ns0:c>
-      <ns0:c r="C15" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0.5s | 1.0s | 1.5s | 2.0s | 2.5s | 3.0s | 4.0s | 5.0s | 8.0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="16">
       <ns0:c r="A16" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>EasingCurveProvider</ns0:t>
+          <ns0:t>DurationProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B16" s="4">
-        <ns0:v>3</ns0:v>
+        <ns0:v>9</ns0:v>
       </ns0:c>
       <ns0:c r="C16" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear</ns0:t>
+          <ns0:t>0.5s | 1.0s | 1.5s | 2.0s | 2.5s | 3.0s | 4.0s | 5.0s | 8.0s</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="17">
       <ns0:c r="A17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamDistanceProvider</ns0:t>
+          <ns0:t>EasingCurveProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B17" s="4">
-        <ns0:v>4</ns0:v>
+        <ns0:v>3</ns0:v>
       </ns0:c>
       <ns0:c r="C17" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="18">
       <ns0:c r="A18" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamHeightProvider</ns0:t>
+          <ns0:t>IntensityMaxProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B18" s="4">
-        <ns0:v>3</ns0:v>
-      </ns0:c>
-      <ns0:c r="C18" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="19">
       <ns0:c r="A19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
+          <ns0:t>KillcamDistanceProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B19" s="4">
@@ -3669,92 +3794,122 @@
       </ns0:c>
       <ns0:c r="C19" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="20">
       <ns0:c r="A20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>MinEnemyGroupProvider</ns0:t>
+          <ns0:t>KillcamHeightProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B20" s="4">
-        <ns0:v>4</ns0:v>
+        <ns0:v>3</ns0:v>
       </ns0:c>
       <ns0:c r="C20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="21">
       <ns0:c r="A21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>PresetProvider</ns0:t>
+          <ns0:t>KillcamOrbitSpeedProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B21" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>4</ns0:v>
+      </ns0:c>
+      <ns0:c r="C21" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="22">
       <ns0:c r="A22" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>QuickTestTriggerProvider</ns0:t>
+          <ns0:t>MinEnemyGroupProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B22" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>4</ns0:v>
+      </ns0:c>
+      <ns0:c r="C22" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1 (every kill) | 2 enemies | 3 enemies | 5 enemies</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="23">
       <ns0:c r="A23" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>ThresholdProvider</ns0:t>
+          <ns0:t>PresetProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B23" s="4">
-        <ns0:v>5</ns0:v>
-      </ns0:c>
-      <ns0:c r="C23" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="24">
       <ns0:c r="A24" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TimeScaleProvider</ns0:t>
+          <ns0:t>QuickTestTriggerProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B24" s="4">
-        <ns0:v>8</ns0:v>
-      </ns0:c>
-      <ns0:c r="C24" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
-        </ns0:is>
+        <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>
     <ns0:row r="25">
       <ns0:c r="A25" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TransitionPresetProvider</ns0:t>
+          <ns0:t>ThresholdProvider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="B25" s="4">
-        <ns0:v>0</ns0:v>
+        <ns0:v>5</ns0:v>
+      </ns0:c>
+      <ns0:c r="C25" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+        </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="26">
       <ns0:c r="A26" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>TimeScaleProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B26" s="4">
+        <ns0:v>8</ns0:v>
+      </ns0:c>
+      <ns0:c r="C26" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0.05x | 0.10x | 0.15x | 0.20x | 0.25x | 0.30x | 0.40x | 0.50x</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="27">
+      <ns0:c r="A27" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TransitionPresetProvider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B27" s="4">
+        <ns0:v>0</ns0:v>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="28">
+      <ns0:c r="A28" t="inlineStr" s="4">
+        <ns0:is>
           <ns0:t>TriggerProfileProvider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="B26" s="4">
+      <ns0:c r="B28" s="4">
         <ns0:v>0</ns0:v>
       </ns0:c>
     </ns0:row>

</xml_diff>

<commit_message>
Add elemental damage type multipliers (Energy/Fire/Lightning)
Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MENU_MOCK.xlsx
+++ b/MENU_MOCK.xlsx
@@ -590,22 +590,20 @@
       </ns0:c>
       <ns0:c r="B20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionIntensityScalingEnabled</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C20" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D20" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionEnergyMultiplier</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C20" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D20" s="4">
+        <ns0:v>1.0</ns0:v>
       </ns0:c>
       <ns0:c r="F20" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Scale slow-mo intensity based on impact force. Off by default.</ns0:t>
+          <ns0:t>Multiplier for energy damage. Higher = more intense slow-mo.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -617,7 +615,7 @@
       </ns0:c>
       <ns0:c r="B21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionIntensityScalingMax</ns0:t>
+          <ns0:t>OptionFireMultiplier</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C21" t="inlineStr" s="7">
@@ -626,100 +624,96 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D21" s="4">
-        <ns0:v>1.5</ns0:v>
+        <ns0:v>1.0</ns0:v>
       </ns0:c>
       <ns0:c r="F21" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Maximum multiplier at full intensity (min is always 1.0x).</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="22"/>
+          <ns0:t>Multiplier for fire damage. Higher = more intense slow-mo.</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="22">
+      <ns0:c r="A22" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryDamageMultipliers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B22" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLightningMultiplier</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C22" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D22" s="4">
+        <ns0:v>1.0</ns0:v>
+      </ns0:c>
+      <ns0:c r="F22" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Multiplier for lightning damage. Higher = more intense slow-mo.</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="23">
-      <ns0:c r="A23" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
+      <ns0:c r="A23" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryDamageMultipliers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B23" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionIntensityScalingEnabled</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C23" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D23" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F23" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Scale slow-mo intensity based on impact force. Off by default.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="24">
       <ns0:c r="A24" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryDamageMultipliers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B24" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionIntensityScalingMax</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C24" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D24" s="4">
+        <ns0:v>1.5</ns0:v>
+      </ns0:c>
+      <ns0:c r="F24" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Maximum multiplier at full intensity (min is always 1.0x).</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="25"/>
+    <ns0:row r="26">
+      <ns0:c r="A26" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B24" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerBasicKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C24" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D24" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F24" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Trigger on any enemy kill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="25">
-      <ns0:c r="A25" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B25" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerThrownImpactKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C25" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D25" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F25" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="26">
-      <ns0:c r="A26" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryTriggers</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B26" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>TriggerCriticalKill</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C26" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D26" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>On</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F26" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -731,7 +725,7 @@
       </ns0:c>
       <ns0:c r="B27" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDismemberment</ns0:t>
+          <ns0:t>TriggerBasicKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C27" t="inlineStr" s="6">
@@ -746,7 +740,7 @@
       </ns0:c>
       <ns0:c r="F27" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when severing limbs</ns0:t>
+          <ns0:t>Trigger on any enemy kill</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -758,7 +752,7 @@
       </ns0:c>
       <ns0:c r="B28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerDecapitation</ns0:t>
+          <ns0:t>TriggerThrownImpactKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C28" t="inlineStr" s="6">
@@ -768,12 +762,12 @@
       </ns0:c>
       <ns0:c r="D28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>On</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F28" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on decapitation</ns0:t>
+          <ns0:t>Also trigger Basic Kill when a recently thrown enemy dies from the environment</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -785,7 +779,7 @@
       </ns0:c>
       <ns0:c r="B29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastEnemy</ns0:t>
+          <ns0:t>TriggerCriticalKill</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C29" t="inlineStr" s="6">
@@ -800,7 +794,7 @@
       </ns0:c>
       <ns0:c r="F29" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+          <ns0:t>Trigger on head/throat kills</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -812,7 +806,7 @@
       </ns0:c>
       <ns0:c r="B30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerLastStand</ns0:t>
+          <ns0:t>TriggerDismemberment</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C30" t="inlineStr" s="6">
@@ -827,7 +821,7 @@
       </ns0:c>
       <ns0:c r="F30" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger when your health drops critically low</ns0:t>
+          <ns0:t>Trigger when severing limbs</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -839,27 +833,22 @@
       </ns0:c>
       <ns0:c r="B31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionLastStandThreshold</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C31" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>TriggerDecapitation</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C31" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>15%</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E31" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+          <ns0:t>On</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F31" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Health % to trigger Last Stand</ns0:t>
+          <ns0:t>Trigger on decapitation</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -871,7 +860,7 @@
       </ns0:c>
       <ns0:c r="B32" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>TriggerParry</ns0:t>
+          <ns0:t>TriggerLastEnemy</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C32" t="inlineStr" s="6">
@@ -886,106 +875,101 @@
       </ns0:c>
       <ns0:c r="F32" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Trigger on successful weapon deflections</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="33"/>
+          <ns0:t>Trigger when killing the final enemy of a wave</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="33">
+      <ns0:c r="A33" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B33" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerLastStand</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C33" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D33" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F33" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger when your health drops critically low</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="34">
-      <ns0:c r="A34" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
+      <ns0:c r="A34" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B34" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionLastStandThreshold</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C34" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D34" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>15%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E34" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>10% | 15% | 20% | 25% | 30%</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F34" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Health % to trigger Last Stand</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="35">
       <ns0:c r="A35" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryTriggers</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B35" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>TriggerParry</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C35" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D35" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>On</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F35" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Trigger on successful weapon deflections</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="36"/>
+    <ns0:row r="37">
+      <ns0:c r="A37" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B35" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCameraDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C35" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D35" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>3m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E35" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F35" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Distance from target</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="36">
-      <ns0:c r="A36" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B36" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionRandomizeDistance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C36" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D36" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F36" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Randomize distance per killcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="37">
-      <ns0:c r="A37" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryKillcam</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B37" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCameraHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C37" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D37" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1.5m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E37" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>1m | 1.5m | 2m</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="F37" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Height offset</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -997,22 +981,27 @@
       </ns0:c>
       <ns0:c r="B38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionRandomizeHeight</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C38" t="inlineStr" s="6">
-        <ns0:is>
-          <ns0:t>Toggle</ns0:t>
+          <ns0:t>OptionCameraDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C38" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Off</ns0:t>
+          <ns0:t>3m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E38" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>2m | 3m | 4m | 5m</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F38" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Randomize height per killcam</ns0:t>
+          <ns0:t>Distance from target</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1024,110 +1013,121 @@
       </ns0:c>
       <ns0:c r="B39" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionOrbitSpeed</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C39" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
+          <ns0:t>OptionRandomizeDistance</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C39" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="D39" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Slow</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E39" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+          <ns0:t>Off</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="F39" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="40"/>
+          <ns0:t>Randomize distance per killcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="40">
+      <ns0:c r="A40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCameraHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C40" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1.5m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>1m | 1.5m | 2m</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F40" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Height offset</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="41">
-      <ns0:c r="A41" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
+      <ns0:c r="A41" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B41" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionRandomizeHeight</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C41" t="inlineStr" s="6">
+        <ns0:is>
+          <ns0:t>Toggle</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D41" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F41" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Randomize height per killcam</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="42">
       <ns0:c r="A42" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryKillcam</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B42" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionOrbitSpeed</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C42" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D42" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Slow</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E42" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>None | Slow | Medium | Fast</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F42" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Camera rotation speed (0 for static)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="43"/>
+    <ns0:row r="44">
+      <ns0:c r="A44" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B42" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionBasicChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C42" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D42" s="4">
-        <ns0:v>0.25</ns0:v>
-      </ns0:c>
-      <ns0:c r="F42" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="43">
-      <ns0:c r="A43" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B43" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionBasicTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C43" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D43" s="4">
-        <ns0:v>0.28</ns0:v>
-      </ns0:c>
-      <ns0:c r="F43" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="44">
-      <ns0:c r="A44" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomBasic</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B44" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionBasicDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C44" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D44" s="4">
-        <ns0:v>2.5</ns0:v>
-      </ns0:c>
-      <ns0:c r="F44" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1139,7 +1139,7 @@
       </ns0:c>
       <ns0:c r="B45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicCooldown</ns0:t>
+          <ns0:t>OptionBasicChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C45" t="inlineStr" s="7">
@@ -1148,16 +1148,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D45" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E45" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.25</ns0:v>
       </ns0:c>
       <ns0:c r="F45" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1169,27 +1164,20 @@
       </ns0:c>
       <ns0:c r="B46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C46" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D46" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E46" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionBasicTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C46" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D46" s="4">
+        <ns0:v>0.28</ns0:v>
       </ns0:c>
       <ns0:c r="F46" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1201,7 +1189,7 @@
       </ns0:c>
       <ns0:c r="B47" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionBasicThirdPerson</ns0:t>
+          <ns0:t>OptionBasicDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C47" t="inlineStr" s="7">
@@ -1209,102 +1197,114 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D47" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E47" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D47" s="4">
+        <ns0:v>2.5</ns0:v>
       </ns0:c>
       <ns0:c r="F47" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="48"/>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="48">
+      <ns0:c r="A48" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B48" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionBasicCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C48" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D48" s="4">
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E48" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F48" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Cooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
     <ns0:row r="49">
-      <ns0:c r="A49" t="inlineStr" s="2">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
+      <ns0:c r="A49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionBasicTransition</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C49" t="inlineStr" s="8">
+        <ns0:is>
+          <ns0:t>Dropdown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Smoothstep</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off | Smoothstep | Linear</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F49" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
     <ns0:row r="50">
       <ns0:c r="A50" t="inlineStr" s="4">
         <ns0:is>
+          <ns0:t>CategoryCustomBasic</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionBasicThirdPerson</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C50" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="E50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F50" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="51"/>
+    <ns0:row r="52">
+      <ns0:c r="A52" t="inlineStr" s="2">
+        <ns0:is>
           <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B50" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCriticalChance</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C50" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D50" s="4">
-        <ns0:v>0.75</ns0:v>
-      </ns0:c>
-      <ns0:c r="F50" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Chance to trigger</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="51">
-      <ns0:c r="A51" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B51" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCriticalTimeScale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C51" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D51" s="4">
-        <ns0:v>0.25</ns0:v>
-      </ns0:c>
-      <ns0:c r="F51" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Time scale</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="52">
-      <ns0:c r="A52" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>CategoryCustomCritical</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="B52" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>OptionCriticalDuration</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C52" t="inlineStr" s="7">
-        <ns0:is>
-          <ns0:t>Slider</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D52" s="4">
-        <ns0:v>3.0</ns0:v>
-      </ns0:c>
-      <ns0:c r="F52" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Duration</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1316,7 +1316,7 @@
       </ns0:c>
       <ns0:c r="B53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalCooldown</ns0:t>
+          <ns0:t>OptionCriticalChance</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C53" t="inlineStr" s="7">
@@ -1325,16 +1325,11 @@
         </ns0:is>
       </ns0:c>
       <ns0:c r="D53" s="4">
-        <ns0:v>10</ns0:v>
-      </ns0:c>
-      <ns0:c r="E53" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>0s</ns0:t>
-        </ns0:is>
+        <ns0:v>0.75</ns0:v>
       </ns0:c>
       <ns0:c r="F53" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Cooldown</ns0:t>
+          <ns0:t>Chance to trigger</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1346,27 +1341,20 @@
       </ns0:c>
       <ns0:c r="B54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalTransition</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="C54" t="inlineStr" s="8">
-        <ns0:is>
-          <ns0:t>Dropdown</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="D54" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Smoothstep</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E54" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off | Smoothstep | Linear</ns0:t>
-        </ns0:is>
+          <ns0:t>OptionCriticalTimeScale</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C54" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D54" s="4">
+        <ns0:v>0.25</ns0:v>
       </ns0:c>
       <ns0:c r="F54" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Transition curve (20% of duration). Off = instant.</ns0:t>
+          <ns0:t>Time scale</ns0:t>
         </ns0:is>
       </ns0:c>
     </ns0:row>
@@ -1378,7 +1366,7 @@
       </ns0:c>
       <ns0:c r="B55" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>OptionCriticalThirdPerson</ns0:t>
+          <ns0:t>OptionCriticalDuration</ns0:t>
         </ns0:is>
       </ns0:c>
       <ns0:c r="C55" t="inlineStr" s="7">
@@ -1386,102 +1374,114 @@
           <ns0:t>Slider</ns0:t>
         </ns0:is>
       </ns0:c>
-      <ns0:c r="D55" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-      <ns0:c r="E55" t="inlineStr" s="4">
-        <ns0:is>
-          <ns0:t>Off (0%) | Rare (40%) | Mixed (100%) | Frequent (140%) | Always (10000%)</ns0:t>
-        </ns0:is>
+      <ns0:c r="D55" s="4">
+        <ns0:v>3.0</ns0:v>
       </ns0:c>
       <ns0:c r="F55" t="inlineStr" s="4">
         <ns0:is>
-          <ns0:t>Third-person killcam frequency multiplier (0% disables)</ns0:t>
-        </ns0:is>
-      </ns0:c>
-    </ns0:row>
-    <ns0:row r="56"/>
+          <ns0:t>Duration</ns0:t>
+        </ns0:is>
+      </ns0:c>
+    </ns0:row>
+    <ns0:row r="56">
+      <ns0:c r="A56" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>CategoryCustomCritical</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="B56" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>OptionCriticalCooldown</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="C56" t="inlineStr" s="7">
+        <ns0:is>
+          <ns0:t>Slider</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="D56" s="4">
+        <ns0:v>10</ns0:v>
+      </ns0:c>
+      <ns0:c r="E56" t="inlineStr" s="4">
+        <ns0:is>
+          <ns0:t>0s</ns0:t>
+        </ns0:is>
+      </ns0:c>
+      <ns0:c r="F56" t="inlineStr" s="4">
+        <ns0:i